<commit_message>
Set GREET2022 as default (the results are not correct yet)
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Box\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2BE5A9-2824-4951-A9EF-6700528FA6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA65358D-D145-47F4-AF7B-4A135BD2342B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="11" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -287,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="352">
   <si>
     <t>Diesel</t>
   </si>
@@ -1343,9 +1343,6 @@
   </si>
   <si>
     <t>from EF: Heavy Heavy-Duty Truck: grams per MMBtu</t>
-  </si>
-  <si>
-    <t>Hydrogen, CO2 from RNG tab (including all the carbon in the NG feedstock. C loss in VOC and CO are not considered here)</t>
   </si>
 </sst>
 </file>
@@ -1646,7 +1643,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1883,9 +1880,6 @@
     <xf numFmtId="3" fontId="2" fillId="16" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="168" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1900,10 +1894,10 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1944,7 +1938,6 @@
       <sheetName val="RNG"/>
       <sheetName val="Pyrolysis_IDL"/>
       <sheetName val="IBR"/>
-      <sheetName val="Fuel_Specs"/>
       <sheetName val="PTF"/>
       <sheetName val="E_fuel"/>
       <sheetName val="Fuel_Prod_TS"/>
@@ -1952,6 +1945,7 @@
       <sheetName val="AgMining_EF_TS"/>
       <sheetName val="EF"/>
       <sheetName val="WCF"/>
+      <sheetName val="Fuel_Specs"/>
       <sheetName val="Car_TS"/>
       <sheetName val="LDT1_TS"/>
       <sheetName val="LDT2_TS"/>
@@ -2004,7 +1998,14 @@
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
-      <sheetData sheetId="17">
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24">
         <row r="171">
           <cell r="C171">
             <v>1000</v>
@@ -2027,13 +2028,6 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
       <sheetData sheetId="25"/>
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
@@ -2613,11 +2607,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
-  <dimension ref="A1:AY24"/>
+  <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AB1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH4" sqref="AH4:AH21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2628,155 +2622,155 @@
     <col min="41" max="41" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="122" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="124" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="123" t="s">
+    <row r="1" spans="1:51" s="121" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="123" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="123" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="123" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="123" t="s">
+      <c r="K1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="123" t="s">
+      <c r="L1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="123" t="s">
+      <c r="M1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="N1" s="123" t="s">
+      <c r="N1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="123" t="s">
+      <c r="O1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="123" t="s">
+      <c r="P1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="123" t="s">
+      <c r="Q1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="123" t="s">
+      <c r="R1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="123" t="s">
+      <c r="S1" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="T1" s="123" t="s">
+      <c r="T1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="U1" s="123" t="s">
+      <c r="U1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="V1" s="123" t="s">
+      <c r="V1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="W1" s="123" t="s">
+      <c r="W1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="X1" s="123" t="s">
+      <c r="X1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="Y1" s="123" t="s">
+      <c r="Y1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="Z1" s="123" t="s">
+      <c r="Z1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="AA1" s="123" t="s">
+      <c r="AA1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="AB1" s="123" t="s">
+      <c r="AB1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="AC1" s="123" t="s">
+      <c r="AC1" s="122" t="s">
         <v>287</v>
       </c>
-      <c r="AD1" s="125" t="s">
+      <c r="AD1" s="124" t="s">
         <v>261</v>
       </c>
-      <c r="AE1" s="125" t="s">
+      <c r="AE1" s="124" t="s">
         <v>37</v>
       </c>
       <c r="AF1" s="113" t="s">
         <v>265</v>
       </c>
-      <c r="AG1" s="126" t="s">
+      <c r="AG1" s="125" t="s">
         <v>264</v>
       </c>
-      <c r="AH1" s="123" t="s">
+      <c r="AH1" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="AI1" s="123" t="s">
+      <c r="AI1" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="AJ1" s="123" t="s">
+      <c r="AJ1" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="AK1" s="123" t="s">
+      <c r="AK1" s="122" t="s">
         <v>208</v>
       </c>
-      <c r="AL1" s="123" t="s">
+      <c r="AL1" s="122" t="s">
         <v>208</v>
       </c>
-      <c r="AM1" s="123" t="s">
+      <c r="AM1" s="122" t="s">
         <v>208</v>
       </c>
-      <c r="AN1" s="123" t="s">
+      <c r="AN1" s="122" t="s">
         <v>292</v>
       </c>
-      <c r="AO1" s="123" t="s">
+      <c r="AO1" s="122" t="s">
         <v>292</v>
       </c>
-      <c r="AP1" s="123" t="s">
+      <c r="AP1" s="122" t="s">
         <v>292</v>
       </c>
-      <c r="AQ1" s="123" t="s">
+      <c r="AQ1" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="AR1" s="123" t="s">
+      <c r="AR1" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="AS1" s="123" t="s">
+      <c r="AS1" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="AT1" s="123" t="s">
+      <c r="AT1" s="122" t="s">
         <v>324</v>
       </c>
-      <c r="AU1" s="123" t="s">
+      <c r="AU1" s="122" t="s">
         <v>324</v>
       </c>
-      <c r="AV1" s="123" t="s">
+      <c r="AV1" s="122" t="s">
         <v>324</v>
       </c>
-      <c r="AW1" s="123" t="s">
+      <c r="AW1" s="122" t="s">
         <v>325</v>
       </c>
-      <c r="AX1" s="123" t="s">
+      <c r="AX1" s="122" t="s">
         <v>325</v>
       </c>
-      <c r="AY1" s="123" t="s">
+      <c r="AY1" s="122" t="s">
         <v>325</v>
       </c>
     </row>
@@ -3179,7 +3173,7 @@
       <c r="AE4" s="115"/>
       <c r="AF4" s="116"/>
       <c r="AG4" s="116"/>
-      <c r="AH4" s="127">
+      <c r="AH4" s="2">
         <v>1000000</v>
       </c>
       <c r="AI4" s="51">
@@ -3340,7 +3334,7 @@
       <c r="AE5" s="115"/>
       <c r="AF5" s="116"/>
       <c r="AG5" s="116"/>
-      <c r="AH5" s="127">
+      <c r="AH5" s="2">
         <v>0</v>
       </c>
       <c r="AI5" s="51">
@@ -3501,7 +3495,7 @@
       <c r="AE6" s="115"/>
       <c r="AF6" s="116"/>
       <c r="AG6" s="116"/>
-      <c r="AH6" s="127">
+      <c r="AH6" s="2">
         <v>0</v>
       </c>
       <c r="AI6" s="51">
@@ -3662,7 +3656,7 @@
       <c r="AE7" s="115"/>
       <c r="AF7" s="116"/>
       <c r="AG7" s="116"/>
-      <c r="AH7" s="127">
+      <c r="AH7" s="2">
         <v>0</v>
       </c>
       <c r="AI7" s="51">
@@ -3823,7 +3817,7 @@
       <c r="AE8" s="115"/>
       <c r="AF8" s="116"/>
       <c r="AG8" s="116"/>
-      <c r="AH8" s="127">
+      <c r="AH8" s="2">
         <v>0</v>
       </c>
       <c r="AI8" s="51">
@@ -3984,7 +3978,7 @@
       <c r="AE9" s="115"/>
       <c r="AF9" s="116"/>
       <c r="AG9" s="116"/>
-      <c r="AH9" s="127">
+      <c r="AH9" s="2">
         <v>0</v>
       </c>
       <c r="AI9" s="51">
@@ -4145,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="AE10" s="117"/>
-      <c r="AH10" s="128">
+      <c r="AH10">
         <v>53.59747463028841</v>
       </c>
       <c r="AI10" s="51">
@@ -4306,7 +4300,7 @@
         <v>0</v>
       </c>
       <c r="AE11" s="117"/>
-      <c r="AH11" s="128">
+      <c r="AH11">
         <v>639.10415070792988</v>
       </c>
       <c r="AI11" s="51">
@@ -4467,7 +4461,7 @@
         <v>0</v>
       </c>
       <c r="AE12" s="117"/>
-      <c r="AH12" s="128">
+      <c r="AH12">
         <v>19.208734314891956</v>
       </c>
       <c r="AI12" s="51">
@@ -4628,7 +4622,7 @@
         <v>0</v>
       </c>
       <c r="AE13" s="117"/>
-      <c r="AH13" s="128">
+      <c r="AH13">
         <v>8.0441472410106218</v>
       </c>
       <c r="AI13" s="51">
@@ -4789,7 +4783,7 @@
         <v>0</v>
       </c>
       <c r="AE14" s="117"/>
-      <c r="AH14" s="128">
+      <c r="AH14">
         <v>1.728649515788488</v>
       </c>
       <c r="AI14" s="51">
@@ -4950,7 +4944,7 @@
         <v>0</v>
       </c>
       <c r="AE15" s="117"/>
-      <c r="AH15" s="128">
+      <c r="AH15">
         <v>0.47886752155609885</v>
       </c>
       <c r="AI15" s="51">
@@ -5107,7 +5101,7 @@
         <v>0</v>
       </c>
       <c r="AE16" s="117"/>
-      <c r="AH16" s="128">
+      <c r="AH16">
         <v>0.47390947465623479</v>
       </c>
       <c r="AI16" s="51">
@@ -5264,7 +5258,7 @@
         <v>0</v>
       </c>
       <c r="AE17" s="117"/>
-      <c r="AH17" s="128">
+      <c r="AH17">
         <v>0.24585827527712426</v>
       </c>
       <c r="AI17" s="51">
@@ -5421,7 +5415,7 @@
         <v>0</v>
       </c>
       <c r="AE18" s="117"/>
-      <c r="AH18" s="128">
+      <c r="AH18">
         <v>3.4141251927898666</v>
       </c>
       <c r="AI18" s="51">
@@ -5578,7 +5572,7 @@
         <v>0</v>
       </c>
       <c r="AE19" s="117"/>
-      <c r="AH19" s="128">
+      <c r="AH19">
         <v>0.91142919415811929</v>
       </c>
       <c r="AI19" s="51">
@@ -5751,7 +5745,7 @@
         <f>-12*6/(12*6+8*1+5*16)*44/12</f>
         <v>-1.6500000000000001</v>
       </c>
-      <c r="AH20" s="128">
+      <c r="AH20">
         <v>71783.505317547926</v>
       </c>
       <c r="AI20" s="51">
@@ -5873,7 +5867,7 @@
       <c r="AC21" s="46">
         <v>-59412.682265174641</v>
       </c>
-      <c r="AH21" s="128">
+      <c r="AH21">
         <v>-72964.246146966863</v>
       </c>
       <c r="AJ21">
@@ -5928,27 +5922,59 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="121" t="s">
+      <c r="B23" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
-      <c r="G23" s="121"/>
-      <c r="H23" s="121"/>
-      <c r="I23" s="121"/>
-      <c r="J23" s="121"/>
-      <c r="K23" s="121"/>
-      <c r="L23" s="121"/>
-      <c r="M23" s="121"/>
-      <c r="N23" s="121"/>
-      <c r="O23" s="121"/>
-      <c r="P23" s="121"/>
-      <c r="Q23" s="121"/>
-      <c r="R23" s="121"/>
-      <c r="S23" s="17" t="s">
-        <v>352</v>
+      <c r="C23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" t="s">
+        <v>351</v>
+      </c>
+      <c r="H23" t="s">
+        <v>351</v>
+      </c>
+      <c r="I23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="J23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="L23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="M23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="O23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="P23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" s="127" t="s">
+        <v>15</v>
+      </c>
+      <c r="S23" s="127" t="s">
+        <v>15</v>
       </c>
       <c r="T23" s="17" t="s">
         <v>289</v>
@@ -5978,18 +6004,7 @@
       </c>
       <c r="AP23" s="51"/>
     </row>
-    <row r="24" spans="1:51" x14ac:dyDescent="0.35">
-      <c r="G24" t="s">
-        <v>351</v>
-      </c>
-      <c r="H24" t="s">
-        <v>351</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B23:R23"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6535,8 +6550,8 @@
   </sheetPr>
   <dimension ref="A1:CF9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9806,11 +9821,11 @@
       <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="121" t="s">
+      <c r="C30" s="126" t="s">
         <v>337</v>
       </c>
-      <c r="D30" s="121"/>
-      <c r="E30" s="121"/>
+      <c r="D30" s="126"/>
+      <c r="E30" s="126"/>
       <c r="G30" s="17" t="s">
         <v>288</v>
       </c>
@@ -15598,39 +15613,39 @@
       <c r="A29" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="121" t="s">
+      <c r="B29" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="121"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="121"/>
-      <c r="I29" s="121"/>
-      <c r="J29" s="121"/>
-      <c r="K29" s="121"/>
-      <c r="L29" s="121"/>
-      <c r="M29" s="121"/>
-      <c r="N29" s="121"/>
-      <c r="O29" s="121"/>
-      <c r="P29" s="121"/>
-      <c r="Q29" s="121"/>
-      <c r="R29" s="121"/>
-      <c r="S29" s="121"/>
-      <c r="T29" s="121"/>
-      <c r="U29" s="121"/>
-      <c r="V29" s="121"/>
-      <c r="W29" s="121"/>
-      <c r="X29" s="121"/>
-      <c r="Y29" s="121"/>
-      <c r="Z29" s="121"/>
-      <c r="AA29" s="121"/>
-      <c r="AB29" s="121"/>
-      <c r="AC29" s="121"/>
-      <c r="AD29" s="121"/>
-      <c r="AE29" s="121"/>
-      <c r="AF29" s="121"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
+      <c r="H29" s="126"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="126"/>
+      <c r="K29" s="126"/>
+      <c r="L29" s="126"/>
+      <c r="M29" s="126"/>
+      <c r="N29" s="126"/>
+      <c r="O29" s="126"/>
+      <c r="P29" s="126"/>
+      <c r="Q29" s="126"/>
+      <c r="R29" s="126"/>
+      <c r="S29" s="126"/>
+      <c r="T29" s="126"/>
+      <c r="U29" s="126"/>
+      <c r="V29" s="126"/>
+      <c r="W29" s="126"/>
+      <c r="X29" s="126"/>
+      <c r="Y29" s="126"/>
+      <c r="Z29" s="126"/>
+      <c r="AA29" s="126"/>
+      <c r="AB29" s="126"/>
+      <c r="AC29" s="126"/>
+      <c r="AD29" s="126"/>
+      <c r="AE29" s="126"/>
+      <c r="AF29" s="126"/>
       <c r="AH29" s="92" t="s">
         <v>340</v>
       </c>
@@ -16799,22 +16814,22 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="121" t="s">
+      <c r="B23" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
-      <c r="G23" s="121"/>
-      <c r="H23" s="121"/>
-      <c r="I23" s="121"/>
-      <c r="J23" s="121"/>
-      <c r="K23" s="121"/>
-      <c r="L23" s="121"/>
-      <c r="M23" s="121"/>
-      <c r="N23" s="121"/>
-      <c r="O23" s="121"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="126"/>
+      <c r="I23" s="126"/>
+      <c r="J23" s="126"/>
+      <c r="K23" s="126"/>
+      <c r="L23" s="126"/>
+      <c r="M23" s="126"/>
+      <c r="N23" s="126"/>
+      <c r="O23" s="126"/>
       <c r="P23" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Fixed errors in the lookup_table file for GREET2022
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA65358D-D145-47F4-AF7B-4A135BD2342B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E88364-0692-422B-A300-DE6CA8E11E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="745" activeTab="1" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
-    <sheet name="Production" sheetId="2" r:id="rId2"/>
-    <sheet name="Chemicals" sheetId="5" r:id="rId3"/>
-    <sheet name="End use" sheetId="3" state="hidden" r:id="rId4"/>
-    <sheet name="Feedstock" sheetId="15" r:id="rId5"/>
-    <sheet name="Units" sheetId="10" r:id="rId6"/>
-    <sheet name="Fuel specs" sheetId="11" r:id="rId7"/>
-    <sheet name="Mass" sheetId="6" r:id="rId8"/>
-    <sheet name="Volume" sheetId="7" r:id="rId9"/>
-    <sheet name="Energy" sheetId="8" r:id="rId10"/>
-    <sheet name="Length" sheetId="9" r:id="rId11"/>
-    <sheet name="Transportation" sheetId="12" r:id="rId12"/>
+    <sheet name="End use supplement" sheetId="16" r:id="rId2"/>
+    <sheet name="Production" sheetId="2" r:id="rId3"/>
+    <sheet name="Chemicals" sheetId="5" r:id="rId4"/>
+    <sheet name="End use" sheetId="3" state="hidden" r:id="rId5"/>
+    <sheet name="Feedstock" sheetId="15" r:id="rId6"/>
+    <sheet name="Units" sheetId="10" r:id="rId7"/>
+    <sheet name="Fuel specs" sheetId="11" r:id="rId8"/>
+    <sheet name="Mass" sheetId="6" r:id="rId9"/>
+    <sheet name="Volume" sheetId="7" r:id="rId10"/>
+    <sheet name="Energy" sheetId="8" r:id="rId11"/>
+    <sheet name="Length" sheetId="9" r:id="rId12"/>
+    <sheet name="Transportation" sheetId="12" r:id="rId13"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="g2T">[1]Fuel_Specs!$B$175</definedName>
@@ -287,7 +288,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="344">
   <si>
     <t>Diesel</t>
   </si>
@@ -1313,30 +1314,6 @@
   </si>
   <si>
     <t>Functional Unit</t>
-  </si>
-  <si>
-    <t>Low-sulfur diesel</t>
-  </si>
-  <si>
-    <t>EtOH-Diesel Additives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isoalkane from waste feedstock </t>
-  </si>
-  <si>
-    <t>Fatty alkyl ether (FAE)</t>
-  </si>
-  <si>
-    <t>FAFE (Fatty acid fusel ester)</t>
-  </si>
-  <si>
-    <t>HTL - Partial Upgrading (Sludge)</t>
-  </si>
-  <si>
-    <t>HTL - Partial Upgrading (Manure)</t>
-  </si>
-  <si>
-    <t>FP (Biomass)</t>
   </si>
   <si>
     <t>Algae Biomass</t>
@@ -1897,7 +1874,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1981,31 +1958,31 @@
       <sheetName val="Forecast_Deleted"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24">
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1">
         <row r="171">
           <cell r="C171">
             <v>1000</v>
@@ -2028,39 +2005,39 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2609,9 +2586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H23" sqref="H23"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AH1" sqref="AH1:AY21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3176,22 +3153,22 @@
       <c r="AH4" s="2">
         <v>1000000</v>
       </c>
-      <c r="AI4" s="51">
-        <v>9216.8702699702171</v>
+      <c r="AI4" s="127">
+        <v>9339.5518419730979</v>
       </c>
       <c r="AJ4">
         <f t="shared" ref="AJ4:AJ10" si="0">AH4+AI4</f>
-        <v>1009216.8702699703</v>
+        <v>1009339.5518419731</v>
       </c>
       <c r="AK4" s="2">
         <v>1000000</v>
       </c>
-      <c r="AL4" s="51">
-        <v>1250.309002469897</v>
+      <c r="AL4" s="127">
+        <v>1253.7917044079659</v>
       </c>
       <c r="AM4">
         <f>AK4+AL4</f>
-        <v>1001250.3090024699</v>
+        <v>1001253.791704408</v>
       </c>
       <c r="AN4" s="2">
         <f>AK4</f>
@@ -3199,11 +3176,11 @@
       </c>
       <c r="AO4">
         <f>AL4</f>
-        <v>1250.309002469897</v>
+        <v>1253.7917044079659</v>
       </c>
       <c r="AP4">
         <f>AN4+AO4</f>
-        <v>1001250.3090024699</v>
+        <v>1001253.791704408</v>
       </c>
       <c r="AQ4" s="2">
         <f>AN4</f>
@@ -3211,11 +3188,11 @@
       </c>
       <c r="AR4">
         <f>AL4</f>
-        <v>1250.309002469897</v>
+        <v>1253.7917044079659</v>
       </c>
       <c r="AS4">
         <f>AQ4+AR4</f>
-        <v>1001250.3090024699</v>
+        <v>1001253.791704408</v>
       </c>
       <c r="AT4" s="2">
         <f>AK4</f>
@@ -3223,11 +3200,11 @@
       </c>
       <c r="AU4">
         <f>AL4</f>
-        <v>1250.309002469897</v>
+        <v>1253.7917044079659</v>
       </c>
       <c r="AV4">
         <f>AT4+AU4</f>
-        <v>1001250.3090024699</v>
+        <v>1001253.791704408</v>
       </c>
       <c r="AW4" s="2">
         <f>AK4</f>
@@ -3235,11 +3212,11 @@
       </c>
       <c r="AX4">
         <f>AL4</f>
-        <v>1250.309002469897</v>
+        <v>1253.7917044079659</v>
       </c>
       <c r="AY4">
         <f>AW4+AX4</f>
-        <v>1001250.3090024699</v>
+        <v>1001253.791704408</v>
       </c>
     </row>
     <row r="5" spans="1:51" x14ac:dyDescent="0.35">
@@ -3337,22 +3314,22 @@
       <c r="AH5" s="2">
         <v>0</v>
       </c>
-      <c r="AI5" s="51">
-        <v>8027.464959570797</v>
+      <c r="AI5" s="127">
+        <v>8169.6873553428004</v>
       </c>
       <c r="AJ5">
         <f t="shared" si="0"/>
-        <v>8027.464959570797</v>
+        <v>8169.6873553428004</v>
       </c>
       <c r="AK5" s="2">
         <v>0</v>
       </c>
-      <c r="AL5" s="51">
-        <v>1199.1725344773329</v>
+      <c r="AL5" s="127">
+        <v>1202.5975456032124</v>
       </c>
       <c r="AM5">
         <f t="shared" ref="AM5:AM9" si="1">AK5+AL5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AN5" s="2">
         <f t="shared" ref="AN5:AN21" si="2">AK5</f>
@@ -3360,11 +3337,11 @@
       </c>
       <c r="AO5">
         <f t="shared" ref="AO5:AO20" si="3">AL5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AP5">
         <f t="shared" ref="AP5:AP9" si="4">AN5+AO5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AQ5" s="2">
         <f t="shared" ref="AQ5:AQ21" si="5">AN5</f>
@@ -3372,11 +3349,11 @@
       </c>
       <c r="AR5">
         <f t="shared" ref="AR5:AR20" si="6">AL5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AS5">
         <f t="shared" ref="AS5:AS9" si="7">AQ5+AR5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AT5" s="2">
         <f t="shared" ref="AT5:AT21" si="8">AK5</f>
@@ -3384,11 +3361,11 @@
       </c>
       <c r="AU5">
         <f t="shared" ref="AU5:AU20" si="9">AL5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AV5">
         <f t="shared" ref="AV5:AV9" si="10">AT5+AU5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AW5" s="2">
         <f t="shared" ref="AW5:AW21" si="11">AK5</f>
@@ -3396,11 +3373,11 @@
       </c>
       <c r="AX5">
         <f t="shared" ref="AX5:AX20" si="12">AL5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
       <c r="AY5">
         <f t="shared" ref="AY5:AY9" si="13">AW5+AX5</f>
-        <v>1199.1725344773329</v>
+        <v>1202.5975456032124</v>
       </c>
     </row>
     <row r="6" spans="1:51" x14ac:dyDescent="0.35">
@@ -3498,22 +3475,22 @@
       <c r="AH6" s="2">
         <v>0</v>
       </c>
-      <c r="AI6" s="51">
-        <v>1664.7217341019561</v>
+      <c r="AI6" s="127">
+        <v>1989.4630119087635</v>
       </c>
       <c r="AJ6">
         <f t="shared" si="0"/>
-        <v>1664.7217341019561</v>
+        <v>1989.4630119087635</v>
       </c>
       <c r="AK6" s="2">
         <v>0</v>
       </c>
-      <c r="AL6" s="51">
-        <v>8.0912620107395146</v>
+      <c r="AL6" s="127">
+        <v>9.9730961197564767</v>
       </c>
       <c r="AM6">
         <f t="shared" si="1"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AN6" s="2">
         <f t="shared" si="2"/>
@@ -3521,11 +3498,11 @@
       </c>
       <c r="AO6">
         <f t="shared" si="3"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AP6">
         <f t="shared" si="4"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AQ6" s="2">
         <f t="shared" si="5"/>
@@ -3533,11 +3510,11 @@
       </c>
       <c r="AR6">
         <f t="shared" si="6"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AS6">
         <f t="shared" si="7"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AT6" s="2">
         <f t="shared" si="8"/>
@@ -3545,11 +3522,11 @@
       </c>
       <c r="AU6">
         <f t="shared" si="9"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AV6">
         <f t="shared" si="10"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AW6" s="2">
         <f t="shared" si="11"/>
@@ -3557,11 +3534,11 @@
       </c>
       <c r="AX6">
         <f t="shared" si="12"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
       <c r="AY6">
         <f t="shared" si="13"/>
-        <v>8.0912620107395146</v>
+        <v>9.9730961197564767</v>
       </c>
     </row>
     <row r="7" spans="1:51" x14ac:dyDescent="0.35">
@@ -3659,22 +3636,22 @@
       <c r="AH7" s="2">
         <v>0</v>
       </c>
-      <c r="AI7" s="51">
-        <v>2963.4305044075732</v>
+      <c r="AI7" s="127">
+        <v>2794.9003158789556</v>
       </c>
       <c r="AJ7">
         <f t="shared" si="0"/>
-        <v>2963.4305044075732</v>
+        <v>2794.9003158789556</v>
       </c>
       <c r="AK7" s="2">
         <v>0</v>
       </c>
-      <c r="AL7" s="51">
-        <v>124.60248498831356</v>
+      <c r="AL7" s="127">
+        <v>126.35657670942828</v>
       </c>
       <c r="AM7">
         <f t="shared" si="1"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AN7" s="2">
         <f t="shared" si="2"/>
@@ -3682,11 +3659,11 @@
       </c>
       <c r="AO7">
         <f t="shared" si="3"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AP7">
         <f t="shared" si="4"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AQ7" s="2">
         <f t="shared" si="5"/>
@@ -3694,11 +3671,11 @@
       </c>
       <c r="AR7">
         <f t="shared" si="6"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AS7">
         <f t="shared" si="7"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AT7" s="2">
         <f t="shared" si="8"/>
@@ -3706,11 +3683,11 @@
       </c>
       <c r="AU7">
         <f t="shared" si="9"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AV7">
         <f t="shared" si="10"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AW7" s="2">
         <f t="shared" si="11"/>
@@ -3718,11 +3695,11 @@
       </c>
       <c r="AX7">
         <f t="shared" si="12"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
       <c r="AY7">
         <f t="shared" si="13"/>
-        <v>124.60248498831356</v>
+        <v>126.35657670942828</v>
       </c>
     </row>
     <row r="8" spans="1:51" x14ac:dyDescent="0.35">
@@ -3820,22 +3797,22 @@
       <c r="AH8" s="2">
         <v>0</v>
       </c>
-      <c r="AI8" s="51">
-        <v>3399.3127210612679</v>
+      <c r="AI8" s="127">
+        <v>3385.324027555082</v>
       </c>
       <c r="AJ8">
         <f t="shared" si="0"/>
-        <v>3399.3127210612679</v>
+        <v>3385.324027555082</v>
       </c>
       <c r="AK8" s="2">
         <v>0</v>
       </c>
-      <c r="AL8" s="51">
-        <v>1066.4787874782799</v>
+      <c r="AL8" s="127">
+        <v>1066.2678727740276</v>
       </c>
       <c r="AM8">
         <f t="shared" si="1"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AN8" s="2">
         <f t="shared" si="2"/>
@@ -3843,11 +3820,11 @@
       </c>
       <c r="AO8">
         <f t="shared" si="3"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AP8">
         <f t="shared" si="4"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AQ8" s="2">
         <f t="shared" si="5"/>
@@ -3855,11 +3832,11 @@
       </c>
       <c r="AR8">
         <f t="shared" si="6"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AS8">
         <f t="shared" si="7"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AT8" s="2">
         <f t="shared" si="8"/>
@@ -3867,11 +3844,11 @@
       </c>
       <c r="AU8">
         <f t="shared" si="9"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AV8">
         <f t="shared" si="10"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AW8" s="2">
         <f t="shared" si="11"/>
@@ -3879,11 +3856,11 @@
       </c>
       <c r="AX8">
         <f t="shared" si="12"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
       <c r="AY8">
         <f t="shared" si="13"/>
-        <v>1066.4787874782799</v>
+        <v>1066.2678727740276</v>
       </c>
     </row>
     <row r="9" spans="1:51" x14ac:dyDescent="0.35">
@@ -3981,22 +3958,22 @@
       <c r="AH9" s="2">
         <v>0</v>
       </c>
-      <c r="AI9" s="51">
-        <v>0.56134131706501467</v>
+      <c r="AI9" s="127">
+        <v>0.53885408384714351</v>
       </c>
       <c r="AJ9">
         <f t="shared" si="0"/>
-        <v>0.56134131706501467</v>
+        <v>0.53885408384714351</v>
       </c>
       <c r="AK9" s="2">
         <v>0</v>
       </c>
-      <c r="AL9" s="51">
-        <v>2.3217600680931635E-2</v>
+      <c r="AL9" s="127">
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AM9">
         <f t="shared" si="1"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AN9" s="2">
         <f t="shared" si="2"/>
@@ -4004,11 +3981,11 @@
       </c>
       <c r="AO9">
         <f t="shared" si="3"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AP9">
         <f t="shared" si="4"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AQ9" s="2">
         <f t="shared" si="5"/>
@@ -4016,11 +3993,11 @@
       </c>
       <c r="AR9">
         <f t="shared" si="6"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AS9">
         <f t="shared" si="7"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AT9" s="2">
         <f t="shared" si="8"/>
@@ -4028,11 +4005,11 @@
       </c>
       <c r="AU9">
         <f t="shared" si="9"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AV9">
         <f t="shared" si="10"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AW9" s="2">
         <f t="shared" si="11"/>
@@ -4040,11 +4017,11 @@
       </c>
       <c r="AX9">
         <f t="shared" si="12"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
       <c r="AY9">
         <f t="shared" si="13"/>
-        <v>2.3217600680931635E-2</v>
+        <v>2.362854580449477E-2</v>
       </c>
     </row>
     <row r="10" spans="1:51" x14ac:dyDescent="0.35">
@@ -4142,22 +4119,22 @@
       <c r="AH10">
         <v>53.59747463028841</v>
       </c>
-      <c r="AI10" s="51">
-        <v>0.12380376798091507</v>
+      <c r="AI10" s="127">
+        <v>0.12683831523481029</v>
       </c>
       <c r="AJ10">
         <f t="shared" si="0"/>
-        <v>53.721278398269327</v>
+        <v>53.724312945523224</v>
       </c>
       <c r="AK10">
         <v>40.352647182660228</v>
       </c>
-      <c r="AL10" s="51">
-        <v>1.4111608204643369E-2</v>
+      <c r="AL10" s="127">
+        <v>1.424806237772471E-2</v>
       </c>
       <c r="AM10">
         <f>AK10+AL10</f>
-        <v>40.366758790864871</v>
+        <v>40.366895245037952</v>
       </c>
       <c r="AN10" s="2">
         <f t="shared" si="2"/>
@@ -4165,11 +4142,11 @@
       </c>
       <c r="AO10">
         <f t="shared" si="3"/>
-        <v>1.4111608204643369E-2</v>
+        <v>1.424806237772471E-2</v>
       </c>
       <c r="AP10">
         <f>AN10+AO10</f>
-        <v>40.366758790864871</v>
+        <v>40.366895245037952</v>
       </c>
       <c r="AQ10" s="2">
         <f t="shared" si="5"/>
@@ -4177,11 +4154,11 @@
       </c>
       <c r="AR10">
         <f t="shared" si="6"/>
-        <v>1.4111608204643369E-2</v>
+        <v>1.424806237772471E-2</v>
       </c>
       <c r="AS10">
         <f>AQ10+AR10</f>
-        <v>40.366758790864871</v>
+        <v>40.366895245037952</v>
       </c>
       <c r="AT10" s="2">
         <f t="shared" si="8"/>
@@ -4189,11 +4166,11 @@
       </c>
       <c r="AU10">
         <f t="shared" si="9"/>
-        <v>1.4111608204643369E-2</v>
+        <v>1.424806237772471E-2</v>
       </c>
       <c r="AV10">
         <f>AT10+AU10</f>
-        <v>40.366758790864871</v>
+        <v>40.366895245037952</v>
       </c>
       <c r="AW10" s="2">
         <f t="shared" si="11"/>
@@ -4201,11 +4178,11 @@
       </c>
       <c r="AX10">
         <f t="shared" si="12"/>
-        <v>1.4111608204643369E-2</v>
+        <v>1.424806237772471E-2</v>
       </c>
       <c r="AY10">
         <f>AW10+AX10</f>
-        <v>40.366758790864871</v>
+        <v>40.366895245037952</v>
       </c>
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.35">
@@ -4303,22 +4280,22 @@
       <c r="AH11">
         <v>639.10415070792988</v>
       </c>
-      <c r="AI11" s="51">
-        <v>0.53001711985689259</v>
+      <c r="AI11" s="127">
+        <v>0.54395091021563391</v>
       </c>
       <c r="AJ11">
         <f t="shared" ref="AJ11:AJ21" si="14">AH11+AI11</f>
-        <v>639.63416782778677</v>
+        <v>639.64810161814546</v>
       </c>
       <c r="AK11">
         <v>993.80073264760836</v>
       </c>
-      <c r="AL11" s="51">
-        <v>0.19579254162294349</v>
+      <c r="AL11" s="127">
+        <v>0.19647676496293282</v>
       </c>
       <c r="AM11">
         <f t="shared" ref="AM11:AM21" si="15">AK11+AL11</f>
-        <v>993.99652518923131</v>
+        <v>993.99720941257124</v>
       </c>
       <c r="AN11" s="2">
         <f t="shared" si="2"/>
@@ -4326,11 +4303,11 @@
       </c>
       <c r="AO11">
         <f t="shared" si="3"/>
-        <v>0.19579254162294349</v>
+        <v>0.19647676496293282</v>
       </c>
       <c r="AP11">
         <f t="shared" ref="AP11:AP21" si="16">AN11+AO11</f>
-        <v>993.99652518923131</v>
+        <v>993.99720941257124</v>
       </c>
       <c r="AQ11" s="2">
         <f t="shared" si="5"/>
@@ -4338,11 +4315,11 @@
       </c>
       <c r="AR11">
         <f t="shared" si="6"/>
-        <v>0.19579254162294349</v>
+        <v>0.19647676496293282</v>
       </c>
       <c r="AS11">
         <f t="shared" ref="AS11:AS21" si="17">AQ11+AR11</f>
-        <v>993.99652518923131</v>
+        <v>993.99720941257124</v>
       </c>
       <c r="AT11" s="2">
         <f t="shared" si="8"/>
@@ -4350,11 +4327,11 @@
       </c>
       <c r="AU11">
         <f t="shared" si="9"/>
-        <v>0.19579254162294349</v>
+        <v>0.19647676496293282</v>
       </c>
       <c r="AV11">
         <f t="shared" ref="AV11:AV21" si="18">AT11+AU11</f>
-        <v>993.99652518923131</v>
+        <v>993.99720941257124</v>
       </c>
       <c r="AW11" s="2">
         <f t="shared" si="11"/>
@@ -4362,11 +4339,11 @@
       </c>
       <c r="AX11">
         <f t="shared" si="12"/>
-        <v>0.19579254162294349</v>
+        <v>0.19647676496293282</v>
       </c>
       <c r="AY11">
         <f t="shared" ref="AY11:AY21" si="19">AW11+AX11</f>
-        <v>993.99652518923131</v>
+        <v>993.99720941257124</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.35">
@@ -4464,22 +4441,22 @@
       <c r="AH12">
         <v>19.208734314891956</v>
       </c>
-      <c r="AI12" s="51">
-        <v>1.4390708093838975</v>
+      <c r="AI12" s="127">
+        <v>1.4670490677357695</v>
       </c>
       <c r="AJ12">
         <f t="shared" si="14"/>
-        <v>20.647805124275852</v>
+        <v>20.675783382627724</v>
       </c>
       <c r="AK12">
         <v>27.387619255967515</v>
       </c>
-      <c r="AL12" s="51">
-        <v>0.13356807901983217</v>
+      <c r="AL12" s="127">
+        <v>0.13480292599982197</v>
       </c>
       <c r="AM12">
         <f t="shared" si="15"/>
-        <v>27.521187334987346</v>
+        <v>27.522422181967336</v>
       </c>
       <c r="AN12" s="2">
         <f t="shared" si="2"/>
@@ -4487,11 +4464,11 @@
       </c>
       <c r="AO12">
         <f t="shared" si="3"/>
-        <v>0.13356807901983217</v>
+        <v>0.13480292599982197</v>
       </c>
       <c r="AP12">
         <f t="shared" si="16"/>
-        <v>27.521187334987346</v>
+        <v>27.522422181967336</v>
       </c>
       <c r="AQ12" s="2">
         <f t="shared" si="5"/>
@@ -4499,11 +4476,11 @@
       </c>
       <c r="AR12">
         <f t="shared" si="6"/>
-        <v>0.13356807901983217</v>
+        <v>0.13480292599982197</v>
       </c>
       <c r="AS12">
         <f t="shared" si="17"/>
-        <v>27.521187334987346</v>
+        <v>27.522422181967336</v>
       </c>
       <c r="AT12" s="2">
         <f t="shared" si="8"/>
@@ -4511,11 +4488,11 @@
       </c>
       <c r="AU12">
         <f t="shared" si="9"/>
-        <v>0.13356807901983217</v>
+        <v>0.13480292599982197</v>
       </c>
       <c r="AV12">
         <f t="shared" si="18"/>
-        <v>27.521187334987346</v>
+        <v>27.522422181967336</v>
       </c>
       <c r="AW12" s="2">
         <f t="shared" si="11"/>
@@ -4523,11 +4500,11 @@
       </c>
       <c r="AX12">
         <f t="shared" si="12"/>
-        <v>0.13356807901983217</v>
+        <v>0.13480292599982197</v>
       </c>
       <c r="AY12">
         <f t="shared" si="19"/>
-        <v>27.521187334987346</v>
+        <v>27.522422181967336</v>
       </c>
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.35">
@@ -4625,22 +4602,22 @@
       <c r="AH13">
         <v>8.0441472410106218</v>
       </c>
-      <c r="AI13" s="51">
-        <v>6.8025222126898502E-2</v>
+      <c r="AI13" s="127">
+        <v>7.2523053711609858E-2</v>
       </c>
       <c r="AJ13">
         <f t="shared" si="14"/>
-        <v>8.1121724631375205</v>
+        <v>8.1166702947222316</v>
       </c>
       <c r="AK13">
         <v>9.458769751780995</v>
       </c>
-      <c r="AL13" s="51">
-        <v>7.5116168079741932E-3</v>
+      <c r="AL13" s="127">
+        <v>7.5690024594833967E-3</v>
       </c>
       <c r="AM13">
         <f t="shared" si="15"/>
-        <v>9.4662813685889695</v>
+        <v>9.4663387542404784</v>
       </c>
       <c r="AN13" s="2">
         <f t="shared" si="2"/>
@@ -4648,11 +4625,11 @@
       </c>
       <c r="AO13">
         <f t="shared" si="3"/>
-        <v>7.5116168079741932E-3</v>
+        <v>7.5690024594833967E-3</v>
       </c>
       <c r="AP13">
         <f t="shared" si="16"/>
-        <v>9.4662813685889695</v>
+        <v>9.4663387542404784</v>
       </c>
       <c r="AQ13" s="2">
         <f t="shared" si="5"/>
@@ -4660,11 +4637,11 @@
       </c>
       <c r="AR13">
         <f t="shared" si="6"/>
-        <v>7.5116168079741932E-3</v>
+        <v>7.5690024594833967E-3</v>
       </c>
       <c r="AS13">
         <f t="shared" si="17"/>
-        <v>9.4662813685889695</v>
+        <v>9.4663387542404784</v>
       </c>
       <c r="AT13" s="2">
         <f t="shared" si="8"/>
@@ -4672,11 +4649,11 @@
       </c>
       <c r="AU13">
         <f t="shared" si="9"/>
-        <v>7.5116168079741932E-3</v>
+        <v>7.5690024594833967E-3</v>
       </c>
       <c r="AV13">
         <f t="shared" si="18"/>
-        <v>9.4662813685889695</v>
+        <v>9.4663387542404784</v>
       </c>
       <c r="AW13" s="2">
         <f t="shared" si="11"/>
@@ -4684,11 +4661,11 @@
       </c>
       <c r="AX13">
         <f t="shared" si="12"/>
-        <v>7.5116168079741932E-3</v>
+        <v>7.5690024594833967E-3</v>
       </c>
       <c r="AY13">
         <f t="shared" si="19"/>
-        <v>9.4662813685889695</v>
+        <v>9.4663387542404784</v>
       </c>
     </row>
     <row r="14" spans="1:51" x14ac:dyDescent="0.35">
@@ -4786,22 +4763,22 @@
       <c r="AH14">
         <v>1.728649515788488</v>
       </c>
-      <c r="AI14" s="51">
-        <v>4.6442748659862865E-2</v>
+      <c r="AI14" s="127">
+        <v>4.8091315083300508E-2</v>
       </c>
       <c r="AJ14">
         <f t="shared" si="14"/>
-        <v>1.7750922644483509</v>
+        <v>1.7767408308717885</v>
       </c>
       <c r="AK14">
         <v>1.8922698715311803</v>
       </c>
-      <c r="AL14" s="51">
-        <v>2.1809956805283149E-3</v>
+      <c r="AL14" s="127">
+        <v>2.2203423357761371E-3</v>
       </c>
       <c r="AM14">
         <f t="shared" si="15"/>
-        <v>1.8944508672117086</v>
+        <v>1.8944902138669564</v>
       </c>
       <c r="AN14" s="2">
         <f t="shared" si="2"/>
@@ -4809,11 +4786,11 @@
       </c>
       <c r="AO14">
         <f t="shared" si="3"/>
-        <v>2.1809956805283149E-3</v>
+        <v>2.2203423357761371E-3</v>
       </c>
       <c r="AP14">
         <f t="shared" si="16"/>
-        <v>1.8944508672117086</v>
+        <v>1.8944902138669564</v>
       </c>
       <c r="AQ14" s="2">
         <f t="shared" si="5"/>
@@ -4821,11 +4798,11 @@
       </c>
       <c r="AR14">
         <f t="shared" si="6"/>
-        <v>2.1809956805283149E-3</v>
+        <v>2.2203423357761371E-3</v>
       </c>
       <c r="AS14">
         <f t="shared" si="17"/>
-        <v>1.8944508672117086</v>
+        <v>1.8944902138669564</v>
       </c>
       <c r="AT14" s="2">
         <f t="shared" si="8"/>
@@ -4833,11 +4810,11 @@
       </c>
       <c r="AU14">
         <f t="shared" si="9"/>
-        <v>2.1809956805283149E-3</v>
+        <v>2.2203423357761371E-3</v>
       </c>
       <c r="AV14">
         <f t="shared" si="18"/>
-        <v>1.8944508672117086</v>
+        <v>1.8944902138669564</v>
       </c>
       <c r="AW14" s="2">
         <f t="shared" si="11"/>
@@ -4845,11 +4822,11 @@
       </c>
       <c r="AX14">
         <f t="shared" si="12"/>
-        <v>2.1809956805283149E-3</v>
+        <v>2.2203423357761371E-3</v>
       </c>
       <c r="AY14">
         <f t="shared" si="19"/>
-        <v>1.8944508672117086</v>
+        <v>1.8944902138669564</v>
       </c>
     </row>
     <row r="15" spans="1:51" x14ac:dyDescent="0.35">
@@ -4947,22 +4924,22 @@
       <c r="AH15">
         <v>0.47886752155609885</v>
       </c>
-      <c r="AI15" s="51">
-        <v>0.22128373782612412</v>
+      <c r="AI15" s="127">
+        <v>0.25121575444697092</v>
       </c>
       <c r="AJ15">
         <f t="shared" si="14"/>
-        <v>0.700151259382223</v>
+        <v>0.73008327600306977</v>
       </c>
       <c r="AK15">
         <v>0</v>
       </c>
-      <c r="AL15" s="51">
-        <v>5.3987418408876558E-3</v>
+      <c r="AL15" s="127">
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AM15">
         <f t="shared" si="15"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AN15" s="2">
         <f t="shared" si="2"/>
@@ -4970,11 +4947,11 @@
       </c>
       <c r="AO15">
         <f t="shared" si="3"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AP15">
         <f t="shared" si="16"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AQ15" s="2">
         <f t="shared" si="5"/>
@@ -4982,11 +4959,11 @@
       </c>
       <c r="AR15">
         <f t="shared" si="6"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AS15">
         <f t="shared" si="17"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AT15" s="2">
         <f t="shared" si="8"/>
@@ -4994,11 +4971,11 @@
       </c>
       <c r="AU15">
         <f t="shared" si="9"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AV15">
         <f t="shared" si="18"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AW15" s="2">
         <f t="shared" si="11"/>
@@ -5006,11 +4983,11 @@
       </c>
       <c r="AX15">
         <f t="shared" si="12"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
       <c r="AY15">
         <f t="shared" si="19"/>
-        <v>5.3987418408876558E-3</v>
+        <v>5.86909788230092E-3</v>
       </c>
     </row>
     <row r="16" spans="1:51" x14ac:dyDescent="0.35">
@@ -5104,22 +5081,22 @@
       <c r="AH16">
         <v>0.47390947465623479</v>
       </c>
-      <c r="AI16" s="51">
-        <v>4.2404984619842561E-3</v>
+      <c r="AI16" s="127">
+        <v>4.2349995275388881E-3</v>
       </c>
       <c r="AJ16">
         <f t="shared" si="14"/>
-        <v>0.47814997311821905</v>
+        <v>0.47814447418377365</v>
       </c>
       <c r="AK16">
         <v>0.51210428280035414</v>
       </c>
-      <c r="AL16" s="51">
-        <v>2.0959176112987082E-4</v>
+      <c r="AL16" s="127">
+        <v>2.1219130796210544E-4</v>
       </c>
       <c r="AM16">
         <f t="shared" si="15"/>
-        <v>0.51231387456148403</v>
+        <v>0.51231647410831627</v>
       </c>
       <c r="AN16" s="2">
         <f t="shared" si="2"/>
@@ -5127,11 +5104,11 @@
       </c>
       <c r="AO16">
         <f t="shared" si="3"/>
-        <v>2.0959176112987082E-4</v>
+        <v>2.1219130796210544E-4</v>
       </c>
       <c r="AP16">
         <f t="shared" si="16"/>
-        <v>0.51231387456148403</v>
+        <v>0.51231647410831627</v>
       </c>
       <c r="AQ16" s="2">
         <f t="shared" si="5"/>
@@ -5139,11 +5116,11 @@
       </c>
       <c r="AR16">
         <f t="shared" si="6"/>
-        <v>2.0959176112987082E-4</v>
+        <v>2.1219130796210544E-4</v>
       </c>
       <c r="AS16">
         <f t="shared" si="17"/>
-        <v>0.51231387456148403</v>
+        <v>0.51231647410831627</v>
       </c>
       <c r="AT16" s="2">
         <f t="shared" si="8"/>
@@ -5151,11 +5128,11 @@
       </c>
       <c r="AU16">
         <f t="shared" si="9"/>
-        <v>2.0959176112987082E-4</v>
+        <v>2.1219130796210544E-4</v>
       </c>
       <c r="AV16">
         <f t="shared" si="18"/>
-        <v>0.51231387456148403</v>
+        <v>0.51231647410831627</v>
       </c>
       <c r="AW16" s="2">
         <f t="shared" si="11"/>
@@ -5163,11 +5140,11 @@
       </c>
       <c r="AX16">
         <f t="shared" si="12"/>
-        <v>2.0959176112987082E-4</v>
+        <v>2.1219130796210544E-4</v>
       </c>
       <c r="AY16">
         <f t="shared" si="19"/>
-        <v>0.51231387456148403</v>
+        <v>0.51231647410831627</v>
       </c>
     </row>
     <row r="17" spans="1:51" x14ac:dyDescent="0.35">
@@ -5261,22 +5238,22 @@
       <c r="AH17">
         <v>0.24585827527712426</v>
       </c>
-      <c r="AI17" s="51">
-        <v>2.0700811243651359E-2</v>
+      <c r="AI17" s="127">
+        <v>2.0560277799938402E-2</v>
       </c>
       <c r="AJ17">
         <f t="shared" si="14"/>
-        <v>0.26655908652077559</v>
+        <v>0.26641855307706264</v>
       </c>
       <c r="AK17">
         <v>7.6630038890183744E-2</v>
       </c>
-      <c r="AL17" s="51">
-        <v>3.7216049065244534E-4</v>
+      <c r="AL17" s="127">
+        <v>3.8366125882774188E-4</v>
       </c>
       <c r="AM17">
         <f t="shared" si="15"/>
-        <v>7.7002199380836189E-2</v>
+        <v>7.7013700149011488E-2</v>
       </c>
       <c r="AN17" s="2">
         <f t="shared" si="2"/>
@@ -5284,11 +5261,11 @@
       </c>
       <c r="AO17">
         <f t="shared" si="3"/>
-        <v>3.7216049065244534E-4</v>
+        <v>3.8366125882774188E-4</v>
       </c>
       <c r="AP17">
         <f t="shared" si="16"/>
-        <v>7.7002199380836189E-2</v>
+        <v>7.7013700149011488E-2</v>
       </c>
       <c r="AQ17" s="2">
         <f t="shared" si="5"/>
@@ -5296,11 +5273,11 @@
       </c>
       <c r="AR17">
         <f t="shared" si="6"/>
-        <v>3.7216049065244534E-4</v>
+        <v>3.8366125882774188E-4</v>
       </c>
       <c r="AS17">
         <f t="shared" si="17"/>
-        <v>7.7002199380836189E-2</v>
+        <v>7.7013700149011488E-2</v>
       </c>
       <c r="AT17" s="2">
         <f t="shared" si="8"/>
@@ -5308,11 +5285,11 @@
       </c>
       <c r="AU17">
         <f t="shared" si="9"/>
-        <v>3.7216049065244534E-4</v>
+        <v>3.8366125882774188E-4</v>
       </c>
       <c r="AV17">
         <f t="shared" si="18"/>
-        <v>7.7002199380836189E-2</v>
+        <v>7.7013700149011488E-2</v>
       </c>
       <c r="AW17" s="2">
         <f t="shared" si="11"/>
@@ -5320,11 +5297,11 @@
       </c>
       <c r="AX17">
         <f t="shared" si="12"/>
-        <v>3.7216049065244534E-4</v>
+        <v>3.8366125882774188E-4</v>
       </c>
       <c r="AY17">
         <f t="shared" si="19"/>
-        <v>7.7002199380836189E-2</v>
+        <v>7.7013700149011488E-2</v>
       </c>
     </row>
     <row r="18" spans="1:51" x14ac:dyDescent="0.35">
@@ -5418,22 +5395,22 @@
       <c r="AH18">
         <v>3.4141251927898666</v>
       </c>
-      <c r="AI18" s="51">
-        <v>1.0718762615156343</v>
+      <c r="AI18" s="127">
+        <v>1.0961495941820574</v>
       </c>
       <c r="AJ18">
         <f t="shared" si="14"/>
-        <v>4.4860014543055007</v>
+        <v>4.510274786971924</v>
       </c>
       <c r="AK18">
         <v>25.825694196902546</v>
       </c>
-      <c r="AL18" s="51">
-        <v>0.11248755052026857</v>
+      <c r="AL18" s="127">
+        <v>0.11480309838857856</v>
       </c>
       <c r="AM18">
         <f t="shared" si="15"/>
-        <v>25.938181747422814</v>
+        <v>25.940497295291124</v>
       </c>
       <c r="AN18" s="2">
         <f t="shared" si="2"/>
@@ -5441,11 +5418,11 @@
       </c>
       <c r="AO18">
         <f t="shared" si="3"/>
-        <v>0.11248755052026857</v>
+        <v>0.11480309838857856</v>
       </c>
       <c r="AP18">
         <f t="shared" si="16"/>
-        <v>25.938181747422814</v>
+        <v>25.940497295291124</v>
       </c>
       <c r="AQ18" s="2">
         <f t="shared" si="5"/>
@@ -5453,11 +5430,11 @@
       </c>
       <c r="AR18">
         <f t="shared" si="6"/>
-        <v>0.11248755052026857</v>
+        <v>0.11480309838857856</v>
       </c>
       <c r="AS18">
         <f t="shared" si="17"/>
-        <v>25.938181747422814</v>
+        <v>25.940497295291124</v>
       </c>
       <c r="AT18" s="2">
         <f t="shared" si="8"/>
@@ -5465,11 +5442,11 @@
       </c>
       <c r="AU18">
         <f t="shared" si="9"/>
-        <v>0.11248755052026857</v>
+        <v>0.11480309838857856</v>
       </c>
       <c r="AV18">
         <f t="shared" si="18"/>
-        <v>25.938181747422814</v>
+        <v>25.940497295291124</v>
       </c>
       <c r="AW18" s="2">
         <f t="shared" si="11"/>
@@ -5477,11 +5454,11 @@
       </c>
       <c r="AX18">
         <f t="shared" si="12"/>
-        <v>0.11248755052026857</v>
+        <v>0.11480309838857856</v>
       </c>
       <c r="AY18">
         <f t="shared" si="19"/>
-        <v>25.938181747422814</v>
+        <v>25.940497295291124</v>
       </c>
     </row>
     <row r="19" spans="1:51" x14ac:dyDescent="0.35">
@@ -5575,22 +5552,22 @@
       <c r="AH19">
         <v>0.91142919415811929</v>
       </c>
-      <c r="AI19" s="51">
-        <v>1.1802078079887578E-2</v>
+      <c r="AI19" s="127">
+        <v>1.2419532449195709E-2</v>
       </c>
       <c r="AJ19">
         <f t="shared" si="14"/>
-        <v>0.92323127223800683</v>
+        <v>0.92384872660731499</v>
       </c>
       <c r="AK19">
         <v>0.18877324129794976</v>
       </c>
-      <c r="AL19" s="51">
-        <v>3.4778154884700514E-4</v>
+      <c r="AL19" s="127">
+        <v>3.7018497329376407E-4</v>
       </c>
       <c r="AM19">
         <f t="shared" si="15"/>
-        <v>0.18912102284679677</v>
+        <v>0.18914342627124353</v>
       </c>
       <c r="AN19" s="2">
         <f t="shared" si="2"/>
@@ -5598,11 +5575,11 @@
       </c>
       <c r="AO19">
         <f t="shared" si="3"/>
-        <v>3.4778154884700514E-4</v>
+        <v>3.7018497329376407E-4</v>
       </c>
       <c r="AP19">
         <f t="shared" si="16"/>
-        <v>0.18912102284679677</v>
+        <v>0.18914342627124353</v>
       </c>
       <c r="AQ19" s="2">
         <f t="shared" si="5"/>
@@ -5610,11 +5587,11 @@
       </c>
       <c r="AR19">
         <f t="shared" si="6"/>
-        <v>3.4778154884700514E-4</v>
+        <v>3.7018497329376407E-4</v>
       </c>
       <c r="AS19">
         <f t="shared" si="17"/>
-        <v>0.18912102284679677</v>
+        <v>0.18914342627124353</v>
       </c>
       <c r="AT19" s="2">
         <f t="shared" si="8"/>
@@ -5622,11 +5599,11 @@
       </c>
       <c r="AU19">
         <f t="shared" si="9"/>
-        <v>3.4778154884700514E-4</v>
+        <v>3.7018497329376407E-4</v>
       </c>
       <c r="AV19">
         <f t="shared" si="18"/>
-        <v>0.18912102284679677</v>
+        <v>0.18914342627124353</v>
       </c>
       <c r="AW19" s="2">
         <f t="shared" si="11"/>
@@ -5634,11 +5611,11 @@
       </c>
       <c r="AX19">
         <f t="shared" si="12"/>
-        <v>3.4778154884700514E-4</v>
+        <v>3.7018497329376407E-4</v>
       </c>
       <c r="AY19">
         <f t="shared" si="19"/>
-        <v>0.18912102284679677</v>
+        <v>0.18914342627124353</v>
       </c>
     </row>
     <row r="20" spans="1:51" x14ac:dyDescent="0.35">
@@ -5748,22 +5725,22 @@
       <c r="AH20">
         <v>71783.505317547926</v>
       </c>
-      <c r="AI20" s="51">
-        <v>611.91676387079497</v>
+      <c r="AI20" s="127">
+        <v>633.15471120171344</v>
       </c>
       <c r="AJ20">
         <f t="shared" si="14"/>
-        <v>72395.422081418714</v>
+        <v>72416.66002874964</v>
       </c>
       <c r="AK20">
         <v>74856.053349714566</v>
       </c>
-      <c r="AL20" s="51">
-        <v>92.564589004961775</v>
+      <c r="AL20" s="127">
+        <v>92.811588579119217</v>
       </c>
       <c r="AM20">
         <f t="shared" si="15"/>
-        <v>74948.61793871953</v>
+        <v>74948.864938293686</v>
       </c>
       <c r="AN20" s="2">
         <f t="shared" si="2"/>
@@ -5771,11 +5748,11 @@
       </c>
       <c r="AO20">
         <f t="shared" si="3"/>
-        <v>92.564589004961775</v>
+        <v>92.811588579119217</v>
       </c>
       <c r="AP20">
         <f t="shared" si="16"/>
-        <v>74948.61793871953</v>
+        <v>74948.864938293686</v>
       </c>
       <c r="AQ20" s="2">
         <f t="shared" si="5"/>
@@ -5783,11 +5760,11 @@
       </c>
       <c r="AR20">
         <f t="shared" si="6"/>
-        <v>92.564589004961775</v>
+        <v>92.811588579119217</v>
       </c>
       <c r="AS20">
         <f t="shared" si="17"/>
-        <v>74948.61793871953</v>
+        <v>74948.864938293686</v>
       </c>
       <c r="AT20" s="2">
         <f t="shared" si="8"/>
@@ -5795,11 +5772,11 @@
       </c>
       <c r="AU20">
         <f t="shared" si="9"/>
-        <v>92.564589004961775</v>
+        <v>92.811588579119217</v>
       </c>
       <c r="AV20">
         <f t="shared" si="18"/>
-        <v>74948.61793871953</v>
+        <v>74948.864938293686</v>
       </c>
       <c r="AW20" s="2">
         <f t="shared" si="11"/>
@@ -5807,11 +5784,11 @@
       </c>
       <c r="AX20">
         <f t="shared" si="12"/>
-        <v>92.564589004961775</v>
+        <v>92.811588579119217</v>
       </c>
       <c r="AY20">
         <f t="shared" si="19"/>
-        <v>74948.61793871953</v>
+        <v>74948.864938293686</v>
       </c>
     </row>
     <row r="21" spans="1:51" x14ac:dyDescent="0.35">
@@ -5922,58 +5899,58 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="127" t="s">
+      <c r="B23" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="127" t="s">
+      <c r="C23" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="127" t="s">
+      <c r="D23" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="127" t="s">
+      <c r="E23" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="127" t="s">
+      <c r="F23" t="s">
         <v>15</v>
       </c>
       <c r="G23" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="H23" t="s">
-        <v>351</v>
-      </c>
-      <c r="I23" s="127" t="s">
+        <v>343</v>
+      </c>
+      <c r="I23" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="127" t="s">
+      <c r="J23" t="s">
         <v>15</v>
       </c>
-      <c r="K23" s="127" t="s">
+      <c r="K23" t="s">
         <v>15</v>
       </c>
-      <c r="L23" s="127" t="s">
+      <c r="L23" t="s">
         <v>15</v>
       </c>
-      <c r="M23" s="127" t="s">
+      <c r="M23" t="s">
         <v>15</v>
       </c>
-      <c r="N23" s="127" t="s">
+      <c r="N23" t="s">
         <v>15</v>
       </c>
-      <c r="O23" s="127" t="s">
+      <c r="O23" t="s">
         <v>15</v>
       </c>
-      <c r="P23" s="127" t="s">
+      <c r="P23" t="s">
         <v>15</v>
       </c>
-      <c r="Q23" s="127" t="s">
+      <c r="Q23" t="s">
         <v>15</v>
       </c>
-      <c r="R23" s="127" t="s">
+      <c r="R23" t="s">
         <v>15</v>
       </c>
-      <c r="S23" s="127" t="s">
+      <c r="S23" t="s">
         <v>15</v>
       </c>
       <c r="T23" s="17" t="s">
@@ -6012,6 +5989,141 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8F5E2C-DDF2-4E57-AD59-B511AD831FCD}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="17">
+        <v>1</v>
+      </c>
+      <c r="C2" s="27">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="D2" s="28">
+        <v>1E-3</v>
+      </c>
+      <c r="E2" s="29">
+        <v>3.7854109999999998E-3</v>
+      </c>
+      <c r="F2" s="30">
+        <v>2.8316846999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="19">
+        <v>1000000</v>
+      </c>
+      <c r="C3" s="19">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19">
+        <v>1000.0000000000001</v>
+      </c>
+      <c r="E3" s="19">
+        <v>3785.4110000000001</v>
+      </c>
+      <c r="F3" s="21">
+        <v>28316.847000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="20">
+        <v>1E-3</v>
+      </c>
+      <c r="D4" s="19">
+        <v>1</v>
+      </c>
+      <c r="E4" s="20">
+        <v>3.7854109999999999</v>
+      </c>
+      <c r="F4" s="23">
+        <v>28.316846999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="31">
+        <v>264.17210707106841</v>
+      </c>
+      <c r="C5" s="22">
+        <v>2.6417210707106839E-4</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0.26417210707106842</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1</v>
+      </c>
+      <c r="F5" s="23">
+        <v>7.4805211375990615</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="32">
+        <v>35.314666212661322</v>
+      </c>
+      <c r="C6" s="24">
+        <v>3.5314666212661319E-5</v>
+      </c>
+      <c r="D6" s="25">
+        <v>3.5314666212661321E-2</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0.13368052594273649</v>
+      </c>
+      <c r="F6" s="26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02D7542-6EF2-41EA-86E3-98DE7161C9DB}">
   <dimension ref="A1:J10"/>
   <sheetViews>
@@ -6367,7 +6479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01334582-9977-4CFE-91E6-70D92C4489D0}">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -6543,7 +6655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F07116-128C-456A-A5F4-E4321BD8FA65}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -6733,7 +6845,7 @@
         <v>226</v>
       </c>
       <c r="BA4" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="BB4" t="s">
         <v>227</v>
@@ -7790,6 +7902,422 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498187A9-5554-4C33-80C2-40670D1F38AD}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" s="122" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" s="122" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="122" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="122" t="s">
+        <v>292</v>
+      </c>
+      <c r="G1" s="122" t="s">
+        <v>292</v>
+      </c>
+      <c r="H1" s="122" t="s">
+        <v>293</v>
+      </c>
+      <c r="I1" s="122" t="s">
+        <v>293</v>
+      </c>
+      <c r="J1" s="122" t="s">
+        <v>324</v>
+      </c>
+      <c r="K1" s="122" t="s">
+        <v>324</v>
+      </c>
+      <c r="L1" s="122" t="s">
+        <v>325</v>
+      </c>
+      <c r="M1" s="122" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="78.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="E2" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="H2" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="I2" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="K2" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="L2" s="47" t="s">
+        <v>272</v>
+      </c>
+      <c r="M2" s="47" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="95" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" s="127">
+        <v>2.1781234690476294E-2</v>
+      </c>
+      <c r="C4">
+        <f>B4</f>
+        <v>2.1781234690476294E-2</v>
+      </c>
+      <c r="D4" s="127">
+        <v>0.73563756849253104</v>
+      </c>
+      <c r="F4">
+        <f>D4</f>
+        <v>0.73563756849253104</v>
+      </c>
+      <c r="H4">
+        <f>D4</f>
+        <v>0.73563756849253104</v>
+      </c>
+      <c r="J4">
+        <f>D4</f>
+        <v>0.73563756849253104</v>
+      </c>
+      <c r="L4">
+        <f>D4</f>
+        <v>0.73563756849253104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="95" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="127">
+        <v>0.18381159698546526</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C11" si="0">B5</f>
+        <v>0.18381159698546526</v>
+      </c>
+      <c r="D5" s="127">
+        <v>0.12786171981419567</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ref="F5:F11" si="1">D5</f>
+        <v>0.12786171981419567</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H11" si="2">D5</f>
+        <v>0.12786171981419567</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J11" si="3">D5</f>
+        <v>0.12786171981419567</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L11" si="4">D5</f>
+        <v>0.12786171981419567</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="95" t="s">
+        <v>331</v>
+      </c>
+      <c r="B6" s="127">
+        <v>0.26679009552113131</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.26679009552113131</v>
+      </c>
+      <c r="D6" s="127">
+        <v>8.2023598818784182E-2</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>8.2023598818784182E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>8.2023598818784182E-2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="3"/>
+        <v>8.2023598818784182E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>8.2023598818784182E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="95" t="s">
+        <v>332</v>
+      </c>
+      <c r="B7" s="127">
+        <v>1.6067527224713878E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>1.6067527224713878E-2</v>
+      </c>
+      <c r="D7" s="127">
+        <v>4.7471776286034904E-3</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>4.7471776286034904E-3</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>4.7471776286034904E-3</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="3"/>
+        <v>4.7471776286034904E-3</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>4.7471776286034904E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="95" t="s">
+        <v>333</v>
+      </c>
+      <c r="B8" s="127">
+        <v>1.0925985281165002E-2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1.0925985281165002E-2</v>
+      </c>
+      <c r="D8" s="127">
+        <v>1.1625114789012593E-3</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>1.1625114789012593E-3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>1.1625114789012593E-3</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>1.1625114789012593E-3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>1.1625114789012593E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="95" t="s">
+        <v>334</v>
+      </c>
+      <c r="B9" s="127">
+        <v>7.5973312175973959E-2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>7.5973312175973959E-2</v>
+      </c>
+      <c r="D9" s="127">
+        <v>1.5008027021008762E-3</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>1.5008027021008762E-3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>1.5008027021008762E-3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>1.5008027021008762E-3</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>1.5008027021008762E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="95" t="s">
+        <v>335</v>
+      </c>
+      <c r="B10" s="127">
+        <v>7.7626034636698693E-4</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>7.7626034636698693E-4</v>
+      </c>
+      <c r="D10" s="127">
+        <v>8.0041955215929224E-5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>8.0041955215929224E-5</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>8.0041955215929224E-5</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>8.0041955215929224E-5</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="4"/>
+        <v>8.0041955215929224E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="96" t="s">
+        <v>336</v>
+      </c>
+      <c r="B11" s="127">
+        <v>3.3865871217684512E-3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>3.3865871217684512E-3</v>
+      </c>
+      <c r="D11" s="127">
+        <v>1.2376182810406463E-4</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>1.2376182810406463E-4</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>1.2376182810406463E-4</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>1.2376182810406463E-4</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="4"/>
+        <v>1.2376182810406463E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B12" s="127"/>
+      <c r="D12" s="127"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B13" s="127"/>
+      <c r="D13" s="127"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B14" s="127"/>
+      <c r="D14" s="127"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B15" s="127"/>
+      <c r="D15" s="127"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B16" s="127"/>
+      <c r="D16" s="127"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B17" s="127"/>
+      <c r="D17" s="127"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B18" s="127"/>
+      <c r="D18" s="127"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B19" s="127"/>
+      <c r="D19" s="127"/>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B20" s="127"/>
+      <c r="D20" s="127"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -7797,7 +8325,7 @@
   <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A21" sqref="A21:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10022,7 +10550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1855EF5-F382-4C03-BE02-9E2A728DFED9}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -15758,7 +16286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F728B1BE-12B0-4F72-A3B0-228655F7F3FD}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
@@ -16844,7 +17372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2275C5-799F-4B1B-8AD1-776CB314922E}">
   <sheetPr>
     <tabColor theme="5"/>
@@ -17261,7 +17789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{912BA9E3-4DC6-4F1B-8852-1658C2A4C23D}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -17476,1020 +18004,824 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885F1586-D778-4FB1-B08D-679C42EBE3A6}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:D74"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C1" s="50" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>171</v>
+      </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="111" t="s">
         <v>113</v>
       </c>
-      <c r="B3" s="111" t="s">
-        <v>113</v>
+      <c r="B3" s="111">
+        <v>42.686144171450856</v>
       </c>
       <c r="C3" s="111">
-        <v>42.686144171450856</v>
-      </c>
-      <c r="D3" s="111">
         <v>846.6716031627742</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="51" t="s">
+    <row r="4" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="111" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="111" t="s">
-        <v>114</v>
+      <c r="B4" s="111">
+        <v>43.638128483226296</v>
       </c>
       <c r="C4" s="111">
-        <v>43.638128483226296</v>
-      </c>
-      <c r="D4" s="111">
         <v>862.78610169410933</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="51" t="s">
+    <row r="5" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="111" t="s">
         <v>115</v>
       </c>
-      <c r="B5" s="111" t="s">
-        <v>115</v>
+      <c r="B5" s="111">
+        <v>41.867999896029993</v>
       </c>
       <c r="C5" s="111">
+        <v>1014.3369175627239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="111" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="111">
         <v>41.867999896029993</v>
       </c>
-      <c r="D5" s="111">
+      <c r="C6" s="111">
         <v>1014.3369175627239</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="51" t="s">
-        <v>116</v>
-      </c>
-      <c r="B6" s="111" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="111">
-        <v>41.867999896029993</v>
-      </c>
-      <c r="D6" s="111">
-        <v>1014.3369175627239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="51" t="s">
+    <row r="7" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="111" t="s">
         <v>117</v>
       </c>
-      <c r="B7" s="111" t="s">
-        <v>117</v>
+      <c r="B7" s="111">
+        <v>43.762023620933512</v>
       </c>
       <c r="C7" s="111">
-        <v>43.762023620933512</v>
-      </c>
-      <c r="D7" s="111">
         <v>924.72851371056413</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="51" t="s">
+    <row r="8" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="111" t="s">
         <v>118</v>
       </c>
-      <c r="B8" s="111" t="s">
-        <v>118</v>
+      <c r="B8" s="111">
+        <v>50.025976283884859</v>
       </c>
       <c r="C8" s="111">
-        <v>50.025976283884859</v>
-      </c>
-      <c r="D8" s="111">
         <v>715.64223805552433</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="51" t="s">
+    <row r="9" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="111" t="s">
         <v>119</v>
       </c>
-      <c r="B9" s="111" t="s">
-        <v>119</v>
+      <c r="B9" s="111">
+        <v>42.923806268925297</v>
       </c>
       <c r="C9" s="111">
-        <v>42.923806268925297</v>
-      </c>
-      <c r="D9" s="111">
         <v>815.56195965417839</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="51" t="s">
+    <row r="10" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="111" t="s">
         <v>120</v>
       </c>
-      <c r="B10" s="111" t="s">
-        <v>120</v>
+      <c r="B10" s="111">
+        <v>43.309214561540323</v>
       </c>
       <c r="C10" s="111">
-        <v>43.309214561540323</v>
-      </c>
-      <c r="D10" s="111">
         <v>788.30083565459597</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="51" t="s">
+    <row r="11" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="111" t="s">
         <v>121</v>
       </c>
-      <c r="B11" s="111" t="s">
-        <v>121</v>
+      <c r="B11" s="111">
+        <v>43.448539775274917</v>
       </c>
       <c r="C11" s="111">
+        <v>744.70116983334174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="111" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="111">
+        <v>41.744962588753829</v>
+      </c>
+      <c r="C12" s="111">
+        <v>749.07638827065296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="111" t="s">
+        <v>123</v>
+      </c>
+      <c r="B13" s="111">
+        <v>41.744962588753829</v>
+      </c>
+      <c r="C13" s="111">
+        <v>749.07638827065296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="111" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="111">
+        <v>39.141696278724332</v>
+      </c>
+      <c r="C14" s="111">
+        <v>755.86244135709444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="111" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" s="111">
+        <v>36.618106210801628</v>
+      </c>
+      <c r="C15" s="111">
+        <v>762.55920427134606</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="111" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" s="111">
+        <v>42.791892621566141</v>
+      </c>
+      <c r="C16" s="111">
+        <v>836.63306309407369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="111" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" s="111">
+        <v>42.612885554908658</v>
+      </c>
+      <c r="C17" s="111">
+        <v>846.93577526984518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="51" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="111" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="111">
+        <v>42.791892621566141</v>
+      </c>
+      <c r="C18" s="111">
+        <v>836.63306309407369</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="112" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="111">
+        <v>42.612885554908658</v>
+      </c>
+      <c r="C19" s="111">
+        <v>846.93577526984518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="111" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="111">
+        <v>44.938845166484512</v>
+      </c>
+      <c r="C20" s="111">
+        <v>725.15243391008278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="111" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" s="111">
+        <v>44.020251676687209</v>
+      </c>
+      <c r="C21" s="111">
+        <v>748.62596861099109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="111" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="111">
+        <v>43.20000000000001</v>
+      </c>
+      <c r="C22" s="111">
+        <v>801.99999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="111" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="111">
+        <v>43.29999999999999</v>
+      </c>
+      <c r="C23" s="111">
+        <v>791.99999999999989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="111" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="111">
+        <v>44.383186869860424</v>
+      </c>
+      <c r="C24" s="111">
+        <v>700.32025584540236</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="111" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" s="111">
+        <v>39.466884224580042</v>
+      </c>
+      <c r="C25" s="111">
+        <v>991.17374573064865</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="111" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="111">
+        <v>39.466884224580042</v>
+      </c>
+      <c r="C26" s="111">
+        <v>991.17374573064865</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="111" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="111">
+        <v>20.09379488107119</v>
+      </c>
+      <c r="C27" s="111">
+        <v>794.1013538556316</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="111" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="111">
+        <v>26.951945458668003</v>
+      </c>
+      <c r="C28" s="111">
+        <v>789.34625592835232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="111" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="111">
+        <v>34.366594093458403</v>
+      </c>
+      <c r="C29" s="111">
+        <v>809.68750817282455</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="111" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="111">
+        <v>29.5896179632085</v>
+      </c>
+      <c r="C30" s="111">
+        <v>783.00612535864673</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="111" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="111">
         <v>43.448539775274917</v>
       </c>
-      <c r="D11" s="111">
+      <c r="C31" s="111">
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="111" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" s="111">
-        <v>41.744962588753829</v>
-      </c>
-      <c r="D12" s="111">
-        <v>749.07638827065296</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="51" t="s">
-        <v>123</v>
-      </c>
-      <c r="B13" s="111" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="111">
-        <v>41.744962588753829</v>
-      </c>
-      <c r="D13" s="111">
-        <v>749.07638827065296</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="51" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="111" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="111">
-        <v>39.141696278724332</v>
-      </c>
-      <c r="D14" s="111">
-        <v>755.86244135709444</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="51" t="s">
-        <v>125</v>
-      </c>
-      <c r="B15" s="111" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="111">
-        <v>36.618106210801628</v>
-      </c>
-      <c r="D15" s="111">
-        <v>762.55920427134606</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="51" t="s">
-        <v>126</v>
-      </c>
-      <c r="B16" s="111" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="111">
-        <v>42.791892621566141</v>
-      </c>
-      <c r="D16" s="111">
-        <v>836.63306309407369</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="51" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" s="111" t="s">
-        <v>127</v>
-      </c>
-      <c r="C17" s="111">
-        <v>42.612885554908658</v>
-      </c>
-      <c r="D17" s="111">
-        <v>846.93577526984518</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="51" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="51" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" s="111" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="111">
-        <v>42.791892621566141</v>
-      </c>
-      <c r="D18" s="111">
-        <v>836.63306309407369</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>342</v>
-      </c>
-      <c r="B19" s="112" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="111">
-        <v>42.612885554908658</v>
-      </c>
-      <c r="D19" s="111">
-        <v>846.93577526984518</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" s="111" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="111">
-        <v>44.938845166484512</v>
-      </c>
-      <c r="D20" s="111">
-        <v>725.15243391008278</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" s="111" t="s">
-        <v>130</v>
-      </c>
-      <c r="C21" s="111">
-        <v>44.020251676687209</v>
-      </c>
-      <c r="D21" s="111">
-        <v>748.62596861099109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" s="111" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" s="111">
-        <v>43.20000000000001</v>
-      </c>
-      <c r="D22" s="111">
-        <v>801.99999999999989</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B23" s="111" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" s="111">
-        <v>43.29999999999999</v>
-      </c>
-      <c r="D23" s="111">
-        <v>791.99999999999989</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>133</v>
-      </c>
-      <c r="B24" s="111" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" s="111">
-        <v>44.383186869860424</v>
-      </c>
-      <c r="D24" s="111">
-        <v>700.32025584540236</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>134</v>
-      </c>
-      <c r="B25" s="111" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="111">
-        <v>39.466884224580042</v>
-      </c>
-      <c r="D25" s="111">
-        <v>991.17374573064865</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="111" t="s">
-        <v>135</v>
-      </c>
-      <c r="C26" s="111">
-        <v>39.466884224580042</v>
-      </c>
-      <c r="D26" s="111">
-        <v>991.17374573064865</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>136</v>
-      </c>
-      <c r="B27" s="111" t="s">
-        <v>136</v>
-      </c>
-      <c r="C27" s="111">
-        <v>20.09379488107119</v>
-      </c>
-      <c r="D27" s="111">
-        <v>794.1013538556316</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>137</v>
-      </c>
-      <c r="B28" s="111" t="s">
-        <v>137</v>
-      </c>
-      <c r="C28" s="111">
-        <v>26.951945458668003</v>
-      </c>
-      <c r="D28" s="111">
-        <v>789.34625592835232</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>138</v>
-      </c>
-      <c r="B29" s="111" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" s="111">
-        <v>34.366594093458403</v>
-      </c>
-      <c r="D29" s="111">
-        <v>809.68750817282455</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>139</v>
-      </c>
-      <c r="B30" s="111" t="s">
-        <v>139</v>
-      </c>
-      <c r="C30" s="111">
-        <v>29.5896179632085</v>
-      </c>
-      <c r="D30" s="111">
-        <v>783.00612535864673</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>343</v>
-      </c>
-      <c r="B31" s="111" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="111">
-        <v>43.448539775274917</v>
-      </c>
-      <c r="D31" s="111">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="111" t="s">
+        <v>141</v>
+      </c>
+      <c r="B32" s="111">
+        <v>46.607901433957352</v>
+      </c>
+      <c r="C32" s="111">
+        <v>508.00296189766453</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="111" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" s="111">
+        <v>48.632802660086355</v>
+      </c>
+      <c r="C33" s="111">
+        <v>428.22298556220187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="111" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="111">
+        <v>28.8820491423749</v>
+      </c>
+      <c r="C34" s="111">
+        <v>665.18536560495022</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="111" t="s">
+        <v>144</v>
+      </c>
+      <c r="B35" s="111">
+        <v>23.402467701996926</v>
+      </c>
+      <c r="C35" s="111">
+        <v>859.88020851632757</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="111" t="s">
+        <v>145</v>
+      </c>
+      <c r="B36" s="111">
+        <v>37.841074841430498</v>
+      </c>
+      <c r="C36" s="111">
+        <v>881.08390254321148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="111" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="111">
+        <v>43.2478478520053</v>
+      </c>
+      <c r="C37" s="111">
+        <v>797.00724703341325</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="111" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="111">
+        <v>43.563944530917098</v>
+      </c>
+      <c r="C38" s="111">
+        <v>748.92792354647884</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="111" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="111">
+        <v>43.979867109548842</v>
+      </c>
+      <c r="C39" s="111">
+        <v>778.77937164550963</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="111" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="111">
+        <v>43.400833892223638</v>
+      </c>
+      <c r="C40" s="111">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="111" t="s">
+        <v>150</v>
+      </c>
+      <c r="B41" s="111">
+        <v>43.450098991200285</v>
+      </c>
+      <c r="C41" s="111">
+        <v>798.04417121416941</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>208</v>
+      </c>
+      <c r="B42" s="51">
+        <v>44.291949816853993</v>
+      </c>
+      <c r="C42">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>292</v>
+      </c>
+      <c r="B43" s="51">
+        <v>44.291949816853993</v>
+      </c>
+      <c r="C43">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>293</v>
+      </c>
+      <c r="B44" s="51">
+        <v>43.995102738357922</v>
+      </c>
+      <c r="C44">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>324</v>
+      </c>
+      <c r="B45" s="51">
+        <v>43.975450721892244</v>
+      </c>
+      <c r="C45">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>325</v>
+      </c>
+      <c r="B46" s="51">
+        <v>43.819577184272568</v>
+      </c>
+      <c r="C46">
+        <v>793.37856525946859</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" s="111" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="111">
+        <v>43.239767721042398</v>
+      </c>
+      <c r="C47" s="111">
+        <v>747.6070630111235</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="111" t="s">
+        <v>152</v>
+      </c>
+      <c r="B48" s="111">
+        <v>44.06462340864357</v>
+      </c>
+      <c r="C48" s="111">
+        <v>716.69892648380858</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="111" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="111">
+        <v>41.940509787192262</v>
+      </c>
+      <c r="C49" s="111">
         <v>744.70116983334174</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>141</v>
-      </c>
-      <c r="B32" s="111" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32" s="111">
-        <v>46.607901433957352</v>
-      </c>
-      <c r="D32" s="111">
-        <v>508.00296189766453</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>142</v>
-      </c>
-      <c r="B33" s="111" t="s">
-        <v>142</v>
-      </c>
-      <c r="C33" s="111">
-        <v>48.632802660086355</v>
-      </c>
-      <c r="D33" s="111">
-        <v>428.22298556220187</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>143</v>
-      </c>
-      <c r="B34" s="111" t="s">
-        <v>143</v>
-      </c>
-      <c r="C34" s="111">
-        <v>28.8820491423749</v>
-      </c>
-      <c r="D34" s="111">
-        <v>665.18536560495022</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>144</v>
-      </c>
-      <c r="B35" s="111" t="s">
-        <v>144</v>
-      </c>
-      <c r="C35" s="111">
-        <v>23.402467701996926</v>
-      </c>
-      <c r="D35" s="111">
-        <v>859.88020851632757</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" s="111" t="s">
-        <v>145</v>
-      </c>
-      <c r="C36" s="111">
-        <v>37.841074841430498</v>
-      </c>
-      <c r="D36" s="111">
-        <v>881.08390254321148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>146</v>
-      </c>
-      <c r="B37" s="111" t="s">
-        <v>146</v>
-      </c>
-      <c r="C37" s="111">
-        <v>43.2478478520053</v>
-      </c>
-      <c r="D37" s="111">
-        <v>797.00724703341325</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>147</v>
-      </c>
-      <c r="B38" s="111" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" s="111">
-        <v>43.563944530917098</v>
-      </c>
-      <c r="D38" s="111">
-        <v>748.92792354647884</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>148</v>
-      </c>
-      <c r="B39" s="111" t="s">
-        <v>148</v>
-      </c>
-      <c r="C39" s="111">
-        <v>43.979867109548842</v>
-      </c>
-      <c r="D39" s="111">
-        <v>778.77937164550963</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>149</v>
-      </c>
-      <c r="B40" s="111" t="s">
-        <v>149</v>
-      </c>
-      <c r="C40" s="111">
-        <v>43.400833892223638</v>
-      </c>
-      <c r="D40" s="111">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>150</v>
-      </c>
-      <c r="B41" s="111" t="s">
-        <v>150</v>
-      </c>
-      <c r="C41" s="111">
-        <v>43.450098991200285</v>
-      </c>
-      <c r="D41" s="111">
-        <v>798.04417121416941</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
-        <v>208</v>
-      </c>
-      <c r="C42" s="51">
-        <v>44.291949816853993</v>
-      </c>
-      <c r="D42">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
-        <v>292</v>
-      </c>
-      <c r="C43" s="51">
-        <v>44.291949816853993</v>
-      </c>
-      <c r="D43">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
-        <v>293</v>
-      </c>
-      <c r="C44" s="51">
-        <v>43.995102738357922</v>
-      </c>
-      <c r="D44">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
-        <v>324</v>
-      </c>
-      <c r="C45" s="51">
-        <v>43.975450721892244</v>
-      </c>
-      <c r="D45">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
-        <v>325</v>
-      </c>
-      <c r="C46" s="51">
-        <v>43.819577184272568</v>
-      </c>
-      <c r="D46">
-        <v>793.37856525946859</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>151</v>
-      </c>
-      <c r="B47" s="111" t="s">
-        <v>151</v>
-      </c>
-      <c r="C47" s="111">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="111" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="111">
+        <v>44.100000000000009</v>
+      </c>
+      <c r="C50" s="111">
+        <v>756.99999999999739</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="111" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" s="111">
+        <v>120.0716545708955</v>
+      </c>
+      <c r="C51" s="111">
+        <v>70.798124695046326</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="111" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="111">
+        <v>35.108475350053361</v>
+      </c>
+      <c r="C52" s="111">
+        <v>742.58779297677324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" s="111" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" s="111">
+        <v>36.314947264056933</v>
+      </c>
+      <c r="C53" s="111">
+        <v>742.32362086970215</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" s="111" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="111">
+        <v>36.392726332990044</v>
+      </c>
+      <c r="C54" s="111">
+        <v>769.53334789802227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" s="111" t="s">
+        <v>159</v>
+      </c>
+      <c r="B55" s="111">
+        <v>45.277295108224124</v>
+      </c>
+      <c r="C55" s="111">
+        <v>584.61287294827434</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" s="111" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="111">
+        <v>44.862289825779037</v>
+      </c>
+      <c r="C56" s="111">
+        <v>559.51652277652283</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="111" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" s="111">
+        <v>44.824654221926316</v>
+      </c>
+      <c r="C57" s="111">
+        <v>595.17975723111715</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" s="111" t="s">
+        <v>162</v>
+      </c>
+      <c r="B58" s="111">
+        <v>46.296070501302083</v>
+      </c>
+      <c r="C58" s="111">
+        <v>507.21044557645126</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" s="111" t="s">
+        <v>163</v>
+      </c>
+      <c r="B59" s="111">
+        <v>34.871059262781436</v>
+      </c>
+      <c r="C59" s="111">
+        <v>668.88377510394514</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" s="111" t="s">
+        <v>164</v>
+      </c>
+      <c r="B60" s="111">
+        <v>44.746252156404559</v>
+      </c>
+      <c r="C60" s="111">
+        <v>654.80340179705718</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" s="111" t="s">
+        <v>165</v>
+      </c>
+      <c r="B61" s="111">
+        <v>44.807686766932541</v>
+      </c>
+      <c r="C61" s="111">
+        <v>688.85095964480468</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" s="111" t="s">
+        <v>166</v>
+      </c>
+      <c r="B62" s="111">
+        <v>44.200433259008399</v>
+      </c>
+      <c r="C62" s="111">
+        <v>737.59071339941693</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" s="111" t="s">
+        <v>167</v>
+      </c>
+      <c r="B63" s="111">
+        <v>43.992111747526693</v>
+      </c>
+      <c r="C63" s="111">
+        <v>765.47381512866104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" s="111" t="s">
+        <v>168</v>
+      </c>
+      <c r="B64" s="111">
+        <v>44.298577840334822</v>
+      </c>
+      <c r="C64" s="111">
+        <v>731.67589538225809</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" s="111" t="s">
+        <v>169</v>
+      </c>
+      <c r="B65" s="111">
+        <v>33.200025671240915</v>
+      </c>
+      <c r="C65" s="111">
+        <v>800.00032424653136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" s="111" t="s">
+        <v>170</v>
+      </c>
+      <c r="B66" s="111">
         <v>43.239767721042398</v>
       </c>
-      <c r="D47" s="111">
+      <c r="C66" s="111">
         <v>747.6070630111235</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>152</v>
-      </c>
-      <c r="B48" s="111" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="111">
-        <v>44.06462340864357</v>
-      </c>
-      <c r="D48" s="111">
-        <v>716.69892648380858</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
-        <v>153</v>
-      </c>
-      <c r="B49" s="111" t="s">
-        <v>153</v>
-      </c>
-      <c r="C49" s="111">
-        <v>41.940509787192262</v>
-      </c>
-      <c r="D49" s="111">
-        <v>744.70116983334174</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B50" s="111" t="s">
-        <v>154</v>
-      </c>
-      <c r="C50" s="111">
-        <v>44.100000000000009</v>
-      </c>
-      <c r="D50" s="111">
-        <v>756.99999999999739</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>155</v>
-      </c>
-      <c r="B51" s="111" t="s">
-        <v>155</v>
-      </c>
-      <c r="C51" s="111">
-        <v>120.0716545708955</v>
-      </c>
-      <c r="D51" s="111">
-        <v>70.798124695046326</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>156</v>
-      </c>
-      <c r="B52" s="111" t="s">
-        <v>156</v>
-      </c>
-      <c r="C52" s="111">
-        <v>35.108475350053361</v>
-      </c>
-      <c r="D52" s="111">
-        <v>742.58779297677324</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>157</v>
-      </c>
-      <c r="B53" s="111" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" s="111">
-        <v>36.314947264056933</v>
-      </c>
-      <c r="D53" s="111">
-        <v>742.32362086970215</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>158</v>
-      </c>
-      <c r="B54" s="111" t="s">
-        <v>158</v>
-      </c>
-      <c r="C54" s="111">
-        <v>36.392726332990044</v>
-      </c>
-      <c r="D54" s="111">
-        <v>769.53334789802227</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" s="111" t="s">
-        <v>159</v>
-      </c>
-      <c r="C55" s="111">
-        <v>45.277295108224124</v>
-      </c>
-      <c r="D55" s="111">
-        <v>584.61287294827434</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>160</v>
-      </c>
-      <c r="B56" s="111" t="s">
-        <v>160</v>
-      </c>
-      <c r="C56" s="111">
-        <v>44.862289825779037</v>
-      </c>
-      <c r="D56" s="111">
-        <v>559.51652277652283</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>161</v>
-      </c>
-      <c r="B57" s="111" t="s">
-        <v>161</v>
-      </c>
-      <c r="C57" s="111">
-        <v>44.824654221926316</v>
-      </c>
-      <c r="D57" s="111">
-        <v>595.17975723111715</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>162</v>
-      </c>
-      <c r="B58" s="111" t="s">
-        <v>162</v>
-      </c>
-      <c r="C58" s="111">
-        <v>46.296070501302083</v>
-      </c>
-      <c r="D58" s="111">
-        <v>507.21044557645126</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>163</v>
-      </c>
-      <c r="B59" s="111" t="s">
-        <v>163</v>
-      </c>
-      <c r="C59" s="111">
-        <v>34.871059262781436</v>
-      </c>
-      <c r="D59" s="111">
-        <v>668.88377510394514</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>164</v>
-      </c>
-      <c r="B60" s="111" t="s">
-        <v>164</v>
-      </c>
-      <c r="C60" s="111">
-        <v>44.746252156404559</v>
-      </c>
-      <c r="D60" s="111">
-        <v>654.80340179705718</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>165</v>
-      </c>
-      <c r="B61" s="111" t="s">
-        <v>165</v>
-      </c>
-      <c r="C61" s="111">
-        <v>44.807686766932541</v>
-      </c>
-      <c r="D61" s="111">
-        <v>688.85095964480468</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>166</v>
-      </c>
-      <c r="B62" s="111" t="s">
-        <v>166</v>
-      </c>
-      <c r="C62" s="111">
-        <v>44.200433259008399</v>
-      </c>
-      <c r="D62" s="111">
-        <v>737.59071339941693</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>167</v>
-      </c>
-      <c r="B63" s="111" t="s">
-        <v>167</v>
-      </c>
-      <c r="C63" s="111">
-        <v>43.992111747526693</v>
-      </c>
-      <c r="D63" s="111">
-        <v>765.47381512866104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>168</v>
-      </c>
-      <c r="B64" s="111" t="s">
-        <v>168</v>
-      </c>
-      <c r="C64" s="111">
-        <v>44.298577840334822</v>
-      </c>
-      <c r="D64" s="111">
-        <v>731.67589538225809</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>169</v>
-      </c>
-      <c r="B65" s="111" t="s">
-        <v>169</v>
-      </c>
-      <c r="C65" s="111">
-        <v>33.200025671240915</v>
-      </c>
-      <c r="D65" s="111">
-        <v>800.00032424653136</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>170</v>
-      </c>
-      <c r="B66" s="111" t="s">
-        <v>170</v>
-      </c>
-      <c r="C66" s="111">
-        <v>43.239767721042398</v>
-      </c>
-      <c r="D66" s="111">
-        <v>747.6070630111235</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>344</v>
-      </c>
-      <c r="B67" s="111" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" s="111" t="s">
         <v>174</v>
       </c>
+      <c r="B67" s="111">
+        <v>47.141813661363628</v>
+      </c>
       <c r="C67" s="111">
-        <v>47.141813661363628</v>
-      </c>
-      <c r="D67" s="111">
         <v>0.77692265667854898</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>345</v>
-      </c>
-      <c r="B68" s="111" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" s="111" t="s">
         <v>175</v>
       </c>
+      <c r="B68" s="111">
+        <v>49.999999999999993</v>
+      </c>
       <c r="C68" s="111">
-        <v>49.999999999999993</v>
-      </c>
-      <c r="D68" s="111">
         <v>0.71699999999999986</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>346</v>
-      </c>
-      <c r="B69" s="112" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" s="112" t="s">
         <v>76</v>
       </c>
+      <c r="B69" s="111">
+        <v>119.98674372549019</v>
+      </c>
       <c r="C69" s="111">
+        <v>9.0052398842286357E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" s="112" t="s">
+        <v>320</v>
+      </c>
+      <c r="B70" s="111">
         <v>119.98674372549019</v>
       </c>
-      <c r="D69" s="111">
+      <c r="C70" s="111">
         <v>9.0052398842286357E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>347</v>
-      </c>
-      <c r="B70" s="112" t="s">
-        <v>320</v>
-      </c>
-      <c r="C70" s="111">
-        <v>119.98674372549019</v>
-      </c>
-      <c r="D70" s="111">
-        <v>9.0052398842286357E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>348</v>
-      </c>
-      <c r="B71" s="111" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" s="111" t="s">
         <v>176</v>
       </c>
+      <c r="B71" s="111">
+        <v>0</v>
+      </c>
       <c r="C71" s="111">
-        <v>0</v>
-      </c>
-      <c r="D71" s="111">
         <v>1.9768383817590991</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>349</v>
-      </c>
-      <c r="B72" s="111" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" s="111" t="s">
         <v>177</v>
       </c>
+      <c r="B72" s="111">
+        <v>48.885121247479262</v>
+      </c>
       <c r="C72" s="111">
-        <v>48.885121247479262</v>
-      </c>
-      <c r="D72" s="111">
         <v>0.88356773166440861</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B73" s="50" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" s="50" t="s">
         <v>185</v>
       </c>
-      <c r="D73">
+      <c r="C73">
         <v>1000</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B74" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
         <v>63</v>
       </c>
-      <c r="D74">
+      <c r="C74">
         <v>1000</v>
       </c>
     </row>
@@ -18498,7 +18830,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C295DD4-7C09-4646-A296-16CD0AFAEC63}">
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -18720,139 +19052,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F8F5E2C-DDF2-4E57-AD59-B511AD831FCD}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B1" s="40" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="40" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="17">
-        <v>1</v>
-      </c>
-      <c r="C2" s="27">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="D2" s="28">
-        <v>1E-3</v>
-      </c>
-      <c r="E2" s="29">
-        <v>3.7854109999999998E-3</v>
-      </c>
-      <c r="F2" s="30">
-        <v>2.8316846999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="19">
-        <v>1000000</v>
-      </c>
-      <c r="C3" s="19">
-        <v>1</v>
-      </c>
-      <c r="D3" s="19">
-        <v>1000.0000000000001</v>
-      </c>
-      <c r="E3" s="19">
-        <v>3785.4110000000001</v>
-      </c>
-      <c r="F3" s="21">
-        <v>28316.847000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="19">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="20">
-        <v>1E-3</v>
-      </c>
-      <c r="D4" s="19">
-        <v>1</v>
-      </c>
-      <c r="E4" s="20">
-        <v>3.7854109999999999</v>
-      </c>
-      <c r="F4" s="23">
-        <v>28.316846999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="31">
-        <v>264.17210707106841</v>
-      </c>
-      <c r="C5" s="22">
-        <v>2.6417210707106839E-4</v>
-      </c>
-      <c r="D5" s="20">
-        <v>0.26417210707106842</v>
-      </c>
-      <c r="E5" s="19">
-        <v>1</v>
-      </c>
-      <c r="F5" s="23">
-        <v>7.4805211375990615</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="32">
-        <v>35.314666212661322</v>
-      </c>
-      <c r="C6" s="24">
-        <v>3.5314666212661319E-5</v>
-      </c>
-      <c r="D6" s="25">
-        <v>3.5314666212661321E-2</v>
-      </c>
-      <c r="E6" s="25">
-        <v>0.13368052594273649</v>
-      </c>
-      <c r="F6" s="26">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
1. Modified the backend data file to separate out fuel distribution emissions, 2. Modified the code to handle urban emissions from fuel distribution and fuel combustion separately, 3. The code now can handle end uses for the main product of a preivous stage, 4. Generated a test data file and verfied that the generated LCI file is correct
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78E88364-0692-422B-A300-DE6CA8E11E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B428CC54-1F0B-4E73-83E1-CC9CBBFC82EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="745" activeTab="1" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
-    <sheet name="End use supplement" sheetId="16" r:id="rId2"/>
+    <sheet name="Fuel dist urban" sheetId="16" r:id="rId2"/>
     <sheet name="Production" sheetId="2" r:id="rId3"/>
     <sheet name="Chemicals" sheetId="5" r:id="rId4"/>
     <sheet name="End use" sheetId="3" state="hidden" r:id="rId5"/>
@@ -1620,7 +1620,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1874,7 +1874,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2586,9 +2585,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AH1" sqref="AH1:AY21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR15" sqref="AR15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2596,7 +2595,13 @@
     <col min="1" max="1" width="25.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.1796875" style="86"/>
     <col min="30" max="33" width="8.7265625" style="114"/>
-    <col min="41" max="41" width="13.7265625" customWidth="1"/>
+    <col min="35" max="36" width="8.7265625" style="114"/>
+    <col min="38" max="39" width="8.7265625" style="114"/>
+    <col min="41" max="41" width="13.7265625" style="114" customWidth="1"/>
+    <col min="42" max="42" width="8.7265625" style="114"/>
+    <col min="44" max="45" width="8.7265625" style="114"/>
+    <col min="47" max="48" width="8.7265625" style="114"/>
+    <col min="50" max="51" width="8.7265625" style="114"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:51" s="121" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.35">
@@ -2699,55 +2704,55 @@
       <c r="AH1" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="AI1" s="122" t="s">
+      <c r="AI1" s="124" t="s">
         <v>151</v>
       </c>
-      <c r="AJ1" s="122" t="s">
+      <c r="AJ1" s="124" t="s">
         <v>151</v>
       </c>
       <c r="AK1" s="122" t="s">
         <v>208</v>
       </c>
-      <c r="AL1" s="122" t="s">
+      <c r="AL1" s="124" t="s">
         <v>208</v>
       </c>
-      <c r="AM1" s="122" t="s">
+      <c r="AM1" s="124" t="s">
         <v>208</v>
       </c>
       <c r="AN1" s="122" t="s">
         <v>292</v>
       </c>
-      <c r="AO1" s="122" t="s">
+      <c r="AO1" s="124" t="s">
         <v>292</v>
       </c>
-      <c r="AP1" s="122" t="s">
+      <c r="AP1" s="124" t="s">
         <v>292</v>
       </c>
       <c r="AQ1" s="122" t="s">
         <v>293</v>
       </c>
-      <c r="AR1" s="122" t="s">
+      <c r="AR1" s="124" t="s">
         <v>293</v>
       </c>
-      <c r="AS1" s="122" t="s">
+      <c r="AS1" s="124" t="s">
         <v>293</v>
       </c>
       <c r="AT1" s="122" t="s">
         <v>324</v>
       </c>
-      <c r="AU1" s="122" t="s">
+      <c r="AU1" s="124" t="s">
         <v>324</v>
       </c>
-      <c r="AV1" s="122" t="s">
+      <c r="AV1" s="124" t="s">
         <v>324</v>
       </c>
       <c r="AW1" s="122" t="s">
         <v>325</v>
       </c>
-      <c r="AX1" s="122" t="s">
+      <c r="AX1" s="124" t="s">
         <v>325</v>
       </c>
-      <c r="AY1" s="122" t="s">
+      <c r="AY1" s="124" t="s">
         <v>325</v>
       </c>
     </row>
@@ -2851,55 +2856,55 @@
       <c r="AH2" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="AI2" s="47" t="s">
+      <c r="AI2" s="115" t="s">
         <v>272</v>
       </c>
-      <c r="AJ2" s="47" t="s">
+      <c r="AJ2" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AK2" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="AL2" s="47" t="s">
+      <c r="AL2" s="115" t="s">
         <v>272</v>
       </c>
-      <c r="AM2" s="47" t="s">
+      <c r="AM2" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AN2" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="AO2" s="47" t="s">
+      <c r="AO2" s="115" t="s">
         <v>272</v>
       </c>
-      <c r="AP2" s="47" t="s">
+      <c r="AP2" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AQ2" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="AR2" s="47" t="s">
+      <c r="AR2" s="115" t="s">
         <v>272</v>
       </c>
-      <c r="AS2" s="47" t="s">
+      <c r="AS2" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AT2" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="AU2" s="47" t="s">
+      <c r="AU2" s="115" t="s">
         <v>272</v>
       </c>
-      <c r="AV2" s="47" t="s">
+      <c r="AV2" s="115" t="s">
         <v>273</v>
       </c>
       <c r="AW2" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="AX2" s="47" t="s">
+      <c r="AX2" s="115" t="s">
         <v>272</v>
       </c>
-      <c r="AY2" s="47" t="s">
+      <c r="AY2" s="115" t="s">
         <v>273</v>
       </c>
     </row>
@@ -3006,55 +3011,55 @@
       <c r="AH3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AI3" s="2" t="s">
+      <c r="AI3" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="AJ3" s="2" t="s">
+      <c r="AJ3" s="116" t="s">
         <v>96</v>
       </c>
       <c r="AK3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AL3" s="2" t="s">
+      <c r="AL3" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="AM3" s="2" t="s">
+      <c r="AM3" s="116" t="s">
         <v>96</v>
       </c>
       <c r="AN3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AO3" s="2" t="s">
+      <c r="AO3" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="AP3" s="2" t="s">
+      <c r="AP3" s="116" t="s">
         <v>96</v>
       </c>
       <c r="AQ3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AR3" s="2" t="s">
+      <c r="AR3" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="AS3" s="2" t="s">
+      <c r="AS3" s="116" t="s">
         <v>96</v>
       </c>
       <c r="AT3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AU3" s="2" t="s">
+      <c r="AU3" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="AV3" s="2" t="s">
+      <c r="AV3" s="116" t="s">
         <v>96</v>
       </c>
       <c r="AW3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="AX3" s="2" t="s">
+      <c r="AX3" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="AY3" s="2" t="s">
+      <c r="AY3" s="116" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3153,20 +3158,20 @@
       <c r="AH4" s="2">
         <v>1000000</v>
       </c>
-      <c r="AI4" s="127">
+      <c r="AI4" s="114">
         <v>9339.5518419730979</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="114">
         <f t="shared" ref="AJ4:AJ10" si="0">AH4+AI4</f>
         <v>1009339.5518419731</v>
       </c>
       <c r="AK4" s="2">
         <v>1000000</v>
       </c>
-      <c r="AL4" s="127">
+      <c r="AL4" s="114">
         <v>1253.7917044079659</v>
       </c>
-      <c r="AM4">
+      <c r="AM4" s="114">
         <f>AK4+AL4</f>
         <v>1001253.791704408</v>
       </c>
@@ -3174,11 +3179,11 @@
         <f>AK4</f>
         <v>1000000</v>
       </c>
-      <c r="AO4">
+      <c r="AO4" s="114">
         <f>AL4</f>
         <v>1253.7917044079659</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="114">
         <f>AN4+AO4</f>
         <v>1001253.791704408</v>
       </c>
@@ -3186,11 +3191,11 @@
         <f>AN4</f>
         <v>1000000</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" s="114">
         <f>AL4</f>
         <v>1253.7917044079659</v>
       </c>
-      <c r="AS4">
+      <c r="AS4" s="114">
         <f>AQ4+AR4</f>
         <v>1001253.791704408</v>
       </c>
@@ -3198,11 +3203,11 @@
         <f>AK4</f>
         <v>1000000</v>
       </c>
-      <c r="AU4">
+      <c r="AU4" s="114">
         <f>AL4</f>
         <v>1253.7917044079659</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="114">
         <f>AT4+AU4</f>
         <v>1001253.791704408</v>
       </c>
@@ -3210,11 +3215,11 @@
         <f>AK4</f>
         <v>1000000</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="114">
         <f>AL4</f>
         <v>1253.7917044079659</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" s="114">
         <f>AW4+AX4</f>
         <v>1001253.791704408</v>
       </c>
@@ -3314,20 +3319,20 @@
       <c r="AH5" s="2">
         <v>0</v>
       </c>
-      <c r="AI5" s="127">
+      <c r="AI5" s="114">
         <v>8169.6873553428004</v>
       </c>
-      <c r="AJ5">
+      <c r="AJ5" s="114">
         <f t="shared" si="0"/>
         <v>8169.6873553428004</v>
       </c>
       <c r="AK5" s="2">
         <v>0</v>
       </c>
-      <c r="AL5" s="127">
+      <c r="AL5" s="114">
         <v>1202.5975456032124</v>
       </c>
-      <c r="AM5">
+      <c r="AM5" s="114">
         <f t="shared" ref="AM5:AM9" si="1">AK5+AL5</f>
         <v>1202.5975456032124</v>
       </c>
@@ -3335,11 +3340,11 @@
         <f t="shared" ref="AN5:AN21" si="2">AK5</f>
         <v>0</v>
       </c>
-      <c r="AO5">
+      <c r="AO5" s="114">
         <f t="shared" ref="AO5:AO20" si="3">AL5</f>
         <v>1202.5975456032124</v>
       </c>
-      <c r="AP5">
+      <c r="AP5" s="114">
         <f t="shared" ref="AP5:AP9" si="4">AN5+AO5</f>
         <v>1202.5975456032124</v>
       </c>
@@ -3347,11 +3352,11 @@
         <f t="shared" ref="AQ5:AQ21" si="5">AN5</f>
         <v>0</v>
       </c>
-      <c r="AR5">
+      <c r="AR5" s="114">
         <f t="shared" ref="AR5:AR20" si="6">AL5</f>
         <v>1202.5975456032124</v>
       </c>
-      <c r="AS5">
+      <c r="AS5" s="114">
         <f t="shared" ref="AS5:AS9" si="7">AQ5+AR5</f>
         <v>1202.5975456032124</v>
       </c>
@@ -3359,11 +3364,11 @@
         <f t="shared" ref="AT5:AT21" si="8">AK5</f>
         <v>0</v>
       </c>
-      <c r="AU5">
+      <c r="AU5" s="114">
         <f t="shared" ref="AU5:AU20" si="9">AL5</f>
         <v>1202.5975456032124</v>
       </c>
-      <c r="AV5">
+      <c r="AV5" s="114">
         <f t="shared" ref="AV5:AV9" si="10">AT5+AU5</f>
         <v>1202.5975456032124</v>
       </c>
@@ -3371,11 +3376,11 @@
         <f t="shared" ref="AW5:AW21" si="11">AK5</f>
         <v>0</v>
       </c>
-      <c r="AX5">
+      <c r="AX5" s="114">
         <f t="shared" ref="AX5:AX20" si="12">AL5</f>
         <v>1202.5975456032124</v>
       </c>
-      <c r="AY5">
+      <c r="AY5" s="114">
         <f t="shared" ref="AY5:AY9" si="13">AW5+AX5</f>
         <v>1202.5975456032124</v>
       </c>
@@ -3475,20 +3480,20 @@
       <c r="AH6" s="2">
         <v>0</v>
       </c>
-      <c r="AI6" s="127">
+      <c r="AI6" s="114">
         <v>1989.4630119087635</v>
       </c>
-      <c r="AJ6">
+      <c r="AJ6" s="114">
         <f t="shared" si="0"/>
         <v>1989.4630119087635</v>
       </c>
       <c r="AK6" s="2">
         <v>0</v>
       </c>
-      <c r="AL6" s="127">
+      <c r="AL6" s="114">
         <v>9.9730961197564767</v>
       </c>
-      <c r="AM6">
+      <c r="AM6" s="114">
         <f t="shared" si="1"/>
         <v>9.9730961197564767</v>
       </c>
@@ -3496,11 +3501,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO6">
+      <c r="AO6" s="114">
         <f t="shared" si="3"/>
         <v>9.9730961197564767</v>
       </c>
-      <c r="AP6">
+      <c r="AP6" s="114">
         <f t="shared" si="4"/>
         <v>9.9730961197564767</v>
       </c>
@@ -3508,11 +3513,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AR6">
+      <c r="AR6" s="114">
         <f t="shared" si="6"/>
         <v>9.9730961197564767</v>
       </c>
-      <c r="AS6">
+      <c r="AS6" s="114">
         <f t="shared" si="7"/>
         <v>9.9730961197564767</v>
       </c>
@@ -3520,11 +3525,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AU6">
+      <c r="AU6" s="114">
         <f t="shared" si="9"/>
         <v>9.9730961197564767</v>
       </c>
-      <c r="AV6">
+      <c r="AV6" s="114">
         <f t="shared" si="10"/>
         <v>9.9730961197564767</v>
       </c>
@@ -3532,11 +3537,11 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AX6">
+      <c r="AX6" s="114">
         <f t="shared" si="12"/>
         <v>9.9730961197564767</v>
       </c>
-      <c r="AY6">
+      <c r="AY6" s="114">
         <f t="shared" si="13"/>
         <v>9.9730961197564767</v>
       </c>
@@ -3636,20 +3641,20 @@
       <c r="AH7" s="2">
         <v>0</v>
       </c>
-      <c r="AI7" s="127">
+      <c r="AI7" s="114">
         <v>2794.9003158789556</v>
       </c>
-      <c r="AJ7">
+      <c r="AJ7" s="114">
         <f t="shared" si="0"/>
         <v>2794.9003158789556</v>
       </c>
       <c r="AK7" s="2">
         <v>0</v>
       </c>
-      <c r="AL7" s="127">
+      <c r="AL7" s="114">
         <v>126.35657670942828</v>
       </c>
-      <c r="AM7">
+      <c r="AM7" s="114">
         <f t="shared" si="1"/>
         <v>126.35657670942828</v>
       </c>
@@ -3657,11 +3662,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO7">
+      <c r="AO7" s="114">
         <f t="shared" si="3"/>
         <v>126.35657670942828</v>
       </c>
-      <c r="AP7">
+      <c r="AP7" s="114">
         <f t="shared" si="4"/>
         <v>126.35657670942828</v>
       </c>
@@ -3669,11 +3674,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AR7">
+      <c r="AR7" s="114">
         <f t="shared" si="6"/>
         <v>126.35657670942828</v>
       </c>
-      <c r="AS7">
+      <c r="AS7" s="114">
         <f t="shared" si="7"/>
         <v>126.35657670942828</v>
       </c>
@@ -3681,11 +3686,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AU7">
+      <c r="AU7" s="114">
         <f t="shared" si="9"/>
         <v>126.35657670942828</v>
       </c>
-      <c r="AV7">
+      <c r="AV7" s="114">
         <f t="shared" si="10"/>
         <v>126.35657670942828</v>
       </c>
@@ -3693,11 +3698,11 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AX7">
+      <c r="AX7" s="114">
         <f t="shared" si="12"/>
         <v>126.35657670942828</v>
       </c>
-      <c r="AY7">
+      <c r="AY7" s="114">
         <f t="shared" si="13"/>
         <v>126.35657670942828</v>
       </c>
@@ -3797,20 +3802,20 @@
       <c r="AH8" s="2">
         <v>0</v>
       </c>
-      <c r="AI8" s="127">
+      <c r="AI8" s="114">
         <v>3385.324027555082</v>
       </c>
-      <c r="AJ8">
+      <c r="AJ8" s="114">
         <f t="shared" si="0"/>
         <v>3385.324027555082</v>
       </c>
       <c r="AK8" s="2">
         <v>0</v>
       </c>
-      <c r="AL8" s="127">
+      <c r="AL8" s="114">
         <v>1066.2678727740276</v>
       </c>
-      <c r="AM8">
+      <c r="AM8" s="114">
         <f t="shared" si="1"/>
         <v>1066.2678727740276</v>
       </c>
@@ -3818,11 +3823,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO8">
+      <c r="AO8" s="114">
         <f t="shared" si="3"/>
         <v>1066.2678727740276</v>
       </c>
-      <c r="AP8">
+      <c r="AP8" s="114">
         <f t="shared" si="4"/>
         <v>1066.2678727740276</v>
       </c>
@@ -3830,11 +3835,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AR8">
+      <c r="AR8" s="114">
         <f t="shared" si="6"/>
         <v>1066.2678727740276</v>
       </c>
-      <c r="AS8">
+      <c r="AS8" s="114">
         <f t="shared" si="7"/>
         <v>1066.2678727740276</v>
       </c>
@@ -3842,11 +3847,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AU8">
+      <c r="AU8" s="114">
         <f t="shared" si="9"/>
         <v>1066.2678727740276</v>
       </c>
-      <c r="AV8">
+      <c r="AV8" s="114">
         <f t="shared" si="10"/>
         <v>1066.2678727740276</v>
       </c>
@@ -3854,11 +3859,11 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AX8">
+      <c r="AX8" s="114">
         <f t="shared" si="12"/>
         <v>1066.2678727740276</v>
       </c>
-      <c r="AY8">
+      <c r="AY8" s="114">
         <f t="shared" si="13"/>
         <v>1066.2678727740276</v>
       </c>
@@ -3958,20 +3963,20 @@
       <c r="AH9" s="2">
         <v>0</v>
       </c>
-      <c r="AI9" s="127">
+      <c r="AI9" s="114">
         <v>0.53885408384714351</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="114">
         <f t="shared" si="0"/>
         <v>0.53885408384714351</v>
       </c>
       <c r="AK9" s="2">
         <v>0</v>
       </c>
-      <c r="AL9" s="127">
+      <c r="AL9" s="114">
         <v>2.362854580449477E-2</v>
       </c>
-      <c r="AM9">
+      <c r="AM9" s="114">
         <f t="shared" si="1"/>
         <v>2.362854580449477E-2</v>
       </c>
@@ -3979,11 +3984,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO9">
+      <c r="AO9" s="114">
         <f t="shared" si="3"/>
         <v>2.362854580449477E-2</v>
       </c>
-      <c r="AP9">
+      <c r="AP9" s="114">
         <f t="shared" si="4"/>
         <v>2.362854580449477E-2</v>
       </c>
@@ -3991,11 +3996,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AR9">
+      <c r="AR9" s="114">
         <f t="shared" si="6"/>
         <v>2.362854580449477E-2</v>
       </c>
-      <c r="AS9">
+      <c r="AS9" s="114">
         <f t="shared" si="7"/>
         <v>2.362854580449477E-2</v>
       </c>
@@ -4003,11 +4008,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AU9">
+      <c r="AU9" s="114">
         <f t="shared" si="9"/>
         <v>2.362854580449477E-2</v>
       </c>
-      <c r="AV9">
+      <c r="AV9" s="114">
         <f t="shared" si="10"/>
         <v>2.362854580449477E-2</v>
       </c>
@@ -4015,11 +4020,11 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AX9">
+      <c r="AX9" s="114">
         <f t="shared" si="12"/>
         <v>2.362854580449477E-2</v>
       </c>
-      <c r="AY9">
+      <c r="AY9" s="114">
         <f t="shared" si="13"/>
         <v>2.362854580449477E-2</v>
       </c>
@@ -4119,20 +4124,20 @@
       <c r="AH10">
         <v>53.59747463028841</v>
       </c>
-      <c r="AI10" s="127">
+      <c r="AI10" s="114">
         <v>0.12683831523481029</v>
       </c>
-      <c r="AJ10">
+      <c r="AJ10" s="114">
         <f t="shared" si="0"/>
         <v>53.724312945523224</v>
       </c>
       <c r="AK10">
         <v>40.352647182660228</v>
       </c>
-      <c r="AL10" s="127">
+      <c r="AL10" s="114">
         <v>1.424806237772471E-2</v>
       </c>
-      <c r="AM10">
+      <c r="AM10" s="114">
         <f>AK10+AL10</f>
         <v>40.366895245037952</v>
       </c>
@@ -4140,11 +4145,11 @@
         <f t="shared" si="2"/>
         <v>40.352647182660228</v>
       </c>
-      <c r="AO10">
+      <c r="AO10" s="114">
         <f t="shared" si="3"/>
         <v>1.424806237772471E-2</v>
       </c>
-      <c r="AP10">
+      <c r="AP10" s="114">
         <f>AN10+AO10</f>
         <v>40.366895245037952</v>
       </c>
@@ -4152,11 +4157,11 @@
         <f t="shared" si="5"/>
         <v>40.352647182660228</v>
       </c>
-      <c r="AR10">
+      <c r="AR10" s="114">
         <f t="shared" si="6"/>
         <v>1.424806237772471E-2</v>
       </c>
-      <c r="AS10">
+      <c r="AS10" s="114">
         <f>AQ10+AR10</f>
         <v>40.366895245037952</v>
       </c>
@@ -4164,11 +4169,11 @@
         <f t="shared" si="8"/>
         <v>40.352647182660228</v>
       </c>
-      <c r="AU10">
+      <c r="AU10" s="114">
         <f t="shared" si="9"/>
         <v>1.424806237772471E-2</v>
       </c>
-      <c r="AV10">
+      <c r="AV10" s="114">
         <f>AT10+AU10</f>
         <v>40.366895245037952</v>
       </c>
@@ -4176,11 +4181,11 @@
         <f t="shared" si="11"/>
         <v>40.352647182660228</v>
       </c>
-      <c r="AX10">
+      <c r="AX10" s="114">
         <f t="shared" si="12"/>
         <v>1.424806237772471E-2</v>
       </c>
-      <c r="AY10">
+      <c r="AY10" s="114">
         <f>AW10+AX10</f>
         <v>40.366895245037952</v>
       </c>
@@ -4280,20 +4285,20 @@
       <c r="AH11">
         <v>639.10415070792988</v>
       </c>
-      <c r="AI11" s="127">
+      <c r="AI11" s="114">
         <v>0.54395091021563391</v>
       </c>
-      <c r="AJ11">
+      <c r="AJ11" s="114">
         <f t="shared" ref="AJ11:AJ21" si="14">AH11+AI11</f>
         <v>639.64810161814546</v>
       </c>
       <c r="AK11">
         <v>993.80073264760836</v>
       </c>
-      <c r="AL11" s="127">
+      <c r="AL11" s="114">
         <v>0.19647676496293282</v>
       </c>
-      <c r="AM11">
+      <c r="AM11" s="114">
         <f t="shared" ref="AM11:AM21" si="15">AK11+AL11</f>
         <v>993.99720941257124</v>
       </c>
@@ -4301,11 +4306,11 @@
         <f t="shared" si="2"/>
         <v>993.80073264760836</v>
       </c>
-      <c r="AO11">
+      <c r="AO11" s="114">
         <f t="shared" si="3"/>
         <v>0.19647676496293282</v>
       </c>
-      <c r="AP11">
+      <c r="AP11" s="114">
         <f t="shared" ref="AP11:AP21" si="16">AN11+AO11</f>
         <v>993.99720941257124</v>
       </c>
@@ -4313,11 +4318,11 @@
         <f t="shared" si="5"/>
         <v>993.80073264760836</v>
       </c>
-      <c r="AR11">
+      <c r="AR11" s="114">
         <f t="shared" si="6"/>
         <v>0.19647676496293282</v>
       </c>
-      <c r="AS11">
+      <c r="AS11" s="114">
         <f t="shared" ref="AS11:AS21" si="17">AQ11+AR11</f>
         <v>993.99720941257124</v>
       </c>
@@ -4325,11 +4330,11 @@
         <f t="shared" si="8"/>
         <v>993.80073264760836</v>
       </c>
-      <c r="AU11">
+      <c r="AU11" s="114">
         <f t="shared" si="9"/>
         <v>0.19647676496293282</v>
       </c>
-      <c r="AV11">
+      <c r="AV11" s="114">
         <f t="shared" ref="AV11:AV21" si="18">AT11+AU11</f>
         <v>993.99720941257124</v>
       </c>
@@ -4337,11 +4342,11 @@
         <f t="shared" si="11"/>
         <v>993.80073264760836</v>
       </c>
-      <c r="AX11">
+      <c r="AX11" s="114">
         <f t="shared" si="12"/>
         <v>0.19647676496293282</v>
       </c>
-      <c r="AY11">
+      <c r="AY11" s="114">
         <f t="shared" ref="AY11:AY21" si="19">AW11+AX11</f>
         <v>993.99720941257124</v>
       </c>
@@ -4441,20 +4446,20 @@
       <c r="AH12">
         <v>19.208734314891956</v>
       </c>
-      <c r="AI12" s="127">
+      <c r="AI12" s="114">
         <v>1.4670490677357695</v>
       </c>
-      <c r="AJ12">
+      <c r="AJ12" s="114">
         <f t="shared" si="14"/>
         <v>20.675783382627724</v>
       </c>
       <c r="AK12">
         <v>27.387619255967515</v>
       </c>
-      <c r="AL12" s="127">
+      <c r="AL12" s="114">
         <v>0.13480292599982197</v>
       </c>
-      <c r="AM12">
+      <c r="AM12" s="114">
         <f t="shared" si="15"/>
         <v>27.522422181967336</v>
       </c>
@@ -4462,11 +4467,11 @@
         <f t="shared" si="2"/>
         <v>27.387619255967515</v>
       </c>
-      <c r="AO12">
+      <c r="AO12" s="114">
         <f t="shared" si="3"/>
         <v>0.13480292599982197</v>
       </c>
-      <c r="AP12">
+      <c r="AP12" s="114">
         <f t="shared" si="16"/>
         <v>27.522422181967336</v>
       </c>
@@ -4474,11 +4479,11 @@
         <f t="shared" si="5"/>
         <v>27.387619255967515</v>
       </c>
-      <c r="AR12">
+      <c r="AR12" s="114">
         <f t="shared" si="6"/>
         <v>0.13480292599982197</v>
       </c>
-      <c r="AS12">
+      <c r="AS12" s="114">
         <f t="shared" si="17"/>
         <v>27.522422181967336</v>
       </c>
@@ -4486,11 +4491,11 @@
         <f t="shared" si="8"/>
         <v>27.387619255967515</v>
       </c>
-      <c r="AU12">
+      <c r="AU12" s="114">
         <f t="shared" si="9"/>
         <v>0.13480292599982197</v>
       </c>
-      <c r="AV12">
+      <c r="AV12" s="114">
         <f t="shared" si="18"/>
         <v>27.522422181967336</v>
       </c>
@@ -4498,11 +4503,11 @@
         <f t="shared" si="11"/>
         <v>27.387619255967515</v>
       </c>
-      <c r="AX12">
+      <c r="AX12" s="114">
         <f t="shared" si="12"/>
         <v>0.13480292599982197</v>
       </c>
-      <c r="AY12">
+      <c r="AY12" s="114">
         <f t="shared" si="19"/>
         <v>27.522422181967336</v>
       </c>
@@ -4602,20 +4607,20 @@
       <c r="AH13">
         <v>8.0441472410106218</v>
       </c>
-      <c r="AI13" s="127">
+      <c r="AI13" s="114">
         <v>7.2523053711609858E-2</v>
       </c>
-      <c r="AJ13">
+      <c r="AJ13" s="114">
         <f t="shared" si="14"/>
         <v>8.1166702947222316</v>
       </c>
       <c r="AK13">
         <v>9.458769751780995</v>
       </c>
-      <c r="AL13" s="127">
+      <c r="AL13" s="114">
         <v>7.5690024594833967E-3</v>
       </c>
-      <c r="AM13">
+      <c r="AM13" s="114">
         <f t="shared" si="15"/>
         <v>9.4663387542404784</v>
       </c>
@@ -4623,11 +4628,11 @@
         <f t="shared" si="2"/>
         <v>9.458769751780995</v>
       </c>
-      <c r="AO13">
+      <c r="AO13" s="114">
         <f t="shared" si="3"/>
         <v>7.5690024594833967E-3</v>
       </c>
-      <c r="AP13">
+      <c r="AP13" s="114">
         <f t="shared" si="16"/>
         <v>9.4663387542404784</v>
       </c>
@@ -4635,11 +4640,11 @@
         <f t="shared" si="5"/>
         <v>9.458769751780995</v>
       </c>
-      <c r="AR13">
+      <c r="AR13" s="114">
         <f t="shared" si="6"/>
         <v>7.5690024594833967E-3</v>
       </c>
-      <c r="AS13">
+      <c r="AS13" s="114">
         <f t="shared" si="17"/>
         <v>9.4663387542404784</v>
       </c>
@@ -4647,11 +4652,11 @@
         <f t="shared" si="8"/>
         <v>9.458769751780995</v>
       </c>
-      <c r="AU13">
+      <c r="AU13" s="114">
         <f t="shared" si="9"/>
         <v>7.5690024594833967E-3</v>
       </c>
-      <c r="AV13">
+      <c r="AV13" s="114">
         <f t="shared" si="18"/>
         <v>9.4663387542404784</v>
       </c>
@@ -4659,11 +4664,11 @@
         <f t="shared" si="11"/>
         <v>9.458769751780995</v>
       </c>
-      <c r="AX13">
+      <c r="AX13" s="114">
         <f t="shared" si="12"/>
         <v>7.5690024594833967E-3</v>
       </c>
-      <c r="AY13">
+      <c r="AY13" s="114">
         <f t="shared" si="19"/>
         <v>9.4663387542404784</v>
       </c>
@@ -4763,20 +4768,20 @@
       <c r="AH14">
         <v>1.728649515788488</v>
       </c>
-      <c r="AI14" s="127">
+      <c r="AI14" s="114">
         <v>4.8091315083300508E-2</v>
       </c>
-      <c r="AJ14">
+      <c r="AJ14" s="114">
         <f t="shared" si="14"/>
         <v>1.7767408308717885</v>
       </c>
       <c r="AK14">
         <v>1.8922698715311803</v>
       </c>
-      <c r="AL14" s="127">
+      <c r="AL14" s="114">
         <v>2.2203423357761371E-3</v>
       </c>
-      <c r="AM14">
+      <c r="AM14" s="114">
         <f t="shared" si="15"/>
         <v>1.8944902138669564</v>
       </c>
@@ -4784,11 +4789,11 @@
         <f t="shared" si="2"/>
         <v>1.8922698715311803</v>
       </c>
-      <c r="AO14">
+      <c r="AO14" s="114">
         <f t="shared" si="3"/>
         <v>2.2203423357761371E-3</v>
       </c>
-      <c r="AP14">
+      <c r="AP14" s="114">
         <f t="shared" si="16"/>
         <v>1.8944902138669564</v>
       </c>
@@ -4796,11 +4801,11 @@
         <f t="shared" si="5"/>
         <v>1.8922698715311803</v>
       </c>
-      <c r="AR14">
+      <c r="AR14" s="114">
         <f t="shared" si="6"/>
         <v>2.2203423357761371E-3</v>
       </c>
-      <c r="AS14">
+      <c r="AS14" s="114">
         <f t="shared" si="17"/>
         <v>1.8944902138669564</v>
       </c>
@@ -4808,11 +4813,11 @@
         <f t="shared" si="8"/>
         <v>1.8922698715311803</v>
       </c>
-      <c r="AU14">
+      <c r="AU14" s="114">
         <f t="shared" si="9"/>
         <v>2.2203423357761371E-3</v>
       </c>
-      <c r="AV14">
+      <c r="AV14" s="114">
         <f t="shared" si="18"/>
         <v>1.8944902138669564</v>
       </c>
@@ -4820,11 +4825,11 @@
         <f t="shared" si="11"/>
         <v>1.8922698715311803</v>
       </c>
-      <c r="AX14">
+      <c r="AX14" s="114">
         <f t="shared" si="12"/>
         <v>2.2203423357761371E-3</v>
       </c>
-      <c r="AY14">
+      <c r="AY14" s="114">
         <f t="shared" si="19"/>
         <v>1.8944902138669564</v>
       </c>
@@ -4924,20 +4929,20 @@
       <c r="AH15">
         <v>0.47886752155609885</v>
       </c>
-      <c r="AI15" s="127">
+      <c r="AI15" s="114">
         <v>0.25121575444697092</v>
       </c>
-      <c r="AJ15">
+      <c r="AJ15" s="114">
         <f t="shared" si="14"/>
         <v>0.73008327600306977</v>
       </c>
       <c r="AK15">
         <v>0</v>
       </c>
-      <c r="AL15" s="127">
+      <c r="AL15" s="114">
         <v>5.86909788230092E-3</v>
       </c>
-      <c r="AM15">
+      <c r="AM15" s="114">
         <f t="shared" si="15"/>
         <v>5.86909788230092E-3</v>
       </c>
@@ -4945,11 +4950,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AO15">
+      <c r="AO15" s="114">
         <f t="shared" si="3"/>
         <v>5.86909788230092E-3</v>
       </c>
-      <c r="AP15">
+      <c r="AP15" s="114">
         <f t="shared" si="16"/>
         <v>5.86909788230092E-3</v>
       </c>
@@ -4957,11 +4962,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="AR15">
+      <c r="AR15" s="114">
         <f t="shared" si="6"/>
         <v>5.86909788230092E-3</v>
       </c>
-      <c r="AS15">
+      <c r="AS15" s="114">
         <f t="shared" si="17"/>
         <v>5.86909788230092E-3</v>
       </c>
@@ -4969,11 +4974,11 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AU15">
+      <c r="AU15" s="114">
         <f t="shared" si="9"/>
         <v>5.86909788230092E-3</v>
       </c>
-      <c r="AV15">
+      <c r="AV15" s="114">
         <f t="shared" si="18"/>
         <v>5.86909788230092E-3</v>
       </c>
@@ -4981,11 +4986,11 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AX15">
+      <c r="AX15" s="114">
         <f t="shared" si="12"/>
         <v>5.86909788230092E-3</v>
       </c>
-      <c r="AY15">
+      <c r="AY15" s="114">
         <f t="shared" si="19"/>
         <v>5.86909788230092E-3</v>
       </c>
@@ -5081,20 +5086,20 @@
       <c r="AH16">
         <v>0.47390947465623479</v>
       </c>
-      <c r="AI16" s="127">
+      <c r="AI16" s="114">
         <v>4.2349995275388881E-3</v>
       </c>
-      <c r="AJ16">
+      <c r="AJ16" s="114">
         <f t="shared" si="14"/>
         <v>0.47814447418377365</v>
       </c>
       <c r="AK16">
         <v>0.51210428280035414</v>
       </c>
-      <c r="AL16" s="127">
+      <c r="AL16" s="114">
         <v>2.1219130796210544E-4</v>
       </c>
-      <c r="AM16">
+      <c r="AM16" s="114">
         <f t="shared" si="15"/>
         <v>0.51231647410831627</v>
       </c>
@@ -5102,11 +5107,11 @@
         <f t="shared" si="2"/>
         <v>0.51210428280035414</v>
       </c>
-      <c r="AO16">
+      <c r="AO16" s="114">
         <f t="shared" si="3"/>
         <v>2.1219130796210544E-4</v>
       </c>
-      <c r="AP16">
+      <c r="AP16" s="114">
         <f t="shared" si="16"/>
         <v>0.51231647410831627</v>
       </c>
@@ -5114,11 +5119,11 @@
         <f t="shared" si="5"/>
         <v>0.51210428280035414</v>
       </c>
-      <c r="AR16">
+      <c r="AR16" s="114">
         <f t="shared" si="6"/>
         <v>2.1219130796210544E-4</v>
       </c>
-      <c r="AS16">
+      <c r="AS16" s="114">
         <f t="shared" si="17"/>
         <v>0.51231647410831627</v>
       </c>
@@ -5126,11 +5131,11 @@
         <f t="shared" si="8"/>
         <v>0.51210428280035414</v>
       </c>
-      <c r="AU16">
+      <c r="AU16" s="114">
         <f t="shared" si="9"/>
         <v>2.1219130796210544E-4</v>
       </c>
-      <c r="AV16">
+      <c r="AV16" s="114">
         <f t="shared" si="18"/>
         <v>0.51231647410831627</v>
       </c>
@@ -5138,11 +5143,11 @@
         <f t="shared" si="11"/>
         <v>0.51210428280035414</v>
       </c>
-      <c r="AX16">
+      <c r="AX16" s="114">
         <f t="shared" si="12"/>
         <v>2.1219130796210544E-4</v>
       </c>
-      <c r="AY16">
+      <c r="AY16" s="114">
         <f t="shared" si="19"/>
         <v>0.51231647410831627</v>
       </c>
@@ -5238,20 +5243,20 @@
       <c r="AH17">
         <v>0.24585827527712426</v>
       </c>
-      <c r="AI17" s="127">
+      <c r="AI17" s="114">
         <v>2.0560277799938402E-2</v>
       </c>
-      <c r="AJ17">
+      <c r="AJ17" s="114">
         <f t="shared" si="14"/>
         <v>0.26641855307706264</v>
       </c>
       <c r="AK17">
         <v>7.6630038890183744E-2</v>
       </c>
-      <c r="AL17" s="127">
+      <c r="AL17" s="114">
         <v>3.8366125882774188E-4</v>
       </c>
-      <c r="AM17">
+      <c r="AM17" s="114">
         <f t="shared" si="15"/>
         <v>7.7013700149011488E-2</v>
       </c>
@@ -5259,11 +5264,11 @@
         <f t="shared" si="2"/>
         <v>7.6630038890183744E-2</v>
       </c>
-      <c r="AO17">
+      <c r="AO17" s="114">
         <f t="shared" si="3"/>
         <v>3.8366125882774188E-4</v>
       </c>
-      <c r="AP17">
+      <c r="AP17" s="114">
         <f t="shared" si="16"/>
         <v>7.7013700149011488E-2</v>
       </c>
@@ -5271,11 +5276,11 @@
         <f t="shared" si="5"/>
         <v>7.6630038890183744E-2</v>
       </c>
-      <c r="AR17">
+      <c r="AR17" s="114">
         <f t="shared" si="6"/>
         <v>3.8366125882774188E-4</v>
       </c>
-      <c r="AS17">
+      <c r="AS17" s="114">
         <f t="shared" si="17"/>
         <v>7.7013700149011488E-2</v>
       </c>
@@ -5283,11 +5288,11 @@
         <f t="shared" si="8"/>
         <v>7.6630038890183744E-2</v>
       </c>
-      <c r="AU17">
+      <c r="AU17" s="114">
         <f t="shared" si="9"/>
         <v>3.8366125882774188E-4</v>
       </c>
-      <c r="AV17">
+      <c r="AV17" s="114">
         <f t="shared" si="18"/>
         <v>7.7013700149011488E-2</v>
       </c>
@@ -5295,11 +5300,11 @@
         <f t="shared" si="11"/>
         <v>7.6630038890183744E-2</v>
       </c>
-      <c r="AX17">
+      <c r="AX17" s="114">
         <f t="shared" si="12"/>
         <v>3.8366125882774188E-4</v>
       </c>
-      <c r="AY17">
+      <c r="AY17" s="114">
         <f t="shared" si="19"/>
         <v>7.7013700149011488E-2</v>
       </c>
@@ -5395,20 +5400,20 @@
       <c r="AH18">
         <v>3.4141251927898666</v>
       </c>
-      <c r="AI18" s="127">
+      <c r="AI18" s="114">
         <v>1.0961495941820574</v>
       </c>
-      <c r="AJ18">
+      <c r="AJ18" s="114">
         <f t="shared" si="14"/>
         <v>4.510274786971924</v>
       </c>
       <c r="AK18">
         <v>25.825694196902546</v>
       </c>
-      <c r="AL18" s="127">
+      <c r="AL18" s="114">
         <v>0.11480309838857856</v>
       </c>
-      <c r="AM18">
+      <c r="AM18" s="114">
         <f t="shared" si="15"/>
         <v>25.940497295291124</v>
       </c>
@@ -5416,11 +5421,11 @@
         <f t="shared" si="2"/>
         <v>25.825694196902546</v>
       </c>
-      <c r="AO18">
+      <c r="AO18" s="114">
         <f t="shared" si="3"/>
         <v>0.11480309838857856</v>
       </c>
-      <c r="AP18">
+      <c r="AP18" s="114">
         <f t="shared" si="16"/>
         <v>25.940497295291124</v>
       </c>
@@ -5428,11 +5433,11 @@
         <f t="shared" si="5"/>
         <v>25.825694196902546</v>
       </c>
-      <c r="AR18">
+      <c r="AR18" s="114">
         <f t="shared" si="6"/>
         <v>0.11480309838857856</v>
       </c>
-      <c r="AS18">
+      <c r="AS18" s="114">
         <f t="shared" si="17"/>
         <v>25.940497295291124</v>
       </c>
@@ -5440,11 +5445,11 @@
         <f t="shared" si="8"/>
         <v>25.825694196902546</v>
       </c>
-      <c r="AU18">
+      <c r="AU18" s="114">
         <f t="shared" si="9"/>
         <v>0.11480309838857856</v>
       </c>
-      <c r="AV18">
+      <c r="AV18" s="114">
         <f t="shared" si="18"/>
         <v>25.940497295291124</v>
       </c>
@@ -5452,11 +5457,11 @@
         <f t="shared" si="11"/>
         <v>25.825694196902546</v>
       </c>
-      <c r="AX18">
+      <c r="AX18" s="114">
         <f t="shared" si="12"/>
         <v>0.11480309838857856</v>
       </c>
-      <c r="AY18">
+      <c r="AY18" s="114">
         <f t="shared" si="19"/>
         <v>25.940497295291124</v>
       </c>
@@ -5552,20 +5557,20 @@
       <c r="AH19">
         <v>0.91142919415811929</v>
       </c>
-      <c r="AI19" s="127">
+      <c r="AI19" s="114">
         <v>1.2419532449195709E-2</v>
       </c>
-      <c r="AJ19">
+      <c r="AJ19" s="114">
         <f t="shared" si="14"/>
         <v>0.92384872660731499</v>
       </c>
       <c r="AK19">
         <v>0.18877324129794976</v>
       </c>
-      <c r="AL19" s="127">
+      <c r="AL19" s="114">
         <v>3.7018497329376407E-4</v>
       </c>
-      <c r="AM19">
+      <c r="AM19" s="114">
         <f t="shared" si="15"/>
         <v>0.18914342627124353</v>
       </c>
@@ -5573,11 +5578,11 @@
         <f t="shared" si="2"/>
         <v>0.18877324129794976</v>
       </c>
-      <c r="AO19">
+      <c r="AO19" s="114">
         <f t="shared" si="3"/>
         <v>3.7018497329376407E-4</v>
       </c>
-      <c r="AP19">
+      <c r="AP19" s="114">
         <f t="shared" si="16"/>
         <v>0.18914342627124353</v>
       </c>
@@ -5585,11 +5590,11 @@
         <f t="shared" si="5"/>
         <v>0.18877324129794976</v>
       </c>
-      <c r="AR19">
+      <c r="AR19" s="114">
         <f t="shared" si="6"/>
         <v>3.7018497329376407E-4</v>
       </c>
-      <c r="AS19">
+      <c r="AS19" s="114">
         <f t="shared" si="17"/>
         <v>0.18914342627124353</v>
       </c>
@@ -5597,11 +5602,11 @@
         <f t="shared" si="8"/>
         <v>0.18877324129794976</v>
       </c>
-      <c r="AU19">
+      <c r="AU19" s="114">
         <f t="shared" si="9"/>
         <v>3.7018497329376407E-4</v>
       </c>
-      <c r="AV19">
+      <c r="AV19" s="114">
         <f t="shared" si="18"/>
         <v>0.18914342627124353</v>
       </c>
@@ -5609,11 +5614,11 @@
         <f t="shared" si="11"/>
         <v>0.18877324129794976</v>
       </c>
-      <c r="AX19">
+      <c r="AX19" s="114">
         <f t="shared" si="12"/>
         <v>3.7018497329376407E-4</v>
       </c>
-      <c r="AY19">
+      <c r="AY19" s="114">
         <f t="shared" si="19"/>
         <v>0.18914342627124353</v>
       </c>
@@ -5725,20 +5730,20 @@
       <c r="AH20">
         <v>71783.505317547926</v>
       </c>
-      <c r="AI20" s="127">
+      <c r="AI20" s="114">
         <v>633.15471120171344</v>
       </c>
-      <c r="AJ20">
+      <c r="AJ20" s="114">
         <f t="shared" si="14"/>
         <v>72416.66002874964</v>
       </c>
       <c r="AK20">
         <v>74856.053349714566</v>
       </c>
-      <c r="AL20" s="127">
+      <c r="AL20" s="114">
         <v>92.811588579119217</v>
       </c>
-      <c r="AM20">
+      <c r="AM20" s="114">
         <f t="shared" si="15"/>
         <v>74948.864938293686</v>
       </c>
@@ -5746,11 +5751,11 @@
         <f t="shared" si="2"/>
         <v>74856.053349714566</v>
       </c>
-      <c r="AO20">
+      <c r="AO20" s="114">
         <f t="shared" si="3"/>
         <v>92.811588579119217</v>
       </c>
-      <c r="AP20">
+      <c r="AP20" s="114">
         <f t="shared" si="16"/>
         <v>74948.864938293686</v>
       </c>
@@ -5758,11 +5763,11 @@
         <f t="shared" si="5"/>
         <v>74856.053349714566</v>
       </c>
-      <c r="AR20">
+      <c r="AR20" s="114">
         <f t="shared" si="6"/>
         <v>92.811588579119217</v>
       </c>
-      <c r="AS20">
+      <c r="AS20" s="114">
         <f t="shared" si="17"/>
         <v>74948.864938293686</v>
       </c>
@@ -5770,11 +5775,11 @@
         <f t="shared" si="8"/>
         <v>74856.053349714566</v>
       </c>
-      <c r="AU20">
+      <c r="AU20" s="114">
         <f t="shared" si="9"/>
         <v>92.811588579119217</v>
       </c>
-      <c r="AV20">
+      <c r="AV20" s="114">
         <f t="shared" si="18"/>
         <v>74948.864938293686</v>
       </c>
@@ -5782,11 +5787,11 @@
         <f t="shared" si="11"/>
         <v>74856.053349714566</v>
       </c>
-      <c r="AX20">
+      <c r="AX20" s="114">
         <f t="shared" si="12"/>
         <v>92.811588579119217</v>
       </c>
-      <c r="AY20">
+      <c r="AY20" s="114">
         <f t="shared" si="19"/>
         <v>74948.864938293686</v>
       </c>
@@ -5847,14 +5852,14 @@
       <c r="AH21">
         <v>-72964.246146966863</v>
       </c>
-      <c r="AJ21">
+      <c r="AJ21" s="114">
         <f t="shared" si="14"/>
         <v>-72964.246146966863</v>
       </c>
       <c r="AK21">
         <v>-76614.526624731123</v>
       </c>
-      <c r="AM21">
+      <c r="AM21" s="114">
         <f t="shared" si="15"/>
         <v>-76614.526624731123</v>
       </c>
@@ -5862,7 +5867,7 @@
         <f t="shared" si="2"/>
         <v>-76614.526624731123</v>
       </c>
-      <c r="AP21">
+      <c r="AP21" s="114">
         <f t="shared" si="16"/>
         <v>-76614.526624731123</v>
       </c>
@@ -5870,7 +5875,7 @@
         <f t="shared" si="5"/>
         <v>-76614.526624731123</v>
       </c>
-      <c r="AS21">
+      <c r="AS21" s="114">
         <f t="shared" si="17"/>
         <v>-76614.526624731123</v>
       </c>
@@ -5878,7 +5883,7 @@
         <f t="shared" si="8"/>
         <v>-76614.526624731123</v>
       </c>
-      <c r="AV21">
+      <c r="AV21" s="114">
         <f t="shared" si="18"/>
         <v>-76614.526624731123</v>
       </c>
@@ -5886,7 +5891,7 @@
         <f t="shared" si="11"/>
         <v>-76614.526624731123</v>
       </c>
-      <c r="AY21">
+      <c r="AY21" s="114">
         <f t="shared" si="19"/>
         <v>-76614.526624731123</v>
       </c>
@@ -5968,18 +5973,14 @@
       <c r="AD23" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="AI23" s="51" t="s">
+      <c r="AI23" s="114" t="s">
         <v>274</v>
       </c>
-      <c r="AJ23" s="51"/>
       <c r="AK23" s="51"/>
-      <c r="AL23" s="51"/>
-      <c r="AM23" s="51"/>
       <c r="AN23" s="51"/>
-      <c r="AO23" s="51" t="s">
+      <c r="AO23" s="114" t="s">
         <v>274</v>
       </c>
-      <c r="AP23" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7903,94 +7904,62 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{498187A9-5554-4C33-80C2-40670D1F38AD}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="52.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="52.5" x14ac:dyDescent="0.35">
       <c r="B1" s="122" t="s">
         <v>151</v>
       </c>
       <c r="C1" s="122" t="s">
-        <v>151</v>
+        <v>208</v>
       </c>
       <c r="D1" s="122" t="s">
-        <v>208</v>
+        <v>292</v>
       </c>
       <c r="E1" s="122" t="s">
-        <v>208</v>
+        <v>293</v>
       </c>
       <c r="F1" s="122" t="s">
-        <v>292</v>
+        <v>324</v>
       </c>
       <c r="G1" s="122" t="s">
-        <v>292</v>
-      </c>
-      <c r="H1" s="122" t="s">
-        <v>293</v>
-      </c>
-      <c r="I1" s="122" t="s">
-        <v>293</v>
-      </c>
-      <c r="J1" s="122" t="s">
-        <v>324</v>
-      </c>
-      <c r="K1" s="122" t="s">
-        <v>324</v>
-      </c>
-      <c r="L1" s="122" t="s">
         <v>325</v>
       </c>
-      <c r="M1" s="122" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="78.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" ht="39.5" x14ac:dyDescent="0.35">
       <c r="B2" s="47" t="s">
         <v>272</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D2" s="47" t="s">
         <v>272</v>
       </c>
       <c r="E2" s="47" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F2" s="47" t="s">
         <v>272</v>
       </c>
       <c r="G2" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="H2" s="47" t="s">
         <v>272</v>
       </c>
-      <c r="I2" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="J2" s="47" t="s">
-        <v>272</v>
-      </c>
-      <c r="K2" s="47" t="s">
-        <v>273</v>
-      </c>
-      <c r="L2" s="47" t="s">
-        <v>272</v>
-      </c>
-      <c r="M2" s="47" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>341</v>
+      </c>
       <c r="B3" s="2" t="s">
         <v>96</v>
       </c>
@@ -8009,308 +7978,681 @@
       <c r="G3" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="95" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>9339.5518419730979</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1253.7917044079659</v>
+      </c>
+      <c r="D4" s="2">
+        <f>C4</f>
+        <v>1253.7917044079659</v>
+      </c>
+      <c r="E4" s="2">
+        <f>C4</f>
+        <v>1253.7917044079659</v>
+      </c>
+      <c r="F4" s="2">
+        <f>C4</f>
+        <v>1253.7917044079659</v>
+      </c>
+      <c r="G4" s="2">
+        <f>C4</f>
+        <v>1253.7917044079659</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>8169.6873553428004</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1202.5975456032124</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" ref="D5:D20" si="0">C5</f>
+        <v>1202.5975456032124</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ref="E5:E20" si="1">C5</f>
+        <v>1202.5975456032124</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" ref="F5:F20" si="2">C5</f>
+        <v>1202.5975456032124</v>
+      </c>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G20" si="3">C5</f>
+        <v>1202.5975456032124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1989.4630119087635</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9.9730961197564767</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>9.9730961197564767</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>9.9730961197564767</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="2"/>
+        <v>9.9730961197564767</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" si="3"/>
+        <v>9.9730961197564767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2794.9003158789556</v>
+      </c>
+      <c r="C7" s="2">
+        <v>126.35657670942828</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>126.35657670942828</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>126.35657670942828</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="2"/>
+        <v>126.35657670942828</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="3"/>
+        <v>126.35657670942828</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3385.324027555082</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1066.2678727740276</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>1066.2678727740276</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>1066.2678727740276</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="2"/>
+        <v>1066.2678727740276</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="3"/>
+        <v>1066.2678727740276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.53885408384714351</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.362854580449477E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>2.362854580449477E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>2.362854580449477E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="2"/>
+        <v>2.362854580449477E-2</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="3"/>
+        <v>2.362854580449477E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.12683831523481029</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1.424806237772471E-2</v>
+      </c>
+      <c r="D10" s="2">
+        <f t="shared" si="0"/>
+        <v>1.424806237772471E-2</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="1"/>
+        <v>1.424806237772471E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="2"/>
+        <v>1.424806237772471E-2</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="3"/>
+        <v>1.424806237772471E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.54395091021563391</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.19647676496293282</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.19647676496293282</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="1"/>
+        <v>0.19647676496293282</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.19647676496293282</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="3"/>
+        <v>0.19647676496293282</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1.4670490677357695</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.13480292599982197</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.13480292599982197</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="1"/>
+        <v>0.13480292599982197</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.13480292599982197</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13480292599982197</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>7.2523053711609858E-2</v>
+      </c>
+      <c r="C13" s="2">
+        <v>7.5690024594833967E-3</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>7.5690024594833967E-3</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="1"/>
+        <v>7.5690024594833967E-3</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="2"/>
+        <v>7.5690024594833967E-3</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="3"/>
+        <v>7.5690024594833967E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>4.8091315083300508E-2</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2.2203423357761371E-3</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="0"/>
+        <v>2.2203423357761371E-3</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="1"/>
+        <v>2.2203423357761371E-3</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="2"/>
+        <v>2.2203423357761371E-3</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="3"/>
+        <v>2.2203423357761371E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.25121575444697092</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5.86909788230092E-3</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="0"/>
+        <v>5.86909788230092E-3</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>5.86909788230092E-3</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="2"/>
+        <v>5.86909788230092E-3</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="3"/>
+        <v>5.86909788230092E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4.2349995275388881E-3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2.1219130796210544E-4</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="0"/>
+        <v>2.1219130796210544E-4</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>2.1219130796210544E-4</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1219130796210544E-4</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1219130796210544E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2.0560277799938402E-2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3.8366125882774188E-4</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="0"/>
+        <v>3.8366125882774188E-4</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>3.8366125882774188E-4</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="2"/>
+        <v>3.8366125882774188E-4</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="3"/>
+        <v>3.8366125882774188E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1.0961495941820574</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.11480309838857856</v>
+      </c>
+      <c r="D18" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11480309838857856</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11480309838857856</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="2"/>
+        <v>0.11480309838857856</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.11480309838857856</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.2419532449195709E-2</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3.7018497329376407E-4</v>
+      </c>
+      <c r="D19" s="2">
+        <f t="shared" si="0"/>
+        <v>3.7018497329376407E-4</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>3.7018497329376407E-4</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="2"/>
+        <v>3.7018497329376407E-4</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="3"/>
+        <v>3.7018497329376407E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2">
+        <v>633.15471120171344</v>
+      </c>
+      <c r="C20" s="2">
+        <v>92.811588579119217</v>
+      </c>
+      <c r="D20" s="2">
+        <f t="shared" si="0"/>
+        <v>92.811588579119217</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>92.811588579119217</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="2"/>
+        <v>92.811588579119217</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="3"/>
+        <v>92.811588579119217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="95" t="s">
         <v>329</v>
       </c>
-      <c r="B4" s="127">
+      <c r="B21">
         <v>2.1781234690476294E-2</v>
       </c>
-      <c r="C4">
-        <f>B4</f>
-        <v>2.1781234690476294E-2</v>
-      </c>
-      <c r="D4" s="127">
+      <c r="C21">
         <v>0.73563756849253104</v>
       </c>
-      <c r="F4">
-        <f>D4</f>
+      <c r="D21">
+        <f>C21</f>
         <v>0.73563756849253104</v>
       </c>
-      <c r="H4">
-        <f>D4</f>
+      <c r="E21">
+        <f>C21</f>
         <v>0.73563756849253104</v>
       </c>
-      <c r="J4">
-        <f>D4</f>
+      <c r="F21">
+        <f>C21</f>
         <v>0.73563756849253104</v>
       </c>
-      <c r="L4">
-        <f>D4</f>
+      <c r="G21">
+        <f>C21</f>
         <v>0.73563756849253104</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="95" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="95" t="s">
         <v>330</v>
       </c>
-      <c r="B5" s="127">
+      <c r="B22">
         <v>0.18381159698546526</v>
       </c>
-      <c r="C5">
-        <f t="shared" ref="C5:C11" si="0">B5</f>
-        <v>0.18381159698546526</v>
-      </c>
-      <c r="D5" s="127">
+      <c r="C22">
         <v>0.12786171981419567</v>
       </c>
-      <c r="F5">
-        <f t="shared" ref="F5:F11" si="1">D5</f>
+      <c r="D22">
+        <f t="shared" ref="D22:D28" si="4">C22</f>
         <v>0.12786171981419567</v>
       </c>
-      <c r="H5">
-        <f t="shared" ref="H5:H11" si="2">D5</f>
+      <c r="E22">
+        <f t="shared" ref="E22:E28" si="5">C22</f>
         <v>0.12786171981419567</v>
       </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J11" si="3">D5</f>
+      <c r="F22">
+        <f t="shared" ref="F22:F28" si="6">C22</f>
         <v>0.12786171981419567</v>
       </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L11" si="4">D5</f>
+      <c r="G22">
+        <f t="shared" ref="G22:G28" si="7">C22</f>
         <v>0.12786171981419567</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="95" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="95" t="s">
         <v>331</v>
       </c>
-      <c r="B6" s="127">
+      <c r="B23">
         <v>0.26679009552113131</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>0.26679009552113131</v>
-      </c>
-      <c r="D6" s="127">
+      <c r="C23">
         <v>8.2023598818784182E-2</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>8.2023598818784182E-2</v>
-      </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
-        <v>8.2023598818784182E-2</v>
-      </c>
-      <c r="J6">
-        <f t="shared" si="3"/>
-        <v>8.2023598818784182E-2</v>
-      </c>
-      <c r="L6">
+      <c r="D23">
         <f t="shared" si="4"/>
         <v>8.2023598818784182E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="95" t="s">
+      <c r="E23">
+        <f t="shared" si="5"/>
+        <v>8.2023598818784182E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="6"/>
+        <v>8.2023598818784182E-2</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="7"/>
+        <v>8.2023598818784182E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="95" t="s">
         <v>332</v>
       </c>
-      <c r="B7" s="127">
+      <c r="B24">
         <v>1.6067527224713878E-2</v>
       </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>1.6067527224713878E-2</v>
-      </c>
-      <c r="D7" s="127">
+      <c r="C24">
         <v>4.7471776286034904E-3</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>4.7471776286034904E-3</v>
-      </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
-        <v>4.7471776286034904E-3</v>
-      </c>
-      <c r="J7">
-        <f t="shared" si="3"/>
-        <v>4.7471776286034904E-3</v>
-      </c>
-      <c r="L7">
+      <c r="D24">
         <f t="shared" si="4"/>
         <v>4.7471776286034904E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="95" t="s">
+      <c r="E24">
+        <f t="shared" si="5"/>
+        <v>4.7471776286034904E-3</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="6"/>
+        <v>4.7471776286034904E-3</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="7"/>
+        <v>4.7471776286034904E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="95" t="s">
         <v>333</v>
       </c>
-      <c r="B8" s="127">
+      <c r="B25">
         <v>1.0925985281165002E-2</v>
       </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>1.0925985281165002E-2</v>
-      </c>
-      <c r="D8" s="127">
+      <c r="C25">
         <v>1.1625114789012593E-3</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>1.1625114789012593E-3</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
-        <v>1.1625114789012593E-3</v>
-      </c>
-      <c r="J8">
-        <f t="shared" si="3"/>
-        <v>1.1625114789012593E-3</v>
-      </c>
-      <c r="L8">
+      <c r="D25">
         <f t="shared" si="4"/>
         <v>1.1625114789012593E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="95" t="s">
+      <c r="E25">
+        <f t="shared" si="5"/>
+        <v>1.1625114789012593E-3</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="6"/>
+        <v>1.1625114789012593E-3</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="7"/>
+        <v>1.1625114789012593E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="95" t="s">
         <v>334</v>
       </c>
-      <c r="B9" s="127">
+      <c r="B26">
         <v>7.5973312175973959E-2</v>
       </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>7.5973312175973959E-2</v>
-      </c>
-      <c r="D9" s="127">
+      <c r="C26">
         <v>1.5008027021008762E-3</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>1.5008027021008762E-3</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>1.5008027021008762E-3</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="3"/>
-        <v>1.5008027021008762E-3</v>
-      </c>
-      <c r="L9">
+      <c r="D26">
         <f t="shared" si="4"/>
         <v>1.5008027021008762E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="95" t="s">
+      <c r="E26">
+        <f t="shared" si="5"/>
+        <v>1.5008027021008762E-3</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="6"/>
+        <v>1.5008027021008762E-3</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="7"/>
+        <v>1.5008027021008762E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="95" t="s">
         <v>335</v>
       </c>
-      <c r="B10" s="127">
+      <c r="B27">
         <v>7.7626034636698693E-4</v>
       </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>7.7626034636698693E-4</v>
-      </c>
-      <c r="D10" s="127">
+      <c r="C27">
         <v>8.0041955215929224E-5</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>8.0041955215929224E-5</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>8.0041955215929224E-5</v>
-      </c>
-      <c r="J10">
-        <f t="shared" si="3"/>
-        <v>8.0041955215929224E-5</v>
-      </c>
-      <c r="L10">
+      <c r="D27">
         <f t="shared" si="4"/>
         <v>8.0041955215929224E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="96" t="s">
+      <c r="E27">
+        <f t="shared" si="5"/>
+        <v>8.0041955215929224E-5</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="6"/>
+        <v>8.0041955215929224E-5</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="7"/>
+        <v>8.0041955215929224E-5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="96" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="127">
+      <c r="B28">
         <v>3.3865871217684512E-3</v>
       </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>3.3865871217684512E-3</v>
-      </c>
-      <c r="D11" s="127">
+      <c r="C28">
         <v>1.2376182810406463E-4</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>1.2376182810406463E-4</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>1.2376182810406463E-4</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="3"/>
-        <v>1.2376182810406463E-4</v>
-      </c>
-      <c r="L11">
+      <c r="D28">
         <f t="shared" si="4"/>
         <v>1.2376182810406463E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B12" s="127"/>
-      <c r="D12" s="127"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B13" s="127"/>
-      <c r="D13" s="127"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B14" s="127"/>
-      <c r="D14" s="127"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B15" s="127"/>
-      <c r="D15" s="127"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="B16" s="127"/>
-      <c r="D16" s="127"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B17" s="127"/>
-      <c r="D17" s="127"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B18" s="127"/>
-      <c r="D18" s="127"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B19" s="127"/>
-      <c r="D19" s="127"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B20" s="127"/>
-      <c r="D20" s="127"/>
+      <c r="E28">
+        <f t="shared" si="5"/>
+        <v>1.2376182810406463E-4</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="6"/>
+        <v>1.2376182810406463E-4</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="7"/>
+        <v>1.2376182810406463E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Updated fuel properties for biochem RD; 2. fixed typos; 3. hide supporting tabs in the data files
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58106C58-FE79-4AEE-B374-1BA83D1C594D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AA501E-3473-4B4E-8D76-C3666B0ED710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -164,6 +164,7 @@
     <author>tc={5DABB33C-268A-4D96-8458-8527F4ED3C5B}</author>
     <author>tc={9E8E3EEE-3F0D-41D7-BBDD-62E207BDD908}</author>
     <author>tc={D5B2B26F-4035-42EA-8638-005D102705FB}</author>
+    <author>tc={D2BC83AE-6558-47F4-9655-79E589A783CC}</author>
   </authors>
   <commentList>
     <comment ref="K1" authorId="0" shapeId="0" xr:uid="{044CB3AF-6283-4031-8C05-A50B4C478E65}">
@@ -221,6 +222,14 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     Lipase Enzyme for FAFE pathway: assumed to be 25 mol. % (or 58.49 wt. %) propylene glycol with balance water.</t>
+      </text>
+    </comment>
+    <comment ref="AF1" authorId="7" shapeId="0" xr:uid="{D2BC83AE-6558-47F4-9655-79E589A783CC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Same as WWT polymer.</t>
       </text>
     </comment>
   </commentList>
@@ -288,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="345">
   <si>
     <t>Diesel</t>
   </si>
@@ -1320,6 +1329,9 @@
   </si>
   <si>
     <t>Renewable Diesel - Biochem (BDO)</t>
+  </si>
+  <si>
+    <t>Polymer</t>
   </si>
 </sst>
 </file>
@@ -1340,7 +1352,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
     <numFmt numFmtId="174" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1372,6 +1384,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -2185,6 +2203,7 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <person displayName="Cai, Hao" id="{C9416A2D-8241-4F20-804B-D394F6D9AB2A}" userId="Cai, Hao" providerId="None"/>
   <person displayName="Anant Vyas" id="{865AB77A-77F7-42CA-A3DE-E71A2578FA95}" userId="Anant Vyas" providerId="None"/>
+  <person displayName="Ou, Longwen" id="{8E567C9D-2604-44CA-B4D4-53F9B4196B19}" userId="Ou, Longwen" providerId="None"/>
   <person displayName="Michael Wang" id="{52F93C99-6E2F-47FF-A86C-9CFC6703D7FF}" userId="Michael Wang" providerId="None"/>
   <person displayName="Zaimes, Greg" id="{A45B9717-AF57-475A-955C-29D129E5B0F1}" userId="Zaimes, Greg" providerId="None"/>
   <person displayName="Ou, Longwen" id="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" userId="S::oul@anl.gov::b81c495d-7ec4-42b7-a488-1701327cd6bc" providerId="AD"/>
@@ -2552,6 +2571,9 @@
   <threadedComment ref="AA1" dT="2021-08-26T16:55:14.53" personId="{4D745061-1DBF-40CE-B410-7C7B5B1E43E2}" id="{D5B2B26F-4035-42EA-8638-005D102705FB}">
     <text>Lipase Enzyme for FAFE pathway: assumed to be 25 mol. % (or 58.49 wt. %) propylene glycol with balance water.</text>
   </threadedComment>
+  <threadedComment ref="AF1" dT="2022-12-20T15:55:59.18" personId="{8E567C9D-2604-44CA-B4D4-53F9B4196B19}" id="{D2BC83AE-6558-47F4-9655-79E589A783CC}">
+    <text>Same as WWT polymer.</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -2585,7 +2607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2881F9E-269C-49CF-82E7-32BB9030EB09}">
   <dimension ref="A1:AY23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="AF1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="AN1" sqref="AN1"/>
     </sheetView>
@@ -8667,7 +8689,7 @@
   <dimension ref="A1:X44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A28"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10897,11 +10919,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:BQ29"/>
+  <dimension ref="A1:BR29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ1" sqref="AJ1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AF1" sqref="AF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -10912,9 +10934,10 @@
     <col min="28" max="29" width="13.1796875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="22.453125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="65.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:70" ht="65.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9"/>
       <c r="B1" s="10" t="s">
         <v>268</v>
@@ -11006,119 +11029,122 @@
       <c r="AE1" t="s">
         <v>62</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="AG1" t="s">
         <v>185</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>76</v>
       </c>
-      <c r="AH1" s="92" t="s">
+      <c r="AI1" s="92" t="s">
         <v>319</v>
       </c>
-      <c r="AI1" s="84" t="s">
+      <c r="AJ1" s="84" t="s">
         <v>264</v>
       </c>
-      <c r="AJ1" s="92" t="s">
+      <c r="AK1" s="92" t="s">
         <v>137</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>277</v>
       </c>
-      <c r="AL1" s="87" t="s">
+      <c r="AM1" s="87" t="s">
         <v>280</v>
       </c>
-      <c r="AM1" s="87" t="s">
+      <c r="AN1" s="87" t="s">
         <v>281</v>
       </c>
-      <c r="AN1" s="87" t="s">
+      <c r="AO1" s="87" t="s">
         <v>282</v>
       </c>
-      <c r="AO1" s="87" t="s">
+      <c r="AP1" s="87" t="s">
         <v>279</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>294</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>295</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>296</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>297</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>298</v>
       </c>
-      <c r="AU1" s="90" t="s">
+      <c r="AV1" s="90" t="s">
         <v>301</v>
       </c>
-      <c r="AV1" s="90" t="s">
+      <c r="AW1" s="90" t="s">
         <v>302</v>
       </c>
-      <c r="AW1" s="90" t="s">
+      <c r="AX1" s="90" t="s">
         <v>303</v>
       </c>
-      <c r="AX1" s="91" t="s">
+      <c r="AY1" s="91" t="s">
         <v>304</v>
       </c>
-      <c r="AY1" s="91" t="s">
+      <c r="AZ1" s="91" t="s">
         <v>305</v>
       </c>
-      <c r="AZ1" s="91" t="s">
+      <c r="BA1" s="91" t="s">
         <v>306</v>
       </c>
-      <c r="BA1" s="91" t="s">
+      <c r="BB1" s="91" t="s">
         <v>307</v>
       </c>
-      <c r="BB1" s="91" t="s">
+      <c r="BC1" s="91" t="s">
         <v>308</v>
       </c>
-      <c r="BC1" s="91" t="s">
+      <c r="BD1" s="91" t="s">
         <v>309</v>
       </c>
-      <c r="BD1" s="91" t="s">
+      <c r="BE1" s="91" t="s">
         <v>310</v>
       </c>
-      <c r="BE1" s="91" t="s">
+      <c r="BF1" s="91" t="s">
         <v>311</v>
       </c>
-      <c r="BF1" s="91" t="s">
+      <c r="BG1" s="91" t="s">
         <v>312</v>
       </c>
-      <c r="BG1" s="91" t="s">
+      <c r="BH1" s="91" t="s">
         <v>313</v>
       </c>
-      <c r="BH1" s="91" t="s">
+      <c r="BI1" s="91" t="s">
         <v>314</v>
       </c>
-      <c r="BI1" s="91" t="s">
+      <c r="BJ1" s="91" t="s">
         <v>320</v>
       </c>
-      <c r="BJ1" s="91" t="s">
+      <c r="BK1" s="91" t="s">
         <v>315</v>
       </c>
-      <c r="BK1" s="91" t="s">
+      <c r="BL1" s="91" t="s">
         <v>316</v>
       </c>
-      <c r="BL1" s="91" t="s">
+      <c r="BM1" s="91" t="s">
         <v>317</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>318</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>322</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>325</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>340</v>
       </c>
@@ -11212,22 +11238,22 @@
       <c r="AE2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="AG2" t="s">
         <v>87</v>
       </c>
-      <c r="AG2" s="13" t="s">
+      <c r="AH2" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="AH2" s="93" t="s">
+      <c r="AI2" s="93" t="s">
         <v>96</v>
       </c>
-      <c r="AI2" s="13" t="s">
+      <c r="AJ2" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="AJ2" s="93" t="s">
-        <v>80</v>
-      </c>
-      <c r="AK2" s="107" t="s">
+      <c r="AK2" s="93" t="s">
         <v>80</v>
       </c>
       <c r="AL2" s="107" t="s">
@@ -11323,9 +11349,12 @@
       <c r="BP2" s="107" t="s">
         <v>80</v>
       </c>
-      <c r="BQ2" s="13"/>
-    </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="BQ2" s="107" t="s">
+        <v>80</v>
+      </c>
+      <c r="BR2" s="13"/>
+    </row>
+    <row r="3" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -11420,67 +11449,68 @@
         <v>0</v>
       </c>
       <c r="AF3" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="51">
-        <v>270564.42668605602</v>
+        <f>L3</f>
+        <v>20.016171557898588</v>
+      </c>
+      <c r="AG3" s="97">
+        <v>0</v>
       </c>
       <c r="AH3" s="51">
         <v>270564.42668605602</v>
       </c>
-      <c r="AI3" s="97">
+      <c r="AI3" s="51">
+        <v>270564.42668605602</v>
+      </c>
+      <c r="AJ3" s="97">
         <v>97.941825710919858</v>
       </c>
-      <c r="AJ3" s="51">
+      <c r="AK3" s="51">
         <v>48.245115483353644</v>
       </c>
-      <c r="AK3" s="51">
+      <c r="AL3" s="51">
         <v>4.7260155706877649</v>
       </c>
-      <c r="AL3" s="51">
+      <c r="AM3" s="51">
         <v>126.19882293839159</v>
       </c>
-      <c r="AM3" s="51">
+      <c r="AN3" s="51">
         <v>40.077107640682193</v>
       </c>
-      <c r="AN3" s="51">
+      <c r="AO3" s="51">
         <v>87.533244440424198</v>
       </c>
-      <c r="AO3" s="51">
+      <c r="AP3" s="51">
         <v>265.68525300521844</v>
       </c>
-      <c r="AP3" s="51">
+      <c r="AQ3" s="51">
         <v>23.498660702149103</v>
       </c>
-      <c r="AQ3" s="51">
+      <c r="AR3" s="51">
         <v>0.50627081243840255</v>
       </c>
-      <c r="AR3" s="51">
+      <c r="AS3" s="51">
         <v>26.95801382381368</v>
       </c>
-      <c r="AS3" s="51">
+      <c r="AT3" s="51">
         <v>74.443002747362939</v>
       </c>
-      <c r="AT3" s="51">
+      <c r="AU3" s="51">
         <v>30.395319931136076</v>
       </c>
-      <c r="AU3" s="51">
+      <c r="AV3" s="51">
         <v>15.17575481546759</v>
-      </c>
-      <c r="AV3" s="51">
-        <v>40.077107640682193</v>
       </c>
       <c r="AW3" s="51">
         <v>40.077107640682193</v>
       </c>
       <c r="AX3" s="51">
+        <v>40.077107640682193</v>
+      </c>
+      <c r="AY3" s="51">
         <v>0.36550917489225548</v>
       </c>
-      <c r="AY3" s="51">
+      <c r="AZ3" s="51">
         <v>4.4293339688143134E-2</v>
-      </c>
-      <c r="AZ3" s="51">
-        <v>198.64676190407542</v>
       </c>
       <c r="BA3" s="51">
         <v>198.64676190407542</v>
@@ -11498,40 +11528,43 @@
         <v>198.64676190407542</v>
       </c>
       <c r="BF3" s="51">
+        <v>198.64676190407542</v>
+      </c>
+      <c r="BG3" s="51">
         <v>39.932638092793603</v>
       </c>
-      <c r="BG3" s="51">
+      <c r="BH3" s="51">
         <v>16.340788459612678</v>
       </c>
-      <c r="BH3" s="51">
+      <c r="BI3" s="51">
         <v>198.64676190407542</v>
       </c>
-      <c r="BI3" s="51">
+      <c r="BJ3" s="51">
         <v>2.9697620459995759</v>
       </c>
-      <c r="BJ3" s="51">
+      <c r="BK3" s="51">
         <v>35.607860000000002</v>
       </c>
-      <c r="BK3" s="51">
+      <c r="BL3" s="51">
         <v>63.118172520906064</v>
       </c>
-      <c r="BL3" s="51">
+      <c r="BM3" s="51">
         <v>1789.1938614313462</v>
       </c>
-      <c r="BM3" s="51">
+      <c r="BN3" s="51">
         <v>69.378860802973378</v>
       </c>
-      <c r="BN3" s="51">
+      <c r="BO3" s="51">
         <v>9.0179268254522125</v>
       </c>
-      <c r="BO3" s="51">
+      <c r="BP3" s="51">
         <v>9.5877694417335881</v>
       </c>
-      <c r="BP3" s="51">
+      <c r="BQ3" s="51">
         <v>3.2548179434336486</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -11626,67 +11659,68 @@
         <v>0</v>
       </c>
       <c r="AF4" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG4" s="51">
-        <v>265310.32849319675</v>
+        <f t="shared" ref="AF4:AF27" si="0">L4</f>
+        <v>17.669444719080467</v>
+      </c>
+      <c r="AG4" s="97">
+        <v>0</v>
       </c>
       <c r="AH4" s="51">
         <v>265310.32849319675</v>
       </c>
-      <c r="AI4" s="97">
+      <c r="AI4" s="51">
+        <v>265310.32849319675</v>
+      </c>
+      <c r="AJ4" s="97">
         <v>97.957127354814901</v>
       </c>
-      <c r="AJ4" s="51">
+      <c r="AK4" s="51">
         <v>14.264166786641894</v>
       </c>
-      <c r="AK4" s="51">
+      <c r="AL4" s="51">
         <v>4.6297798831510386</v>
       </c>
-      <c r="AL4" s="51">
+      <c r="AM4" s="51">
         <v>120.2163356099561</v>
       </c>
-      <c r="AM4" s="51">
+      <c r="AN4" s="51">
         <v>35.202656869085949</v>
       </c>
-      <c r="AN4" s="51">
+      <c r="AO4" s="51">
         <v>82.972785598695125</v>
       </c>
-      <c r="AO4" s="51">
+      <c r="AP4" s="51">
         <v>253.21323060996494</v>
       </c>
-      <c r="AP4" s="51">
+      <c r="AQ4" s="51">
         <v>22.362959251662502</v>
       </c>
-      <c r="AQ4" s="51">
+      <c r="AR4" s="51">
         <v>0.45131042523003451</v>
       </c>
-      <c r="AR4" s="51">
+      <c r="AS4" s="51">
         <v>25.173700738277056</v>
       </c>
-      <c r="AS4" s="51">
+      <c r="AT4" s="51">
         <v>71.688868284651093</v>
       </c>
-      <c r="AT4" s="51">
+      <c r="AU4" s="51">
         <v>29.939378514583474</v>
       </c>
-      <c r="AU4" s="51">
+      <c r="AV4" s="51">
         <v>14.107547470255774</v>
-      </c>
-      <c r="AV4" s="51">
-        <v>35.202656869085942</v>
       </c>
       <c r="AW4" s="51">
         <v>35.202656869085942</v>
       </c>
       <c r="AX4" s="51">
+        <v>35.202656869085942</v>
+      </c>
+      <c r="AY4" s="51">
         <v>0.28996126831884061</v>
       </c>
-      <c r="AY4" s="51">
+      <c r="AZ4" s="51">
         <v>4.02816573645291E-2</v>
-      </c>
-      <c r="AZ4" s="51">
-        <v>193.09941239590157</v>
       </c>
       <c r="BA4" s="51">
         <v>193.09941239590157</v>
@@ -11704,40 +11738,43 @@
         <v>193.09941239590157</v>
       </c>
       <c r="BF4" s="51">
+        <v>193.09941239590157</v>
+      </c>
+      <c r="BG4" s="51">
         <v>39.414907554091407</v>
       </c>
-      <c r="BG4" s="51">
+      <c r="BH4" s="51">
         <v>15.48013264899326</v>
       </c>
-      <c r="BH4" s="51">
+      <c r="BI4" s="51">
         <v>193.09941239590157</v>
       </c>
-      <c r="BI4" s="51">
+      <c r="BJ4" s="51">
         <v>2.35593530509058</v>
       </c>
-      <c r="BJ4" s="51">
+      <c r="BK4" s="51">
         <v>34.146839999999997</v>
       </c>
-      <c r="BK4" s="51">
+      <c r="BL4" s="51">
         <v>61.092141088683597</v>
       </c>
-      <c r="BL4" s="51">
+      <c r="BM4" s="51">
         <v>645.20002493956258</v>
       </c>
-      <c r="BM4" s="51">
+      <c r="BN4" s="51">
         <v>66.562363858854823</v>
       </c>
-      <c r="BN4" s="51">
+      <c r="BO4" s="51">
         <v>8.9777607956598811</v>
       </c>
-      <c r="BO4" s="51">
+      <c r="BP4" s="51">
         <v>9.5819504475122663</v>
       </c>
-      <c r="BP4" s="51">
+      <c r="BQ4" s="51">
         <v>3.1019980225698647</v>
       </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -11832,67 +11869,68 @@
         <v>0</v>
       </c>
       <c r="AF5" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="51">
-        <v>8939.4542987875684</v>
+        <f t="shared" si="0"/>
+        <v>3.9928442443419501</v>
+      </c>
+      <c r="AG5" s="97">
+        <v>0</v>
       </c>
       <c r="AH5" s="51">
         <v>8939.4542987875684</v>
       </c>
-      <c r="AI5" s="97">
+      <c r="AI5" s="51">
+        <v>8939.4542987875684</v>
+      </c>
+      <c r="AJ5" s="97">
         <v>-2.7085618926532478E-2</v>
       </c>
-      <c r="AJ5" s="51">
+      <c r="AK5" s="51">
         <v>1.1239589634237839</v>
       </c>
-      <c r="AK5" s="51">
+      <c r="AL5" s="51">
         <v>3.8990536508594245</v>
       </c>
-      <c r="AL5" s="51">
+      <c r="AM5" s="51">
         <v>10.760549801926718</v>
       </c>
-      <c r="AM5" s="51">
+      <c r="AN5" s="51">
         <v>9.6316195636916753</v>
       </c>
-      <c r="AN5" s="51">
+      <c r="AO5" s="51">
         <v>29.13297279594817</v>
       </c>
-      <c r="AO5" s="51">
+      <c r="AP5" s="51">
         <v>40.009650656378795</v>
       </c>
-      <c r="AP5" s="51">
+      <c r="AQ5" s="51">
         <v>1.930871286755997</v>
       </c>
-      <c r="AQ5" s="51">
+      <c r="AR5" s="51">
         <v>0.18491245113269286</v>
       </c>
-      <c r="AR5" s="51">
+      <c r="AS5" s="51">
         <v>18.03733201336857</v>
       </c>
-      <c r="AS5" s="51">
+      <c r="AT5" s="51">
         <v>4.6864369026676123</v>
       </c>
-      <c r="AT5" s="51">
+      <c r="AU5" s="51">
         <v>20.731489834275457</v>
       </c>
-      <c r="AU5" s="51">
+      <c r="AV5" s="51">
         <v>1.8161025484401034</v>
-      </c>
-      <c r="AV5" s="51">
-        <v>9.631619563691677</v>
       </c>
       <c r="AW5" s="51">
         <v>9.631619563691677</v>
       </c>
       <c r="AX5" s="51">
+        <v>9.631619563691677</v>
+      </c>
+      <c r="AY5" s="51">
         <v>0.12854120723978854</v>
       </c>
-      <c r="AY5" s="51">
+      <c r="AZ5" s="51">
         <v>6.7934776101475254E-3</v>
-      </c>
-      <c r="AZ5" s="51">
-        <v>17.076988376901635</v>
       </c>
       <c r="BA5" s="51">
         <v>17.076988376901635</v>
@@ -11910,40 +11948,43 @@
         <v>17.076988376901635</v>
       </c>
       <c r="BF5" s="51">
+        <v>17.076988376901635</v>
+      </c>
+      <c r="BG5" s="51">
         <v>4.0016783327688534</v>
       </c>
-      <c r="BG5" s="51">
+      <c r="BH5" s="51">
         <v>1.4642917062315886</v>
       </c>
-      <c r="BH5" s="51">
+      <c r="BI5" s="51">
         <v>17.076988376901635</v>
       </c>
-      <c r="BI5" s="51">
+      <c r="BJ5" s="51">
         <v>1.0443973088232819</v>
       </c>
-      <c r="BJ5" s="51">
+      <c r="BK5" s="51">
         <v>2.8897429999999997</v>
       </c>
-      <c r="BK5" s="51">
+      <c r="BL5" s="51">
         <v>3.4461514234900887</v>
       </c>
-      <c r="BL5" s="51">
+      <c r="BM5" s="51">
         <v>29.543487415925121</v>
       </c>
-      <c r="BM5" s="51">
+      <c r="BN5" s="51">
         <v>3.5388428925359858</v>
       </c>
-      <c r="BN5" s="51">
+      <c r="BO5" s="51">
         <v>7.0321354472179673E-2</v>
       </c>
-      <c r="BO5" s="51">
+      <c r="BP5" s="51">
         <v>9.875250529459487E-3</v>
       </c>
-      <c r="BP5" s="51">
+      <c r="BQ5" s="51">
         <v>0.5464831258747449</v>
       </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -12038,67 +12079,68 @@
         <v>0</v>
       </c>
       <c r="AF6" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="51">
-        <v>255619.31656445214</v>
+        <f t="shared" si="0"/>
+        <v>13.553771162213316</v>
+      </c>
+      <c r="AG6" s="97">
+        <v>0</v>
       </c>
       <c r="AH6" s="51">
         <v>255619.31656445214</v>
       </c>
-      <c r="AI6" s="97">
+      <c r="AI6" s="51">
+        <v>255619.31656445214</v>
+      </c>
+      <c r="AJ6" s="97">
         <v>94.513039694513239</v>
       </c>
-      <c r="AJ6" s="51">
+      <c r="AK6" s="51">
         <v>11.638318072853059</v>
       </c>
-      <c r="AK6" s="51">
+      <c r="AL6" s="51">
         <v>0.48693590769400102</v>
       </c>
-      <c r="AL6" s="51">
+      <c r="AM6" s="51">
         <v>64.727547223603551</v>
       </c>
-      <c r="AM6" s="51">
+      <c r="AN6" s="51">
         <v>24.99792087060689</v>
       </c>
-      <c r="AN6" s="51">
+      <c r="AO6" s="51">
         <v>50.036880028751753</v>
       </c>
-      <c r="AO6" s="51">
+      <c r="AP6" s="51">
         <v>202.81076409394649</v>
       </c>
-      <c r="AP6" s="51">
+      <c r="AQ6" s="51">
         <v>15.512019009281868</v>
       </c>
-      <c r="AQ6" s="51">
+      <c r="AR6" s="51">
         <v>0.13184574977337188</v>
       </c>
-      <c r="AR6" s="51">
+      <c r="AS6" s="51">
         <v>7.2735884227177143</v>
       </c>
-      <c r="AS6" s="51">
+      <c r="AT6" s="51">
         <v>62.225675032994907</v>
       </c>
-      <c r="AT6" s="51">
+      <c r="AU6" s="51">
         <v>7.4830006405819365</v>
       </c>
-      <c r="AU6" s="51">
+      <c r="AV6" s="51">
         <v>7.6038501700618921</v>
-      </c>
-      <c r="AV6" s="51">
-        <v>24.99792087060689</v>
       </c>
       <c r="AW6" s="51">
         <v>24.99792087060689</v>
       </c>
       <c r="AX6" s="51">
+        <v>24.99792087060689</v>
+      </c>
+      <c r="AY6" s="51">
         <v>0.15757425250265861</v>
       </c>
-      <c r="AY6" s="51">
+      <c r="AZ6" s="51">
         <v>1.2182268278702715E-2</v>
-      </c>
-      <c r="AZ6" s="51">
-        <v>169.11521182545442</v>
       </c>
       <c r="BA6" s="51">
         <v>169.11521182545442</v>
@@ -12116,40 +12158,43 @@
         <v>169.11521182545442</v>
       </c>
       <c r="BF6" s="51">
+        <v>169.11521182545442</v>
+      </c>
+      <c r="BG6" s="51">
         <v>18.657919975763626</v>
       </c>
-      <c r="BG6" s="51">
+      <c r="BH6" s="51">
         <v>13.728640427219338</v>
       </c>
-      <c r="BH6" s="51">
+      <c r="BI6" s="51">
         <v>169.11521182545442</v>
       </c>
-      <c r="BI6" s="51">
+      <c r="BJ6" s="51">
         <v>1.2802908015841012</v>
       </c>
-      <c r="BJ6" s="51">
+      <c r="BK6" s="51">
         <v>22.8813</v>
       </c>
-      <c r="BK6" s="51">
+      <c r="BL6" s="51">
         <v>54.087089973185108</v>
       </c>
-      <c r="BL6" s="51">
+      <c r="BM6" s="51">
         <v>453.86296612981522</v>
       </c>
-      <c r="BM6" s="51">
+      <c r="BN6" s="51">
         <v>47.175363754400323</v>
       </c>
-      <c r="BN6" s="51">
+      <c r="BO6" s="51">
         <v>7.7272886866656796</v>
       </c>
-      <c r="BO6" s="51">
+      <c r="BP6" s="51">
         <v>9.487525944381753</v>
       </c>
-      <c r="BP6" s="51">
+      <c r="BQ6" s="51">
         <v>1.5045324171794181</v>
       </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -12244,67 +12289,68 @@
         <v>0</v>
       </c>
       <c r="AF7" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="51">
-        <v>751.55762995703594</v>
+        <f t="shared" si="0"/>
+        <v>0.12282931252520071</v>
+      </c>
+      <c r="AG7" s="97">
+        <v>0</v>
       </c>
       <c r="AH7" s="51">
         <v>751.55762995703594</v>
       </c>
-      <c r="AI7" s="97">
+      <c r="AI7" s="51">
+        <v>751.55762995703594</v>
+      </c>
+      <c r="AJ7" s="97">
         <v>3.4711732792281844</v>
       </c>
-      <c r="AJ7" s="51">
+      <c r="AK7" s="51">
         <v>1.5018897503650515</v>
       </c>
-      <c r="AK7" s="51">
+      <c r="AL7" s="51">
         <v>0.24379032459761335</v>
       </c>
-      <c r="AL7" s="51">
+      <c r="AM7" s="51">
         <v>44.728238584425839</v>
       </c>
-      <c r="AM7" s="51">
+      <c r="AN7" s="51">
         <v>0.57311643478738505</v>
       </c>
-      <c r="AN7" s="51">
+      <c r="AO7" s="51">
         <v>3.8029327739952028</v>
       </c>
-      <c r="AO7" s="51">
+      <c r="AP7" s="51">
         <v>10.392815859639667</v>
       </c>
-      <c r="AP7" s="51">
+      <c r="AQ7" s="51">
         <v>4.9200689556246351</v>
       </c>
-      <c r="AQ7" s="51">
+      <c r="AR7" s="51">
         <v>0.13455222432396977</v>
       </c>
-      <c r="AR7" s="51">
+      <c r="AS7" s="51">
         <v>-0.13721969780923163</v>
       </c>
-      <c r="AS7" s="51">
+      <c r="AT7" s="51">
         <v>4.7767563489885543</v>
       </c>
-      <c r="AT7" s="51">
+      <c r="AU7" s="51">
         <v>1.7248880397260815</v>
       </c>
-      <c r="AU7" s="51">
+      <c r="AV7" s="51">
         <v>4.687594751753779</v>
-      </c>
-      <c r="AV7" s="51">
-        <v>0.57311643478738505</v>
       </c>
       <c r="AW7" s="51">
         <v>0.57311643478738505</v>
       </c>
       <c r="AX7" s="51">
+        <v>0.57311643478738505</v>
+      </c>
+      <c r="AY7" s="51">
         <v>3.8458085763934152E-3</v>
       </c>
-      <c r="AY7" s="51">
+      <c r="AZ7" s="51">
         <v>2.1305911475678851E-2</v>
-      </c>
-      <c r="AZ7" s="51">
-        <v>6.9072121935455115</v>
       </c>
       <c r="BA7" s="51">
         <v>6.9072121935455115</v>
@@ -12322,40 +12368,43 @@
         <v>6.9072121935455115</v>
       </c>
       <c r="BF7" s="51">
+        <v>6.9072121935455115</v>
+      </c>
+      <c r="BG7" s="51">
         <v>16.755309245558927</v>
       </c>
-      <c r="BG7" s="51">
+      <c r="BH7" s="51">
         <v>0.28720051554233039</v>
       </c>
-      <c r="BH7" s="51">
+      <c r="BI7" s="51">
         <v>6.9072121935455115</v>
       </c>
-      <c r="BI7" s="51">
+      <c r="BJ7" s="51">
         <v>3.1247194683196498E-2</v>
       </c>
-      <c r="BJ7" s="51">
+      <c r="BK7" s="51">
         <v>8.3757970000000004</v>
       </c>
-      <c r="BK7" s="51">
+      <c r="BL7" s="51">
         <v>3.5588996920083935</v>
       </c>
-      <c r="BL7" s="51">
+      <c r="BM7" s="51">
         <v>161.79357139382219</v>
       </c>
-      <c r="BM7" s="51">
+      <c r="BN7" s="51">
         <v>15.848157211918526</v>
       </c>
-      <c r="BN7" s="51">
+      <c r="BO7" s="51">
         <v>1.1801507545220213</v>
       </c>
-      <c r="BO7" s="51">
+      <c r="BP7" s="51">
         <v>8.4549252601055933E-2</v>
       </c>
-      <c r="BP7" s="51">
+      <c r="BQ7" s="51">
         <v>1.0509824795157012</v>
       </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -12450,67 +12499,68 @@
         <v>0</v>
       </c>
       <c r="AF8" s="97">
+        <f t="shared" si="0"/>
+        <v>9.733778630854604E-4</v>
+      </c>
+      <c r="AG8" s="97">
         <v>1</v>
-      </c>
-      <c r="AG8" s="51">
-        <v>42.404553314283064</v>
       </c>
       <c r="AH8" s="51">
         <v>42.404553314283064</v>
       </c>
-      <c r="AI8" s="97">
+      <c r="AI8" s="51">
+        <v>42.404553314283064</v>
+      </c>
+      <c r="AJ8" s="97">
         <v>2.9292853558009185E-3</v>
       </c>
-      <c r="AJ8" s="51">
+      <c r="AK8" s="51">
         <v>1.0520870555878569E-2</v>
       </c>
-      <c r="AK8" s="51">
+      <c r="AL8" s="51">
         <v>1.2296962254580426E-3</v>
       </c>
-      <c r="AL8" s="51">
+      <c r="AM8" s="51">
         <v>9.3759544958936947E-3</v>
       </c>
-      <c r="AM8" s="51">
+      <c r="AN8" s="51">
         <v>2.109093616469005E-3</v>
       </c>
-      <c r="AN8" s="51">
+      <c r="AO8" s="51">
         <v>1.1427987301686452E-2</v>
       </c>
-      <c r="AO8" s="51">
+      <c r="AP8" s="51">
         <v>1.6116391261875276E-2</v>
       </c>
-      <c r="AP8" s="51">
+      <c r="AQ8" s="51">
         <v>9.7340351016242718E-3</v>
       </c>
-      <c r="AQ8" s="51">
+      <c r="AR8" s="51">
         <v>1.604287118647296E-4</v>
       </c>
-      <c r="AR8" s="51">
+      <c r="AS8" s="51">
         <v>8.3213246414534799E-4</v>
       </c>
-      <c r="AS8" s="51">
+      <c r="AT8" s="51">
         <v>2.4412039012312228E-3</v>
       </c>
-      <c r="AT8" s="51">
+      <c r="AU8" s="51">
         <v>2.9200234321583908E-4</v>
       </c>
-      <c r="AU8" s="51">
+      <c r="AV8" s="51">
         <v>9.6545502029114702E-3</v>
-      </c>
-      <c r="AV8" s="51">
-        <v>2.109093616469005E-3</v>
       </c>
       <c r="AW8" s="51">
         <v>2.109093616469005E-3</v>
       </c>
       <c r="AX8" s="51">
+        <v>2.109093616469005E-3</v>
+      </c>
+      <c r="AY8" s="51">
         <v>3.0530248815791281E-5</v>
       </c>
-      <c r="AY8" s="51">
+      <c r="AZ8" s="51">
         <v>1.3453070785644059E-4</v>
-      </c>
-      <c r="AZ8" s="51">
-        <v>5.6451275302559353E-3</v>
       </c>
       <c r="BA8" s="51">
         <v>5.6451275302559353E-3</v>
@@ -12528,40 +12578,43 @@
         <v>5.6451275302559353E-3</v>
       </c>
       <c r="BF8" s="51">
+        <v>5.6451275302559353E-3</v>
+      </c>
+      <c r="BG8" s="51">
         <v>7.4067591398331448E-4</v>
       </c>
-      <c r="BG8" s="51">
+      <c r="BH8" s="51">
         <v>6.6082443834203212E-4</v>
       </c>
-      <c r="BH8" s="51">
+      <c r="BI8" s="51">
         <v>5.6451275302559353E-3</v>
       </c>
-      <c r="BI8" s="51">
+      <c r="BJ8" s="51">
         <v>2.4805827162830416E-4</v>
       </c>
-      <c r="BJ8" s="51">
+      <c r="BK8" s="51">
         <v>1.8195209999999999E-3</v>
       </c>
-      <c r="BK8" s="51">
+      <c r="BL8" s="51">
         <v>1.8415962095976479E-3</v>
       </c>
-      <c r="BL8" s="51">
+      <c r="BM8" s="51">
         <v>2.3737943475385142E-2</v>
       </c>
-      <c r="BM8" s="51">
+      <c r="BN8" s="51">
         <v>1.2571786330539047E-3</v>
       </c>
-      <c r="BN8" s="51">
+      <c r="BO8" s="51">
         <v>1.2103002161038088E-3</v>
       </c>
-      <c r="BO8" s="51">
+      <c r="BP8" s="51">
         <v>3.1310844776686155E-5</v>
       </c>
-      <c r="BP8" s="51">
+      <c r="BQ8" s="51">
         <v>5.5892063883909704E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>48</v>
       </c>
@@ -12656,67 +12709,68 @@
         <v>0</v>
       </c>
       <c r="AF9" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="51">
-        <v>13.853129850764713</v>
+        <f t="shared" si="0"/>
+        <v>1.8924912108795632E-4</v>
+      </c>
+      <c r="AG9" s="97">
+        <v>0</v>
       </c>
       <c r="AH9" s="51">
         <v>13.853129850764713</v>
       </c>
-      <c r="AI9" s="97">
+      <c r="AI9" s="51">
+        <v>13.853129850764713</v>
+      </c>
+      <c r="AJ9" s="97">
         <v>3.219463789855906E-3</v>
       </c>
-      <c r="AJ9" s="51">
+      <c r="AK9" s="51">
         <v>1.5404428409087317E-3</v>
       </c>
-      <c r="AK9" s="51">
+      <c r="AL9" s="51">
         <v>9.9761797169438908E-5</v>
       </c>
-      <c r="AL9" s="51">
+      <c r="AM9" s="51">
         <v>1.9438336635204136E-3</v>
       </c>
-      <c r="AM9" s="51">
+      <c r="AN9" s="51">
         <v>3.8047101002084251E-4</v>
       </c>
-      <c r="AN9" s="51">
+      <c r="AO9" s="51">
         <v>9.5091884528415141E-4</v>
       </c>
-      <c r="AO9" s="51">
+      <c r="AP9" s="51">
         <v>4.9094990479613305E-3</v>
       </c>
-      <c r="AP9" s="51">
+      <c r="AQ9" s="51">
         <v>1.4544023990644757E-3</v>
       </c>
-      <c r="AQ9" s="108">
+      <c r="AR9" s="108">
         <v>8.0752850663760964E-5</v>
       </c>
-      <c r="AR9" s="108">
+      <c r="AS9" s="108">
         <v>2.6078019206617377E-3</v>
       </c>
-      <c r="AS9" s="108">
+      <c r="AT9" s="108">
         <v>8.934585296938661E-4</v>
       </c>
-      <c r="AT9" s="108">
+      <c r="AU9" s="108">
         <v>1.8643725389676437E-3</v>
       </c>
-      <c r="AU9" s="51">
+      <c r="AV9" s="51">
         <v>3.2770668334754449E-4</v>
-      </c>
-      <c r="AV9" s="51">
-        <v>3.8047101002084251E-4</v>
       </c>
       <c r="AW9" s="51">
         <v>3.8047101002084251E-4</v>
       </c>
       <c r="AX9" s="51">
+        <v>3.8047101002084251E-4</v>
+      </c>
+      <c r="AY9" s="51">
         <v>2.6691689270569509E-6</v>
       </c>
-      <c r="AY9" s="51">
+      <c r="AZ9" s="51">
         <v>7.5112438296346698E-7</v>
-      </c>
-      <c r="AZ9" s="51">
-        <v>2.8160601075936523E-3</v>
       </c>
       <c r="BA9" s="51">
         <v>2.8160601075936523E-3</v>
@@ -12734,40 +12788,43 @@
         <v>2.8160601075936523E-3</v>
       </c>
       <c r="BF9" s="51">
+        <v>2.8160601075936523E-3</v>
+      </c>
+      <c r="BG9" s="51">
         <v>3.4393994834084024E-4</v>
       </c>
-      <c r="BG9" s="51">
+      <c r="BH9" s="51">
         <v>1.6622324935140995E-4</v>
       </c>
-      <c r="BH9" s="51">
+      <c r="BI9" s="51">
         <v>2.8160601075936523E-3</v>
       </c>
-      <c r="BI9" s="51">
+      <c r="BJ9" s="51">
         <v>2.168699753233773E-5</v>
       </c>
-      <c r="BJ9" s="51">
+      <c r="BK9" s="51">
         <v>1.2273030000000001E-3</v>
       </c>
-      <c r="BK9" s="51">
+      <c r="BL9" s="51">
         <v>1.5547557883063921E-3</v>
       </c>
-      <c r="BL9" s="51">
+      <c r="BM9" s="51">
         <v>7.3696832078651645E-2</v>
       </c>
-      <c r="BM9" s="51">
+      <c r="BN9" s="51">
         <v>9.6751445371123475E-4</v>
       </c>
-      <c r="BN9" s="51">
+      <c r="BO9" s="51">
         <v>1.1666453033932554E-3</v>
       </c>
-      <c r="BO9" s="51">
+      <c r="BP9" s="51">
         <v>1.175228065630124E-4</v>
       </c>
-      <c r="BP9" s="51">
+      <c r="BQ9" s="51">
         <v>6.2238427722671554E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>49</v>
       </c>
@@ -12862,67 +12919,68 @@
         <v>0</v>
       </c>
       <c r="AF10" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="51">
-        <v>36.132779310734101</v>
+        <f t="shared" si="0"/>
+        <v>7.428948222380189E-4</v>
+      </c>
+      <c r="AG10" s="97">
+        <v>0</v>
       </c>
       <c r="AH10" s="51">
         <v>36.132779310734101</v>
       </c>
-      <c r="AI10" s="97">
+      <c r="AI10" s="51">
+        <v>36.132779310734101</v>
+      </c>
+      <c r="AJ10" s="97">
         <v>4.930081576499711E-3</v>
       </c>
-      <c r="AJ10" s="51">
+      <c r="AK10" s="51">
         <v>1.1017991189333064E-3</v>
       </c>
-      <c r="AK10" s="51">
+      <c r="AL10" s="51">
         <v>4.6836811428169385E-4</v>
       </c>
-      <c r="AL10" s="51">
+      <c r="AM10" s="51">
         <v>1.0684624756801942E-2</v>
       </c>
-      <c r="AM10" s="51">
+      <c r="AN10" s="51">
         <v>1.5694782736866014E-3</v>
       </c>
-      <c r="AN10" s="51">
+      <c r="AO10" s="51">
         <v>3.8712232201269735E-3</v>
       </c>
-      <c r="AO10" s="51">
+      <c r="AP10" s="51">
         <v>1.2193815603813246E-2</v>
       </c>
-      <c r="AP10" s="51">
+      <c r="AQ10" s="51">
         <v>2.1154365243611899E-3</v>
       </c>
-      <c r="AQ10" s="108">
+      <c r="AR10" s="108">
         <v>1.3581385731758483E-4</v>
       </c>
-      <c r="AR10" s="108">
+      <c r="AS10" s="108">
         <v>1.8852251001991446E-2</v>
       </c>
-      <c r="AS10" s="108">
+      <c r="AT10" s="108">
         <v>1.6990498192349802E-3</v>
       </c>
-      <c r="AT10" s="108">
+      <c r="AU10" s="108">
         <v>1.0559020914774062E-3</v>
       </c>
-      <c r="AU10" s="51">
+      <c r="AV10" s="51">
         <v>9.3113688992334915E-4</v>
-      </c>
-      <c r="AV10" s="51">
-        <v>1.5694782736866014E-3</v>
       </c>
       <c r="AW10" s="51">
         <v>1.5694782736866014E-3</v>
       </c>
       <c r="AX10" s="51">
+        <v>1.5694782736866014E-3</v>
+      </c>
+      <c r="AY10" s="51">
         <v>9.5591172832866281E-6</v>
       </c>
-      <c r="AY10" s="51">
+      <c r="AZ10" s="51">
         <v>5.5482577449629409E-6</v>
-      </c>
-      <c r="AZ10" s="51">
-        <v>9.7111092889849929E-3</v>
       </c>
       <c r="BA10" s="51">
         <v>9.7111092889849929E-3</v>
@@ -12940,40 +12998,43 @@
         <v>9.7111092889849929E-3</v>
       </c>
       <c r="BF10" s="51">
+        <v>9.7111092889849929E-3</v>
+      </c>
+      <c r="BG10" s="51">
         <v>1.2403250904839793E-3</v>
       </c>
-      <c r="BG10" s="51">
+      <c r="BH10" s="51">
         <v>5.1924141354754445E-4</v>
       </c>
-      <c r="BH10" s="51">
+      <c r="BI10" s="51">
         <v>9.7111092889849929E-3</v>
       </c>
-      <c r="BI10" s="51">
+      <c r="BJ10" s="51">
         <v>7.7667827926703852E-5</v>
       </c>
-      <c r="BJ10" s="51">
+      <c r="BK10" s="51">
         <v>1.9763879999999999E-3</v>
       </c>
-      <c r="BK10" s="51">
+      <c r="BL10" s="51">
         <v>2.3251750578326884E-3</v>
       </c>
-      <c r="BL10" s="51">
+      <c r="BM10" s="51">
         <v>5.5469635646732587E-2</v>
       </c>
-      <c r="BM10" s="51">
+      <c r="BN10" s="51">
         <v>6.9227894123971819E-3</v>
       </c>
-      <c r="BN10" s="51">
+      <c r="BO10" s="51">
         <v>1.3144165437702056E-3</v>
       </c>
-      <c r="BO10" s="51">
+      <c r="BP10" s="51">
         <v>5.1486233608696841E-4</v>
       </c>
-      <c r="BP10" s="51">
+      <c r="BQ10" s="51">
         <v>2.1294457385628157E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>50</v>
       </c>
@@ -13068,67 +13129,68 @@
         <v>0</v>
       </c>
       <c r="AF11" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="51">
-        <v>43.548992461514736</v>
+        <f t="shared" si="0"/>
+        <v>1.1424999878425083E-3</v>
+      </c>
+      <c r="AG11" s="97">
+        <v>0</v>
       </c>
       <c r="AH11" s="51">
         <v>43.548992461514736</v>
       </c>
-      <c r="AI11" s="97">
+      <c r="AI11" s="51">
+        <v>43.548992461514736</v>
+      </c>
+      <c r="AJ11" s="97">
         <v>3.6459857349944745E-2</v>
       </c>
-      <c r="AJ11" s="51">
+      <c r="AK11" s="51">
         <v>2.3136533851042017E-3</v>
       </c>
-      <c r="AK11" s="51">
+      <c r="AL11" s="51">
         <v>2.6612080177163829E-4</v>
       </c>
-      <c r="AL11" s="51">
+      <c r="AM11" s="51">
         <v>1.1044252611762412E-2</v>
       </c>
-      <c r="AM11" s="51">
+      <c r="AN11" s="51">
         <v>2.2828941925211151E-3</v>
       </c>
-      <c r="AN11" s="51">
+      <c r="AO11" s="51">
         <v>2.6103933233382521E-2</v>
       </c>
-      <c r="AO11" s="51">
+      <c r="AP11" s="51">
         <v>1.3088118020022285E-2</v>
       </c>
-      <c r="AP11" s="51">
+      <c r="AQ11" s="51">
         <v>4.9304899021517237E-3</v>
       </c>
-      <c r="AQ11" s="108">
+      <c r="AR11" s="108">
         <v>1.584360662882161E-4</v>
       </c>
-      <c r="AR11" s="108">
+      <c r="AS11" s="108">
         <v>2.4527023312705476E-3</v>
       </c>
-      <c r="AS11" s="108">
+      <c r="AT11" s="108">
         <v>2.425075797096791E-3</v>
       </c>
-      <c r="AT11" s="108">
+      <c r="AU11" s="108">
         <v>1.3946845087155903E-3</v>
       </c>
-      <c r="AU11" s="51">
+      <c r="AV11" s="51">
         <v>4.4692722488138218E-3</v>
-      </c>
-      <c r="AV11" s="51">
-        <v>2.2828941925211151E-3</v>
       </c>
       <c r="AW11" s="51">
         <v>2.2828941925211151E-3</v>
       </c>
       <c r="AX11" s="51">
+        <v>2.2828941925211151E-3</v>
+      </c>
+      <c r="AY11" s="51">
         <v>1.7317487340960441E-5</v>
       </c>
-      <c r="AY11" s="51">
+      <c r="AZ11" s="51">
         <v>9.0004178322438038E-6</v>
-      </c>
-      <c r="AZ11" s="51">
-        <v>1.2930569792365848E-2</v>
       </c>
       <c r="BA11" s="51">
         <v>1.2930569792365848E-2</v>
@@ -13146,40 +13208,43 @@
         <v>1.2930569792365848E-2</v>
       </c>
       <c r="BF11" s="51">
+        <v>1.2930569792365848E-2</v>
+      </c>
+      <c r="BG11" s="51">
         <v>2.2124387505511618E-3</v>
       </c>
-      <c r="BG11" s="51">
+      <c r="BH11" s="51">
         <v>7.3207162164031544E-4</v>
       </c>
-      <c r="BH11" s="51">
+      <c r="BI11" s="51">
         <v>1.2930569792365848E-2</v>
       </c>
-      <c r="BI11" s="51">
+      <c r="BJ11" s="51">
         <v>1.4070458464530359E-4</v>
       </c>
-      <c r="BJ11" s="51">
+      <c r="BK11" s="51">
         <v>3.2296099999999999E-3</v>
       </c>
-      <c r="BK11" s="51">
+      <c r="BL11" s="51">
         <v>2.37089654009001E-3</v>
       </c>
-      <c r="BL11" s="51">
+      <c r="BM11" s="51">
         <v>9.8354638645194128E-2</v>
       </c>
-      <c r="BM11" s="51">
+      <c r="BN11" s="51">
         <v>3.724647449968985E-3</v>
       </c>
-      <c r="BN11" s="51">
+      <c r="BO11" s="51">
         <v>1.7996322569381546E-3</v>
       </c>
-      <c r="BO11" s="51">
+      <c r="BP11" s="51">
         <v>6.9221614546950412E-4</v>
       </c>
-      <c r="BP11" s="51">
+      <c r="BQ11" s="51">
         <v>1.0201356388362432E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>51</v>
       </c>
@@ -13274,67 +13339,68 @@
         <v>0</v>
       </c>
       <c r="AF12" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG12" s="51">
-        <v>2.1916273923414038</v>
+        <f t="shared" si="0"/>
+        <v>1.1147539929989985E-4</v>
+      </c>
+      <c r="AG12" s="97">
+        <v>0</v>
       </c>
       <c r="AH12" s="51">
         <v>2.1916273923414038</v>
       </c>
-      <c r="AI12" s="97">
+      <c r="AI12" s="51">
+        <v>2.1916273923414038</v>
+      </c>
+      <c r="AJ12" s="97">
         <v>3.1270187115295611E-4</v>
       </c>
-      <c r="AJ12" s="51">
+      <c r="AK12" s="51">
         <v>4.1823212657618296E-4</v>
       </c>
-      <c r="AK12" s="51">
+      <c r="AL12" s="51">
         <v>1.3882235872714782E-4</v>
       </c>
-      <c r="AL12" s="51">
+      <c r="AM12" s="51">
         <v>4.2164737460304589E-3</v>
       </c>
-      <c r="AM12" s="51">
+      <c r="AN12" s="51">
         <v>2.6908731030060075E-4</v>
       </c>
-      <c r="AN12" s="51">
+      <c r="AO12" s="51">
         <v>6.9545693450555454E-4</v>
       </c>
-      <c r="AO12" s="51">
+      <c r="AP12" s="51">
         <v>1.4589095422337696E-3</v>
       </c>
-      <c r="AP12" s="51">
+      <c r="AQ12" s="51">
         <v>1.0599637127928867E-3</v>
       </c>
-      <c r="AQ12" s="108">
+      <c r="AR12" s="108">
         <v>7.6493149989187494E-5</v>
       </c>
-      <c r="AR12" s="108">
+      <c r="AS12" s="108">
         <v>1.4350523600710626E-3</v>
       </c>
-      <c r="AS12" s="108">
+      <c r="AT12" s="108">
         <v>1.8527574111123216E-4</v>
       </c>
-      <c r="AT12" s="108">
+      <c r="AU12" s="108">
         <v>9.2759211769203231E-4</v>
       </c>
-      <c r="AU12" s="51">
+      <c r="AV12" s="51">
         <v>1.044547668945385E-3</v>
-      </c>
-      <c r="AV12" s="51">
-        <v>2.6908731030060075E-4</v>
       </c>
       <c r="AW12" s="51">
         <v>2.6908731030060075E-4</v>
       </c>
       <c r="AX12" s="51">
+        <v>2.6908731030060075E-4</v>
+      </c>
+      <c r="AY12" s="51">
         <v>2.6102000331794207E-6</v>
       </c>
-      <c r="AY12" s="51">
+      <c r="AZ12" s="51">
         <v>4.9495938610220581E-6</v>
-      </c>
-      <c r="AZ12" s="51">
-        <v>1.0634913488805668E-3</v>
       </c>
       <c r="BA12" s="51">
         <v>1.0634913488805668E-3</v>
@@ -13352,40 +13418,43 @@
         <v>1.0634913488805668E-3</v>
       </c>
       <c r="BF12" s="51">
+        <v>1.0634913488805668E-3</v>
+      </c>
+      <c r="BG12" s="51">
         <v>1.6627469622985393E-4</v>
       </c>
-      <c r="BG12" s="51">
+      <c r="BH12" s="51">
         <v>6.0947369538356957E-5</v>
       </c>
-      <c r="BH12" s="51">
+      <c r="BI12" s="51">
         <v>1.0634913488805668E-3</v>
       </c>
-      <c r="BI12" s="51">
+      <c r="BJ12" s="51">
         <v>2.120787526958279E-5</v>
       </c>
-      <c r="BJ12" s="51">
+      <c r="BK12" s="51">
         <v>2.01041E-4</v>
       </c>
-      <c r="BK12" s="51">
+      <c r="BL12" s="51">
         <v>1.6220539941598399E-4</v>
       </c>
-      <c r="BL12" s="51">
+      <c r="BM12" s="51">
         <v>6.9839409218922892E-3</v>
       </c>
-      <c r="BM12" s="51">
+      <c r="BN12" s="51">
         <v>3.9233022845947815E-4</v>
       </c>
-      <c r="BN12" s="51">
+      <c r="BO12" s="51">
         <v>7.4279147469320404E-5</v>
       </c>
-      <c r="BO12" s="51">
+      <c r="BP12" s="51">
         <v>3.398798089930026E-5</v>
       </c>
-      <c r="BP12" s="51">
+      <c r="BQ12" s="51">
         <v>8.245826402391268E-5</v>
       </c>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>52</v>
       </c>
@@ -13480,67 +13549,68 @@
         <v>0</v>
       </c>
       <c r="AF13" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="51">
-        <v>2.0504089814962967</v>
+        <f t="shared" si="0"/>
+        <v>7.4767003995855185E-5</v>
+      </c>
+      <c r="AG13" s="97">
+        <v>0</v>
       </c>
       <c r="AH13" s="51">
         <v>2.0504089814962967</v>
       </c>
-      <c r="AI13" s="97">
+      <c r="AI13" s="51">
+        <v>2.0504089814962967</v>
+      </c>
+      <c r="AJ13" s="97">
         <v>2.9407544343232545E-4</v>
       </c>
-      <c r="AJ13" s="51">
+      <c r="AK13" s="51">
         <v>1.5602644631362996E-4</v>
       </c>
-      <c r="AK13" s="51">
+      <c r="AL13" s="51">
         <v>1.0508828417083725E-4</v>
       </c>
-      <c r="AL13" s="51">
+      <c r="AM13" s="51">
         <v>8.1868321354229697E-4</v>
       </c>
-      <c r="AM13" s="51">
+      <c r="AN13" s="51">
         <v>1.7491465796201544E-4</v>
       </c>
-      <c r="AN13" s="51">
+      <c r="AO13" s="51">
         <v>4.1378137391431141E-4</v>
       </c>
-      <c r="AO13" s="51">
+      <c r="AP13" s="51">
         <v>1.0168576839743771E-3</v>
       </c>
-      <c r="AP13" s="51">
+      <c r="AQ13" s="51">
         <v>8.3419110835793436E-4</v>
       </c>
-      <c r="AQ13" s="108">
+      <c r="AR13" s="108">
         <v>2.6501667394179705E-5</v>
       </c>
-      <c r="AR13" s="108">
+      <c r="AS13" s="108">
         <v>6.9239656736841285E-4</v>
       </c>
-      <c r="AS13" s="108">
+      <c r="AT13" s="108">
         <v>1.368227648988548E-4</v>
       </c>
-      <c r="AT13" s="108">
+      <c r="AU13" s="108">
         <v>4.2434005302537548E-4</v>
       </c>
-      <c r="AU13" s="51">
+      <c r="AV13" s="51">
         <v>8.2010946996604207E-4</v>
-      </c>
-      <c r="AV13" s="51">
-        <v>1.7491465796201544E-4</v>
       </c>
       <c r="AW13" s="51">
         <v>1.7491465796201544E-4</v>
       </c>
       <c r="AX13" s="51">
+        <v>1.7491465796201544E-4</v>
+      </c>
+      <c r="AY13" s="51">
         <v>1.4318903971349838E-6</v>
       </c>
-      <c r="AY13" s="51">
+      <c r="AZ13" s="51">
         <v>2.7154446379280947E-6</v>
-      </c>
-      <c r="AZ13" s="51">
-        <v>8.5485325088438557E-4</v>
       </c>
       <c r="BA13" s="51">
         <v>8.5485325088438557E-4</v>
@@ -13558,40 +13628,43 @@
         <v>8.5485325088438557E-4</v>
       </c>
       <c r="BF13" s="51">
+        <v>8.5485325088438557E-4</v>
+      </c>
+      <c r="BG13" s="51">
         <v>1.2868340296769327E-4</v>
       </c>
-      <c r="BG13" s="51">
+      <c r="BH13" s="51">
         <v>4.3722343457981401E-5</v>
       </c>
-      <c r="BH13" s="51">
+      <c r="BI13" s="51">
         <v>8.5485325088438557E-4</v>
       </c>
-      <c r="BI13" s="51">
+      <c r="BJ13" s="51">
         <v>1.1634109476721748E-5</v>
       </c>
-      <c r="BJ13" s="51">
+      <c r="BK13" s="51">
         <v>1.60686E-4</v>
       </c>
-      <c r="BK13" s="51">
+      <c r="BL13" s="51">
         <v>1.2564456786316416E-4</v>
       </c>
-      <c r="BL13" s="51">
+      <c r="BM13" s="51">
         <v>5.9956379317822623E-3</v>
       </c>
-      <c r="BM13" s="51">
+      <c r="BN13" s="51">
         <v>2.0326514725382689E-4</v>
       </c>
-      <c r="BN13" s="51">
+      <c r="BO13" s="51">
         <v>6.4530878468949487E-5</v>
       </c>
-      <c r="BO13" s="51">
+      <c r="BP13" s="51">
         <v>3.3383269367365187E-5</v>
       </c>
-      <c r="BP13" s="51">
+      <c r="BQ13" s="51">
         <v>7.2056775732025927E-5</v>
       </c>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>53</v>
       </c>
@@ -13686,67 +13759,68 @@
         <v>0</v>
       </c>
       <c r="AF14" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG14" s="51">
-        <v>13.508553407967</v>
+        <f t="shared" si="0"/>
+        <v>5.6358026481416771E-4</v>
+      </c>
+      <c r="AG14" s="97">
+        <v>0</v>
       </c>
       <c r="AH14" s="51">
         <v>13.508553407967</v>
       </c>
-      <c r="AI14" s="97">
+      <c r="AI14" s="51">
+        <v>13.508553407967</v>
+      </c>
+      <c r="AJ14" s="97">
         <v>1.853105547938629E-3</v>
       </c>
-      <c r="AJ14" s="51">
+      <c r="AK14" s="51">
         <v>6.5035646998658919E-4</v>
       </c>
-      <c r="AK14" s="51">
+      <c r="AL14" s="51">
         <v>1.4036898131768901E-4</v>
       </c>
-      <c r="AL14" s="51">
+      <c r="AM14" s="51">
         <v>7.511526190629933E-3</v>
       </c>
-      <c r="AM14" s="51">
+      <c r="AN14" s="51">
         <v>1.1898636051740278E-3</v>
       </c>
-      <c r="AN14" s="51">
+      <c r="AO14" s="51">
         <v>6.1402604767802202E-3</v>
       </c>
-      <c r="AO14" s="51">
+      <c r="AP14" s="51">
         <v>3.0619331573313643E-2</v>
       </c>
-      <c r="AP14" s="51">
+      <c r="AQ14" s="51">
         <v>1.1066924513396071E-2</v>
       </c>
-      <c r="AQ14" s="108">
+      <c r="AR14" s="108">
         <v>3.8188885462792113E-5</v>
       </c>
-      <c r="AR14" s="108">
+      <c r="AS14" s="108">
         <v>9.2300987745307112E-3</v>
       </c>
-      <c r="AS14" s="108">
+      <c r="AT14" s="108">
         <v>1.176737721847586E-3</v>
       </c>
-      <c r="AT14" s="108">
+      <c r="AU14" s="108">
         <v>3.2216592053520257E-3</v>
       </c>
-      <c r="AU14" s="51">
+      <c r="AV14" s="51">
         <v>1.0968511328533553E-2</v>
-      </c>
-      <c r="AV14" s="51">
-        <v>1.1898636051740278E-3</v>
       </c>
       <c r="AW14" s="51">
         <v>1.1898636051740278E-3</v>
       </c>
       <c r="AX14" s="51">
+        <v>1.1898636051740278E-3</v>
+      </c>
+      <c r="AY14" s="51">
         <v>1.5287602234490922E-5</v>
       </c>
-      <c r="AY14" s="51">
+      <c r="AZ14" s="51">
         <v>6.8998478822275319E-6</v>
-      </c>
-      <c r="AZ14" s="51">
-        <v>6.7826237856860143E-3</v>
       </c>
       <c r="BA14" s="51">
         <v>6.7826237856860143E-3</v>
@@ -13764,40 +13838,43 @@
         <v>6.7826237856860143E-3</v>
       </c>
       <c r="BF14" s="51">
+        <v>6.7826237856860143E-3</v>
+      </c>
+      <c r="BG14" s="51">
         <v>1.058226135590116E-3</v>
       </c>
-      <c r="BG14" s="51">
+      <c r="BH14" s="51">
         <v>3.2176741797676966E-4</v>
       </c>
-      <c r="BH14" s="51">
+      <c r="BI14" s="51">
         <v>6.7826237856860143E-3</v>
       </c>
-      <c r="BI14" s="51">
+      <c r="BJ14" s="51">
         <v>1.2421176815523871E-4</v>
       </c>
-      <c r="BJ14" s="51">
+      <c r="BK14" s="51">
         <v>1.652819E-3</v>
       </c>
-      <c r="BK14" s="51">
+      <c r="BL14" s="51">
         <v>1.0024671553281843E-3</v>
       </c>
-      <c r="BL14" s="51">
+      <c r="BM14" s="51">
         <v>2.182482145703642E-2</v>
       </c>
-      <c r="BM14" s="51">
+      <c r="BN14" s="51">
         <v>1.3557166453407658E-2</v>
       </c>
-      <c r="BN14" s="51">
+      <c r="BO14" s="51">
         <v>5.4168132644715134E-4</v>
       </c>
-      <c r="BO14" s="51">
+      <c r="BP14" s="51">
         <v>9.8507999946265097E-5</v>
       </c>
-      <c r="BP14" s="51">
+      <c r="BQ14" s="51">
         <v>6.0822760339839291E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>54</v>
       </c>
@@ -13892,67 +13969,68 @@
         <v>0</v>
       </c>
       <c r="AF15" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG15" s="51">
-        <v>0.18585087123256866</v>
+        <f t="shared" si="0"/>
+        <v>7.4628800560922671E-6</v>
+      </c>
+      <c r="AG15" s="97">
+        <v>0</v>
       </c>
       <c r="AH15" s="51">
         <v>0.18585087123256866</v>
       </c>
-      <c r="AI15" s="97">
+      <c r="AI15" s="51">
+        <v>0.18585087123256866</v>
+      </c>
+      <c r="AJ15" s="97">
         <v>4.1759752642281592E-5</v>
       </c>
-      <c r="AJ15" s="51">
+      <c r="AK15" s="51">
         <v>1.7872477884974561E-5</v>
       </c>
-      <c r="AK15" s="51">
+      <c r="AL15" s="51">
         <v>8.5961918351453069E-6</v>
       </c>
-      <c r="AL15" s="51">
+      <c r="AM15" s="51">
         <v>6.118662096424913E-5</v>
       </c>
-      <c r="AM15" s="51">
+      <c r="AN15" s="51">
         <v>1.4993960373938642E-5</v>
       </c>
-      <c r="AN15" s="51">
+      <c r="AO15" s="51">
         <v>4.1240169230845359E-5</v>
       </c>
-      <c r="AO15" s="51">
+      <c r="AP15" s="51">
         <v>1.0272973218978136E-4</v>
       </c>
-      <c r="AP15" s="51">
+      <c r="AQ15" s="51">
         <v>4.7521443376567185E-5</v>
       </c>
-      <c r="AQ15" s="108">
+      <c r="AR15" s="108">
         <v>1.0074152413072438E-6</v>
       </c>
-      <c r="AR15" s="108">
+      <c r="AS15" s="108">
         <v>8.1880009979099035E-6</v>
       </c>
-      <c r="AS15" s="108">
+      <c r="AT15" s="108">
         <v>1.2194979869284162E-5</v>
       </c>
-      <c r="AT15" s="108">
+      <c r="AU15" s="108">
         <v>6.1688220508681354E-6</v>
       </c>
-      <c r="AU15" s="51">
+      <c r="AV15" s="51">
         <v>4.4858455906128154E-5</v>
-      </c>
-      <c r="AV15" s="51">
-        <v>1.499396037393864E-5</v>
       </c>
       <c r="AW15" s="51">
         <v>1.499396037393864E-5</v>
       </c>
       <c r="AX15" s="51">
+        <v>1.499396037393864E-5</v>
+      </c>
+      <c r="AY15" s="51">
         <v>7.5197981910804767E-8</v>
       </c>
-      <c r="AY15" s="51">
+      <c r="AZ15" s="51">
         <v>1.065325835898643E-7</v>
-      </c>
-      <c r="AZ15" s="51">
-        <v>1.065287447716148E-4</v>
       </c>
       <c r="BA15" s="51">
         <v>1.065287447716148E-4</v>
@@ -13970,40 +14048,43 @@
         <v>1.065287447716148E-4</v>
       </c>
       <c r="BF15" s="51">
+        <v>1.065287447716148E-4</v>
+      </c>
+      <c r="BG15" s="51">
         <v>1.6443972177294838E-5</v>
       </c>
-      <c r="BG15" s="51">
+      <c r="BH15" s="51">
         <v>4.0128658904944647E-6</v>
       </c>
-      <c r="BH15" s="51">
+      <c r="BI15" s="51">
         <v>1.065287447716148E-4</v>
       </c>
-      <c r="BI15" s="51">
+      <c r="BJ15" s="51">
         <v>6.1098360302528867E-7</v>
       </c>
-      <c r="BJ15" s="51">
+      <c r="BK15" s="51">
         <v>2.4223000000000002E-5</v>
       </c>
-      <c r="BK15" s="51">
+      <c r="BL15" s="51">
         <v>1.3277447299330108E-5</v>
       </c>
-      <c r="BL15" s="51">
+      <c r="BM15" s="51">
         <v>2.363582970813479E-3</v>
       </c>
-      <c r="BM15" s="51">
+      <c r="BN15" s="51">
         <v>3.2718107917875022E-5</v>
       </c>
-      <c r="BN15" s="51">
+      <c r="BO15" s="51">
         <v>9.7172067289831399E-6</v>
       </c>
-      <c r="BO15" s="51">
+      <c r="BP15" s="51">
         <v>5.6266433702982988E-6</v>
       </c>
-      <c r="BP15" s="51">
+      <c r="BQ15" s="51">
         <v>1.1192972181725723E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>55</v>
       </c>
@@ -14098,67 +14179,68 @@
         <v>0</v>
       </c>
       <c r="AF16" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG16" s="51">
-        <v>0.44413558847092516</v>
+        <f t="shared" si="0"/>
+        <v>2.4302538521693214E-5</v>
+      </c>
+      <c r="AG16" s="97">
+        <v>0</v>
       </c>
       <c r="AH16" s="51">
         <v>0.44413558847092516</v>
       </c>
-      <c r="AI16" s="97">
+      <c r="AI16" s="51">
+        <v>0.44413558847092516</v>
+      </c>
+      <c r="AJ16" s="97">
         <v>1.0849974006181372E-4</v>
       </c>
-      <c r="AJ16" s="51">
+      <c r="AK16" s="51">
         <v>2.6269817949653039E-5</v>
       </c>
-      <c r="AK16" s="51">
+      <c r="AL16" s="51">
         <v>1.6404056370215794E-5</v>
       </c>
-      <c r="AL16" s="51">
+      <c r="AM16" s="51">
         <v>1.3089373181002996E-4</v>
       </c>
-      <c r="AM16" s="51">
+      <c r="AN16" s="51">
         <v>4.8181655814015295E-5</v>
       </c>
-      <c r="AN16" s="51">
+      <c r="AO16" s="51">
         <v>1.0351629331675042E-4</v>
       </c>
-      <c r="AO16" s="51">
+      <c r="AP16" s="51">
         <v>2.0829394365546249E-4</v>
       </c>
-      <c r="AP16" s="51">
+      <c r="AQ16" s="51">
         <v>1.054226407172321E-4</v>
       </c>
-      <c r="AQ16" s="108">
+      <c r="AR16" s="108">
         <v>2.4143630282031166E-6</v>
       </c>
-      <c r="AR16" s="108">
+      <c r="AS16" s="108">
         <v>2.3944614337886097E-5</v>
       </c>
-      <c r="AS16" s="108">
+      <c r="AT16" s="108">
         <v>4.3084645016142185E-5</v>
       </c>
-      <c r="AT16" s="108">
+      <c r="AU16" s="108">
         <v>1.6265424272844858E-5</v>
       </c>
-      <c r="AU16" s="51">
+      <c r="AV16" s="51">
         <v>9.8372876122563224E-5</v>
-      </c>
-      <c r="AV16" s="51">
-        <v>4.8181655814015295E-5</v>
       </c>
       <c r="AW16" s="51">
         <v>4.8181655814015295E-5</v>
       </c>
       <c r="AX16" s="51">
+        <v>4.8181655814015295E-5</v>
+      </c>
+      <c r="AY16" s="51">
         <v>3.6538217627142357E-7</v>
       </c>
-      <c r="AY16" s="51">
+      <c r="AZ16" s="51">
         <v>1.5091160608896177E-7</v>
-      </c>
-      <c r="AZ16" s="51">
-        <v>2.7484911916987408E-4</v>
       </c>
       <c r="BA16" s="51">
         <v>2.7484911916987408E-4</v>
@@ -14176,40 +14258,43 @@
         <v>2.7484911916987408E-4</v>
       </c>
       <c r="BF16" s="51">
+        <v>2.7484911916987408E-4</v>
+      </c>
+      <c r="BG16" s="51">
         <v>4.0677473538700538E-5</v>
       </c>
-      <c r="BG16" s="51">
+      <c r="BH16" s="51">
         <v>1.1434508270900258E-5</v>
       </c>
-      <c r="BH16" s="51">
+      <c r="BI16" s="51">
         <v>2.7484911916987408E-4</v>
       </c>
-      <c r="BI16" s="51">
+      <c r="BJ16" s="51">
         <v>2.9687301822053166E-6</v>
       </c>
-      <c r="BJ16" s="51">
+      <c r="BK16" s="51">
         <v>5.9191000000000003E-5</v>
       </c>
-      <c r="BK16" s="51">
+      <c r="BL16" s="51">
         <v>4.246923512610396E-5</v>
       </c>
-      <c r="BL16" s="51">
+      <c r="BM16" s="51">
         <v>1.2090940693830438E-3</v>
       </c>
-      <c r="BM16" s="51">
+      <c r="BN16" s="51">
         <v>5.3261285895382865E-5</v>
       </c>
-      <c r="BN16" s="51">
+      <c r="BO16" s="51">
         <v>2.5692709376555415E-5</v>
       </c>
-      <c r="BO16" s="51">
+      <c r="BP16" s="51">
         <v>1.4215912657140629E-5</v>
       </c>
-      <c r="BP16" s="51">
+      <c r="BQ16" s="51">
         <v>2.7449972577494612E-5</v>
       </c>
     </row>
-    <row r="17" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>56</v>
       </c>
@@ -14304,67 +14389,68 @@
         <v>0</v>
       </c>
       <c r="AF17" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG17" s="51">
-        <v>253.36281754574139</v>
+        <f t="shared" si="0"/>
+        <v>3.2311322785073021E-3</v>
+      </c>
+      <c r="AG17" s="97">
+        <v>0</v>
       </c>
       <c r="AH17" s="51">
         <v>253.36281754574139</v>
       </c>
-      <c r="AI17" s="97">
+      <c r="AI17" s="51">
+        <v>253.36281754574139</v>
+      </c>
+      <c r="AJ17" s="97">
         <v>2.2322295843704987E-2</v>
       </c>
-      <c r="AJ17" s="51">
+      <c r="AK17" s="51">
         <v>3.2264463834966333E-3</v>
       </c>
-      <c r="AK17" s="51">
+      <c r="AL17" s="51">
         <v>6.8302849678478087E-4</v>
       </c>
-      <c r="AL17" s="51">
+      <c r="AM17" s="51">
         <v>1.9069747889327696E-2</v>
       </c>
-      <c r="AM17" s="51">
+      <c r="AN17" s="51">
         <v>6.2965892828091927E-3</v>
       </c>
-      <c r="AN17" s="51">
+      <c r="AO17" s="51">
         <v>1.5000607598845347E-2</v>
       </c>
-      <c r="AO17" s="51">
+      <c r="AP17" s="51">
         <v>5.2474264130324251E-2</v>
       </c>
-      <c r="AP17" s="51">
+      <c r="AQ17" s="51">
         <v>6.8300938248962439E-3</v>
       </c>
-      <c r="AQ17" s="108">
+      <c r="AR17" s="108">
         <v>4.4725954808079494E-5</v>
       </c>
-      <c r="AR17" s="108">
+      <c r="AS17" s="108">
         <v>4.0645412083838168E-3</v>
       </c>
-      <c r="AS17" s="108">
+      <c r="AT17" s="108">
         <v>9.9076876694219069E-3</v>
       </c>
-      <c r="AT17" s="108">
+      <c r="AU17" s="108">
         <v>4.2538513876070484E-3</v>
       </c>
-      <c r="AU17" s="51">
+      <c r="AV17" s="51">
         <v>2.1559627906224867E-3</v>
-      </c>
-      <c r="AV17" s="51">
-        <v>6.2965892828091927E-3</v>
       </c>
       <c r="AW17" s="51">
         <v>6.2965892828091927E-3</v>
       </c>
       <c r="AX17" s="51">
+        <v>6.2965892828091927E-3</v>
+      </c>
+      <c r="AY17" s="51">
         <v>4.7791147055317132E-5</v>
       </c>
-      <c r="AY17" s="51">
+      <c r="AZ17" s="51">
         <v>5.0919237194982617E-6</v>
-      </c>
-      <c r="AZ17" s="51">
-        <v>3.6518829969822073E-2</v>
       </c>
       <c r="BA17" s="51">
         <v>3.6518829969822073E-2</v>
@@ -14382,40 +14468,43 @@
         <v>3.6518829969822073E-2</v>
       </c>
       <c r="BF17" s="51">
+        <v>3.6518829969822073E-2</v>
+      </c>
+      <c r="BG17" s="51">
         <v>5.7378016001246286E-3</v>
       </c>
-      <c r="BG17" s="51">
+      <c r="BH17" s="51">
         <v>2.9641347912872651E-3</v>
       </c>
-      <c r="BH17" s="51">
+      <c r="BI17" s="51">
         <v>3.6518829969822073E-2</v>
       </c>
-      <c r="BI17" s="51">
+      <c r="BJ17" s="51">
         <v>3.8830306982445172E-4</v>
       </c>
-      <c r="BJ17" s="51">
+      <c r="BK17" s="51">
         <v>5.8936729999999994E-3</v>
       </c>
-      <c r="BK17" s="51">
+      <c r="BL17" s="51">
         <v>1.1430134964912938E-2</v>
       </c>
-      <c r="BL17" s="51">
+      <c r="BM17" s="51">
         <v>0.12226143774674139</v>
       </c>
-      <c r="BM17" s="51">
+      <c r="BN17" s="51">
         <v>1.9528710437986155E-2</v>
       </c>
-      <c r="BN17" s="51">
+      <c r="BO17" s="51">
         <v>4.7292925714375123E-3</v>
       </c>
-      <c r="BO17" s="51">
+      <c r="BP17" s="51">
         <v>1.9215986089099715E-3</v>
       </c>
-      <c r="BP17" s="51">
+      <c r="BQ17" s="51">
         <v>4.6679297023467672E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>57</v>
       </c>
@@ -14510,67 +14599,68 @@
         <v>0</v>
       </c>
       <c r="AF18" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG18" s="51">
-        <v>1.7377733095783761</v>
+        <f t="shared" si="0"/>
+        <v>3.1113524280317462E-5</v>
+      </c>
+      <c r="AG18" s="97">
+        <v>0</v>
       </c>
       <c r="AH18" s="51">
         <v>1.7377733095783761</v>
       </c>
-      <c r="AI18" s="97">
+      <c r="AI18" s="51">
+        <v>1.7377733095783761</v>
+      </c>
+      <c r="AJ18" s="97">
         <v>1.7437257460515478E-2</v>
       </c>
-      <c r="AJ18" s="51">
+      <c r="AK18" s="51">
         <v>1.002250951053452E-3</v>
       </c>
-      <c r="AK18" s="51">
+      <c r="AL18" s="51">
         <v>1.2334276856587168E-6</v>
       </c>
-      <c r="AL18" s="51">
+      <c r="AM18" s="51">
         <v>5.2290508742300628E-4</v>
       </c>
-      <c r="AM18" s="51">
+      <c r="AN18" s="51">
         <v>5.6079243682504259E-5</v>
       </c>
-      <c r="AN18" s="51">
+      <c r="AO18" s="51">
         <v>3.3711915727577973E-4</v>
       </c>
-      <c r="AO18" s="51">
+      <c r="AP18" s="51">
         <v>4.6923403382535925E-4</v>
       </c>
-      <c r="AP18" s="51">
+      <c r="AQ18" s="51">
         <v>3.4540205401445904E-5</v>
       </c>
-      <c r="AQ18" s="108">
+      <c r="AR18" s="108">
         <v>7.7673225037144343E-7</v>
       </c>
-      <c r="AR18" s="108">
+      <c r="AS18" s="108">
         <v>2.3104473467376116E-5</v>
       </c>
-      <c r="AS18" s="108">
+      <c r="AT18" s="108">
         <v>4.0808361892545356E-5</v>
       </c>
-      <c r="AT18" s="108">
+      <c r="AU18" s="108">
         <v>1.7384511736016079E-5</v>
       </c>
-      <c r="AU18" s="51">
+      <c r="AV18" s="51">
         <v>2.439264208002629E-5</v>
-      </c>
-      <c r="AV18" s="51">
-        <v>5.6079243682504252E-5</v>
       </c>
       <c r="AW18" s="51">
         <v>5.6079243682504252E-5</v>
       </c>
       <c r="AX18" s="51">
+        <v>5.6079243682504252E-5</v>
+      </c>
+      <c r="AY18" s="51">
         <v>4.5807200562031658E-7</v>
       </c>
-      <c r="AY18" s="51">
+      <c r="AZ18" s="51">
         <v>5.891145581849599E-8</v>
-      </c>
-      <c r="AZ18" s="51">
-        <v>2.7965297583711242E-4</v>
       </c>
       <c r="BA18" s="51">
         <v>2.7965297583711242E-4</v>
@@ -14588,40 +14678,43 @@
         <v>2.7965297583711242E-4</v>
       </c>
       <c r="BF18" s="51">
+        <v>2.7965297583711242E-4</v>
+      </c>
+      <c r="BG18" s="51">
         <v>4.2891207360095945E-5</v>
       </c>
-      <c r="BG18" s="51">
+      <c r="BH18" s="51">
         <v>2.349282321281286E-5</v>
       </c>
-      <c r="BH18" s="51">
+      <c r="BI18" s="51">
         <v>2.7965297583711242E-4</v>
       </c>
-      <c r="BI18" s="51">
+      <c r="BJ18" s="51">
         <v>3.7218350456650725E-6</v>
       </c>
-      <c r="BJ18" s="51">
+      <c r="BK18" s="51">
         <v>2.0967329999999999E-3</v>
       </c>
-      <c r="BK18" s="51">
+      <c r="BL18" s="51">
         <v>4.462441199518442E-5</v>
       </c>
-      <c r="BL18" s="51">
+      <c r="BM18" s="51">
         <v>6.2487234523302231E-2</v>
       </c>
-      <c r="BM18" s="51">
+      <c r="BN18" s="51">
         <v>8.8356010400824942E-5</v>
       </c>
-      <c r="BN18" s="51">
+      <c r="BO18" s="51">
         <v>3.6622673706587653E-3</v>
       </c>
-      <c r="BO18" s="51">
+      <c r="BP18" s="51">
         <v>1.6813938869836862E-5</v>
       </c>
-      <c r="BP18" s="51">
+      <c r="BQ18" s="51">
         <v>4.8283115828002249E-6</v>
       </c>
     </row>
-    <row r="19" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>58</v>
       </c>
@@ -14716,67 +14809,68 @@
         <v>0</v>
       </c>
       <c r="AF19" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG19" s="51">
-        <v>75408.791415255429</v>
+        <f t="shared" si="0"/>
+        <v>1.2135062343035297</v>
+      </c>
+      <c r="AG19" s="97">
+        <v>0</v>
       </c>
       <c r="AH19" s="51">
         <v>75408.791415255429</v>
       </c>
-      <c r="AI19" s="98">
+      <c r="AI19" s="51">
+        <v>75408.791415255429</v>
+      </c>
+      <c r="AJ19" s="98">
         <v>4.1671233462981707</v>
       </c>
-      <c r="AJ19" s="51">
+      <c r="AK19" s="51">
         <v>1.1157612238478314</v>
       </c>
-      <c r="AK19" s="51">
+      <c r="AL19" s="51">
         <v>1.2627002352231111</v>
       </c>
-      <c r="AL19" s="51">
+      <c r="AM19" s="51">
         <v>8.6708238175555881</v>
       </c>
-      <c r="AM19" s="51">
+      <c r="AN19" s="51">
         <v>3.0835751219721632</v>
       </c>
-      <c r="AN19" s="51">
+      <c r="AO19" s="51">
         <v>6.3943752486573908</v>
       </c>
-      <c r="AO19" s="51">
+      <c r="AP19" s="51">
         <v>10.880109009531633</v>
       </c>
-      <c r="AP19" s="51">
+      <c r="AQ19" s="51">
         <v>1.5203390780174186</v>
       </c>
-      <c r="AQ19" s="108">
+      <c r="AR19" s="108">
         <v>9.4841874510463234E-2</v>
       </c>
-      <c r="AR19" s="108">
+      <c r="AS19" s="108">
         <v>2.285979415679499</v>
       </c>
-      <c r="AS19" s="108">
+      <c r="AT19" s="108">
         <v>1.8023928088902272</v>
       </c>
-      <c r="AT19" s="108">
+      <c r="AU19" s="108">
         <v>0.79472117156330102</v>
       </c>
-      <c r="AU19" s="51">
+      <c r="AV19" s="51">
         <v>1.0114638889108551</v>
-      </c>
-      <c r="AV19" s="51">
-        <v>3.0835751219721628</v>
       </c>
       <c r="AW19" s="51">
         <v>3.0835751219721628</v>
       </c>
       <c r="AX19" s="51">
+        <v>3.0835751219721628</v>
+      </c>
+      <c r="AY19" s="51">
         <v>2.2540237665439691E-2</v>
       </c>
-      <c r="AY19" s="51">
+      <c r="AZ19" s="51">
         <v>3.8465275441921408E-3</v>
-      </c>
-      <c r="AZ19" s="51">
-        <v>11.027823611486687</v>
       </c>
       <c r="BA19" s="51">
         <v>11.027823611486687</v>
@@ -14794,40 +14888,43 @@
         <v>11.027823611486687</v>
       </c>
       <c r="BF19" s="51">
+        <v>11.027823611486687</v>
+      </c>
+      <c r="BG19" s="51">
         <v>1.9038082662446976</v>
       </c>
-      <c r="BG19" s="51">
+      <c r="BH19" s="51">
         <v>0.98516450405410128</v>
       </c>
-      <c r="BH19" s="51">
+      <c r="BI19" s="51">
         <v>11.027823611486687</v>
       </c>
-      <c r="BI19" s="51">
+      <c r="BJ19" s="51">
         <v>0.18313943103169752</v>
       </c>
-      <c r="BJ19" s="51">
+      <c r="BK19" s="51">
         <v>1.9748460000000001</v>
       </c>
-      <c r="BK19" s="51">
+      <c r="BL19" s="51">
         <v>2.4082502303115878</v>
       </c>
-      <c r="BL19" s="51">
+      <c r="BM19" s="51">
         <v>33.662755662531829</v>
       </c>
-      <c r="BM19" s="51">
+      <c r="BN19" s="51">
         <v>2.6286261463371274</v>
       </c>
-      <c r="BN19" s="51">
+      <c r="BO19" s="51">
         <v>0.83876126877143187</v>
       </c>
-      <c r="BO19" s="51">
+      <c r="BP19" s="51">
         <v>0.56982490603351421</v>
       </c>
-      <c r="BP19" s="51">
+      <c r="BQ19" s="51">
         <v>0.22939459728231432</v>
       </c>
     </row>
-    <row r="20" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A20" s="95" t="s">
         <v>328</v>
       </c>
@@ -14922,67 +15019,68 @@
         <v>0</v>
       </c>
       <c r="AF20" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG20" s="51">
-        <v>0.98473222509014713</v>
+        <f t="shared" si="0"/>
+        <v>1.0183577867439129E-5</v>
+      </c>
+      <c r="AG20" s="97">
+        <v>0</v>
       </c>
       <c r="AH20" s="51">
         <v>0.98473222509014713</v>
       </c>
-      <c r="AI20" s="97">
+      <c r="AI20" s="51">
+        <v>0.98473222509014713</v>
+      </c>
+      <c r="AJ20" s="97">
         <v>2.6301349442907818E-4</v>
       </c>
-      <c r="AJ20" s="51">
+      <c r="AK20" s="51">
         <v>3.5052431602284993E-4</v>
       </c>
-      <c r="AK20" s="51">
+      <c r="AL20" s="51">
         <v>1.1174985015707548E-6</v>
       </c>
-      <c r="AL20" s="51">
+      <c r="AM20" s="51">
         <v>1.5654051881137926E-4</v>
       </c>
-      <c r="AM20" s="51">
+      <c r="AN20" s="51">
         <v>2.0232628915214837E-5</v>
       </c>
-      <c r="AN20" s="51">
+      <c r="AO20" s="51">
         <v>5.1798395209010816E-5</v>
       </c>
-      <c r="AO20" s="51">
+      <c r="AP20" s="51">
         <v>1.4991638071334959E-4</v>
       </c>
-      <c r="AP20" s="51">
+      <c r="AQ20" s="51">
         <v>2.7500515449821973E-5</v>
       </c>
-      <c r="AQ20" s="109">
+      <c r="AR20" s="109">
         <v>4.400560658140986E-5</v>
       </c>
-      <c r="AR20" s="110">
+      <c r="AS20" s="110">
         <v>5.7831542283699589E-6</v>
       </c>
-      <c r="AS20" s="110">
+      <c r="AT20" s="110">
         <v>2.733836622065192E-4</v>
       </c>
-      <c r="AT20" s="109">
+      <c r="AU20" s="109">
         <v>9.3270335485895916E-6</v>
       </c>
-      <c r="AU20" s="51">
+      <c r="AV20" s="51">
         <v>2.2900198522228669E-5</v>
-      </c>
-      <c r="AV20" s="51">
-        <v>2.0232628915214837E-5</v>
       </c>
       <c r="AW20" s="51">
         <v>2.0232628915214837E-5</v>
       </c>
       <c r="AX20" s="51">
+        <v>2.0232628915214837E-5</v>
+      </c>
+      <c r="AY20" s="51">
         <v>1.7901963056516892E-7</v>
       </c>
-      <c r="AY20" s="51">
+      <c r="AZ20" s="51">
         <v>7.389858991106616E-8</v>
-      </c>
-      <c r="AZ20" s="51">
-        <v>2.3478130550948399E-4</v>
       </c>
       <c r="BA20" s="51">
         <v>2.3478130550948399E-4</v>
@@ -15000,40 +15098,43 @@
         <v>2.3478130550948399E-4</v>
       </c>
       <c r="BF20" s="51">
+        <v>2.3478130550948399E-4</v>
+      </c>
+      <c r="BG20" s="51">
         <v>4.5126418033472775E-5</v>
       </c>
-      <c r="BG20" s="51">
+      <c r="BH20" s="51">
         <v>1.1157978124787627E-5</v>
       </c>
-      <c r="BH20" s="51">
+      <c r="BI20" s="51">
         <v>2.3478130550948399E-4</v>
       </c>
-      <c r="BI20" s="51">
+      <c r="BJ20" s="51">
         <v>1.4545344983419976E-6</v>
       </c>
-      <c r="BJ20" s="51">
+      <c r="BK20" s="51">
         <v>1.8387899999999999E-4</v>
       </c>
-      <c r="BK20" s="51">
+      <c r="BL20" s="51">
         <v>1.9894937474460199E-4</v>
       </c>
-      <c r="BL20" s="51">
+      <c r="BM20" s="51">
         <v>2.2701246598357708E-3</v>
       </c>
-      <c r="BM20" s="51">
+      <c r="BN20" s="51">
         <v>4.379079485914717E-5</v>
       </c>
-      <c r="BN20" s="51">
+      <c r="BO20" s="51">
         <v>8.2226444843980003E-6</v>
       </c>
-      <c r="BO20" s="51">
+      <c r="BP20" s="51">
         <v>5.2800697979831783E-6</v>
       </c>
-      <c r="BP20" s="51">
+      <c r="BQ20" s="51">
         <v>5.1344722992501993E-6</v>
       </c>
     </row>
-    <row r="21" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A21" s="95" t="s">
         <v>329</v>
       </c>
@@ -15128,67 +15229,68 @@
         <v>0</v>
       </c>
       <c r="AF21" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG21" s="51">
-        <v>2.4637161821866642</v>
+        <f t="shared" si="0"/>
+        <v>8.9012827370724037E-5</v>
+      </c>
+      <c r="AG21" s="97">
+        <v>0</v>
       </c>
       <c r="AH21" s="51">
         <v>2.4637161821866642</v>
       </c>
       <c r="AI21" s="51">
+        <v>2.4637161821866642</v>
+      </c>
+      <c r="AJ21" s="51">
         <v>2.5209135850464039E-4</v>
       </c>
-      <c r="AJ21" s="51">
+      <c r="AK21" s="51">
         <v>5.2265362765144044E-5</v>
       </c>
-      <c r="AK21" s="51">
+      <c r="AL21" s="51">
         <v>3.9301129456925813E-6</v>
       </c>
-      <c r="AL21" s="51">
+      <c r="AM21" s="51">
         <v>3.6480895206674136E-4</v>
       </c>
-      <c r="AM21" s="51">
+      <c r="AN21" s="51">
         <v>1.7710347972885423E-4</v>
       </c>
-      <c r="AN21" s="51">
+      <c r="AO21" s="51">
         <v>4.5409676337714191E-4</v>
       </c>
-      <c r="AO21" s="51">
+      <c r="AP21" s="51">
         <v>7.5386616496120665E-4</v>
       </c>
-      <c r="AP21" s="51">
+      <c r="AQ21" s="51">
         <v>8.8351732360253017E-5</v>
       </c>
-      <c r="AQ21" s="110">
+      <c r="AR21" s="110">
         <v>3.6934187099323884E-5</v>
       </c>
-      <c r="AR21" s="110">
+      <c r="AS21" s="110">
         <v>5.9977046235993406E-5</v>
       </c>
-      <c r="AS21" s="110">
+      <c r="AT21" s="110">
         <v>3.3932464975774002E-4</v>
       </c>
-      <c r="AT21" s="110">
+      <c r="AU21" s="110">
         <v>3.294676430669605E-5</v>
       </c>
-      <c r="AU21" s="51">
+      <c r="AV21" s="51">
         <v>6.7095975498083116E-5</v>
-      </c>
-      <c r="AV21" s="51">
-        <v>1.7710347972885423E-4</v>
       </c>
       <c r="AW21" s="51">
         <v>1.7710347972885423E-4</v>
       </c>
       <c r="AX21" s="51">
+        <v>1.7710347972885423E-4</v>
+      </c>
+      <c r="AY21" s="51">
         <v>2.1385118764832851E-6</v>
       </c>
-      <c r="AY21" s="51">
+      <c r="AZ21" s="51">
         <v>1.5199824644066077E-7</v>
-      </c>
-      <c r="AZ21" s="51">
-        <v>6.1286116874635155E-4</v>
       </c>
       <c r="BA21" s="51">
         <v>6.1286116874635155E-4</v>
@@ -15206,40 +15308,43 @@
         <v>6.1286116874635155E-4</v>
       </c>
       <c r="BF21" s="51">
+        <v>6.1286116874635155E-4</v>
+      </c>
+      <c r="BG21" s="51">
         <v>7.7651203836893998E-5</v>
       </c>
-      <c r="BG21" s="51">
+      <c r="BH21" s="51">
         <v>4.8764874941060923E-5</v>
       </c>
-      <c r="BH21" s="51">
+      <c r="BI21" s="51">
         <v>6.1286116874635155E-4</v>
       </c>
-      <c r="BI21" s="51">
+      <c r="BJ21" s="51">
         <v>1.7375408996426691E-5</v>
       </c>
-      <c r="BJ21" s="51">
+      <c r="BK21" s="51">
         <v>1.6558400000000001E-4</v>
       </c>
-      <c r="BK21" s="51">
+      <c r="BL21" s="51">
         <v>2.6624821484953976E-4</v>
       </c>
-      <c r="BL21" s="51">
+      <c r="BM21" s="51">
         <v>2.0635038603674534E-3</v>
       </c>
-      <c r="BM21" s="51">
+      <c r="BN21" s="51">
         <v>1.6681578164179269E-4</v>
       </c>
-      <c r="BN21" s="51">
+      <c r="BO21" s="51">
         <v>2.7269050726089581E-5</v>
       </c>
-      <c r="BO21" s="51">
+      <c r="BP21" s="51">
         <v>2.4990313595886678E-5</v>
       </c>
-      <c r="BP21" s="51">
+      <c r="BQ21" s="51">
         <v>1.2548404837591077E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A22" s="95" t="s">
         <v>330</v>
       </c>
@@ -15334,67 +15439,68 @@
         <v>0</v>
       </c>
       <c r="AF22" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG22" s="51">
-        <v>3.2111856117297162</v>
+        <f t="shared" si="0"/>
+        <v>1.6760640385155267E-4</v>
+      </c>
+      <c r="AG22" s="97">
+        <v>0</v>
       </c>
       <c r="AH22" s="51">
         <v>3.2111856117297162</v>
       </c>
       <c r="AI22" s="51">
+        <v>3.2111856117297162</v>
+      </c>
+      <c r="AJ22" s="51">
         <v>4.0568812500610244E-4</v>
       </c>
-      <c r="AJ22" s="51">
+      <c r="AK22" s="51">
         <v>8.5498017104933708E-5</v>
       </c>
-      <c r="AK22" s="51">
+      <c r="AL22" s="51">
         <v>8.2271496004231284E-6</v>
       </c>
-      <c r="AL22" s="51">
+      <c r="AM22" s="51">
         <v>6.2611894234368437E-4</v>
       </c>
-      <c r="AM22" s="51">
+      <c r="AN22" s="51">
         <v>3.3943981679371304E-4</v>
       </c>
-      <c r="AN22" s="51">
+      <c r="AO22" s="51">
         <v>9.3692296015765637E-4</v>
       </c>
-      <c r="AO22" s="51">
+      <c r="AP22" s="51">
         <v>1.2035052695230119E-3</v>
       </c>
-      <c r="AP22" s="51">
+      <c r="AQ22" s="51">
         <v>2.6619353376776395E-4</v>
       </c>
-      <c r="AQ22" s="110">
+      <c r="AR22" s="110">
         <v>4.4375230969019702E-5</v>
       </c>
-      <c r="AR22" s="110">
+      <c r="AS22" s="110">
         <v>1.2182106474267705E-4</v>
       </c>
-      <c r="AS22" s="110">
+      <c r="AT22" s="110">
         <v>5.8909439567317529E-4</v>
       </c>
-      <c r="AT22" s="110">
+      <c r="AU22" s="110">
         <v>5.6037647497470983E-5</v>
       </c>
-      <c r="AU22" s="51">
+      <c r="AV22" s="51">
         <v>2.3561964897809859E-4</v>
-      </c>
-      <c r="AV22" s="51">
-        <v>3.3943981679371304E-4</v>
       </c>
       <c r="AW22" s="51">
         <v>3.3943981679371304E-4</v>
       </c>
       <c r="AX22" s="51">
+        <v>3.3943981679371304E-4</v>
+      </c>
+      <c r="AY22" s="51">
         <v>4.5382343409995544E-6</v>
       </c>
-      <c r="AY22" s="51">
+      <c r="AZ22" s="51">
         <v>2.9678687275179186E-7</v>
-      </c>
-      <c r="AZ22" s="51">
-        <v>9.4554734028597619E-4</v>
       </c>
       <c r="BA22" s="51">
         <v>9.4554734028597619E-4</v>
@@ -15412,40 +15518,43 @@
         <v>9.4554734028597619E-4</v>
       </c>
       <c r="BF22" s="51">
+        <v>9.4554734028597619E-4</v>
+      </c>
+      <c r="BG22" s="51">
         <v>1.1467817423225097E-4</v>
       </c>
-      <c r="BG22" s="51">
+      <c r="BH22" s="51">
         <v>8.1836597552782057E-5</v>
       </c>
-      <c r="BH22" s="51">
+      <c r="BI22" s="51">
         <v>9.4554734028597619E-4</v>
       </c>
-      <c r="BI22" s="51">
+      <c r="BJ22" s="51">
         <v>3.6873154020621375E-5</v>
       </c>
-      <c r="BJ22" s="51">
+      <c r="BK22" s="51">
         <v>2.7946700000000004E-4</v>
       </c>
-      <c r="BK22" s="51">
+      <c r="BL22" s="51">
         <v>4.5272564863293758E-4</v>
       </c>
-      <c r="BL22" s="51">
+      <c r="BM22" s="51">
         <v>3.3014385315858906E-3</v>
       </c>
-      <c r="BM22" s="51">
+      <c r="BN22" s="51">
         <v>2.4408338495687793E-4</v>
       </c>
-      <c r="BN22" s="51">
+      <c r="BO22" s="51">
         <v>6.4202379676730369E-5</v>
       </c>
-      <c r="BO22" s="51">
+      <c r="BP22" s="51">
         <v>2.9669429137698592E-5</v>
       </c>
-      <c r="BP22" s="51">
+      <c r="BQ22" s="51">
         <v>5.5377491729647921E-5</v>
       </c>
     </row>
-    <row r="23" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A23" s="95" t="s">
         <v>331</v>
       </c>
@@ -15540,67 +15649,68 @@
         <v>0</v>
       </c>
       <c r="AF23" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG23" s="51">
-        <v>0.4385859244279543</v>
+        <f t="shared" si="0"/>
+        <v>1.5963877712870554E-5</v>
+      </c>
+      <c r="AG23" s="97">
+        <v>0</v>
       </c>
       <c r="AH23" s="51">
         <v>0.4385859244279543</v>
       </c>
       <c r="AI23" s="51">
+        <v>0.4385859244279543</v>
+      </c>
+      <c r="AJ23" s="51">
         <v>2.8907411102190626E-5</v>
       </c>
-      <c r="AJ23" s="51">
+      <c r="AK23" s="51">
         <v>4.8130896756620812E-6</v>
       </c>
-      <c r="AK23" s="51">
+      <c r="AL23" s="51">
         <v>7.7678045563531458E-7</v>
       </c>
-      <c r="AL23" s="51">
+      <c r="AM23" s="51">
         <v>6.0536702990039917E-5</v>
       </c>
-      <c r="AM23" s="51">
+      <c r="AN23" s="51">
         <v>3.3272110660970326E-5</v>
       </c>
-      <c r="AN23" s="51">
+      <c r="AO23" s="51">
         <v>8.7860573616982326E-5</v>
       </c>
-      <c r="AO23" s="51">
+      <c r="AP23" s="51">
         <v>6.84584302105892E-5</v>
       </c>
-      <c r="AP23" s="51">
+      <c r="AQ23" s="51">
         <v>2.11681357881779E-5</v>
       </c>
-      <c r="AQ23" s="110">
+      <c r="AR23" s="110">
         <v>3.5072175874221158E-5</v>
       </c>
-      <c r="AR23" s="110">
+      <c r="AS23" s="110">
         <v>1.2038027229429136E-5</v>
       </c>
-      <c r="AS23" s="110">
+      <c r="AT23" s="110">
         <v>6.128887743398559E-5</v>
       </c>
-      <c r="AT23" s="110">
+      <c r="AU23" s="110">
         <v>3.9723126148773418E-6</v>
       </c>
-      <c r="AU23" s="51">
+      <c r="AV23" s="51">
         <v>2.01636950280847E-5</v>
-      </c>
-      <c r="AV23" s="51">
-        <v>3.3272110660970326E-5</v>
       </c>
       <c r="AW23" s="51">
         <v>3.3272110660970326E-5</v>
       </c>
       <c r="AX23" s="51">
+        <v>3.3272110660970326E-5</v>
+      </c>
+      <c r="AY23" s="51">
         <v>5.1181415742549008E-7</v>
       </c>
-      <c r="AY23" s="51">
+      <c r="AZ23" s="51">
         <v>3.6498848986230218E-8</v>
-      </c>
-      <c r="AZ23" s="51">
-        <v>6.0107320944489042E-5</v>
       </c>
       <c r="BA23" s="51">
         <v>6.0107320944489042E-5</v>
@@ -15618,40 +15728,43 @@
         <v>6.0107320944489042E-5</v>
       </c>
       <c r="BF23" s="51">
+        <v>6.0107320944489042E-5</v>
+      </c>
+      <c r="BG23" s="51">
         <v>1.012121030067036E-5</v>
       </c>
-      <c r="BG23" s="51">
+      <c r="BH23" s="51">
         <v>8.9487470517714616E-6</v>
       </c>
-      <c r="BH23" s="51">
+      <c r="BI23" s="51">
         <v>6.0107320944489042E-5</v>
       </c>
-      <c r="BI23" s="51">
+      <c r="BJ23" s="51">
         <v>4.1584900290821074E-6</v>
       </c>
-      <c r="BJ23" s="51">
+      <c r="BK23" s="51">
         <v>2.3753000000000001E-5</v>
       </c>
-      <c r="BK23" s="51">
+      <c r="BL23" s="51">
         <v>4.4142716312102229E-5</v>
       </c>
-      <c r="BL23" s="51">
+      <c r="BM23" s="51">
         <v>2.6442232352743027E-4</v>
       </c>
-      <c r="BM23" s="51">
+      <c r="BN23" s="51">
         <v>1.3852998794338467E-5</v>
       </c>
-      <c r="BN23" s="51">
+      <c r="BO23" s="51">
         <v>3.8653995310932731E-6</v>
       </c>
-      <c r="BO23" s="51">
+      <c r="BP23" s="51">
         <v>1.4667107987881394E-7</v>
       </c>
-      <c r="BP23" s="51">
+      <c r="BQ23" s="51">
         <v>4.6867225865551064E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A24" s="95" t="s">
         <v>332</v>
       </c>
@@ -15746,67 +15859,68 @@
         <v>0</v>
       </c>
       <c r="AF24" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="51">
-        <v>0.42133548984070207</v>
+        <f t="shared" si="0"/>
+        <v>1.324280729521896E-5</v>
+      </c>
+      <c r="AG24" s="97">
+        <v>0</v>
       </c>
       <c r="AH24" s="51">
         <v>0.42133548984070207</v>
       </c>
       <c r="AI24" s="51">
+        <v>0.42133548984070207</v>
+      </c>
+      <c r="AJ24" s="51">
         <v>2.6910449371340887E-5</v>
       </c>
-      <c r="AJ24" s="51">
+      <c r="AK24" s="51">
         <v>3.9201574142665707E-6</v>
       </c>
-      <c r="AK24" s="51">
+      <c r="AL24" s="51">
         <v>6.5018658387501317E-7</v>
       </c>
-      <c r="AL24" s="51">
+      <c r="AM24" s="51">
         <v>5.0895229106867355E-5</v>
       </c>
-      <c r="AM24" s="51">
+      <c r="AN24" s="51">
         <v>2.7603157083585251E-5</v>
       </c>
-      <c r="AN24" s="51">
+      <c r="AO24" s="51">
         <v>6.9973419938251018E-5</v>
       </c>
-      <c r="AO24" s="51">
+      <c r="AP24" s="51">
         <v>5.6767270865275495E-5</v>
       </c>
-      <c r="AP24" s="51">
+      <c r="AQ24" s="51">
         <v>1.8574845175646637E-5</v>
       </c>
-      <c r="AQ24" s="110">
+      <c r="AR24" s="110">
         <v>1.0817800973810079E-5</v>
       </c>
-      <c r="AR24" s="110">
+      <c r="AS24" s="110">
         <v>9.9813764499091004E-6</v>
       </c>
-      <c r="AS24" s="110">
+      <c r="AT24" s="110">
         <v>5.4860346027767251E-5</v>
       </c>
-      <c r="AT24" s="110">
+      <c r="AU24" s="110">
         <v>3.3348908758563838E-6</v>
       </c>
-      <c r="AU24" s="51">
+      <c r="AV24" s="51">
         <v>1.772706730365577E-5</v>
-      </c>
-      <c r="AV24" s="51">
-        <v>2.7603157083585251E-5</v>
       </c>
       <c r="AW24" s="51">
         <v>2.7603157083585251E-5</v>
       </c>
       <c r="AX24" s="51">
+        <v>2.7603157083585251E-5</v>
+      </c>
+      <c r="AY24" s="51">
         <v>4.2425595376950953E-7</v>
       </c>
-      <c r="AY24" s="51">
+      <c r="AZ24" s="51">
         <v>3.0590768523713289E-8</v>
-      </c>
-      <c r="AZ24" s="51">
-        <v>5.2121440525578443E-5</v>
       </c>
       <c r="BA24" s="51">
         <v>5.2121440525578443E-5</v>
@@ -15824,40 +15938,43 @@
         <v>5.2121440525578443E-5</v>
       </c>
       <c r="BF24" s="51">
+        <v>5.2121440525578443E-5</v>
+      </c>
+      <c r="BG24" s="51">
         <v>8.71211221374498E-6</v>
       </c>
-      <c r="BG24" s="51">
+      <c r="BH24" s="51">
         <v>7.8572693796801896E-6</v>
       </c>
-      <c r="BH24" s="51">
+      <c r="BI24" s="51">
         <v>5.2121440525578443E-5</v>
       </c>
-      <c r="BI24" s="51">
+      <c r="BJ24" s="51">
         <v>3.4470796243772649E-6</v>
       </c>
-      <c r="BJ24" s="51">
+      <c r="BK24" s="51">
         <v>2.0438999999999999E-5</v>
       </c>
-      <c r="BK24" s="51">
+      <c r="BL24" s="51">
         <v>3.9446456437112961E-5</v>
       </c>
-      <c r="BL24" s="51">
+      <c r="BM24" s="51">
         <v>2.1591083475339714E-4</v>
       </c>
-      <c r="BM24" s="51">
+      <c r="BN24" s="51">
         <v>1.1762524852776183E-5</v>
       </c>
-      <c r="BN24" s="51">
+      <c r="BO24" s="51">
         <v>3.3919928363608214E-6</v>
       </c>
-      <c r="BO24" s="51">
+      <c r="BP24" s="51">
         <v>1.3360622294773735E-7</v>
       </c>
-      <c r="BP24" s="51">
+      <c r="BQ24" s="51">
         <v>4.2006686128196504E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A25" s="95" t="s">
         <v>333</v>
       </c>
@@ -15952,67 +16069,68 @@
         <v>0</v>
       </c>
       <c r="AF25" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG25" s="51">
-        <v>0.45346404218117098</v>
+        <f t="shared" si="0"/>
+        <v>1.4762406834840445E-4</v>
+      </c>
+      <c r="AG25" s="97">
+        <v>0</v>
       </c>
       <c r="AH25" s="51">
         <v>0.45346404218117098</v>
       </c>
       <c r="AI25" s="51">
+        <v>0.45346404218117098</v>
+      </c>
+      <c r="AJ25" s="51">
         <v>6.2473013870428226E-5</v>
       </c>
-      <c r="AJ25" s="51">
+      <c r="AK25" s="51">
         <v>3.3781830590020848E-5</v>
       </c>
-      <c r="AK25" s="51">
+      <c r="AL25" s="51">
         <v>6.2149425430376577E-6</v>
       </c>
-      <c r="AL25" s="51">
+      <c r="AM25" s="51">
         <v>4.1455863831335208E-4</v>
       </c>
-      <c r="AM25" s="51">
+      <c r="AN25" s="51">
         <v>3.065329171447868E-4</v>
       </c>
-      <c r="AN25" s="51">
+      <c r="AO25" s="51">
         <v>9.8441460933476176E-4</v>
       </c>
-      <c r="AO25" s="51">
+      <c r="AP25" s="51">
         <v>6.1990859296870893E-4</v>
       </c>
-      <c r="AP25" s="51">
+      <c r="AQ25" s="51">
         <v>1.6074752135619512E-4</v>
       </c>
-      <c r="AQ25" s="110">
+      <c r="AR25" s="110">
         <v>1.0676087497513601E-5</v>
       </c>
-      <c r="AR25" s="110">
+      <c r="AS25" s="110">
         <v>1.1162388724473391E-4</v>
       </c>
-      <c r="AS25" s="110">
+      <c r="AT25" s="110">
         <v>2.0784784843161662E-4</v>
       </c>
-      <c r="AT25" s="110">
+      <c r="AU25" s="110">
         <v>3.0345362238736868E-5</v>
       </c>
-      <c r="AU25" s="51">
+      <c r="AV25" s="51">
         <v>1.5292043990073654E-4</v>
-      </c>
-      <c r="AV25" s="51">
-        <v>3.065329171447868E-4</v>
       </c>
       <c r="AW25" s="51">
         <v>3.065329171447868E-4</v>
       </c>
       <c r="AX25" s="51">
+        <v>3.065329171447868E-4</v>
+      </c>
+      <c r="AY25" s="51">
         <v>4.7242480331211364E-6</v>
       </c>
-      <c r="AY25" s="51">
+      <c r="AZ25" s="51">
         <v>2.6507093903463427E-7</v>
-      </c>
-      <c r="AZ25" s="51">
-        <v>3.650623486055222E-4</v>
       </c>
       <c r="BA25" s="51">
         <v>3.650623486055222E-4</v>
@@ -16030,40 +16148,43 @@
         <v>3.650623486055222E-4</v>
       </c>
       <c r="BF25" s="51">
+        <v>3.650623486055222E-4</v>
+      </c>
+      <c r="BG25" s="51">
         <v>4.5506305390834834E-5</v>
       </c>
-      <c r="BG25" s="51">
+      <c r="BH25" s="51">
         <v>5.5179874181620383E-5</v>
       </c>
-      <c r="BH25" s="51">
+      <c r="BI25" s="51">
         <v>3.650623486055222E-4</v>
       </c>
-      <c r="BI25" s="51">
+      <c r="BJ25" s="51">
         <v>3.8384515269109238E-5</v>
       </c>
-      <c r="BJ25" s="51">
+      <c r="BK25" s="51">
         <v>2.6927800000000002E-4</v>
       </c>
-      <c r="BK25" s="51">
+      <c r="BL25" s="51">
         <v>1.5545445618026779E-4</v>
       </c>
-      <c r="BL25" s="51">
+      <c r="BM25" s="51">
         <v>1.4324939219529306E-3</v>
       </c>
-      <c r="BM25" s="51">
+      <c r="BN25" s="51">
         <v>1.0697126249591312E-4</v>
       </c>
-      <c r="BN25" s="51">
+      <c r="BO25" s="51">
         <v>2.6360729593556294E-5</v>
       </c>
-      <c r="BO25" s="51">
+      <c r="BP25" s="51">
         <v>1.3775427757572883E-6</v>
       </c>
-      <c r="BP25" s="51">
+      <c r="BQ25" s="51">
         <v>3.5239600659423857E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A26" s="95" t="s">
         <v>334</v>
       </c>
@@ -16158,67 +16279,68 @@
         <v>0</v>
       </c>
       <c r="AF26" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG26" s="51">
-        <v>2.639049099011706E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.1848166024042453E-7</v>
+      </c>
+      <c r="AG26" s="97">
+        <v>0</v>
       </c>
       <c r="AH26" s="51">
         <v>2.639049099011706E-2</v>
       </c>
       <c r="AI26" s="51">
+        <v>2.639049099011706E-2</v>
+      </c>
+      <c r="AJ26" s="51">
         <v>2.2325602930793059E-6</v>
       </c>
-      <c r="AJ26" s="51">
+      <c r="AK26" s="51">
         <v>3.1839512520469493E-7</v>
       </c>
-      <c r="AK26" s="51">
+      <c r="AL26" s="51">
         <v>3.8370324737054715E-8</v>
       </c>
-      <c r="AL26" s="51">
+      <c r="AM26" s="51">
         <v>3.969824278385659E-6</v>
       </c>
-      <c r="AM26" s="51">
+      <c r="AN26" s="51">
         <v>1.2945748897856043E-6</v>
       </c>
-      <c r="AN26" s="51">
+      <c r="AO26" s="51">
         <v>3.3444954934160299E-6</v>
       </c>
-      <c r="AO26" s="51">
+      <c r="AP26" s="51">
         <v>3.767688526735234E-6</v>
       </c>
-      <c r="AP26" s="51">
+      <c r="AQ26" s="51">
         <v>2.0595701624397093E-6</v>
       </c>
-      <c r="AQ26" s="110">
+      <c r="AR26" s="110">
         <v>3.6020833388199609E-7</v>
       </c>
-      <c r="AR26" s="110">
+      <c r="AS26" s="110">
         <v>4.58697733747854E-7</v>
       </c>
-      <c r="AS26" s="110">
+      <c r="AT26" s="110">
         <v>3.4988011310911198E-6</v>
       </c>
-      <c r="AT26" s="110">
+      <c r="AU26" s="110">
         <v>2.1988725829967597E-7</v>
       </c>
-      <c r="AU26" s="51">
+      <c r="AV26" s="51">
         <v>1.9725252370026831E-6</v>
-      </c>
-      <c r="AV26" s="51">
-        <v>1.2945748897856043E-6</v>
       </c>
       <c r="AW26" s="51">
         <v>1.2945748897856043E-6</v>
       </c>
       <c r="AX26" s="51">
+        <v>1.2945748897856043E-6</v>
+      </c>
+      <c r="AY26" s="51">
         <v>1.9491098096921769E-8</v>
       </c>
-      <c r="AY26" s="51">
+      <c r="AZ26" s="51">
         <v>2.0874162596806422E-9</v>
-      </c>
-      <c r="AZ26" s="51">
-        <v>3.3310773544400239E-6</v>
       </c>
       <c r="BA26" s="51">
         <v>3.3310773544400239E-6</v>
@@ -16236,40 +16358,43 @@
         <v>3.3310773544400239E-6</v>
       </c>
       <c r="BF26" s="51">
+        <v>3.3310773544400239E-6</v>
+      </c>
+      <c r="BG26" s="51">
         <v>8.2982042603282386E-7</v>
       </c>
-      <c r="BG26" s="51">
+      <c r="BH26" s="51">
         <v>4.21607644625354E-7</v>
       </c>
-      <c r="BH26" s="51">
+      <c r="BI26" s="51">
         <v>3.3310773544400239E-6</v>
       </c>
-      <c r="BI26" s="51">
+      <c r="BJ26" s="51">
         <v>1.5836517203748938E-7</v>
       </c>
-      <c r="BJ26" s="51">
+      <c r="BK26" s="51">
         <v>1.8669999999999999E-6</v>
       </c>
-      <c r="BK26" s="51">
+      <c r="BL26" s="51">
         <v>2.5275068230518082E-6</v>
       </c>
-      <c r="BL26" s="51">
+      <c r="BM26" s="51">
         <v>1.740086709904541E-5</v>
       </c>
-      <c r="BM26" s="51">
+      <c r="BN26" s="51">
         <v>7.3281634985847891E-7</v>
       </c>
-      <c r="BN26" s="51">
+      <c r="BO26" s="51">
         <v>4.7057747941947738E-7</v>
       </c>
-      <c r="BO26" s="51">
+      <c r="BP26" s="51">
         <v>1.9825468972662552E-8</v>
       </c>
-      <c r="BP26" s="51">
+      <c r="BQ26" s="51">
         <v>5.2754901013355671E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A27" s="96" t="s">
         <v>335</v>
       </c>
@@ -16364,67 +16489,68 @@
         <v>0</v>
       </c>
       <c r="AF27" s="97">
-        <v>0</v>
-      </c>
-      <c r="AG27" s="51">
-        <v>7.1373626246069508E-2</v>
+        <f t="shared" si="0"/>
+        <v>3.3340404990608108E-6</v>
+      </c>
+      <c r="AG27" s="97">
+        <v>0</v>
       </c>
       <c r="AH27" s="51">
         <v>7.1373626246069508E-2</v>
       </c>
       <c r="AI27" s="51">
+        <v>7.1373626246069508E-2</v>
+      </c>
+      <c r="AJ27" s="51">
         <v>7.8852757030381768E-6</v>
       </c>
-      <c r="AJ27" s="51">
+      <c r="AK27" s="51">
         <v>1.1239714888415085E-6</v>
       </c>
-      <c r="AK27" s="51">
+      <c r="AL27" s="51">
         <v>1.6658747020650673E-7</v>
       </c>
-      <c r="AL27" s="51">
+      <c r="AM27" s="51">
         <v>1.1388907815843227E-5</v>
       </c>
-      <c r="AM27" s="51">
+      <c r="AN27" s="51">
         <v>6.939345283315578E-6</v>
       </c>
-      <c r="AN27" s="51">
+      <c r="AO27" s="51">
         <v>9.6955857953731394E-6</v>
       </c>
-      <c r="AO27" s="51">
+      <c r="AP27" s="51">
         <v>1.2961733623408748E-5</v>
       </c>
-      <c r="AP27" s="51">
+      <c r="AQ27" s="51">
         <v>6.1485280328407163E-6</v>
       </c>
-      <c r="AQ27" s="110">
+      <c r="AR27" s="110">
         <v>8.7548264896605068E-7</v>
       </c>
-      <c r="AR27" s="110">
+      <c r="AS27" s="110">
         <v>2.5680335984512118E-6</v>
       </c>
-      <c r="AS27" s="110">
+      <c r="AT27" s="110">
         <v>1.6345840744560085E-5</v>
       </c>
-      <c r="AT27" s="110">
+      <c r="AU27" s="110">
         <v>8.4226744328682021E-7</v>
       </c>
-      <c r="AU27" s="51">
+      <c r="AV27" s="51">
         <v>5.8834021649830369E-6</v>
-      </c>
-      <c r="AV27" s="51">
-        <v>6.9393452833155772E-6</v>
       </c>
       <c r="AW27" s="51">
         <v>6.9393452833155772E-6</v>
       </c>
       <c r="AX27" s="51">
+        <v>6.9393452833155772E-6</v>
+      </c>
+      <c r="AY27" s="51">
         <v>1.0646107695121333E-7</v>
       </c>
-      <c r="AY27" s="51">
+      <c r="AZ27" s="51">
         <v>7.001744334547597E-9</v>
-      </c>
-      <c r="AZ27" s="51">
-        <v>1.4066006393739066E-5</v>
       </c>
       <c r="BA27" s="51">
         <v>1.4066006393739066E-5</v>
@@ -16442,44 +16568,47 @@
         <v>1.4066006393739066E-5</v>
       </c>
       <c r="BF27" s="51">
+        <v>1.4066006393739066E-5</v>
+      </c>
+      <c r="BG27" s="51">
         <v>1.7119688011449312E-6</v>
       </c>
-      <c r="BG27" s="51">
+      <c r="BH27" s="51">
         <v>1.7108203064563108E-6</v>
       </c>
-      <c r="BH27" s="51">
+      <c r="BI27" s="51">
         <v>1.4066006393739066E-5</v>
       </c>
-      <c r="BI27" s="51">
+      <c r="BJ27" s="51">
         <v>8.649962502286083E-7</v>
       </c>
-      <c r="BJ27" s="51">
+      <c r="BK27" s="51">
         <v>5.6119999999999998E-6</v>
       </c>
-      <c r="BK27" s="51">
+      <c r="BL27" s="51">
         <v>1.1749175134387463E-5</v>
       </c>
-      <c r="BL27" s="51">
+      <c r="BM27" s="51">
         <v>5.1312158850442524E-5</v>
       </c>
-      <c r="BM27" s="51">
+      <c r="BN27" s="51">
         <v>3.2496215635210682E-6</v>
       </c>
-      <c r="BN27" s="51">
+      <c r="BO27" s="51">
         <v>1.2232802247868837E-6</v>
       </c>
-      <c r="BO27" s="51">
+      <c r="BP27" s="51">
         <v>4.3047618520767291E-8</v>
       </c>
-      <c r="BP27" s="51">
+      <c r="BQ27" s="51">
         <v>1.4711785884205773E-6</v>
       </c>
     </row>
-    <row r="28" spans="1:68" x14ac:dyDescent="0.35">
-      <c r="AH28" s="92"/>
-      <c r="AJ28" s="92"/>
-    </row>
-    <row r="29" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:69" x14ac:dyDescent="0.35">
+      <c r="AI28" s="92"/>
+      <c r="AK28" s="92"/>
+    </row>
+    <row r="29" spans="1:69" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -16516,17 +16645,15 @@
       <c r="AD29" s="126"/>
       <c r="AE29" s="126"/>
       <c r="AF29" s="126"/>
-      <c r="AH29" s="92" t="s">
+      <c r="AG29" s="126"/>
+      <c r="AI29" s="92" t="s">
         <v>339</v>
       </c>
-      <c r="AJ29" s="92" t="s">
+      <c r="AK29" s="92" t="s">
         <v>300</v>
       </c>
-      <c r="AK29" t="s">
+      <c r="AL29" t="s">
         <v>278</v>
-      </c>
-      <c r="AL29" t="s">
-        <v>283</v>
       </c>
       <c r="AM29" t="s">
         <v>283</v>
@@ -16538,10 +16665,10 @@
         <v>283</v>
       </c>
       <c r="AP29" t="s">
+        <v>283</v>
+      </c>
+      <c r="AQ29" t="s">
         <v>299</v>
-      </c>
-      <c r="AQ29" t="s">
-        <v>300</v>
       </c>
       <c r="AR29" t="s">
         <v>300</v>
@@ -16610,18 +16737,21 @@
         <v>300</v>
       </c>
       <c r="BN29" t="s">
+        <v>300</v>
+      </c>
+      <c r="BO29" t="s">
         <v>321</v>
-      </c>
-      <c r="BO29" t="s">
-        <v>300</v>
       </c>
       <c r="BP29" t="s">
         <v>300</v>
       </c>
+      <c r="BQ29" t="s">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B29:AF29"/>
+    <mergeCell ref="B29:AG29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -18353,8 +18483,8 @@
   </sheetPr>
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18825,8 +18955,8 @@
       <c r="A43" t="s">
         <v>343</v>
       </c>
-      <c r="B43" s="51">
-        <v>44.291949816853993</v>
+      <c r="B43" s="111">
+        <v>44.290551348177281</v>
       </c>
       <c r="C43">
         <v>793.37856525946859</v>
@@ -18836,8 +18966,8 @@
       <c r="A44" t="s">
         <v>292</v>
       </c>
-      <c r="B44" s="51">
-        <v>43.995102738357922</v>
+      <c r="B44" s="111">
+        <v>43.995071666669872</v>
       </c>
       <c r="C44">
         <v>793.37856525946859</v>

</xml_diff>

<commit_message>
Minor updates: 1. Conformed and corrected urban emission ratios for 2022 SOT pathways; 2. Hided supporting tabs in 2022 SOT files
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D307636-B25B-4A27-9C57-ADB0B8D06D6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88311583-1B1A-4086-8C0A-F4D693B0CBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="1" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -1641,7 +1641,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1891,10 +1891,11 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7937,8 +7938,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8470,7 +8471,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="127" t="s">
         <v>328</v>
       </c>
       <c r="B21">
@@ -8497,7 +8498,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="127" t="s">
         <v>329</v>
       </c>
       <c r="B22">
@@ -8524,7 +8525,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="127" t="s">
         <v>330</v>
       </c>
       <c r="B23">
@@ -8551,7 +8552,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="127" t="s">
         <v>331</v>
       </c>
       <c r="B24">
@@ -8578,7 +8579,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="94" t="s">
+      <c r="A25" s="127" t="s">
         <v>332</v>
       </c>
       <c r="B25">
@@ -8605,7 +8606,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="94" t="s">
+      <c r="A26" s="127" t="s">
         <v>333</v>
       </c>
       <c r="B26">
@@ -8632,7 +8633,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="94" t="s">
+      <c r="A27" s="127" t="s">
         <v>334</v>
       </c>
       <c r="B27">
@@ -8659,7 +8660,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="95" t="s">
+      <c r="A28" s="127" t="s">
         <v>335</v>
       </c>
       <c r="B28">
@@ -8697,8 +8698,8 @@
   </sheetPr>
   <dimension ref="A1:X44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8860,22 +8861,22 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="126">
+      <c r="B3" s="125">
         <v>186094.49507276824</v>
       </c>
-      <c r="C3" s="126">
+      <c r="C3" s="125">
         <v>2072402.1612015334</v>
       </c>
-      <c r="D3" s="126">
+      <c r="D3" s="125">
         <v>3108119.3839218104</v>
       </c>
-      <c r="E3" s="126">
-        <v>0</v>
-      </c>
-      <c r="F3" s="126">
+      <c r="E3" s="125">
+        <v>0</v>
+      </c>
+      <c r="F3" s="125">
         <v>113249.59303072518</v>
       </c>
-      <c r="G3" s="126">
+      <c r="G3" s="125">
         <v>0</v>
       </c>
       <c r="H3" s="50">
@@ -8934,22 +8935,22 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="126">
+      <c r="B4" s="125">
         <v>180156.32120244121</v>
       </c>
-      <c r="C4" s="126">
+      <c r="C4" s="125">
         <v>1644052.7363118604</v>
       </c>
-      <c r="D4" s="126">
+      <c r="D4" s="125">
         <v>3105649.4651196641</v>
       </c>
-      <c r="E4" s="126">
-        <v>0</v>
-      </c>
-      <c r="F4" s="126">
+      <c r="E4" s="125">
+        <v>0</v>
+      </c>
+      <c r="F4" s="125">
         <v>112621.05874733524</v>
       </c>
-      <c r="G4" s="126">
+      <c r="G4" s="125">
         <v>0</v>
       </c>
       <c r="H4" s="50">
@@ -9008,22 +9009,22 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="126">
+      <c r="B5" s="125">
         <v>9786.9918916111783</v>
       </c>
-      <c r="C5" s="126">
+      <c r="C5" s="125">
         <v>728816.38543196069</v>
       </c>
-      <c r="D5" s="126">
+      <c r="D5" s="125">
         <v>3048641.6698973337</v>
       </c>
-      <c r="E5" s="126">
-        <v>0</v>
-      </c>
-      <c r="F5" s="126">
+      <c r="E5" s="125">
+        <v>0</v>
+      </c>
+      <c r="F5" s="125">
         <v>1069.2908903426282</v>
       </c>
-      <c r="G5" s="126">
+      <c r="G5" s="125">
         <v>0</v>
       </c>
       <c r="H5" s="50">
@@ -9082,22 +9083,22 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="126">
+      <c r="B6" s="125">
         <v>123998.68374447372</v>
       </c>
-      <c r="C6" s="126">
+      <c r="C6" s="125">
         <v>893430.9830457418</v>
       </c>
-      <c r="D6" s="126">
+      <c r="D6" s="125">
         <v>10305.909398414617</v>
       </c>
-      <c r="E6" s="126">
-        <v>0</v>
-      </c>
-      <c r="F6" s="126">
+      <c r="E6" s="125">
+        <v>0</v>
+      </c>
+      <c r="F6" s="125">
         <v>111088.13476192606</v>
       </c>
-      <c r="G6" s="126">
+      <c r="G6" s="125">
         <v>0</v>
       </c>
       <c r="H6" s="50">
@@ -9156,22 +9157,22 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="126">
+      <c r="B7" s="125">
         <v>46370.645566356325</v>
       </c>
-      <c r="C7" s="126">
+      <c r="C7" s="125">
         <v>21805.367834157689</v>
       </c>
-      <c r="D7" s="126">
+      <c r="D7" s="125">
         <v>46701.885823915771</v>
       </c>
-      <c r="E7" s="126">
-        <v>0</v>
-      </c>
-      <c r="F7" s="126">
+      <c r="E7" s="125">
+        <v>0</v>
+      </c>
+      <c r="F7" s="125">
         <v>463.63309506655048</v>
       </c>
-      <c r="G7" s="126">
+      <c r="G7" s="125">
         <v>0</v>
       </c>
       <c r="H7" s="50">
@@ -9230,22 +9231,22 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="126">
+      <c r="B8" s="125">
         <v>23.187622321321854</v>
       </c>
-      <c r="C8" s="126">
+      <c r="C8" s="125">
         <v>173.10359896305576</v>
       </c>
-      <c r="D8" s="126">
+      <c r="D8" s="125">
         <v>135.66242385197384</v>
       </c>
-      <c r="E8" s="126">
-        <v>0</v>
-      </c>
-      <c r="F8" s="126">
+      <c r="E8" s="125">
+        <v>0</v>
+      </c>
+      <c r="F8" s="125">
         <v>3.4611542510826787</v>
       </c>
-      <c r="G8" s="126">
+      <c r="G8" s="125">
         <v>0</v>
       </c>
       <c r="H8" s="50">
@@ -9304,22 +9305,22 @@
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="126">
+      <c r="B9" s="125">
         <v>7.5011532988214453</v>
       </c>
-      <c r="C9" s="126">
+      <c r="C9" s="125">
         <v>15.133933244426496</v>
       </c>
-      <c r="D9" s="126">
+      <c r="D9" s="125">
         <v>26.541650933703714</v>
       </c>
-      <c r="E9" s="126">
-        <v>0</v>
-      </c>
-      <c r="F9" s="126">
+      <c r="E9" s="125">
+        <v>0</v>
+      </c>
+      <c r="F9" s="125">
         <v>11.110765191701168</v>
       </c>
-      <c r="G9" s="126">
+      <c r="G9" s="125">
         <v>-28.216209696614314</v>
       </c>
       <c r="H9" s="50">
@@ -9378,22 +9379,22 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="126">
+      <c r="B10" s="125">
         <v>12.422546675550979</v>
       </c>
-      <c r="C10" s="126">
+      <c r="C10" s="125">
         <v>54.19928329542428</v>
       </c>
-      <c r="D10" s="126">
+      <c r="D10" s="125">
         <v>97.11129587282521</v>
       </c>
-      <c r="E10" s="126">
-        <v>0</v>
-      </c>
-      <c r="F10" s="126">
+      <c r="E10" s="125">
+        <v>0</v>
+      </c>
+      <c r="F10" s="125">
         <v>35.025568879881035</v>
       </c>
-      <c r="G10" s="126">
+      <c r="G10" s="125">
         <v>-42.331377382329954</v>
       </c>
       <c r="H10" s="50">
@@ -9452,22 +9453,22 @@
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="126">
+      <c r="B11" s="125">
         <v>19.071196687104383</v>
       </c>
-      <c r="C11" s="126">
+      <c r="C11" s="125">
         <v>98.188501567890555</v>
       </c>
-      <c r="D11" s="126">
+      <c r="D11" s="125">
         <v>234.94388554989396</v>
       </c>
-      <c r="E11" s="126">
-        <v>0</v>
-      </c>
-      <c r="F11" s="126">
+      <c r="E11" s="125">
+        <v>0</v>
+      </c>
+      <c r="F11" s="125">
         <v>41.227954149828165</v>
       </c>
-      <c r="G11" s="126">
+      <c r="G11" s="125">
         <v>-13.685436653377941</v>
       </c>
       <c r="H11" s="50">
@@ -9526,22 +9527,22 @@
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="126">
+      <c r="B12" s="125">
         <v>1.3608058322593073</v>
       </c>
-      <c r="C12" s="126">
+      <c r="C12" s="125">
         <v>14.79958524029915</v>
       </c>
-      <c r="D12" s="126">
+      <c r="D12" s="125">
         <v>49.490926461655775</v>
       </c>
-      <c r="E12" s="126">
-        <v>0</v>
-      </c>
-      <c r="F12" s="126">
+      <c r="E12" s="125">
+        <v>0</v>
+      </c>
+      <c r="F12" s="125">
         <v>0.41029045603247111</v>
       </c>
-      <c r="G12" s="126">
+      <c r="G12" s="125">
         <v>-5.4061596857689773</v>
       </c>
       <c r="H12" s="50">
@@ -9600,22 +9601,22 @@
       <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="126">
+      <c r="B13" s="125">
         <v>1.1438709851240312</v>
       </c>
-      <c r="C13" s="126">
+      <c r="C13" s="125">
         <v>8.1186819852087329</v>
       </c>
-      <c r="D13" s="126">
+      <c r="D13" s="125">
         <v>21.975169116137472</v>
       </c>
-      <c r="E13" s="126">
-        <v>0</v>
-      </c>
-      <c r="F13" s="126">
+      <c r="E13" s="125">
+        <v>0</v>
+      </c>
+      <c r="F13" s="125">
         <v>0.38679426325231481</v>
       </c>
-      <c r="G13" s="126">
+      <c r="G13" s="125">
         <v>-5.4061596857689773</v>
       </c>
       <c r="H13" s="50">
@@ -9674,22 +9675,22 @@
       <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="126">
+      <c r="B14" s="125">
         <v>5.2148770711776189</v>
       </c>
-      <c r="C14" s="126">
+      <c r="C14" s="125">
         <v>86.6792466145004</v>
       </c>
-      <c r="D14" s="126">
+      <c r="D14" s="125">
         <v>310.86145005871089</v>
       </c>
-      <c r="E14" s="126">
-        <v>0</v>
-      </c>
-      <c r="F14" s="126">
+      <c r="E14" s="125">
+        <v>0</v>
+      </c>
+      <c r="F14" s="125">
         <v>11.227367678749063</v>
       </c>
-      <c r="G14" s="126">
+      <c r="G14" s="125">
         <v>-0.27393692777212614</v>
       </c>
       <c r="H14" s="50">
@@ -9748,22 +9749,22 @@
       <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="126">
+      <c r="B15" s="125">
         <v>0.17301768179602184</v>
       </c>
-      <c r="C15" s="126">
+      <c r="C15" s="125">
         <v>0.4263653854267383</v>
       </c>
-      <c r="D15" s="126">
+      <c r="D15" s="125">
         <v>0.89779545683120388</v>
       </c>
-      <c r="E15" s="126">
-        <v>0</v>
-      </c>
-      <c r="F15" s="126">
+      <c r="E15" s="125">
+        <v>0</v>
+      </c>
+      <c r="F15" s="125">
         <v>7.9067379883375796E-2</v>
       </c>
-      <c r="G15" s="126">
+      <c r="G15" s="125">
         <v>-5.72954763659021</v>
       </c>
       <c r="H15" s="50">
@@ -9822,22 +9823,22 @@
       <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="126">
+      <c r="B16" s="125">
         <v>0.3110698001896765</v>
       </c>
-      <c r="C16" s="126">
+      <c r="C16" s="125">
         <v>2.0716820911339098</v>
       </c>
-      <c r="D16" s="126">
+      <c r="D16" s="125">
         <v>1.7266356010456643</v>
       </c>
-      <c r="E16" s="126">
-        <v>0</v>
-      </c>
-      <c r="F16" s="126">
+      <c r="E16" s="125">
+        <v>0</v>
+      </c>
+      <c r="F16" s="125">
         <v>0.16211356019619858</v>
       </c>
-      <c r="G16" s="126">
+      <c r="G16" s="125">
         <v>0.13580324168234237</v>
       </c>
       <c r="H16" s="50">
@@ -9896,22 +9897,22 @@
       <c r="A17" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="126">
+      <c r="B17" s="125">
         <v>111.77224464924271</v>
       </c>
-      <c r="C17" s="126">
+      <c r="C17" s="125">
         <v>270.97124572299776</v>
       </c>
-      <c r="D17" s="126">
+      <c r="D17" s="125">
         <v>498.39393522009186</v>
       </c>
-      <c r="E17" s="126">
-        <v>0</v>
-      </c>
-      <c r="F17" s="126">
+      <c r="E17" s="125">
+        <v>0</v>
+      </c>
+      <c r="F17" s="125">
         <v>223.18874113291389</v>
       </c>
-      <c r="G17" s="126">
+      <c r="G17" s="125">
         <v>384.29844655783586</v>
       </c>
       <c r="H17" s="50">
@@ -9970,22 +9971,22 @@
       <c r="A18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="126">
+      <c r="B18" s="125">
         <v>0.24401582180145484</v>
       </c>
-      <c r="C18" s="126">
+      <c r="C18" s="125">
         <v>2.597224583249659</v>
       </c>
-      <c r="D18" s="126">
+      <c r="D18" s="125">
         <v>7.1656826033797216</v>
       </c>
-      <c r="E18" s="126">
-        <v>0</v>
-      </c>
-      <c r="F18" s="126">
+      <c r="E18" s="125">
+        <v>0</v>
+      </c>
+      <c r="F18" s="125">
         <v>1.4177914985569811</v>
       </c>
-      <c r="G18" s="126">
+      <c r="G18" s="125">
         <v>-1.3019529375153069</v>
       </c>
       <c r="H18" s="50">
@@ -10044,22 +10045,22 @@
       <c r="A19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="126">
+      <c r="B19" s="125">
         <v>13186.722667602997</v>
       </c>
-      <c r="C19" s="126">
+      <c r="C19" s="125">
         <v>127800.99778787572</v>
       </c>
-      <c r="D19" s="126">
+      <c r="D19" s="125">
         <v>309025.2744712985</v>
       </c>
-      <c r="E19" s="126">
-        <v>0</v>
-      </c>
-      <c r="F19" s="126">
+      <c r="E19" s="125">
+        <v>0</v>
+      </c>
+      <c r="F19" s="125">
         <v>6612.5157742586298</v>
       </c>
-      <c r="G19" s="126">
+      <c r="G19" s="125">
         <v>258.20196307358003</v>
       </c>
       <c r="H19" s="50">
@@ -10118,33 +10119,33 @@
       <c r="A20" s="57" t="s">
         <v>327</v>
       </c>
-      <c r="B20" s="126"/>
-      <c r="C20" s="126"/>
-      <c r="D20" s="126"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="126"/>
-      <c r="G20" s="126"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="125"/>
+      <c r="D20" s="125"/>
+      <c r="E20" s="125"/>
+      <c r="F20" s="125"/>
+      <c r="G20" s="125"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="94" t="s">
         <v>328</v>
       </c>
-      <c r="B21" s="126">
+      <c r="B21" s="125">
         <v>2.7709518164194042</v>
       </c>
-      <c r="C21" s="126">
+      <c r="C21" s="125">
         <v>1.0150242313072426</v>
       </c>
-      <c r="D21" s="126">
+      <c r="D21" s="125">
         <v>1.7601979147913644</v>
       </c>
-      <c r="E21" s="126">
-        <v>0</v>
-      </c>
-      <c r="F21" s="126">
+      <c r="E21" s="125">
+        <v>0</v>
+      </c>
+      <c r="F21" s="125">
         <v>0.59395466241739103</v>
       </c>
-      <c r="G21" s="126">
+      <c r="G21" s="125">
         <v>-14.108104848307157</v>
       </c>
       <c r="H21" s="50">
@@ -10203,22 +10204,22 @@
       <c r="A22" s="94" t="s">
         <v>329</v>
       </c>
-      <c r="B22" s="126">
+      <c r="B22" s="125">
         <v>1.9100704704858615</v>
       </c>
-      <c r="C22" s="126">
+      <c r="C22" s="125">
         <v>12.125158379090005</v>
       </c>
-      <c r="D22" s="126">
+      <c r="D22" s="125">
         <v>35.018256654548495</v>
       </c>
-      <c r="E22" s="126">
-        <v>0</v>
-      </c>
-      <c r="F22" s="126">
+      <c r="E22" s="125">
+        <v>0</v>
+      </c>
+      <c r="F22" s="125">
         <v>2.9123286674356534</v>
       </c>
-      <c r="G22" s="126">
+      <c r="G22" s="125">
         <v>-21.165688691164977</v>
       </c>
       <c r="H22" s="50">
@@ -10277,22 +10278,22 @@
       <c r="A23" s="94" t="s">
         <v>330</v>
       </c>
-      <c r="B23" s="126">
+      <c r="B23" s="125">
         <v>2.9398748358909206</v>
       </c>
-      <c r="C23" s="126">
+      <c r="C23" s="125">
         <v>25.731355879367204</v>
       </c>
-      <c r="D23" s="126">
+      <c r="D23" s="125">
         <v>84.059425624626655</v>
       </c>
-      <c r="E23" s="126">
-        <v>0</v>
-      </c>
-      <c r="F23" s="126">
+      <c r="E23" s="125">
+        <v>0</v>
+      </c>
+      <c r="F23" s="125">
         <v>3.4515556640320058</v>
       </c>
-      <c r="G23" s="126">
+      <c r="G23" s="125">
         <v>-6.8427183266889706</v>
       </c>
       <c r="H23" s="50">
@@ -10351,22 +10352,22 @@
       <c r="A24" s="94" t="s">
         <v>331</v>
       </c>
-      <c r="B24" s="126">
+      <c r="B24" s="125">
         <v>0.50272862517322592</v>
       </c>
-      <c r="C24" s="126">
+      <c r="C24" s="125">
         <v>2.9019374583272644</v>
       </c>
-      <c r="D24" s="126">
+      <c r="D24" s="125">
         <v>9.0062308603196826</v>
       </c>
-      <c r="E24" s="126">
-        <v>0</v>
-      </c>
-      <c r="F24" s="126">
+      <c r="E24" s="125">
+        <v>0</v>
+      </c>
+      <c r="F24" s="125">
         <v>1.2654757316781947E-2</v>
       </c>
-      <c r="G24" s="126">
+      <c r="G24" s="125">
         <v>-2.7030798428844887</v>
       </c>
       <c r="H24" s="50">
@@ -10425,22 +10426,22 @@
       <c r="A25" s="94" t="s">
         <v>332</v>
       </c>
-      <c r="B25" s="126">
+      <c r="B25" s="125">
         <v>0.43181700206063867</v>
       </c>
-      <c r="C25" s="126">
+      <c r="C25" s="125">
         <v>2.405490794461528</v>
       </c>
-      <c r="D25" s="126">
+      <c r="D25" s="125">
         <v>7.0122492369158884</v>
       </c>
-      <c r="E25" s="126">
-        <v>0</v>
-      </c>
-      <c r="F25" s="126">
+      <c r="E25" s="125">
+        <v>0</v>
+      </c>
+      <c r="F25" s="125">
         <v>1.1763463500421619E-2</v>
       </c>
-      <c r="G25" s="126">
+      <c r="G25" s="125">
         <v>-2.7030798428844887</v>
       </c>
       <c r="H25" s="50">
@@ -10499,22 +10500,22 @@
       <c r="A26" s="94" t="s">
         <v>333</v>
       </c>
-      <c r="B26" s="126">
+      <c r="B26" s="125">
         <v>1.0996774442050521</v>
       </c>
-      <c r="C26" s="126">
+      <c r="C26" s="125">
         <v>26.786035772640684</v>
       </c>
-      <c r="D26" s="126">
+      <c r="D26" s="125">
         <v>110.45566063925806</v>
       </c>
-      <c r="E26" s="126">
-        <v>0</v>
-      </c>
-      <c r="F26" s="126">
+      <c r="E26" s="125">
+        <v>0</v>
+      </c>
+      <c r="F26" s="125">
         <v>0.15155791049396339</v>
       </c>
-      <c r="G26" s="126">
+      <c r="G26" s="125">
         <v>-0.13696846388606307</v>
       </c>
       <c r="H26" s="50">
@@ -10573,22 +10574,22 @@
       <c r="A27" s="94" t="s">
         <v>334</v>
       </c>
-      <c r="B27" s="126">
+      <c r="B27" s="125">
         <v>5.4426729883429829E-2</v>
       </c>
-      <c r="C27" s="126">
+      <c r="C27" s="125">
         <v>0.11051266724606544</v>
       </c>
-      <c r="D27" s="126">
+      <c r="D27" s="125">
         <v>0.3037489980061826</v>
       </c>
-      <c r="E27" s="126">
-        <v>0</v>
-      </c>
-      <c r="F27" s="126">
+      <c r="E27" s="125">
+        <v>0</v>
+      </c>
+      <c r="F27" s="125">
         <v>1.8326759701175711E-3</v>
       </c>
-      <c r="G27" s="126">
+      <c r="G27" s="125">
         <v>-2.864773818295105</v>
       </c>
       <c r="H27" s="50">
@@ -10647,22 +10648,22 @@
       <c r="A28" s="95" t="s">
         <v>335</v>
       </c>
-      <c r="B28" s="126">
+      <c r="B28" s="125">
         <v>7.6631367002745324E-2</v>
       </c>
-      <c r="C28" s="126">
+      <c r="C28" s="125">
         <v>0.60362415258816537</v>
       </c>
-      <c r="D28" s="126">
+      <c r="D28" s="125">
         <v>0.58301417405342637</v>
       </c>
-      <c r="E28" s="126">
-        <v>0</v>
-      </c>
-      <c r="F28" s="126">
+      <c r="E28" s="125">
+        <v>0</v>
+      </c>
+      <c r="F28" s="125">
         <v>4.3544808165781679E-3</v>
       </c>
-      <c r="G28" s="126">
+      <c r="G28" s="125">
         <v>6.7901620841171184E-2</v>
       </c>
       <c r="H28" s="50">
@@ -10727,11 +10728,11 @@
       <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="125" t="s">
+      <c r="C30" s="126" t="s">
         <v>336</v>
       </c>
-      <c r="D30" s="125"/>
-      <c r="E30" s="125"/>
+      <c r="D30" s="126"/>
+      <c r="E30" s="126"/>
       <c r="G30" s="17" t="s">
         <v>288</v>
       </c>
@@ -16626,40 +16627,40 @@
       <c r="A29" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="125" t="s">
+      <c r="B29" s="126" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="125"/>
-      <c r="D29" s="125"/>
-      <c r="E29" s="125"/>
-      <c r="F29" s="125"/>
-      <c r="G29" s="125"/>
-      <c r="H29" s="125"/>
-      <c r="I29" s="125"/>
-      <c r="J29" s="125"/>
-      <c r="K29" s="125"/>
-      <c r="L29" s="125"/>
-      <c r="M29" s="125"/>
-      <c r="N29" s="125"/>
-      <c r="O29" s="125"/>
-      <c r="P29" s="125"/>
-      <c r="Q29" s="125"/>
-      <c r="R29" s="125"/>
-      <c r="S29" s="125"/>
-      <c r="T29" s="125"/>
-      <c r="U29" s="125"/>
-      <c r="V29" s="125"/>
-      <c r="W29" s="125"/>
-      <c r="X29" s="125"/>
-      <c r="Y29" s="125"/>
-      <c r="Z29" s="125"/>
-      <c r="AA29" s="125"/>
-      <c r="AB29" s="125"/>
-      <c r="AC29" s="125"/>
-      <c r="AD29" s="125"/>
-      <c r="AE29" s="125"/>
-      <c r="AF29" s="125"/>
-      <c r="AG29" s="125"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
+      <c r="H29" s="126"/>
+      <c r="I29" s="126"/>
+      <c r="J29" s="126"/>
+      <c r="K29" s="126"/>
+      <c r="L29" s="126"/>
+      <c r="M29" s="126"/>
+      <c r="N29" s="126"/>
+      <c r="O29" s="126"/>
+      <c r="P29" s="126"/>
+      <c r="Q29" s="126"/>
+      <c r="R29" s="126"/>
+      <c r="S29" s="126"/>
+      <c r="T29" s="126"/>
+      <c r="U29" s="126"/>
+      <c r="V29" s="126"/>
+      <c r="W29" s="126"/>
+      <c r="X29" s="126"/>
+      <c r="Y29" s="126"/>
+      <c r="Z29" s="126"/>
+      <c r="AA29" s="126"/>
+      <c r="AB29" s="126"/>
+      <c r="AC29" s="126"/>
+      <c r="AD29" s="126"/>
+      <c r="AE29" s="126"/>
+      <c r="AF29" s="126"/>
+      <c r="AG29" s="126"/>
       <c r="AI29" s="91" t="s">
         <v>339</v>
       </c>
@@ -17828,22 +17829,22 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="125" t="s">
+      <c r="B23" s="126" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="125"/>
-      <c r="D23" s="125"/>
-      <c r="E23" s="125"/>
-      <c r="F23" s="125"/>
-      <c r="G23" s="125"/>
-      <c r="H23" s="125"/>
-      <c r="I23" s="125"/>
-      <c r="J23" s="125"/>
-      <c r="K23" s="125"/>
-      <c r="L23" s="125"/>
-      <c r="M23" s="125"/>
-      <c r="N23" s="125"/>
-      <c r="O23" s="125"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="126"/>
+      <c r="I23" s="126"/>
+      <c r="J23" s="126"/>
+      <c r="K23" s="126"/>
+      <c r="L23" s="126"/>
+      <c r="M23" s="126"/>
+      <c r="N23" s="126"/>
+      <c r="O23" s="126"/>
       <c r="P23" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Updated renewable diesel properties for Algae CAP
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88311583-1B1A-4086-8C0A-F4D693B0CBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CE6D02-76B3-4391-A861-712E6D912243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="1" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" activeTab="7" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -1641,7 +1641,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1895,7 +1895,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7938,7 +7937,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
@@ -8471,7 +8470,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="127" t="s">
+      <c r="A21" s="6" t="s">
         <v>328</v>
       </c>
       <c r="B21">
@@ -8498,7 +8497,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" s="127" t="s">
+      <c r="A22" s="6" t="s">
         <v>329</v>
       </c>
       <c r="B22">
@@ -8525,7 +8524,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="127" t="s">
+      <c r="A23" s="6" t="s">
         <v>330</v>
       </c>
       <c r="B23">
@@ -8552,7 +8551,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="127" t="s">
+      <c r="A24" s="6" t="s">
         <v>331</v>
       </c>
       <c r="B24">
@@ -8579,7 +8578,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="127" t="s">
+      <c r="A25" s="6" t="s">
         <v>332</v>
       </c>
       <c r="B25">
@@ -8606,7 +8605,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="127" t="s">
+      <c r="A26" s="6" t="s">
         <v>333</v>
       </c>
       <c r="B26">
@@ -8633,7 +8632,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="127" t="s">
+      <c r="A27" s="6" t="s">
         <v>334</v>
       </c>
       <c r="B27">
@@ -8660,7 +8659,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="127" t="s">
+      <c r="A28" s="6" t="s">
         <v>335</v>
       </c>
       <c r="B28">
@@ -18582,8 +18581,8 @@
   </sheetPr>
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19043,8 +19042,8 @@
       <c r="A42" t="s">
         <v>208</v>
       </c>
-      <c r="B42" s="50">
-        <v>44.291949816853993</v>
+      <c r="B42" s="110">
+        <v>43.979867109548849</v>
       </c>
       <c r="C42">
         <v>793.37856525946859</v>
@@ -19076,8 +19075,8 @@
       <c r="A45" t="s">
         <v>323</v>
       </c>
-      <c r="B45" s="50">
-        <v>43.975450721892244</v>
+      <c r="B45" s="110">
+        <v>43.9700528928783</v>
       </c>
       <c r="C45">
         <v>793.37856525946859</v>
@@ -19087,8 +19086,8 @@
       <c r="A46" t="s">
         <v>324</v>
       </c>
-      <c r="B46" s="50">
-        <v>43.819577184272568</v>
+      <c r="B46" s="110">
+        <v>43.820862210478118</v>
       </c>
       <c r="C46">
         <v>793.37856525946859</v>

</xml_diff>

<commit_message>
Fixed the emissions from RD distribution for algae CAP and HTL pathways, also changed the RD distribution loss factor (but that does not seem to affect the result becuase 'distribution' is not in the end use of the final product)
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CE6D02-76B3-4391-A861-712E6D912243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7069D5C-7D77-4D5F-8C1E-C6F137E6F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" tabRatio="745" activeTab="7" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="745" activeTab="1" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -7937,8 +7937,8 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8018,23 +8018,23 @@
         <v>9339.5518419730979</v>
       </c>
       <c r="C4" s="2">
-        <v>1253.7917044079659</v>
+        <v>5093.7824552240209</v>
       </c>
       <c r="D4" s="2">
         <f>C4</f>
-        <v>1253.7917044079659</v>
+        <v>5093.7824552240209</v>
       </c>
       <c r="E4" s="2">
         <f>C4</f>
-        <v>1253.7917044079659</v>
+        <v>5093.7824552240209</v>
       </c>
       <c r="F4" s="2">
         <f>C4</f>
-        <v>1253.7917044079659</v>
+        <v>5093.7824552240209</v>
       </c>
       <c r="G4" s="2">
         <f>C4</f>
-        <v>1253.7917044079659</v>
+        <v>5093.7824552240209</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -8045,23 +8045,23 @@
         <v>8169.6873553428004</v>
       </c>
       <c r="C5" s="2">
-        <v>1202.5975456032124</v>
+        <v>5023.1958652604862</v>
       </c>
       <c r="D5" s="2">
         <f t="shared" ref="D5:D20" si="0">C5</f>
-        <v>1202.5975456032124</v>
+        <v>5023.1958652604862</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" ref="E5:E20" si="1">C5</f>
-        <v>1202.5975456032124</v>
+        <v>5023.1958652604862</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" ref="F5:F20" si="2">C5</f>
-        <v>1202.5975456032124</v>
+        <v>5023.1958652604862</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" ref="G5:G20" si="3">C5</f>
-        <v>1202.5975456032124</v>
+        <v>5023.1958652604862</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -8072,23 +8072,23 @@
         <v>1989.4630119087635</v>
       </c>
       <c r="C6" s="2">
-        <v>9.9730961197564767</v>
+        <v>41.657173986229949</v>
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>9.9730961197564767</v>
+        <v>41.657173986229949</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="1"/>
-        <v>9.9730961197564767</v>
+        <v>41.657173986229949</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="2"/>
-        <v>9.9730961197564767</v>
+        <v>41.657173986229949</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="3"/>
-        <v>9.9730961197564767</v>
+        <v>41.657173986229949</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -8099,23 +8099,23 @@
         <v>2794.9003158789556</v>
       </c>
       <c r="C7" s="2">
-        <v>126.35657670942828</v>
+        <v>527.78573845908159</v>
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>126.35657670942828</v>
+        <v>527.78573845908159</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="1"/>
-        <v>126.35657670942828</v>
+        <v>527.78573845908159</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="2"/>
-        <v>126.35657670942828</v>
+        <v>527.78573845908159</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="3"/>
-        <v>126.35657670942828</v>
+        <v>527.78573845908159</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -8126,23 +8126,23 @@
         <v>3385.324027555082</v>
       </c>
       <c r="C8" s="2">
-        <v>1066.2678727740276</v>
+        <v>4453.7529528151745</v>
       </c>
       <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>1066.2678727740276</v>
+        <v>4453.7529528151745</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="1"/>
-        <v>1066.2678727740276</v>
+        <v>4453.7529528151745</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="2"/>
-        <v>1066.2678727740276</v>
+        <v>4453.7529528151745</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="3"/>
-        <v>1066.2678727740276</v>
+        <v>4453.7529528151745</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -8153,23 +8153,23 @@
         <v>0.53885408384714351</v>
       </c>
       <c r="C9" s="2">
-        <v>2.362854580449477E-2</v>
+        <v>9.869537321209304E-2</v>
       </c>
       <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>2.362854580449477E-2</v>
+        <v>9.869537321209304E-2</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="1"/>
-        <v>2.362854580449477E-2</v>
+        <v>9.869537321209304E-2</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="2"/>
-        <v>2.362854580449477E-2</v>
+        <v>9.869537321209304E-2</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="3"/>
-        <v>2.362854580449477E-2</v>
+        <v>9.869537321209304E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -8180,23 +8180,23 @@
         <v>0.12683831523481029</v>
       </c>
       <c r="C10" s="2">
-        <v>1.424806237772471E-2</v>
+        <v>1.1883133447180589</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>1.424806237772471E-2</v>
+        <v>1.1883133447180589</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="1"/>
-        <v>1.424806237772471E-2</v>
+        <v>1.1883133447180589</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="2"/>
-        <v>1.424806237772471E-2</v>
+        <v>1.1883133447180589</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="3"/>
-        <v>1.424806237772471E-2</v>
+        <v>1.1883133447180589</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -8207,23 +8207,23 @@
         <v>0.54395091021563391</v>
       </c>
       <c r="C11" s="2">
-        <v>0.19647676496293282</v>
+        <v>0.60557378989801824</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>0.19647676496293282</v>
+        <v>0.60557378989801824</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="1"/>
-        <v>0.19647676496293282</v>
+        <v>0.60557378989801824</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="2"/>
-        <v>0.19647676496293282</v>
+        <v>0.60557378989801824</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="3"/>
-        <v>0.19647676496293282</v>
+        <v>0.60557378989801824</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -8234,23 +8234,23 @@
         <v>1.4670490677357695</v>
       </c>
       <c r="C12" s="2">
-        <v>0.13480292599982197</v>
+        <v>1.3472060329660924</v>
       </c>
       <c r="D12" s="2">
         <f t="shared" si="0"/>
-        <v>0.13480292599982197</v>
+        <v>1.3472060329660924</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="1"/>
-        <v>0.13480292599982197</v>
+        <v>1.3472060329660924</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="2"/>
-        <v>0.13480292599982197</v>
+        <v>1.3472060329660924</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="3"/>
-        <v>0.13480292599982197</v>
+        <v>1.3472060329660924</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -8261,23 +8261,23 @@
         <v>7.2523053711609858E-2</v>
       </c>
       <c r="C13" s="2">
-        <v>7.5690024594833967E-3</v>
+        <v>4.077408879999693E-2</v>
       </c>
       <c r="D13" s="2">
         <f t="shared" si="0"/>
-        <v>7.5690024594833967E-3</v>
+        <v>4.077408879999693E-2</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="1"/>
-        <v>7.5690024594833967E-3</v>
+        <v>4.077408879999693E-2</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="2"/>
-        <v>7.5690024594833967E-3</v>
+        <v>4.077408879999693E-2</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="3"/>
-        <v>7.5690024594833967E-3</v>
+        <v>4.077408879999693E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -8288,23 +8288,23 @@
         <v>4.8091315083300508E-2</v>
       </c>
       <c r="C14" s="2">
-        <v>2.2203423357761371E-3</v>
+        <v>2.866035992117464E-2</v>
       </c>
       <c r="D14" s="2">
         <f t="shared" si="0"/>
-        <v>2.2203423357761371E-3</v>
+        <v>2.866035992117464E-2</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="1"/>
-        <v>2.2203423357761371E-3</v>
+        <v>2.866035992117464E-2</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="2"/>
-        <v>2.2203423357761371E-3</v>
+        <v>2.866035992117464E-2</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="3"/>
-        <v>2.2203423357761371E-3</v>
+        <v>2.866035992117464E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -8315,23 +8315,23 @@
         <v>0.25121575444697092</v>
       </c>
       <c r="C15" s="2">
-        <v>5.86909788230092E-3</v>
+        <v>2.4510023670013949E-2</v>
       </c>
       <c r="D15" s="2">
         <f t="shared" si="0"/>
-        <v>5.86909788230092E-3</v>
+        <v>2.4510023670013949E-2</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="1"/>
-        <v>5.86909788230092E-3</v>
+        <v>2.4510023670013949E-2</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="2"/>
-        <v>5.86909788230092E-3</v>
+        <v>2.4510023670013949E-2</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="3"/>
-        <v>5.86909788230092E-3</v>
+        <v>2.4510023670013949E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -8342,23 +8342,23 @@
         <v>4.2349995275388881E-3</v>
       </c>
       <c r="C16" s="2">
-        <v>2.1219130796210544E-4</v>
+        <v>3.3183046022218594E-3</v>
       </c>
       <c r="D16" s="2">
         <f t="shared" si="0"/>
-        <v>2.1219130796210544E-4</v>
+        <v>3.3183046022218594E-3</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="1"/>
-        <v>2.1219130796210544E-4</v>
+        <v>3.3183046022218594E-3</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="2"/>
-        <v>2.1219130796210544E-4</v>
+        <v>3.3183046022218594E-3</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="3"/>
-        <v>2.1219130796210544E-4</v>
+        <v>3.3183046022218594E-3</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -8369,23 +8369,23 @@
         <v>2.0560277799938402E-2</v>
       </c>
       <c r="C17" s="2">
-        <v>3.8366125882774188E-4</v>
+        <v>1.5425727512154881E-2</v>
       </c>
       <c r="D17" s="2">
         <f t="shared" si="0"/>
-        <v>3.8366125882774188E-4</v>
+        <v>1.5425727512154881E-2</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="1"/>
-        <v>3.8366125882774188E-4</v>
+        <v>1.5425727512154881E-2</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="2"/>
-        <v>3.8366125882774188E-4</v>
+        <v>1.5425727512154881E-2</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="3"/>
-        <v>3.8366125882774188E-4</v>
+        <v>1.5425727512154881E-2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -8396,23 +8396,23 @@
         <v>1.0961495941820574</v>
       </c>
       <c r="C18" s="2">
-        <v>0.11480309838857856</v>
+        <v>0.48940655600260441</v>
       </c>
       <c r="D18" s="2">
         <f t="shared" si="0"/>
-        <v>0.11480309838857856</v>
+        <v>0.48940655600260441</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="1"/>
-        <v>0.11480309838857856</v>
+        <v>0.48940655600260441</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="2"/>
-        <v>0.11480309838857856</v>
+        <v>0.48940655600260441</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="3"/>
-        <v>0.11480309838857856</v>
+        <v>0.48940655600260441</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -8423,23 +8423,23 @@
         <v>1.2419532449195709E-2</v>
       </c>
       <c r="C19" s="2">
-        <v>3.7018497329376407E-4</v>
+        <v>5.8402637809921217E-3</v>
       </c>
       <c r="D19" s="2">
         <f t="shared" si="0"/>
-        <v>3.7018497329376407E-4</v>
+        <v>5.8402637809921217E-3</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="1"/>
-        <v>3.7018497329376407E-4</v>
+        <v>5.8402637809921217E-3</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="2"/>
-        <v>3.7018497329376407E-4</v>
+        <v>5.8402637809921217E-3</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="3"/>
-        <v>3.7018497329376407E-4</v>
+        <v>5.8402637809921217E-3</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -8450,23 +8450,23 @@
         <v>633.15471120171344</v>
       </c>
       <c r="C20" s="2">
-        <v>92.811588579119217</v>
+        <v>387.85040331686662</v>
       </c>
       <c r="D20" s="2">
         <f t="shared" si="0"/>
-        <v>92.811588579119217</v>
+        <v>387.85040331686662</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="1"/>
-        <v>92.811588579119217</v>
+        <v>387.85040331686662</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="2"/>
-        <v>92.811588579119217</v>
+        <v>387.85040331686662</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="3"/>
-        <v>92.811588579119217</v>
+        <v>387.85040331686662</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -8477,23 +8477,23 @@
         <v>2.1781234690476294E-2</v>
       </c>
       <c r="C21">
-        <v>0.73563756849253104</v>
+        <v>0.26551552589021865</v>
       </c>
       <c r="D21">
         <f>C21</f>
-        <v>0.73563756849253104</v>
+        <v>0.26551552589021865</v>
       </c>
       <c r="E21">
         <f>C21</f>
-        <v>0.73563756849253104</v>
+        <v>0.26551552589021865</v>
       </c>
       <c r="F21">
         <f>C21</f>
-        <v>0.73563756849253104</v>
+        <v>0.26551552589021865</v>
       </c>
       <c r="G21">
         <f>C21</f>
-        <v>0.73563756849253104</v>
+        <v>0.26551552589021865</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -8504,23 +8504,23 @@
         <v>0.18381159698546526</v>
       </c>
       <c r="C22">
-        <v>0.12786171981419567</v>
+        <v>0.17288665151109295</v>
       </c>
       <c r="D22">
         <f t="shared" ref="D22:D28" si="4">C22</f>
-        <v>0.12786171981419567</v>
+        <v>0.17288665151109295</v>
       </c>
       <c r="E22">
         <f t="shared" ref="E22:E28" si="5">C22</f>
-        <v>0.12786171981419567</v>
+        <v>0.17288665151109295</v>
       </c>
       <c r="F22">
         <f t="shared" ref="F22:F28" si="6">C22</f>
-        <v>0.12786171981419567</v>
+        <v>0.17288665151109295</v>
       </c>
       <c r="G22">
         <f t="shared" ref="G22:G28" si="7">C22</f>
-        <v>0.12786171981419567</v>
+        <v>0.17288665151109295</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -8531,23 +8531,23 @@
         <v>0.26679009552113131</v>
       </c>
       <c r="C23">
-        <v>8.2023598818784182E-2</v>
+        <v>0.21330355735173617</v>
       </c>
       <c r="D23">
         <f t="shared" si="4"/>
-        <v>8.2023598818784182E-2</v>
+        <v>0.21330355735173617</v>
       </c>
       <c r="E23">
         <f t="shared" si="5"/>
-        <v>8.2023598818784182E-2</v>
+        <v>0.21330355735173617</v>
       </c>
       <c r="F23">
         <f t="shared" si="6"/>
-        <v>8.2023598818784182E-2</v>
+        <v>0.21330355735173617</v>
       </c>
       <c r="G23">
         <f t="shared" si="7"/>
-        <v>8.2023598818784182E-2</v>
+        <v>0.21330355735173617</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -8558,23 +8558,23 @@
         <v>1.6067527224713878E-2</v>
       </c>
       <c r="C24">
-        <v>4.7471776286034904E-3</v>
+        <v>9.4740252492059081E-3</v>
       </c>
       <c r="D24">
         <f t="shared" si="4"/>
-        <v>4.7471776286034904E-3</v>
+        <v>9.4740252492059081E-3</v>
       </c>
       <c r="E24">
         <f t="shared" si="5"/>
-        <v>4.7471776286034904E-3</v>
+        <v>9.4740252492059081E-3</v>
       </c>
       <c r="F24">
         <f t="shared" si="6"/>
-        <v>4.7471776286034904E-3</v>
+        <v>9.4740252492059081E-3</v>
       </c>
       <c r="G24">
         <f t="shared" si="7"/>
-        <v>4.7471776286034904E-3</v>
+        <v>9.4740252492059081E-3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -8585,23 +8585,23 @@
         <v>1.0925985281165002E-2</v>
       </c>
       <c r="C25">
-        <v>1.1625114789012593E-3</v>
+        <v>5.0442745092267195E-3</v>
       </c>
       <c r="D25">
         <f t="shared" si="4"/>
-        <v>1.1625114789012593E-3</v>
+        <v>5.0442745092267195E-3</v>
       </c>
       <c r="E25">
         <f t="shared" si="5"/>
-        <v>1.1625114789012593E-3</v>
+        <v>5.0442745092267195E-3</v>
       </c>
       <c r="F25">
         <f t="shared" si="6"/>
-        <v>1.1625114789012593E-3</v>
+        <v>5.0442745092267195E-3</v>
       </c>
       <c r="G25">
         <f t="shared" si="7"/>
-        <v>1.1625114789012593E-3</v>
+        <v>5.0442745092267195E-3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -8612,23 +8612,23 @@
         <v>7.5973312175973959E-2</v>
       </c>
       <c r="C26">
-        <v>1.5008027021008762E-3</v>
+        <v>5.2423279836688944E-3</v>
       </c>
       <c r="D26">
         <f t="shared" si="4"/>
-        <v>1.5008027021008762E-3</v>
+        <v>5.2423279836688944E-3</v>
       </c>
       <c r="E26">
         <f t="shared" si="5"/>
-        <v>1.5008027021008762E-3</v>
+        <v>5.2423279836688944E-3</v>
       </c>
       <c r="F26">
         <f t="shared" si="6"/>
-        <v>1.5008027021008762E-3</v>
+        <v>5.2423279836688944E-3</v>
       </c>
       <c r="G26">
         <f t="shared" si="7"/>
-        <v>1.5008027021008762E-3</v>
+        <v>5.2423279836688944E-3</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -8639,23 +8639,23 @@
         <v>7.7626034636698693E-4</v>
       </c>
       <c r="C27">
-        <v>8.0041955215929224E-5</v>
+        <v>5.4229333446464761E-4</v>
       </c>
       <c r="D27">
         <f t="shared" si="4"/>
-        <v>8.0041955215929224E-5</v>
+        <v>5.4229333446464761E-4</v>
       </c>
       <c r="E27">
         <f t="shared" si="5"/>
-        <v>8.0041955215929224E-5</v>
+        <v>5.4229333446464761E-4</v>
       </c>
       <c r="F27">
         <f t="shared" si="6"/>
-        <v>8.0041955215929224E-5</v>
+        <v>5.4229333446464761E-4</v>
       </c>
       <c r="G27">
         <f t="shared" si="7"/>
-        <v>8.0041955215929224E-5</v>
+        <v>5.4229333446464761E-4</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -8666,23 +8666,23 @@
         <v>3.3865871217684512E-3</v>
       </c>
       <c r="C28">
-        <v>1.2376182810406463E-4</v>
+        <v>1.8571109385136862E-3</v>
       </c>
       <c r="D28">
         <f t="shared" si="4"/>
-        <v>1.2376182810406463E-4</v>
+        <v>1.8571109385136862E-3</v>
       </c>
       <c r="E28">
         <f t="shared" si="5"/>
-        <v>1.2376182810406463E-4</v>
+        <v>1.8571109385136862E-3</v>
       </c>
       <c r="F28">
         <f t="shared" si="6"/>
-        <v>1.2376182810406463E-4</v>
+        <v>1.8571109385136862E-3</v>
       </c>
       <c r="G28">
         <f t="shared" si="7"/>
-        <v>1.2376182810406463E-4</v>
+        <v>1.8571109385136862E-3</v>
       </c>
     </row>
   </sheetData>
@@ -18581,7 +18581,7 @@
   </sheetPr>
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added chemicals to the background GREET 2022 database for the PNNL sludge HTL paper
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7069D5C-7D77-4D5F-8C1E-C6F137E6F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9A1225-9420-4D3B-99EA-596A63211903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="745" activeTab="1" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -297,7 +297,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="349">
   <si>
     <t>Diesel</t>
   </si>
@@ -1335,6 +1335,15 @@
   </si>
   <si>
     <t>EtOH</t>
+  </si>
+  <si>
+    <t>(NH4)2SO4</t>
+  </si>
+  <si>
+    <t>Coal-Based Activated Carbon</t>
+  </si>
+  <si>
+    <t>Need to adjust a cell in GREET and copy/paste manually</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1489,6 +1498,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1641,7 +1656,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1895,6 +1910,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7937,7 +7953,7 @@
   </sheetPr>
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -8695,10 +8711,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:X44"/>
+  <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="AB27" sqref="AB27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8711,7 +8727,7 @@
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -8781,8 +8797,14 @@
       <c r="X1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y1" t="s">
+        <v>346</v>
+      </c>
+      <c r="Z1" s="127" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>340</v>
       </c>
@@ -8855,8 +8877,14 @@
       <c r="X2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z2" s="127" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8929,8 +8957,14 @@
       <c r="X3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y3">
+        <v>10.092966734864383</v>
+      </c>
+      <c r="Z3" s="127">
+        <v>159.61294596442238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9003,8 +9037,14 @@
       <c r="X4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y4">
+        <v>10.037274812679371</v>
+      </c>
+      <c r="Z4" s="127">
+        <v>159.01572660266299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -9077,8 +9117,14 @@
       <c r="X5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y5">
+        <v>9.4476222834829759E-2</v>
+      </c>
+      <c r="Z5" s="127">
+        <v>84.252817189850219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -9151,8 +9197,14 @@
       <c r="X6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y6">
+        <v>9.0114461776113988</v>
+      </c>
+      <c r="Z6" s="127">
+        <v>70.123245507139814</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -9225,8 +9277,14 @@
       <c r="X7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y7">
+        <v>0.93135241223314247</v>
+      </c>
+      <c r="Z7" s="127">
+        <v>4.63966390567297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -9299,8 +9357,14 @@
       <c r="X8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y8">
+        <v>1.8850254189575909E-4</v>
+      </c>
+      <c r="Z8" s="127">
+        <v>7.9911248903944939E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -9373,8 +9437,14 @@
       <c r="X9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y9">
+        <v>1.3351720663121653E-3</v>
+      </c>
+      <c r="Z9" s="127">
+        <v>1.4991020819976521E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -9447,8 +9517,14 @@
       <c r="X10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y10">
+        <v>1.458359822850299E-3</v>
+      </c>
+      <c r="Z10" s="127">
+        <v>4.1850710755000908E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -9521,8 +9597,14 @@
       <c r="X11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y11">
+        <v>8.1362048922501589E-4</v>
+      </c>
+      <c r="Z11" s="127">
+        <v>5.8889140492385424E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -9595,8 +9677,14 @@
       <c r="X12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y12">
+        <v>4.0834205013456504E-5</v>
+      </c>
+      <c r="Z12" s="127">
+        <v>2.4491257687576568E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -9669,8 +9757,14 @@
       <c r="X13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y13">
+        <v>3.520397730589998E-5</v>
+      </c>
+      <c r="Z13" s="127">
+        <v>3.8207677812154074E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -9743,8 +9837,14 @@
       <c r="X14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y14">
+        <v>1.7762640197414279E-3</v>
+      </c>
+      <c r="Z14" s="127">
+        <v>1.3876605774230375E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -9817,8 +9917,14 @@
       <c r="X15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y15">
+        <v>5.3094217795047773E-6</v>
+      </c>
+      <c r="Z15" s="127">
+        <v>5.4894128620987762E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -9891,8 +9997,14 @@
       <c r="X16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y16">
+        <v>1.4374911737179876E-5</v>
+      </c>
+      <c r="Z16" s="127">
+        <v>1.191254767832926E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -9965,8 +10077,14 @@
       <c r="X17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y17">
+        <v>5.4762278993310248E-3</v>
+      </c>
+      <c r="Z17" s="127">
+        <v>2.6773045154859922E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -10039,8 +10157,14 @@
       <c r="X18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y18">
+        <v>1.2020606510860481E-5</v>
+      </c>
+      <c r="Z18" s="127">
+        <v>1.3028316422886578E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -10113,8 +10237,14 @@
       <c r="X19">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y19">
+        <v>0.62984762096725244</v>
+      </c>
+      <c r="Z19" s="127">
+        <v>8.6166537276591537</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="57" t="s">
         <v>327</v>
       </c>
@@ -10124,8 +10254,9 @@
       <c r="E20" s="125"/>
       <c r="F20" s="125"/>
       <c r="G20" s="125"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Z20" s="127"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="94" t="s">
         <v>328</v>
       </c>
@@ -10198,8 +10329,14 @@
       <c r="X21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y21">
+        <v>7.5802039323866825E-6</v>
+      </c>
+      <c r="Z21" s="127">
+        <v>5.1830773072089746E-5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="94" t="s">
         <v>329</v>
       </c>
@@ -10272,8 +10409,14 @@
       <c r="X22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y22">
+        <v>2.8580049446178005E-5</v>
+      </c>
+      <c r="Z22" s="127">
+        <v>2.0603336772959054E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="94" t="s">
         <v>330</v>
       </c>
@@ -10346,8 +10489,14 @@
       <c r="X23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y23">
+        <v>4.9199020008530993E-5</v>
+      </c>
+      <c r="Z23" s="127">
+        <v>2.8134101377039379E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" s="94" t="s">
         <v>331</v>
       </c>
@@ -10420,8 +10569,14 @@
       <c r="X24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y24">
+        <v>2.2234737484796388E-6</v>
+      </c>
+      <c r="Z24" s="127">
+        <v>6.9961764575117456E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" s="94" t="s">
         <v>332</v>
       </c>
@@ -10494,8 +10649,14 @@
       <c r="X25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y25">
+        <v>1.8762312745581416E-6</v>
+      </c>
+      <c r="Z25" s="127">
+        <v>5.9939614248582743E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" s="94" t="s">
         <v>333</v>
       </c>
@@ -10568,8 +10729,14 @@
       <c r="X26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y26">
+        <v>1.4049061779183859E-5</v>
+      </c>
+      <c r="Z26" s="127">
+        <v>4.7494585709469088E-5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" s="94" t="s">
         <v>334</v>
       </c>
@@ -10642,8 +10809,14 @@
       <c r="X27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y27">
+        <v>2.3730644005080313E-7</v>
+      </c>
+      <c r="Z27" s="127">
+        <v>5.2149778991018595E-7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="95" t="s">
         <v>335</v>
       </c>
@@ -10716,11 +10889,17 @@
       <c r="X28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Y28">
+        <v>6.4012408493445377E-7</v>
+      </c>
+      <c r="Z28" s="127">
+        <v>1.6882066883636638E-6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -10736,8 +10915,11 @@
         <v>288</v>
       </c>
       <c r="H30" s="17"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="Z30" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>

</xml_diff>

<commit_message>
Added catalyst data for the PNNL sludge HTL paper
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Documents\dash_development_in_github\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Longwen Ou\Desktop\dash_development\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC9A1225-9420-4D3B-99EA-596A63211903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FDB7BE-2CAC-4F47-80FE-887CCB1460DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="2610" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="745" activeTab="2" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -157,6 +157,33 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={4344998C-BEB8-4ECE-8A72-0F44640DAAC9}</author>
+    <author>tc={359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}</author>
+  </authors>
+  <commentList>
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{4344998C-BEB8-4ECE-8A72-0F44640DAAC9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ZSM-5 as surrogate</t>
+      </text>
+    </comment>
+    <comment ref="AB1" authorId="1" shapeId="0" xr:uid="{359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Source: Life cycle greenhouse gas emissions analysis of catalysts for hydrotreating of fast pyrolysis bio-oil | Elsevier Enhanced Reader </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
     <author>tc={044CB3AF-6283-4031-8C05-A50B4C478E65}</author>
     <author>tc={AC7E57AA-E1E8-4F84-B9FC-C85A72059020}</author>
     <author>tc={DE17457E-03BF-4211-B5F5-8525E651A0CD}</author>
@@ -236,7 +263,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={AB144FDA-22B0-44A8-8FFE-47B0095C1B54}</author>
@@ -297,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="351">
   <si>
     <t>Diesel</t>
   </si>
@@ -1344,6 +1371,12 @@
   </si>
   <si>
     <t>Need to adjust a cell in GREET and copy/paste manually</t>
+  </si>
+  <si>
+    <t>ZnZr</t>
+  </si>
+  <si>
+    <t>Ru/C</t>
   </si>
 </sst>
 </file>
@@ -1364,7 +1397,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
     <numFmt numFmtId="174" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1396,6 +1429,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1907,10 +1946,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1931,7 +1970,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Overview"/>
@@ -2080,7 +2119,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Overview"/>
@@ -2568,6 +2607,23 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="AA1" dT="2023-02-10T05:48:42.89" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{4344998C-BEB8-4ECE-8A72-0F44640DAAC9}">
+    <text>ZSM-5 as surrogate</text>
+  </threadedComment>
+  <threadedComment ref="AB1" dT="2023-02-10T05:50:24.14" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}">
+    <text xml:space="preserve">Source: Life cycle greenhouse gas emissions analysis of catalysts for hydrotreating of fast pyrolysis bio-oil | Elsevier Enhanced Reader </text>
+    <extLst>
+      <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
+        <xltc2:checksum>591062682</xltc2:checksum>
+        <xltc2:hyperlink startIndex="8" length="128" url="https://reader.elsevier.com/reader/sd/pii/S0961953416300198?token=197C119E27C335F9678717D6D7609BE9B44D3B43386B54E1F704E6FA0D6C10F3D4B2186A94D0C193546B89BEFA4A65E7&amp;originRegion=us-east-1&amp;originCreation=20230210053151"/>
+      </x:ext>
+    </extLst>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="K1" personId="{C9416A2D-8241-4F20-804B-D394F6D9AB2A}" id="{044CB3AF-6283-4031-8C05-A50B4C478E65}">
     <text>CO2 transportation for algae cultivation is used here as surrogate.</text>
   </threadedComment>
@@ -2596,7 +2652,7 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="G2" personId="{52F93C99-6E2F-47FF-A86C-9CFC6703D7FF}" id="{AB144FDA-22B0-44A8-8FFE-47B0095C1B54}">
     <text>Emsisions factors are for large industrial boilers. 
@@ -8707,14 +8763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB773631-DDD5-4A77-BD33-C58835457A60}">
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="AB27" sqref="AB27"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8727,7 +8783,7 @@
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -8800,11 +8856,17 @@
       <c r="Y1" t="s">
         <v>346</v>
       </c>
-      <c r="Z1" s="127" t="s">
+      <c r="Z1" s="126" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA1" t="s">
+        <v>349</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
         <v>340</v>
       </c>
@@ -8880,11 +8942,17 @@
       <c r="Y2" t="s">
         <v>80</v>
       </c>
-      <c r="Z2" s="127" t="s">
+      <c r="Z2" s="126" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -8960,11 +9028,14 @@
       <c r="Y3">
         <v>10.092966734864383</v>
       </c>
-      <c r="Z3" s="127">
+      <c r="Z3" s="126">
         <v>159.61294596442238</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AB3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9040,11 +9111,14 @@
       <c r="Y4">
         <v>10.037274812679371</v>
       </c>
-      <c r="Z4" s="127">
+      <c r="Z4" s="126">
         <v>159.01572660266299</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AB4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -9120,11 +9194,14 @@
       <c r="Y5">
         <v>9.4476222834829759E-2</v>
       </c>
-      <c r="Z5" s="127">
+      <c r="Z5" s="126">
         <v>84.252817189850219</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AB5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -9200,11 +9277,14 @@
       <c r="Y6">
         <v>9.0114461776113988</v>
       </c>
-      <c r="Z6" s="127">
+      <c r="Z6" s="126">
         <v>70.123245507139814</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AB6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -9280,11 +9360,14 @@
       <c r="Y7">
         <v>0.93135241223314247</v>
       </c>
-      <c r="Z7" s="127">
+      <c r="Z7" s="126">
         <v>4.63966390567297</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AB7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -9360,11 +9443,14 @@
       <c r="Y8">
         <v>1.8850254189575909E-4</v>
       </c>
-      <c r="Z8" s="127">
+      <c r="Z8" s="126">
         <v>7.9911248903944939E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AB8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -9440,11 +9526,17 @@
       <c r="Y9">
         <v>1.3351720663121653E-3</v>
       </c>
-      <c r="Z9" s="127">
+      <c r="Z9" s="126">
         <v>1.4991020819976521E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA9">
+        <v>1.5661402605072106E-3</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -9520,11 +9612,17 @@
       <c r="Y10">
         <v>1.458359822850299E-3</v>
       </c>
-      <c r="Z10" s="127">
+      <c r="Z10" s="126">
         <v>4.1850710755000908E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA10">
+        <v>5.5321968067478938E-3</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -9600,11 +9698,17 @@
       <c r="Y11">
         <v>8.1362048922501589E-4</v>
       </c>
-      <c r="Z11" s="127">
+      <c r="Z11" s="126">
         <v>5.8889140492385424E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA11">
+        <v>7.3649533909408496E-3</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -9680,11 +9784,17 @@
       <c r="Y12">
         <v>4.0834205013456504E-5</v>
       </c>
-      <c r="Z12" s="127">
+      <c r="Z12" s="126">
         <v>2.4491257687576568E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA12">
+        <v>6.7802056095251913E-4</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -9760,11 +9870,17 @@
       <c r="Y13">
         <v>3.520397730589998E-5</v>
       </c>
-      <c r="Z13" s="127">
+      <c r="Z13" s="126">
         <v>3.8207677812154074E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA13">
+        <v>5.3144359219302675E-4</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -9840,11 +9956,17 @@
       <c r="Y14">
         <v>1.7762640197414279E-3</v>
       </c>
-      <c r="Z14" s="127">
+      <c r="Z14" s="126">
         <v>1.3876605774230375E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA14">
+        <v>4.6796326638847349E-3</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -9920,11 +10042,17 @@
       <c r="Y15">
         <v>5.3094217795047773E-6</v>
       </c>
-      <c r="Z15" s="127">
+      <c r="Z15" s="126">
         <v>5.4894128620987762E-5</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA15">
+        <v>6.2195971551301605E-5</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -10000,11 +10128,17 @@
       <c r="Y16">
         <v>1.4374911737179876E-5</v>
       </c>
-      <c r="Z16" s="127">
+      <c r="Z16" s="126">
         <v>1.191254767832926E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA16">
+        <v>1.589609941075944E-4</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -10080,11 +10214,17 @@
       <c r="Y17">
         <v>5.4762278993310248E-3</v>
       </c>
-      <c r="Z17" s="127">
+      <c r="Z17" s="126">
         <v>2.6773045154859922E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA17">
+        <v>2.0196219200983769E-2</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -10160,11 +10300,17 @@
       <c r="Y18">
         <v>1.2020606510860481E-5</v>
       </c>
-      <c r="Z18" s="127">
+      <c r="Z18" s="126">
         <v>1.3028316422886578E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA18">
+        <v>1.5448196096900553E-4</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -10240,11 +10386,17 @@
       <c r="Y19">
         <v>0.62984762096725244</v>
       </c>
-      <c r="Z19" s="127">
+      <c r="Z19" s="126">
         <v>8.6166537276591537</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="AA19">
+        <v>6.3624128058164002</v>
+      </c>
+      <c r="AB19">
+        <v>80.400000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" s="57" t="s">
         <v>327</v>
       </c>
@@ -10254,9 +10406,9 @@
       <c r="E20" s="125"/>
       <c r="F20" s="125"/>
       <c r="G20" s="125"/>
-      <c r="Z20" s="127"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="Z20" s="126"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" s="94" t="s">
         <v>328</v>
       </c>
@@ -10332,11 +10484,11 @@
       <c r="Y21">
         <v>7.5802039323866825E-6</v>
       </c>
-      <c r="Z21" s="127">
+      <c r="Z21" s="126">
         <v>5.1830773072089746E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A22" s="94" t="s">
         <v>329</v>
       </c>
@@ -10412,11 +10564,11 @@
       <c r="Y22">
         <v>2.8580049446178005E-5</v>
       </c>
-      <c r="Z22" s="127">
+      <c r="Z22" s="126">
         <v>2.0603336772959054E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A23" s="94" t="s">
         <v>330</v>
       </c>
@@ -10492,11 +10644,11 @@
       <c r="Y23">
         <v>4.9199020008530993E-5</v>
       </c>
-      <c r="Z23" s="127">
+      <c r="Z23" s="126">
         <v>2.8134101377039379E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A24" s="94" t="s">
         <v>331</v>
       </c>
@@ -10572,11 +10724,11 @@
       <c r="Y24">
         <v>2.2234737484796388E-6</v>
       </c>
-      <c r="Z24" s="127">
+      <c r="Z24" s="126">
         <v>6.9961764575117456E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A25" s="94" t="s">
         <v>332</v>
       </c>
@@ -10652,11 +10804,11 @@
       <c r="Y25">
         <v>1.8762312745581416E-6</v>
       </c>
-      <c r="Z25" s="127">
+      <c r="Z25" s="126">
         <v>5.9939614248582743E-6</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A26" s="94" t="s">
         <v>333</v>
       </c>
@@ -10732,11 +10884,11 @@
       <c r="Y26">
         <v>1.4049061779183859E-5</v>
       </c>
-      <c r="Z26" s="127">
+      <c r="Z26" s="126">
         <v>4.7494585709469088E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A27" s="94" t="s">
         <v>334</v>
       </c>
@@ -10812,11 +10964,11 @@
       <c r="Y27">
         <v>2.3730644005080313E-7</v>
       </c>
-      <c r="Z27" s="127">
+      <c r="Z27" s="126">
         <v>5.2149778991018595E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A28" s="95" t="s">
         <v>335</v>
       </c>
@@ -10892,25 +11044,25 @@
       <c r="Y28">
         <v>6.4012408493445377E-7</v>
       </c>
-      <c r="Z28" s="127">
+      <c r="Z28" s="126">
         <v>1.6882066883636638E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="C30" s="126" t="s">
+      <c r="C30" s="127" t="s">
         <v>336</v>
       </c>
-      <c r="D30" s="126"/>
-      <c r="E30" s="126"/>
+      <c r="D30" s="127"/>
+      <c r="E30" s="127"/>
       <c r="G30" s="17" t="s">
         <v>288</v>
       </c>
@@ -10919,7 +11071,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -11107,6 +11259,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16808,40 +16961,40 @@
       <c r="A29" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="126" t="s">
+      <c r="B29" s="127" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="126"/>
-      <c r="D29" s="126"/>
-      <c r="E29" s="126"/>
-      <c r="F29" s="126"/>
-      <c r="G29" s="126"/>
-      <c r="H29" s="126"/>
-      <c r="I29" s="126"/>
-      <c r="J29" s="126"/>
-      <c r="K29" s="126"/>
-      <c r="L29" s="126"/>
-      <c r="M29" s="126"/>
-      <c r="N29" s="126"/>
-      <c r="O29" s="126"/>
-      <c r="P29" s="126"/>
-      <c r="Q29" s="126"/>
-      <c r="R29" s="126"/>
-      <c r="S29" s="126"/>
-      <c r="T29" s="126"/>
-      <c r="U29" s="126"/>
-      <c r="V29" s="126"/>
-      <c r="W29" s="126"/>
-      <c r="X29" s="126"/>
-      <c r="Y29" s="126"/>
-      <c r="Z29" s="126"/>
-      <c r="AA29" s="126"/>
-      <c r="AB29" s="126"/>
-      <c r="AC29" s="126"/>
-      <c r="AD29" s="126"/>
-      <c r="AE29" s="126"/>
-      <c r="AF29" s="126"/>
-      <c r="AG29" s="126"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="127"/>
+      <c r="F29" s="127"/>
+      <c r="G29" s="127"/>
+      <c r="H29" s="127"/>
+      <c r="I29" s="127"/>
+      <c r="J29" s="127"/>
+      <c r="K29" s="127"/>
+      <c r="L29" s="127"/>
+      <c r="M29" s="127"/>
+      <c r="N29" s="127"/>
+      <c r="O29" s="127"/>
+      <c r="P29" s="127"/>
+      <c r="Q29" s="127"/>
+      <c r="R29" s="127"/>
+      <c r="S29" s="127"/>
+      <c r="T29" s="127"/>
+      <c r="U29" s="127"/>
+      <c r="V29" s="127"/>
+      <c r="W29" s="127"/>
+      <c r="X29" s="127"/>
+      <c r="Y29" s="127"/>
+      <c r="Z29" s="127"/>
+      <c r="AA29" s="127"/>
+      <c r="AB29" s="127"/>
+      <c r="AC29" s="127"/>
+      <c r="AD29" s="127"/>
+      <c r="AE29" s="127"/>
+      <c r="AF29" s="127"/>
+      <c r="AG29" s="127"/>
       <c r="AI29" s="91" t="s">
         <v>339</v>
       </c>
@@ -18010,22 +18163,22 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="126" t="s">
+      <c r="B23" s="127" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="126"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="126"/>
-      <c r="F23" s="126"/>
-      <c r="G23" s="126"/>
-      <c r="H23" s="126"/>
-      <c r="I23" s="126"/>
-      <c r="J23" s="126"/>
-      <c r="K23" s="126"/>
-      <c r="L23" s="126"/>
-      <c r="M23" s="126"/>
-      <c r="N23" s="126"/>
-      <c r="O23" s="126"/>
+      <c r="C23" s="127"/>
+      <c r="D23" s="127"/>
+      <c r="E23" s="127"/>
+      <c r="F23" s="127"/>
+      <c r="G23" s="127"/>
+      <c r="H23" s="127"/>
+      <c r="I23" s="127"/>
+      <c r="J23" s="127"/>
+      <c r="K23" s="127"/>
+      <c r="L23" s="127"/>
+      <c r="M23" s="127"/>
+      <c r="N23" s="127"/>
+      <c r="O23" s="127"/>
       <c r="P23" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
Added CFP pathways but still need to debug the results
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\oulongwen\projects\Interactive-SCSA_Dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Box\Temp\interactive SCSA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB576BBA-1AC5-4BA4-9678-0EB209586B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF48C9C-403C-486B-847C-CB8480DCA96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="3" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -161,7 +161,7 @@
     <author>tc={359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}</author>
   </authors>
   <commentList>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{4344998C-BEB8-4ECE-8A72-0F44640DAAC9}">
+    <comment ref="AB1" authorId="0" shapeId="0" xr:uid="{4344998C-BEB8-4ECE-8A72-0F44640DAAC9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -169,7 +169,7 @@
     ZSM-5 as surrogate</t>
       </text>
     </comment>
-    <comment ref="AB1" authorId="1" shapeId="0" xr:uid="{359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}">
+    <comment ref="AC1" authorId="1" shapeId="0" xr:uid="{359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="380">
   <si>
     <t>Diesel</t>
   </si>
@@ -1443,6 +1443,45 @@
   </si>
   <si>
     <t>Cooling Tower Chemicals</t>
+  </si>
+  <si>
+    <t>HDS (reforming cleanup)</t>
+  </si>
+  <si>
+    <t>Steam reforming catalyst</t>
+  </si>
+  <si>
+    <t>PSA adsorbent</t>
+  </si>
+  <si>
+    <t>Pyrolysis_IDL!P335</t>
+  </si>
+  <si>
+    <t>Fixed-Bed VPU Catalyst</t>
+  </si>
+  <si>
+    <t>Hydrotreating catalyst</t>
+  </si>
+  <si>
+    <t>Hydrocracking Catalyst</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>ZSM-5 Catalyst</t>
+  </si>
+  <si>
+    <t>Fossil fuel gas</t>
+  </si>
+  <si>
+    <t>Biogenic fuel gas</t>
+  </si>
+  <si>
+    <t>Fuel gas</t>
+  </si>
+  <si>
+    <t>Boiler</t>
   </si>
 </sst>
 </file>
@@ -1463,7 +1502,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
     <numFmt numFmtId="174" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1495,12 +1534,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="20">
@@ -2020,10 +2053,10 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2681,10 +2714,10 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="AA1" dT="2023-02-10T05:48:42.89" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{4344998C-BEB8-4ECE-8A72-0F44640DAAC9}">
+  <threadedComment ref="AB1" dT="2023-02-10T05:48:42.89" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{4344998C-BEB8-4ECE-8A72-0F44640DAAC9}">
     <text>ZSM-5 as surrogate</text>
   </threadedComment>
-  <threadedComment ref="AB1" dT="2023-02-10T05:50:24.14" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}">
+  <threadedComment ref="AC1" dT="2023-02-10T05:50:24.14" personId="{E68499E2-350F-4BF2-80B7-ADA89A480BB6}" id="{359B2A39-4F3E-48A6-B6AE-D35BCCC7B69C}">
     <text xml:space="preserve">Source: Life cycle greenhouse gas emissions analysis of catalysts for hydrotreating of fast pyrolysis bio-oil | Elsevier Enhanced Reader </text>
     <extLst>
       <x:ext xmlns:xltc2="http://schemas.microsoft.com/office/spreadsheetml/2020/threadedcomments2" uri="{F7C98A9C-CBB3-438F-8F68-D28B6AF4A901}">
@@ -2763,11 +2796,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AY23"/>
+  <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BB3" sqref="BB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,7 +2817,7 @@
     <col min="50" max="51" width="8.7109375" style="113"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="120" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:54" s="120" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="121" t="s">
         <v>0</v>
       </c>
@@ -2935,8 +2968,17 @@
       <c r="AY1" s="123" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="2" spans="1:51" ht="77.25" x14ac:dyDescent="0.25">
+      <c r="AZ1" t="s">
+        <v>378</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>377</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:54" ht="77.25" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
@@ -3087,8 +3129,17 @@
       <c r="AY2" s="114" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ2" t="s">
+        <v>10</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>338</v>
       </c>
@@ -3242,8 +3293,17 @@
       <c r="AY3" s="115" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BB3" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -3403,8 +3463,18 @@
         <f>AW4+AX4</f>
         <v>1001253.791704408</v>
       </c>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ4" s="2">
+        <f>AN4</f>
+        <v>1000000</v>
+      </c>
+      <c r="BA4" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="BB4" s="2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -3564,8 +3634,17 @@
         <f t="shared" ref="AY5:AY9" si="13">AW5+AX5</f>
         <v>1202.5975456032124</v>
       </c>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ5" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="BA5" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3725,8 +3804,18 @@
         <f t="shared" si="13"/>
         <v>9.9730961197564767</v>
       </c>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ6" s="2">
+        <f t="shared" ref="AZ6:AZ9" si="14">AN6</f>
+        <v>0</v>
+      </c>
+      <c r="BA6" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3886,8 +3975,17 @@
         <f t="shared" si="13"/>
         <v>126.35657670942828</v>
       </c>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ7" s="2">
+        <v>1000000</v>
+      </c>
+      <c r="BA7" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -4047,8 +4145,18 @@
         <f t="shared" si="13"/>
         <v>1066.2678727740276</v>
       </c>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ8" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BA8" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4208,8 +4316,18 @@
         <f t="shared" si="13"/>
         <v>2.362854580449477E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ9" s="2">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BA9" s="2">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>16</v>
       </c>
@@ -4369,8 +4487,17 @@
         <f>AW10+AX10</f>
         <v>40.366895245037952</v>
       </c>
-    </row>
-    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ10">
+        <v>2.54</v>
+      </c>
+      <c r="BA10">
+        <v>2.54</v>
+      </c>
+      <c r="BB10">
+        <v>1.4950000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -4469,7 +4596,7 @@
         <v>0.54395091021563391</v>
       </c>
       <c r="AJ11" s="113">
-        <f t="shared" ref="AJ11:AJ21" si="14">AH11+AI11</f>
+        <f t="shared" ref="AJ11:AJ21" si="15">AH11+AI11</f>
         <v>639.64810161814546</v>
       </c>
       <c r="AK11">
@@ -4479,7 +4606,7 @@
         <v>0.19647676496293282</v>
       </c>
       <c r="AM11" s="113">
-        <f t="shared" ref="AM11:AM21" si="15">AK11+AL11</f>
+        <f t="shared" ref="AM11:AM21" si="16">AK11+AL11</f>
         <v>993.99720941257124</v>
       </c>
       <c r="AN11" s="2">
@@ -4491,7 +4618,7 @@
         <v>0.19647676496293282</v>
       </c>
       <c r="AP11" s="113">
-        <f t="shared" ref="AP11:AP21" si="16">AN11+AO11</f>
+        <f t="shared" ref="AP11:AP21" si="17">AN11+AO11</f>
         <v>993.99720941257124</v>
       </c>
       <c r="AQ11" s="2">
@@ -4503,7 +4630,7 @@
         <v>0.19647676496293282</v>
       </c>
       <c r="AS11" s="113">
-        <f t="shared" ref="AS11:AS21" si="17">AQ11+AR11</f>
+        <f t="shared" ref="AS11:AS21" si="18">AQ11+AR11</f>
         <v>993.99720941257124</v>
       </c>
       <c r="AT11" s="2">
@@ -4515,7 +4642,7 @@
         <v>0.19647676496293282</v>
       </c>
       <c r="AV11" s="113">
-        <f t="shared" ref="AV11:AV21" si="18">AT11+AU11</f>
+        <f t="shared" ref="AV11:AV21" si="19">AT11+AU11</f>
         <v>993.99720941257124</v>
       </c>
       <c r="AW11" s="2">
@@ -4527,11 +4654,20 @@
         <v>0.19647676496293282</v>
       </c>
       <c r="AY11" s="113">
-        <f t="shared" ref="AY11:AY21" si="19">AW11+AX11</f>
+        <f t="shared" ref="AY11:AY21" si="20">AW11+AX11</f>
         <v>993.99720941257124</v>
       </c>
-    </row>
-    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ11">
+        <v>22.21</v>
+      </c>
+      <c r="BA11">
+        <v>22.21</v>
+      </c>
+      <c r="BB11">
+        <v>12.417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>1</v>
       </c>
@@ -4630,7 +4766,7 @@
         <v>1.4670490677357695</v>
       </c>
       <c r="AJ12" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>20.675783382627724</v>
       </c>
       <c r="AK12">
@@ -4640,7 +4776,7 @@
         <v>0.13480292599982197</v>
       </c>
       <c r="AM12" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>27.522422181967336</v>
       </c>
       <c r="AN12" s="2">
@@ -4652,7 +4788,7 @@
         <v>0.13480292599982197</v>
       </c>
       <c r="AP12" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>27.522422181967336</v>
       </c>
       <c r="AQ12" s="2">
@@ -4664,7 +4800,7 @@
         <v>0.13480292599982197</v>
       </c>
       <c r="AS12" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>27.522422181967336</v>
       </c>
       <c r="AT12" s="2">
@@ -4676,7 +4812,7 @@
         <v>0.13480292599982197</v>
       </c>
       <c r="AV12" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>27.522422181967336</v>
       </c>
       <c r="AW12" s="2">
@@ -4688,11 +4824,20 @@
         <v>0.13480292599982197</v>
       </c>
       <c r="AY12" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>27.522422181967336</v>
       </c>
-    </row>
-    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ12">
+        <v>36.4</v>
+      </c>
+      <c r="BA12">
+        <v>36.4</v>
+      </c>
+      <c r="BB12">
+        <v>116.035</v>
+      </c>
+    </row>
+    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -4791,7 +4936,7 @@
         <v>7.2523053711609858E-2</v>
       </c>
       <c r="AJ13" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>8.1166702947222316</v>
       </c>
       <c r="AK13">
@@ -4801,7 +4946,7 @@
         <v>7.5690024594833967E-3</v>
       </c>
       <c r="AM13" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>9.4663387542404784</v>
       </c>
       <c r="AN13" s="2">
@@ -4813,7 +4958,7 @@
         <v>7.5690024594833967E-3</v>
       </c>
       <c r="AP13" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>9.4663387542404784</v>
       </c>
       <c r="AQ13" s="2">
@@ -4825,7 +4970,7 @@
         <v>7.5690024594833967E-3</v>
       </c>
       <c r="AS13" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>9.4663387542404784</v>
       </c>
       <c r="AT13" s="2">
@@ -4837,7 +4982,7 @@
         <v>7.5690024594833967E-3</v>
       </c>
       <c r="AV13" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>9.4663387542404784</v>
       </c>
       <c r="AW13" s="2">
@@ -4849,11 +4994,20 @@
         <v>7.5690024594833967E-3</v>
       </c>
       <c r="AY13" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>9.4663387542404784</v>
       </c>
-    </row>
-    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ13">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="BA13">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="BB13">
+        <v>22.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>19</v>
       </c>
@@ -4952,7 +5106,7 @@
         <v>4.8091315083300508E-2</v>
       </c>
       <c r="AJ14" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1.7767408308717885</v>
       </c>
       <c r="AK14">
@@ -4962,7 +5116,7 @@
         <v>2.2203423357761371E-3</v>
       </c>
       <c r="AM14" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>1.8944902138669564</v>
       </c>
       <c r="AN14" s="2">
@@ -4974,7 +5128,7 @@
         <v>2.2203423357761371E-3</v>
       </c>
       <c r="AP14" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>1.8944902138669564</v>
       </c>
       <c r="AQ14" s="2">
@@ -4986,7 +5140,7 @@
         <v>2.2203423357761371E-3</v>
       </c>
       <c r="AS14" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.8944902138669564</v>
       </c>
       <c r="AT14" s="2">
@@ -4998,7 +5152,7 @@
         <v>2.2203423357761371E-3</v>
       </c>
       <c r="AV14" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1.8944902138669564</v>
       </c>
       <c r="AW14" s="2">
@@ -5010,11 +5164,20 @@
         <v>2.2203423357761371E-3</v>
       </c>
       <c r="AY14" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1.8944902138669564</v>
       </c>
-    </row>
-    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ14">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="BA14">
+        <v>3.5070000000000001</v>
+      </c>
+      <c r="BB14">
+        <v>16.93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>20</v>
       </c>
@@ -5113,7 +5276,7 @@
         <v>0.25121575444697092</v>
       </c>
       <c r="AJ15" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.73008327600306977</v>
       </c>
       <c r="AK15">
@@ -5123,7 +5286,7 @@
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AM15" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AN15" s="2">
@@ -5135,7 +5298,7 @@
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AP15" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AQ15" s="2">
@@ -5147,7 +5310,7 @@
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AS15" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AT15" s="2">
@@ -5159,7 +5322,7 @@
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AV15" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AW15" s="2">
@@ -5171,11 +5334,20 @@
         <v>5.86909788230092E-3</v>
       </c>
       <c r="AY15" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>5.86909788230092E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ15">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="BA15">
+        <v>0.26856561546286878</v>
+      </c>
+      <c r="BB15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>21</v>
       </c>
@@ -5270,7 +5442,7 @@
         <v>4.2349995275388881E-3</v>
       </c>
       <c r="AJ16" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.47814447418377365</v>
       </c>
       <c r="AK16">
@@ -5280,7 +5452,7 @@
         <v>2.1219130796210544E-4</v>
       </c>
       <c r="AM16" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.51231647410831627</v>
       </c>
       <c r="AN16" s="2">
@@ -5292,7 +5464,7 @@
         <v>2.1219130796210544E-4</v>
       </c>
       <c r="AP16" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.51231647410831627</v>
       </c>
       <c r="AQ16" s="2">
@@ -5304,7 +5476,7 @@
         <v>2.1219130796210544E-4</v>
       </c>
       <c r="AS16" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.51231647410831627</v>
       </c>
       <c r="AT16" s="2">
@@ -5316,7 +5488,7 @@
         <v>2.1219130796210544E-4</v>
       </c>
       <c r="AV16" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.51231647410831627</v>
       </c>
       <c r="AW16" s="2">
@@ -5328,11 +5500,20 @@
         <v>2.1219130796210544E-4</v>
       </c>
       <c r="AY16" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.51231647410831627</v>
       </c>
-    </row>
-    <row r="17" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ16">
+        <v>0.57865500000000003</v>
+      </c>
+      <c r="BA16">
+        <v>0.57865500000000003</v>
+      </c>
+      <c r="BB16">
+        <v>0.72798999999999991</v>
+      </c>
+    </row>
+    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>22</v>
       </c>
@@ -5427,7 +5608,7 @@
         <v>2.0560277799938402E-2</v>
       </c>
       <c r="AJ17" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.26641855307706264</v>
       </c>
       <c r="AK17">
@@ -5437,7 +5618,7 @@
         <v>3.8366125882774188E-4</v>
       </c>
       <c r="AM17" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>7.7013700149011488E-2</v>
       </c>
       <c r="AN17" s="2">
@@ -5449,7 +5630,7 @@
         <v>3.8366125882774188E-4</v>
       </c>
       <c r="AP17" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>7.7013700149011488E-2</v>
       </c>
       <c r="AQ17" s="2">
@@ -5461,7 +5642,7 @@
         <v>3.8366125882774188E-4</v>
       </c>
       <c r="AS17" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>7.7013700149011488E-2</v>
       </c>
       <c r="AT17" s="2">
@@ -5473,7 +5654,7 @@
         <v>3.8366125882774188E-4</v>
       </c>
       <c r="AV17" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>7.7013700149011488E-2</v>
       </c>
       <c r="AW17" s="2">
@@ -5485,11 +5666,20 @@
         <v>3.8366125882774188E-4</v>
       </c>
       <c r="AY17" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>7.7013700149011488E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ17">
+        <v>1.5009959999999998</v>
+      </c>
+      <c r="BA17">
+        <v>1.5009959999999998</v>
+      </c>
+      <c r="BB17">
+        <v>1.3713299999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
@@ -5584,7 +5774,7 @@
         <v>1.0961495941820574</v>
       </c>
       <c r="AJ18" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>4.510274786971924</v>
       </c>
       <c r="AK18">
@@ -5594,7 +5784,7 @@
         <v>0.11480309838857856</v>
       </c>
       <c r="AM18" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>25.940497295291124</v>
       </c>
       <c r="AN18" s="2">
@@ -5606,7 +5796,7 @@
         <v>0.11480309838857856</v>
       </c>
       <c r="AP18" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>25.940497295291124</v>
       </c>
       <c r="AQ18" s="2">
@@ -5618,7 +5808,7 @@
         <v>0.11480309838857856</v>
       </c>
       <c r="AS18" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>25.940497295291124</v>
       </c>
       <c r="AT18" s="2">
@@ -5630,7 +5820,7 @@
         <v>0.11480309838857856</v>
       </c>
       <c r="AV18" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>25.940497295291124</v>
       </c>
       <c r="AW18" s="2">
@@ -5642,11 +5832,20 @@
         <v>0.11480309838857856</v>
       </c>
       <c r="AY18" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>25.940497295291124</v>
       </c>
-    </row>
-    <row r="19" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ18">
+        <v>1.06</v>
+      </c>
+      <c r="BA18">
+        <v>1.06</v>
+      </c>
+      <c r="BB18">
+        <v>1.0580000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>24</v>
       </c>
@@ -5741,7 +5940,7 @@
         <v>1.2419532449195709E-2</v>
       </c>
       <c r="AJ19" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.92384872660731499</v>
       </c>
       <c r="AK19">
@@ -5751,7 +5950,7 @@
         <v>3.7018497329376407E-4</v>
       </c>
       <c r="AM19" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.18914342627124353</v>
       </c>
       <c r="AN19" s="2">
@@ -5763,7 +5962,7 @@
         <v>3.7018497329376407E-4</v>
       </c>
       <c r="AP19" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.18914342627124353</v>
       </c>
       <c r="AQ19" s="2">
@@ -5775,7 +5974,7 @@
         <v>3.7018497329376407E-4</v>
       </c>
       <c r="AS19" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.18914342627124353</v>
       </c>
       <c r="AT19" s="2">
@@ -5787,7 +5986,7 @@
         <v>3.7018497329376407E-4</v>
       </c>
       <c r="AV19" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.18914342627124353</v>
       </c>
       <c r="AW19" s="2">
@@ -5799,11 +5998,20 @@
         <v>3.7018497329376407E-4</v>
       </c>
       <c r="AY19" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.18914342627124353</v>
       </c>
-    </row>
-    <row r="20" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ19">
+        <v>0.75</v>
+      </c>
+      <c r="BA19">
+        <v>0.75</v>
+      </c>
+      <c r="BB19">
+        <v>1.5860000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>25</v>
       </c>
@@ -5914,7 +6122,7 @@
         <v>633.15471120171344</v>
       </c>
       <c r="AJ20" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>72416.66002874964</v>
       </c>
       <c r="AK20">
@@ -5924,7 +6132,7 @@
         <v>92.811588579119217</v>
       </c>
       <c r="AM20" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>74948.864938293686</v>
       </c>
       <c r="AN20" s="2">
@@ -5936,7 +6144,7 @@
         <v>92.811588579119217</v>
       </c>
       <c r="AP20" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>74948.864938293686</v>
       </c>
       <c r="AQ20" s="2">
@@ -5948,7 +6156,7 @@
         <v>92.811588579119217</v>
       </c>
       <c r="AS20" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>74948.864938293686</v>
       </c>
       <c r="AT20" s="2">
@@ -5960,7 +6168,7 @@
         <v>92.811588579119217</v>
       </c>
       <c r="AV20" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>74948.864938293686</v>
       </c>
       <c r="AW20" s="2">
@@ -5972,11 +6180,20 @@
         <v>92.811588579119217</v>
       </c>
       <c r="AY20" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>74948.864938293686</v>
       </c>
-    </row>
-    <row r="21" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="AZ20">
+        <v>60873.708109661638</v>
+      </c>
+      <c r="BA20">
+        <v>60873.708109661638</v>
+      </c>
+      <c r="BB20">
+        <v>90002.849570264574</v>
+      </c>
+    </row>
+    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>26</v>
       </c>
@@ -6033,14 +6250,14 @@
         <v>-72964.246146966863</v>
       </c>
       <c r="AJ21" s="113">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-72964.246146966863</v>
       </c>
       <c r="AK21">
         <v>-76614.526624731123</v>
       </c>
       <c r="AM21" s="113">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-76614.526624731123</v>
       </c>
       <c r="AN21" s="2">
@@ -6048,7 +6265,7 @@
         <v>-76614.526624731123</v>
       </c>
       <c r="AP21" s="113">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>-76614.526624731123</v>
       </c>
       <c r="AQ21" s="2">
@@ -6056,7 +6273,7 @@
         <v>-76614.526624731123</v>
       </c>
       <c r="AS21" s="113">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>-76614.526624731123</v>
       </c>
       <c r="AT21" s="2">
@@ -6064,7 +6281,7 @@
         <v>-76614.526624731123</v>
       </c>
       <c r="AV21" s="113">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>-76614.526624731123</v>
       </c>
       <c r="AW21" s="2">
@@ -6072,15 +6289,21 @@
         <v>-76614.526624731123</v>
       </c>
       <c r="AY21" s="113">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>-76614.526624731123</v>
       </c>
-    </row>
-    <row r="22" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="BA21">
+        <v>-60919.440871566396</v>
+      </c>
+      <c r="BB21">
+        <v>-90029.930915502671</v>
+      </c>
+    </row>
+    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="P22" s="45"/>
     </row>
-    <row r="23" spans="1:51" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -8847,10 +9070,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AC44"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8861,9 +9084,10 @@
     <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -8892,61 +9116,64 @@
         <v>290</v>
       </c>
       <c r="K1" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1" t="s">
         <v>274</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>283</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>17</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>273</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>343</v>
       </c>
-      <c r="Z1" s="126" t="s">
+      <c r="AA1" s="126" t="s">
         <v>344</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>346</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>338</v>
       </c>
@@ -8978,7 +9205,7 @@
         <v>95</v>
       </c>
       <c r="K2" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="L2" t="s">
         <v>79</v>
@@ -9022,17 +9249,20 @@
       <c r="Y2" t="s">
         <v>79</v>
       </c>
-      <c r="Z2" s="126" t="s">
+      <c r="Z2" t="s">
         <v>79</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AA2" s="126" t="s">
         <v>79</v>
       </c>
       <c r="AB2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -9064,12 +9294,12 @@
         <v>0</v>
       </c>
       <c r="K3" s="50">
-        <v>0</v>
+        <v>148630.95890589131</v>
       </c>
       <c r="L3" s="50">
         <v>0</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="50">
         <v>0</v>
       </c>
       <c r="N3">
@@ -9106,16 +9336,19 @@
         <v>0</v>
       </c>
       <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
         <v>10.092966734864383</v>
       </c>
-      <c r="Z3" s="126">
+      <c r="AA3" s="126">
         <v>159.61294596442238</v>
       </c>
-      <c r="AB3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -9147,12 +9380,12 @@
         <v>0</v>
       </c>
       <c r="K4" s="50">
-        <v>0</v>
+        <v>145478.15070756595</v>
       </c>
       <c r="L4" s="50">
         <v>0</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="50">
         <v>0</v>
       </c>
       <c r="N4">
@@ -9189,16 +9422,19 @@
         <v>0</v>
       </c>
       <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
         <v>10.037274812679371</v>
       </c>
-      <c r="Z4" s="126">
+      <c r="AA4" s="126">
         <v>159.01572660266299</v>
       </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -9230,12 +9466,12 @@
         <v>0</v>
       </c>
       <c r="K5" s="50">
-        <v>0</v>
+        <v>5282.7465061676921</v>
       </c>
       <c r="L5" s="50">
         <v>0</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="50">
         <v>0</v>
       </c>
       <c r="N5">
@@ -9272,16 +9508,19 @@
         <v>0</v>
       </c>
       <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
         <v>9.4476222834829759E-2</v>
       </c>
-      <c r="Z5" s="126">
+      <c r="AA5" s="126">
         <v>84.252817189850219</v>
       </c>
-      <c r="AB5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -9313,12 +9552,12 @@
         <v>0</v>
       </c>
       <c r="K6" s="50">
-        <v>0</v>
+        <v>120337.19982245468</v>
       </c>
       <c r="L6" s="50">
         <v>0</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="50">
         <v>0</v>
       </c>
       <c r="N6">
@@ -9355,16 +9594,19 @@
         <v>0</v>
       </c>
       <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
         <v>9.0114461776113988</v>
       </c>
-      <c r="Z6" s="126">
+      <c r="AA6" s="126">
         <v>70.123245507139814</v>
       </c>
-      <c r="AB6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -9396,12 +9638,12 @@
         <v>0</v>
       </c>
       <c r="K7" s="50">
-        <v>0</v>
+        <v>19858.204378943552</v>
       </c>
       <c r="L7" s="50">
         <v>0</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="50">
         <v>0</v>
       </c>
       <c r="N7">
@@ -9438,16 +9680,19 @@
         <v>0</v>
       </c>
       <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
         <v>0.93135241223314247</v>
       </c>
-      <c r="Z7" s="126">
+      <c r="AA7" s="126">
         <v>4.63966390567297</v>
       </c>
-      <c r="AB7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -9479,12 +9724,12 @@
         <v>0</v>
       </c>
       <c r="K8" s="50">
-        <v>0</v>
+        <v>9.5578960223641065</v>
       </c>
       <c r="L8" s="50">
         <v>0</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="50">
         <v>0</v>
       </c>
       <c r="N8">
@@ -9521,16 +9766,19 @@
         <v>0</v>
       </c>
       <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
         <v>1.8850254189575909E-4</v>
       </c>
-      <c r="Z8" s="126">
+      <c r="AA8" s="126">
         <v>7.9911248903944939E-4</v>
       </c>
-      <c r="AB8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -9562,17 +9810,17 @@
         <v>0</v>
       </c>
       <c r="K9" s="50">
-        <v>0</v>
+        <v>12.328628903057187</v>
       </c>
       <c r="L9" s="50">
         <v>0</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="50">
+        <v>0</v>
+      </c>
+      <c r="N9">
         <v>1</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
       <c r="O9">
         <v>0</v>
       </c>
@@ -9604,19 +9852,22 @@
         <v>0</v>
       </c>
       <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
         <v>1.3351720663121653E-3</v>
       </c>
-      <c r="Z9" s="126">
+      <c r="AA9" s="126">
         <v>1.4991020819976521E-3</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <v>1.5661402605072106E-3</v>
       </c>
-      <c r="AB9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -9648,20 +9899,20 @@
         <v>0</v>
       </c>
       <c r="K10" s="50">
-        <v>0</v>
+        <v>18.492428858048552</v>
       </c>
       <c r="L10" s="50">
         <v>0</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="50">
         <v>0</v>
       </c>
       <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
         <v>1</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
       <c r="P10">
         <v>0</v>
       </c>
@@ -9690,19 +9941,22 @@
         <v>0</v>
       </c>
       <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
         <v>1.458359822850299E-3</v>
       </c>
-      <c r="Z10" s="126">
+      <c r="AA10" s="126">
         <v>4.1850710755000908E-3</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>5.5321968067478938E-3</v>
       </c>
-      <c r="AB10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -9734,23 +9988,23 @@
         <v>0</v>
       </c>
       <c r="K11" s="50">
-        <v>0</v>
+        <v>23.607747661082556</v>
       </c>
       <c r="L11" s="50">
         <v>0</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="50">
         <v>0</v>
       </c>
       <c r="N11">
         <v>0</v>
       </c>
       <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
         <v>1</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
       <c r="Q11">
         <v>0</v>
       </c>
@@ -9776,19 +10030,22 @@
         <v>0</v>
       </c>
       <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
         <v>8.1362048922501589E-4</v>
       </c>
-      <c r="Z11" s="126">
+      <c r="AA11" s="126">
         <v>5.8889140492385424E-3</v>
       </c>
-      <c r="AA11">
+      <c r="AB11">
         <v>7.3649533909408496E-3</v>
       </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -9820,12 +10077,12 @@
         <v>0</v>
       </c>
       <c r="K12" s="50">
-        <v>0</v>
+        <v>0.96378103867189679</v>
       </c>
       <c r="L12" s="50">
         <v>0</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="50">
         <v>0</v>
       </c>
       <c r="N12">
@@ -9835,11 +10092,11 @@
         <v>0</v>
       </c>
       <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
         <v>1</v>
       </c>
-      <c r="Q12">
-        <v>0</v>
-      </c>
       <c r="R12">
         <v>0</v>
       </c>
@@ -9862,19 +10119,22 @@
         <v>0</v>
       </c>
       <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
         <v>4.0834205013456504E-5</v>
       </c>
-      <c r="Z12" s="126">
+      <c r="AA12" s="126">
         <v>2.4491257687576568E-3</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <v>6.7802056095251913E-4</v>
       </c>
-      <c r="AB12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -9906,12 +10166,12 @@
         <v>0</v>
       </c>
       <c r="K13" s="50">
-        <v>0</v>
+        <v>0.84020166567630694</v>
       </c>
       <c r="L13" s="50">
         <v>0</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="50">
         <v>0</v>
       </c>
       <c r="N13">
@@ -9924,11 +10184,11 @@
         <v>0</v>
       </c>
       <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
         <v>1</v>
       </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
       <c r="S13">
         <v>0</v>
       </c>
@@ -9948,19 +10208,22 @@
         <v>0</v>
       </c>
       <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
         <v>3.520397730589998E-5</v>
       </c>
-      <c r="Z13" s="126">
+      <c r="AA13" s="126">
         <v>3.8207677812154074E-4</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <v>5.3144359219302675E-4</v>
       </c>
-      <c r="AB13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -9992,12 +10255,12 @@
         <v>0</v>
       </c>
       <c r="K14" s="50">
-        <v>0</v>
+        <v>18.312368016828625</v>
       </c>
       <c r="L14" s="50">
         <v>0</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="50">
         <v>0</v>
       </c>
       <c r="N14">
@@ -10013,11 +10276,11 @@
         <v>0</v>
       </c>
       <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
         <v>1</v>
       </c>
-      <c r="S14">
-        <v>0</v>
-      </c>
       <c r="T14">
         <v>0</v>
       </c>
@@ -10034,19 +10297,22 @@
         <v>0</v>
       </c>
       <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
         <v>1.7762640197414279E-3</v>
       </c>
-      <c r="Z14" s="126">
+      <c r="AA14" s="126">
         <v>1.3876605774230375E-3</v>
       </c>
-      <c r="AA14">
+      <c r="AB14">
         <v>4.6796326638847349E-3</v>
       </c>
-      <c r="AB14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -10078,12 +10344,12 @@
         <v>0</v>
       </c>
       <c r="K15" s="50">
-        <v>0</v>
+        <v>0.11782516711423591</v>
       </c>
       <c r="L15" s="50">
         <v>0</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="50">
         <v>0</v>
       </c>
       <c r="N15">
@@ -10102,11 +10368,11 @@
         <v>0</v>
       </c>
       <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
         <v>1</v>
       </c>
-      <c r="T15">
-        <v>0</v>
-      </c>
       <c r="U15">
         <v>0</v>
       </c>
@@ -10120,19 +10386,22 @@
         <v>0</v>
       </c>
       <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
         <v>5.3094217795047773E-6</v>
       </c>
-      <c r="Z15" s="126">
+      <c r="AA15" s="126">
         <v>5.4894128620987762E-5</v>
       </c>
-      <c r="AA15">
+      <c r="AB15">
         <v>6.2195971551301605E-5</v>
       </c>
-      <c r="AB15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -10164,12 +10433,12 @@
         <v>0</v>
       </c>
       <c r="K16" s="50">
-        <v>0</v>
+        <v>0.27120930382192787</v>
       </c>
       <c r="L16" s="50">
         <v>0</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="50">
         <v>0</v>
       </c>
       <c r="N16">
@@ -10191,11 +10460,11 @@
         <v>0</v>
       </c>
       <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
         <v>1</v>
       </c>
-      <c r="U16">
-        <v>0</v>
-      </c>
       <c r="V16">
         <v>0</v>
       </c>
@@ -10206,19 +10475,22 @@
         <v>0</v>
       </c>
       <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
         <v>1.4374911737179876E-5</v>
       </c>
-      <c r="Z16" s="126">
+      <c r="AA16" s="126">
         <v>1.191254767832926E-4</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <v>1.589609941075944E-4</v>
       </c>
-      <c r="AB16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -10250,12 +10522,12 @@
         <v>0</v>
       </c>
       <c r="K17" s="50">
-        <v>0</v>
+        <v>143.92225199052672</v>
       </c>
       <c r="L17" s="50">
         <v>0</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="50">
         <v>0</v>
       </c>
       <c r="N17">
@@ -10280,11 +10552,11 @@
         <v>0</v>
       </c>
       <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
         <v>1</v>
       </c>
-      <c r="V17">
-        <v>0</v>
-      </c>
       <c r="W17">
         <v>0</v>
       </c>
@@ -10292,19 +10564,22 @@
         <v>0</v>
       </c>
       <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
         <v>5.4762278993310248E-3</v>
       </c>
-      <c r="Z17" s="126">
+      <c r="AA17" s="126">
         <v>2.6773045154859922E-2</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <v>2.0196219200983769E-2</v>
       </c>
-      <c r="AB17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -10336,12 +10611,12 @@
         <v>0</v>
       </c>
       <c r="K18" s="50">
-        <v>0</v>
+        <v>0.19004615754683868</v>
       </c>
       <c r="L18" s="50">
         <v>0</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="50">
         <v>0</v>
       </c>
       <c r="N18">
@@ -10369,28 +10644,31 @@
         <v>0</v>
       </c>
       <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
         <v>1</v>
       </c>
-      <c r="W18">
-        <v>0</v>
-      </c>
       <c r="X18">
         <v>0</v>
       </c>
       <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
         <v>1.2020606510860481E-5</v>
       </c>
-      <c r="Z18" s="126">
+      <c r="AA18" s="126">
         <v>1.3028316422886578E-4</v>
       </c>
-      <c r="AA18">
+      <c r="AB18">
         <v>1.5448196096900553E-4</v>
       </c>
-      <c r="AB18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AC18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -10422,12 +10700,12 @@
         <v>0</v>
       </c>
       <c r="K19" s="50">
-        <v>0</v>
+        <v>10270.907185152539</v>
       </c>
       <c r="L19" s="50">
         <v>0</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="50">
         <v>0</v>
       </c>
       <c r="N19">
@@ -10458,25 +10736,28 @@
         <v>0</v>
       </c>
       <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
         <v>1</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>-1</v>
       </c>
-      <c r="Y19">
+      <c r="Z19">
         <v>0.62984762096725244</v>
       </c>
-      <c r="Z19" s="126">
+      <c r="AA19" s="126">
         <v>8.6166537276591537</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <v>6.3624128058164002</v>
       </c>
-      <c r="AB19">
+      <c r="AC19">
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="57" t="s">
         <v>325</v>
       </c>
@@ -10486,9 +10767,9 @@
       <c r="E20" s="125"/>
       <c r="F20" s="125"/>
       <c r="G20" s="125"/>
-      <c r="Z20" s="126"/>
-    </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AA20" s="126"/>
+    </row>
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="94" t="s">
         <v>326</v>
       </c>
@@ -10520,17 +10801,17 @@
         <v>0</v>
       </c>
       <c r="K21" s="50">
-        <v>0</v>
+        <v>1.4166539330738113</v>
       </c>
       <c r="L21" s="50">
         <v>0</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="50">
+        <v>0</v>
+      </c>
+      <c r="N21">
         <v>1</v>
       </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
       <c r="O21">
         <v>0</v>
       </c>
@@ -10562,13 +10843,16 @@
         <v>0</v>
       </c>
       <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
         <v>7.5802039323866825E-6</v>
       </c>
-      <c r="Z21" s="126">
+      <c r="AA21" s="126">
         <v>5.1830773072089746E-5</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="94" t="s">
         <v>327</v>
       </c>
@@ -10600,20 +10884,20 @@
         <v>0</v>
       </c>
       <c r="K22" s="50">
-        <v>0</v>
+        <v>1.2297288565054236</v>
       </c>
       <c r="L22" s="50">
         <v>0</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="50">
         <v>0</v>
       </c>
       <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
         <v>1</v>
       </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
       <c r="P22">
         <v>0</v>
       </c>
@@ -10642,13 +10926,16 @@
         <v>0</v>
       </c>
       <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
         <v>2.8580049446178005E-5</v>
       </c>
-      <c r="Z22" s="126">
+      <c r="AA22" s="126">
         <v>2.0603336772959054E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="94" t="s">
         <v>328</v>
       </c>
@@ -10680,23 +10967,23 @@
         <v>0</v>
       </c>
       <c r="K23" s="50">
-        <v>0</v>
+        <v>1.570003471186205</v>
       </c>
       <c r="L23" s="50">
         <v>0</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="50">
         <v>0</v>
       </c>
       <c r="N23">
         <v>0</v>
       </c>
       <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
         <v>1</v>
       </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
       <c r="Q23">
         <v>0</v>
       </c>
@@ -10722,13 +11009,16 @@
         <v>0</v>
       </c>
       <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
         <v>4.9199020008530993E-5</v>
       </c>
-      <c r="Z23" s="126">
+      <c r="AA23" s="126">
         <v>2.8134101377039379E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="94" t="s">
         <v>329</v>
       </c>
@@ -10760,12 +11050,12 @@
         <v>0</v>
       </c>
       <c r="K24" s="50">
-        <v>0</v>
+        <v>0.25621937777363929</v>
       </c>
       <c r="L24" s="50">
         <v>0</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="50">
         <v>0</v>
       </c>
       <c r="N24">
@@ -10775,11 +11065,11 @@
         <v>0</v>
       </c>
       <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
         <v>1</v>
       </c>
-      <c r="Q24">
-        <v>0</v>
-      </c>
       <c r="R24">
         <v>0</v>
       </c>
@@ -10802,13 +11092,16 @@
         <v>0</v>
       </c>
       <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
         <v>2.2234737484796388E-6</v>
       </c>
-      <c r="Z24" s="126">
+      <c r="AA24" s="126">
         <v>6.9961764575117456E-6</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="94" t="s">
         <v>330</v>
       </c>
@@ -10840,12 +11133,12 @@
         <v>0</v>
       </c>
       <c r="K25" s="50">
-        <v>0</v>
+        <v>0.22030796358502358</v>
       </c>
       <c r="L25" s="50">
         <v>0</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="50">
         <v>0</v>
       </c>
       <c r="N25">
@@ -10858,11 +11151,11 @@
         <v>0</v>
       </c>
       <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
         <v>1</v>
       </c>
-      <c r="R25">
-        <v>0</v>
-      </c>
       <c r="S25">
         <v>0</v>
       </c>
@@ -10882,13 +11175,16 @@
         <v>0</v>
       </c>
       <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
         <v>1.8762312745581416E-6</v>
       </c>
-      <c r="Z25" s="126">
+      <c r="AA25" s="126">
         <v>5.9939614248582743E-6</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="94" t="s">
         <v>331</v>
       </c>
@@ -10920,12 +11216,12 @@
         <v>0</v>
       </c>
       <c r="K26" s="50">
-        <v>0</v>
+        <v>0.93145736364298237</v>
       </c>
       <c r="L26" s="50">
         <v>0</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="50">
         <v>0</v>
       </c>
       <c r="N26">
@@ -10941,11 +11237,11 @@
         <v>0</v>
       </c>
       <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
         <v>1</v>
       </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
       <c r="T26">
         <v>0</v>
       </c>
@@ -10962,13 +11258,16 @@
         <v>0</v>
       </c>
       <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
         <v>1.4049061779183859E-5</v>
       </c>
-      <c r="Z26" s="126">
+      <c r="AA26" s="126">
         <v>4.7494585709469088E-5</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="94" t="s">
         <v>332</v>
       </c>
@@ -11000,12 +11299,12 @@
         <v>0</v>
       </c>
       <c r="K27" s="50">
-        <v>0</v>
+        <v>1.7553469241045817E-2</v>
       </c>
       <c r="L27" s="50">
         <v>0</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="50">
         <v>0</v>
       </c>
       <c r="N27">
@@ -11024,11 +11323,11 @@
         <v>0</v>
       </c>
       <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
         <v>1</v>
       </c>
-      <c r="T27">
-        <v>0</v>
-      </c>
       <c r="U27">
         <v>0</v>
       </c>
@@ -11042,13 +11341,16 @@
         <v>0</v>
       </c>
       <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
         <v>2.3730644005080313E-7</v>
       </c>
-      <c r="Z27" s="126">
+      <c r="AA27" s="126">
         <v>5.2149778991018595E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="95" t="s">
         <v>333</v>
       </c>
@@ -11080,12 +11382,12 @@
         <v>0</v>
       </c>
       <c r="K28" s="50">
-        <v>0</v>
+        <v>2.7968317794105035E-2</v>
       </c>
       <c r="L28" s="50">
         <v>0</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="50">
         <v>0</v>
       </c>
       <c r="N28">
@@ -11107,11 +11409,11 @@
         <v>0</v>
       </c>
       <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
         <v>1</v>
       </c>
-      <c r="U28">
-        <v>0</v>
-      </c>
       <c r="V28">
         <v>0</v>
       </c>
@@ -11122,36 +11424,39 @@
         <v>0</v>
       </c>
       <c r="Y28">
+        <v>0</v>
+      </c>
+      <c r="Z28">
         <v>6.4012408493445377E-7</v>
       </c>
-      <c r="Z28" s="126">
+      <c r="AA28" s="126">
         <v>1.6882066883636638E-6</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="6"/>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
       <c r="B30" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="128" t="s">
+      <c r="C30" s="129" t="s">
         <v>334</v>
       </c>
-      <c r="D30" s="128"/>
-      <c r="E30" s="128"/>
+      <c r="D30" s="129"/>
+      <c r="E30" s="129"/>
       <c r="G30" s="17" t="s">
         <v>286</v>
       </c>
       <c r="H30" s="17"/>
-      <c r="Z30" t="s">
+      <c r="AA30" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -11164,8 +11469,9 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
       <c r="M32" s="5"/>
-    </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="5"/>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -11178,8 +11484,9 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
       <c r="M33" s="2"/>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -11192,8 +11499,9 @@
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="3"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -11206,8 +11514,9 @@
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="3"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -11220,8 +11529,9 @@
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="3"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -11234,8 +11544,9 @@
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="3"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -11248,8 +11559,9 @@
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="3"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -11262,8 +11574,9 @@
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="3"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -11276,8 +11589,9 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="3"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -11290,8 +11604,9 @@
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="3"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -11304,8 +11619,9 @@
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="3"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -11318,8 +11634,9 @@
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="3"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -11331,7 +11648,8 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="4"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11348,11 +11666,11 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:CE29"/>
+  <dimension ref="A1:CP29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="BL1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="CD2" sqref="CD2"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="CK19" sqref="CK19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11366,7 +11684,7 @@
     <col min="32" max="32" width="22.42578125" style="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" ht="64.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:94" ht="64.5" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="10" t="s">
         <v>266</v>
@@ -11605,17 +11923,50 @@
       <c r="CB1" t="s">
         <v>364</v>
       </c>
-      <c r="CC1" s="129" t="s">
+      <c r="CC1" s="128" t="s">
         <v>365</v>
       </c>
-      <c r="CD1" s="129" t="s">
+      <c r="CD1" s="128" t="s">
         <v>366</v>
       </c>
       <c r="CE1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF1" s="128" t="s">
+        <v>374</v>
+      </c>
+      <c r="CG1" s="128" t="s">
+        <v>371</v>
+      </c>
+      <c r="CH1" s="128" t="s">
+        <v>372</v>
+      </c>
+      <c r="CI1" s="128" t="s">
+        <v>373</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>368</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>369</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>375</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>376</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>377</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>338</v>
       </c>
@@ -11865,8 +12216,41 @@
       <c r="CE2" s="106" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CG2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CH2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CI2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CJ2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CK2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CL2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CM2" s="106" t="s">
+        <v>79</v>
+      </c>
+      <c r="CN2" s="106" t="s">
+        <v>110</v>
+      </c>
+      <c r="CO2" s="106" t="s">
+        <v>110</v>
+      </c>
+      <c r="CP2" s="106" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -12117,8 +12501,41 @@
       <c r="CE3">
         <v>0.56381800000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF3">
+        <v>0.36550917489225554</v>
+      </c>
+      <c r="CG3">
+        <v>1278.7519820492755</v>
+      </c>
+      <c r="CH3">
+        <v>126.19882293839159</v>
+      </c>
+      <c r="CI3">
+        <v>87.533244440424198</v>
+      </c>
+      <c r="CJ3">
+        <v>265.68525300521844</v>
+      </c>
+      <c r="CK3">
+        <v>112.51424973860428</v>
+      </c>
+      <c r="CL3">
+        <v>110.8118639322022</v>
+      </c>
+      <c r="CM3">
+        <v>198.64676190407542</v>
+      </c>
+      <c r="CN3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO3" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP3" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -12369,8 +12786,41 @@
       <c r="CE4">
         <v>0.46926200000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF4">
+        <v>0.28996126831884061</v>
+      </c>
+      <c r="CG4">
+        <v>1224.8589733034305</v>
+      </c>
+      <c r="CH4">
+        <v>120.2163356099561</v>
+      </c>
+      <c r="CI4">
+        <v>82.972785598695125</v>
+      </c>
+      <c r="CJ4">
+        <v>253.21323060996494</v>
+      </c>
+      <c r="CK4">
+        <v>17.204122267782704</v>
+      </c>
+      <c r="CL4">
+        <v>107.44231988182482</v>
+      </c>
+      <c r="CM4">
+        <v>193.09941239590157</v>
+      </c>
+      <c r="CN4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO4" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP4" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -12621,8 +13071,41 @@
       <c r="CE5">
         <v>0.160883</v>
       </c>
-    </row>
-    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF5">
+        <v>0.12854120723978857</v>
+      </c>
+      <c r="CG5">
+        <v>1125.6129414096276</v>
+      </c>
+      <c r="CH5">
+        <v>10.760549801926718</v>
+      </c>
+      <c r="CI5">
+        <v>29.13297279594817</v>
+      </c>
+      <c r="CJ5">
+        <v>40.009650656378795</v>
+      </c>
+      <c r="CK5">
+        <v>3.4766115890860837E-2</v>
+      </c>
+      <c r="CL5">
+        <v>11.618702094777317</v>
+      </c>
+      <c r="CM5">
+        <v>17.076988376901635</v>
+      </c>
+      <c r="CN5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO5" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP5" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -12873,8 +13356,41 @@
       <c r="CE6">
         <v>0.30352499999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF6">
+        <v>0.15757425250265861</v>
+      </c>
+      <c r="CG6">
+        <v>17.621666187300175</v>
+      </c>
+      <c r="CH6">
+        <v>64.727547223603551</v>
+      </c>
+      <c r="CI6">
+        <v>50.036880028751753</v>
+      </c>
+      <c r="CJ6">
+        <v>202.81076409394649</v>
+      </c>
+      <c r="CK6">
+        <v>14.958453386831092</v>
+      </c>
+      <c r="CL6">
+        <v>91.516171226200328</v>
+      </c>
+      <c r="CM6">
+        <v>169.11521182545442</v>
+      </c>
+      <c r="CN6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO6" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -13125,8 +13641,41 @@
       <c r="CE7">
         <v>4.8549999999999999E-3</v>
       </c>
-    </row>
-    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF7">
+        <v>3.8458085763934152E-3</v>
+      </c>
+      <c r="CG7">
+        <v>81.624365706502559</v>
+      </c>
+      <c r="CH7">
+        <v>44.728238584425839</v>
+      </c>
+      <c r="CI7">
+        <v>3.8029327739952028</v>
+      </c>
+      <c r="CJ7">
+        <v>10.392815859639667</v>
+      </c>
+      <c r="CK7">
+        <v>2.2109027650607489</v>
+      </c>
+      <c r="CL7">
+        <v>4.3074465608471844</v>
+      </c>
+      <c r="CM7">
+        <v>6.9072121935455124</v>
+      </c>
+      <c r="CN7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO7" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -13377,8 +13926,41 @@
       <c r="CE8">
         <v>2.34E-4</v>
       </c>
-    </row>
-    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF8">
+        <v>3.0530248815791281E-5</v>
+      </c>
+      <c r="CG8">
+        <v>0.25163755992739434</v>
+      </c>
+      <c r="CH8">
+        <v>9.3759544958936947E-3</v>
+      </c>
+      <c r="CI8">
+        <v>1.1427987301686452E-2</v>
+      </c>
+      <c r="CJ8">
+        <v>1.6116391261875276E-2</v>
+      </c>
+      <c r="CK8">
+        <v>9.4641038685311103E-5</v>
+      </c>
+      <c r="CL8">
+        <v>3.2994223318611234E-3</v>
+      </c>
+      <c r="CM8">
+        <v>5.6451275302559353E-3</v>
+      </c>
+      <c r="CN8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO8" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP8" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>48</v>
       </c>
@@ -13629,8 +14211,41 @@
       <c r="CE9" s="127">
         <v>4.6500000000000004E-6</v>
       </c>
-    </row>
-    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF9">
+        <v>2.6691689270569514E-6</v>
+      </c>
+      <c r="CG9">
+        <v>1.0625898581138974E-2</v>
+      </c>
+      <c r="CH9">
+        <v>1.9438336635204136E-3</v>
+      </c>
+      <c r="CI9">
+        <v>9.5091884528415141E-4</v>
+      </c>
+      <c r="CJ9">
+        <v>4.9094990479613305E-3</v>
+      </c>
+      <c r="CK9">
+        <v>2.3374762580479847E-4</v>
+      </c>
+      <c r="CL9">
+        <v>1.5661402605072106E-3</v>
+      </c>
+      <c r="CM9">
+        <v>2.8160601075936527E-3</v>
+      </c>
+      <c r="CN9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO9" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>49</v>
       </c>
@@ -13881,8 +14496,41 @@
       <c r="CE10" s="127">
         <v>1.7600000000000001E-5</v>
       </c>
-    </row>
-    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF10">
+        <v>9.5591172832866281E-6</v>
+      </c>
+      <c r="CG10">
+        <v>4.7344426448157735E-2</v>
+      </c>
+      <c r="CH10">
+        <v>1.0684624756801942E-2</v>
+      </c>
+      <c r="CI10">
+        <v>3.8712232201269735E-3</v>
+      </c>
+      <c r="CJ10">
+        <v>1.2193815603813246E-2</v>
+      </c>
+      <c r="CK10">
+        <v>1.1947011466289727E-3</v>
+      </c>
+      <c r="CL10">
+        <v>5.5321968067478938E-3</v>
+      </c>
+      <c r="CM10">
+        <v>9.7111092889849929E-3</v>
+      </c>
+      <c r="CN10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO10" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>50</v>
       </c>
@@ -14133,8 +14781,41 @@
       <c r="CE11" s="127">
         <v>2.9300000000000001E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF11">
+        <v>1.7317487340960441E-5</v>
+      </c>
+      <c r="CG11">
+        <v>9.9766479732465413E-2</v>
+      </c>
+      <c r="CH11">
+        <v>1.1044252611762412E-2</v>
+      </c>
+      <c r="CI11">
+        <v>2.6103933233382521E-2</v>
+      </c>
+      <c r="CJ11">
+        <v>1.3088118020022285E-2</v>
+      </c>
+      <c r="CK11">
+        <v>1.5686755363868124E-3</v>
+      </c>
+      <c r="CL11">
+        <v>7.3649533909408496E-3</v>
+      </c>
+      <c r="CM11">
+        <v>1.2930569792365848E-2</v>
+      </c>
+      <c r="CN11" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO11" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP11" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>51</v>
       </c>
@@ -14385,8 +15066,41 @@
       <c r="CE12" s="127">
         <v>3.6399999999999999E-6</v>
       </c>
-    </row>
-    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF12">
+        <v>2.6102000331794207E-6</v>
+      </c>
+      <c r="CG12">
+        <v>1.8328068085285788E-2</v>
+      </c>
+      <c r="CH12">
+        <v>4.2164737460304589E-3</v>
+      </c>
+      <c r="CI12">
+        <v>6.9545693450555454E-4</v>
+      </c>
+      <c r="CJ12">
+        <v>1.4589095422337696E-3</v>
+      </c>
+      <c r="CK12">
+        <v>8.533018687642064E-5</v>
+      </c>
+      <c r="CL12">
+        <v>6.7802056095251913E-4</v>
+      </c>
+      <c r="CM12">
+        <v>1.063491348880567E-3</v>
+      </c>
+      <c r="CN12" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO12" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP12" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>52</v>
       </c>
@@ -14637,8 +15351,41 @@
       <c r="CE13" s="127">
         <v>2.1600000000000001E-6</v>
       </c>
-    </row>
-    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF13">
+        <v>1.431890397134984E-6</v>
+      </c>
+      <c r="CG13">
+        <v>8.0328967275118436E-3</v>
+      </c>
+      <c r="CH13">
+        <v>8.1868321354229697E-4</v>
+      </c>
+      <c r="CI13">
+        <v>4.1378137391431141E-4</v>
+      </c>
+      <c r="CJ13">
+        <v>1.0168576839743771E-3</v>
+      </c>
+      <c r="CK13">
+        <v>7.6956843263033565E-5</v>
+      </c>
+      <c r="CL13">
+        <v>5.3144359219302675E-4</v>
+      </c>
+      <c r="CM13">
+        <v>8.5485325088438557E-4</v>
+      </c>
+      <c r="CN13" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO13" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP13" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>53</v>
       </c>
@@ -14889,8 +15636,41 @@
       <c r="CE14">
         <v>6.1324999999999998E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF14">
+        <v>1.5287602234490922E-5</v>
+      </c>
+      <c r="CG14">
+        <v>0.12629039698608727</v>
+      </c>
+      <c r="CH14">
+        <v>7.511526190629933E-3</v>
+      </c>
+      <c r="CI14">
+        <v>6.1402604767802202E-3</v>
+      </c>
+      <c r="CJ14">
+        <v>3.0619331573313643E-2</v>
+      </c>
+      <c r="CK14">
+        <v>1.641346511695967E-4</v>
+      </c>
+      <c r="CL14">
+        <v>4.6796326638847349E-3</v>
+      </c>
+      <c r="CM14">
+        <v>6.7826237856860143E-3</v>
+      </c>
+      <c r="CN14" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO14" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>54</v>
       </c>
@@ -15141,8 +15921,41 @@
       <c r="CE15" s="127">
         <v>1.5699999999999999E-7</v>
       </c>
-    </row>
-    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF15">
+        <v>7.5197981910804781E-8</v>
+      </c>
+      <c r="CG15">
+        <v>3.7961070133254608E-4</v>
+      </c>
+      <c r="CH15">
+        <v>6.118662096424913E-5</v>
+      </c>
+      <c r="CI15">
+        <v>4.1240169230845359E-5</v>
+      </c>
+      <c r="CJ15">
+        <v>1.0272973218978136E-4</v>
+      </c>
+      <c r="CK15">
+        <v>2.5783422327621937E-5</v>
+      </c>
+      <c r="CL15">
+        <v>6.2195971551301605E-5</v>
+      </c>
+      <c r="CM15">
+        <v>1.0652874477161482E-4</v>
+      </c>
+      <c r="CN15" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO15" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>55</v>
       </c>
@@ -15393,8 +16206,41 @@
       <c r="CE16" s="127">
         <v>6.1600000000000001E-7</v>
       </c>
-    </row>
-    <row r="17" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF16">
+        <v>3.6538217627142357E-7</v>
+      </c>
+      <c r="CG16">
+        <v>6.6205133776358227E-4</v>
+      </c>
+      <c r="CH16">
+        <v>1.3089373181002996E-4</v>
+      </c>
+      <c r="CI16">
+        <v>1.0351629331675042E-4</v>
+      </c>
+      <c r="CJ16">
+        <v>2.0829394365546249E-4</v>
+      </c>
+      <c r="CK16">
+        <v>2.7299660131106907E-5</v>
+      </c>
+      <c r="CL16">
+        <v>1.589609941075944E-4</v>
+      </c>
+      <c r="CM16">
+        <v>2.7484911916987408E-4</v>
+      </c>
+      <c r="CN16" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO16" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP16" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>56</v>
       </c>
@@ -15645,8 +16491,41 @@
       <c r="CE17" s="127">
         <v>8.1299999999999997E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF17">
+        <v>4.7791147055317132E-5</v>
+      </c>
+      <c r="CG17">
+        <v>0.19084049531698805</v>
+      </c>
+      <c r="CH17">
+        <v>1.9069747889327696E-2</v>
+      </c>
+      <c r="CI17">
+        <v>1.5000607598845347E-2</v>
+      </c>
+      <c r="CJ17">
+        <v>5.2474264130324251E-2</v>
+      </c>
+      <c r="CK17">
+        <v>3.2043305680193282E-3</v>
+      </c>
+      <c r="CL17">
+        <v>2.0196219200983769E-2</v>
+      </c>
+      <c r="CM17">
+        <v>3.6518829969822073E-2</v>
+      </c>
+      <c r="CN17" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO17" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP17" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>57</v>
       </c>
@@ -15897,8 +16776,41 @@
       <c r="CE18" s="127">
         <v>7.61E-7</v>
       </c>
-    </row>
-    <row r="19" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF18">
+        <v>4.5807200562031658E-7</v>
+      </c>
+      <c r="CG18">
+        <v>2.5638343795105385E-3</v>
+      </c>
+      <c r="CH18">
+        <v>5.2290508742300628E-4</v>
+      </c>
+      <c r="CI18">
+        <v>3.3711915727577973E-4</v>
+      </c>
+      <c r="CJ18">
+        <v>4.6923403382535925E-4</v>
+      </c>
+      <c r="CK18">
+        <v>2.8179590282616181E-5</v>
+      </c>
+      <c r="CL18">
+        <v>1.5448196096900553E-4</v>
+      </c>
+      <c r="CM18">
+        <v>2.7965297583711242E-4</v>
+      </c>
+      <c r="CN18" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO18" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>58</v>
       </c>
@@ -16149,8 +17061,41 @@
       <c r="CE19">
         <v>3.4513000000000002E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF19">
+        <v>2.2540237665439691E-2</v>
+      </c>
+      <c r="CG19">
+        <v>120.01963713376205</v>
+      </c>
+      <c r="CH19">
+        <v>8.6708238175555881</v>
+      </c>
+      <c r="CI19">
+        <v>6.3943752486573908</v>
+      </c>
+      <c r="CJ19">
+        <v>10.880109009531633</v>
+      </c>
+      <c r="CK19">
+        <v>-2.3087886543311078</v>
+      </c>
+      <c r="CL19">
+        <v>6.3624128058164002</v>
+      </c>
+      <c r="CM19">
+        <v>11.027823611486689</v>
+      </c>
+      <c r="CN19" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO19" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP19" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A20" s="94" t="s">
         <v>326</v>
       </c>
@@ -16401,8 +17346,41 @@
       <c r="CE20" s="127">
         <v>2.8099999999999999E-7</v>
       </c>
-    </row>
-    <row r="21" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF20">
+        <v>1.7901963056516892E-7</v>
+      </c>
+      <c r="CG20">
+        <v>7.7760045383131664E-4</v>
+      </c>
+      <c r="CH20">
+        <v>1.5654051881137926E-4</v>
+      </c>
+      <c r="CI20">
+        <v>5.1798395209010816E-5</v>
+      </c>
+      <c r="CJ20">
+        <v>1.4991638071334959E-4</v>
+      </c>
+      <c r="CK20">
+        <v>1.4117009921472009E-5</v>
+      </c>
+      <c r="CL20">
+        <v>1.2422426901355897E-4</v>
+      </c>
+      <c r="CM20">
+        <v>2.3478130550948399E-4</v>
+      </c>
+      <c r="CN20" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO20" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP20" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A21" s="94" t="s">
         <v>327</v>
       </c>
@@ -16653,8 +17631,41 @@
       <c r="CE21" s="127">
         <v>2.9500000000000001E-6</v>
       </c>
-    </row>
-    <row r="22" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF21">
+        <v>2.1385118764832846E-6</v>
+      </c>
+      <c r="CG21">
+        <v>1.2051438863717444E-2</v>
+      </c>
+      <c r="CH21">
+        <v>3.6480895206674136E-4</v>
+      </c>
+      <c r="CI21">
+        <v>4.5409676337714191E-4</v>
+      </c>
+      <c r="CJ21">
+        <v>7.5386616496120665E-4</v>
+      </c>
+      <c r="CK21">
+        <v>5.4287132681996822E-5</v>
+      </c>
+      <c r="CL21">
+        <v>3.4022742365625127E-4</v>
+      </c>
+      <c r="CM21">
+        <v>6.1286116874635155E-4</v>
+      </c>
+      <c r="CN21" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO21" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP21" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A22" s="94" t="s">
         <v>328</v>
       </c>
@@ -16905,8 +17916,41 @@
       <c r="CE22" s="127">
         <v>6.0100000000000001E-6</v>
       </c>
-    </row>
-    <row r="23" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF22">
+        <v>4.5382343409995544E-6</v>
+      </c>
+      <c r="CG22">
+        <v>2.8818144673219474E-2</v>
+      </c>
+      <c r="CH22">
+        <v>6.2611894234368437E-4</v>
+      </c>
+      <c r="CI22">
+        <v>9.3692296015765637E-4</v>
+      </c>
+      <c r="CJ22">
+        <v>1.2035052695230119E-3</v>
+      </c>
+      <c r="CK22">
+        <v>5.9218466568400222E-5</v>
+      </c>
+      <c r="CL22">
+        <v>5.3695919103006074E-4</v>
+      </c>
+      <c r="CM22">
+        <v>9.4554734028597619E-4</v>
+      </c>
+      <c r="CN22" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO22" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP22" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A23" s="94" t="s">
         <v>329</v>
       </c>
@@ -17157,8 +18201,41 @@
       <c r="CE23" s="127">
         <v>6.4099999999999998E-7</v>
       </c>
-    </row>
-    <row r="24" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF23">
+        <v>5.1181415742549008E-7</v>
+      </c>
+      <c r="CG23">
+        <v>3.0950633631833769E-3</v>
+      </c>
+      <c r="CH23">
+        <v>6.0536702990039917E-5</v>
+      </c>
+      <c r="CI23">
+        <v>8.7860573616982326E-5</v>
+      </c>
+      <c r="CJ23">
+        <v>6.84584302105892E-5</v>
+      </c>
+      <c r="CK23">
+        <v>1.6214902882341074E-6</v>
+      </c>
+      <c r="CL23">
+        <v>3.5071088029088972E-5</v>
+      </c>
+      <c r="CM23">
+        <v>6.0107320944489042E-5</v>
+      </c>
+      <c r="CN23" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO23" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A24" s="94" t="s">
         <v>330</v>
       </c>
@@ -17409,8 +18486,41 @@
       <c r="CE24" s="127">
         <v>5.3200000000000005E-7</v>
       </c>
-    </row>
-    <row r="25" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF24">
+        <v>4.2425595376950953E-7</v>
+      </c>
+      <c r="CG24">
+        <v>2.4125385375629981E-3</v>
+      </c>
+      <c r="CH24">
+        <v>5.0895229106867355E-5</v>
+      </c>
+      <c r="CI24">
+        <v>6.9973419938251018E-5</v>
+      </c>
+      <c r="CJ24">
+        <v>5.6767270865275495E-5</v>
+      </c>
+      <c r="CK24">
+        <v>1.132826554072982E-6</v>
+      </c>
+      <c r="CL24">
+        <v>3.0294426000665246E-5</v>
+      </c>
+      <c r="CM24">
+        <v>5.2121440525578443E-5</v>
+      </c>
+      <c r="CN24" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO24" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A25" s="94" t="s">
         <v>331</v>
       </c>
@@ -17661,8 +18771,41 @@
       <c r="CE25" s="127">
         <v>5.9200000000000001E-6</v>
       </c>
-    </row>
-    <row r="26" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF25">
+        <v>4.7242480331211372E-6</v>
+      </c>
+      <c r="CG25">
+        <v>3.7631870191036587E-2</v>
+      </c>
+      <c r="CH25">
+        <v>4.1455863831335208E-4</v>
+      </c>
+      <c r="CI25">
+        <v>9.8441460933476176E-4</v>
+      </c>
+      <c r="CJ25">
+        <v>6.1990859296870893E-4</v>
+      </c>
+      <c r="CK25">
+        <v>4.3573058347259474E-6</v>
+      </c>
+      <c r="CL25">
+        <v>2.252279876039111E-4</v>
+      </c>
+      <c r="CM25">
+        <v>3.6506234860552225E-4</v>
+      </c>
+      <c r="CN25" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO25" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A26" s="94" t="s">
         <v>332</v>
       </c>
@@ -17913,8 +19056,41 @@
       <c r="CE26" s="127">
         <v>2.4599999999999999E-8</v>
       </c>
-    </row>
-    <row r="27" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF26">
+        <v>1.9491098096921769E-8</v>
+      </c>
+      <c r="CG26">
+        <v>1.0679125522103036E-4</v>
+      </c>
+      <c r="CH26">
+        <v>3.969824278385659E-6</v>
+      </c>
+      <c r="CI26">
+        <v>3.3444954934160299E-6</v>
+      </c>
+      <c r="CJ26">
+        <v>3.767688526735234E-6</v>
+      </c>
+      <c r="CK26">
+        <v>1.4121435618797454E-7</v>
+      </c>
+      <c r="CL26">
+        <v>1.9446357626832362E-6</v>
+      </c>
+      <c r="CM26">
+        <v>3.3310773544400243E-6</v>
+      </c>
+      <c r="CN26" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO26" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A27" s="95" t="s">
         <v>333</v>
       </c>
@@ -18165,49 +19341,82 @@
       <c r="CE27" s="127">
         <v>1.3400000000000001E-7</v>
       </c>
-    </row>
-    <row r="28" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF27">
+        <v>1.0646107695121333E-7</v>
+      </c>
+      <c r="CG27">
+        <v>2.0367301853471361E-4</v>
+      </c>
+      <c r="CH27">
+        <v>1.1388907815843227E-5</v>
+      </c>
+      <c r="CI27">
+        <v>9.6955857953731394E-6</v>
+      </c>
+      <c r="CJ27">
+        <v>1.2961733623408748E-5</v>
+      </c>
+      <c r="CK27">
+        <v>2.2332519909467878E-7</v>
+      </c>
+      <c r="CL27">
+        <v>8.1755836463894652E-6</v>
+      </c>
+      <c r="CM27">
+        <v>1.4066006393739068E-5</v>
+      </c>
+      <c r="CN27" s="16">
+        <v>0</v>
+      </c>
+      <c r="CO27" s="16">
+        <v>0</v>
+      </c>
+      <c r="CP27" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:94" x14ac:dyDescent="0.25">
       <c r="AI28" s="91"/>
       <c r="AK28" s="91"/>
     </row>
-    <row r="29" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="128" t="s">
+      <c r="B29" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="128"/>
-      <c r="D29" s="128"/>
-      <c r="E29" s="128"/>
-      <c r="F29" s="128"/>
-      <c r="G29" s="128"/>
-      <c r="H29" s="128"/>
-      <c r="I29" s="128"/>
-      <c r="J29" s="128"/>
-      <c r="K29" s="128"/>
-      <c r="L29" s="128"/>
-      <c r="M29" s="128"/>
-      <c r="N29" s="128"/>
-      <c r="O29" s="128"/>
-      <c r="P29" s="128"/>
-      <c r="Q29" s="128"/>
-      <c r="R29" s="128"/>
-      <c r="S29" s="128"/>
-      <c r="T29" s="128"/>
-      <c r="U29" s="128"/>
-      <c r="V29" s="128"/>
-      <c r="W29" s="128"/>
-      <c r="X29" s="128"/>
-      <c r="Y29" s="128"/>
-      <c r="Z29" s="128"/>
-      <c r="AA29" s="128"/>
-      <c r="AB29" s="128"/>
-      <c r="AC29" s="128"/>
-      <c r="AD29" s="128"/>
-      <c r="AE29" s="128"/>
-      <c r="AF29" s="128"/>
-      <c r="AG29" s="128"/>
+      <c r="C29" s="129"/>
+      <c r="D29" s="129"/>
+      <c r="E29" s="129"/>
+      <c r="F29" s="129"/>
+      <c r="G29" s="129"/>
+      <c r="H29" s="129"/>
+      <c r="I29" s="129"/>
+      <c r="J29" s="129"/>
+      <c r="K29" s="129"/>
+      <c r="L29" s="129"/>
+      <c r="M29" s="129"/>
+      <c r="N29" s="129"/>
+      <c r="O29" s="129"/>
+      <c r="P29" s="129"/>
+      <c r="Q29" s="129"/>
+      <c r="R29" s="129"/>
+      <c r="S29" s="129"/>
+      <c r="T29" s="129"/>
+      <c r="U29" s="129"/>
+      <c r="V29" s="129"/>
+      <c r="W29" s="129"/>
+      <c r="X29" s="129"/>
+      <c r="Y29" s="129"/>
+      <c r="Z29" s="129"/>
+      <c r="AA29" s="129"/>
+      <c r="AB29" s="129"/>
+      <c r="AC29" s="129"/>
+      <c r="AD29" s="129"/>
+      <c r="AE29" s="129"/>
+      <c r="AF29" s="129"/>
+      <c r="AG29" s="129"/>
       <c r="AI29" s="91" t="s">
         <v>337</v>
       </c>
@@ -18310,10 +19519,19 @@
       <c r="BQ29" t="s">
         <v>298</v>
       </c>
+      <c r="CF29" s="129" t="s">
+        <v>370</v>
+      </c>
+      <c r="CG29" s="129"/>
+      <c r="CH29" s="129"/>
+      <c r="CI29" s="129"/>
+      <c r="CJ29" s="129"/>
+      <c r="CK29" s="129"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B29:AG29"/>
+    <mergeCell ref="CF29:CK29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -19376,22 +20594,22 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="C23" s="128"/>
-      <c r="D23" s="128"/>
-      <c r="E23" s="128"/>
-      <c r="F23" s="128"/>
-      <c r="G23" s="128"/>
-      <c r="H23" s="128"/>
-      <c r="I23" s="128"/>
-      <c r="J23" s="128"/>
-      <c r="K23" s="128"/>
-      <c r="L23" s="128"/>
-      <c r="M23" s="128"/>
-      <c r="N23" s="128"/>
-      <c r="O23" s="128"/>
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="129"/>
+      <c r="F23" s="129"/>
+      <c r="G23" s="129"/>
+      <c r="H23" s="129"/>
+      <c r="I23" s="129"/>
+      <c r="J23" s="129"/>
+      <c r="K23" s="129"/>
+      <c r="L23" s="129"/>
+      <c r="M23" s="129"/>
+      <c r="N23" s="129"/>
+      <c r="O23" s="129"/>
       <c r="P23" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
1.updated the background GREET2023 file; 2. added algae HTL 2023 file
</commit_message>
<xml_diff>
--- a/Lookup table_prototyping_greet2022.xlsx
+++ b/Lookup table_prototyping_greet2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oul\Box\Temp\interactive SCSA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\oulongwen\projects\Interactive-SCSA_Dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF48C9C-403C-486B-847C-CB8480DCA96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD30194F-A955-41C2-808C-5BA9968CD8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="745" activeTab="1" xr2:uid="{A628798E-305C-4246-A75A-2AB1A71444C5}"/>
   </bookViews>
   <sheets>
     <sheet name="End use test" sheetId="14" r:id="rId1"/>
@@ -342,7 +342,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="382">
   <si>
     <t>Diesel</t>
   </si>
@@ -1482,6 +1482,12 @@
   </si>
   <si>
     <t>Boiler</t>
+  </si>
+  <si>
+    <t>Pyrolysis_IDL!CX261</t>
+  </si>
+  <si>
+    <t>Sum(Algae!Z591:AA591)</t>
   </si>
 </sst>
 </file>
@@ -1800,7 +1806,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2057,6 +2063,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2377,9 +2384,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2417,7 +2424,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2523,7 +2530,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2665,7 +2672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2798,8 +2805,8 @@
   </sheetPr>
   <dimension ref="A1:BB23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="BB3" sqref="BB3"/>
     </sheetView>
   </sheetViews>
@@ -8310,10 +8317,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9058,6 +9065,14 @@
       <c r="G28">
         <f t="shared" si="7"/>
         <v>1.8571109385136862E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="130" t="s">
+        <v>380</v>
+      </c>
+      <c r="C30" s="130" t="s">
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>